<commit_message>
Aded grand jury indicator
</commit_message>
<xml_diff>
--- a/schemas/ChargeFiling_iepd/artifacts/ChargeFiling_MappingSpreadsheet.xlsx
+++ b/schemas/ChargeFiling_iepd/artifacts/ChargeFiling_MappingSpreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JamesCabral\git\JTMP-Data-Exchange-Specs\schemas\ChargeFiling_iepd\artifacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47152B53-5272-4B67-BEA4-829BF8C9B9E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F52C61D3-B739-42DE-A29F-42FD5B75EEE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" tabRatio="781" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13335" yWindow="-21225" windowWidth="22755" windowHeight="19890" tabRatio="781" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="9" state="hidden" r:id="rId1"/>
@@ -149,7 +149,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="834" uniqueCount="486">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="836" uniqueCount="488">
   <si>
     <t>Definition</t>
   </si>
@@ -2304,6 +2304,12 @@
   </si>
   <si>
     <t>A unique identifier of a law, rule, or ordinance within a jurisdiction that a person is accused of violating.</t>
+  </si>
+  <si>
+    <t>Grand Jury Indicator</t>
+  </si>
+  <si>
+    <t>True if this filing is a grand jury indictment</t>
   </si>
 </sst>
 </file>
@@ -2663,7 +2669,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2887,13 +2893,7 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2975,258 +2975,6 @@
   </cellStyles>
   <dxfs count="124">
     <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -3912,6 +3660,258 @@
         <color theme="0"/>
         <name val="Calibri"/>
         <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -4134,43 +4134,43 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{733D753A-1A77-494A-B62C-0EC743EEA49A}" name="Table10" displayName="Table10" ref="A1:N2" totalsRowShown="0" headerRowDxfId="56" dataDxfId="55" tableBorderDxfId="54" headerRowCellStyle="Accent2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{733D753A-1A77-494A-B62C-0EC743EEA49A}" name="Table10" displayName="Table10" ref="A1:N2" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28" tableBorderDxfId="27" headerRowCellStyle="Accent2">
   <autoFilter ref="A1:N2" xr:uid="{E1E5EF99-DFA3-4734-B0F5-3FD6CA399E33}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{E1238927-B089-4D9E-8088-75D3EC35BFBA}" name="Source_x000a_NS Prefix" dataDxfId="53"/>
-    <tableColumn id="2" xr3:uid="{9410951A-EE35-4F3C-8F36-8BEE201CF8AF}" name="URI" dataDxfId="52"/>
-    <tableColumn id="3" xr3:uid="{2B517D23-941B-4B3E-A7DD-F7786E3924D5}" name="Definition" dataDxfId="51"/>
-    <tableColumn id="4" xr3:uid="{7DD55007-8311-4C82-A5D2-EBEDF474C65D}" name="Mapping_x000a_Code" dataDxfId="50"/>
-    <tableColumn id="5" xr3:uid="{0E949C96-18B4-4EB9-95F2-53DB84718832}" name="Description" dataDxfId="49"/>
-    <tableColumn id="6" xr3:uid="{E124F618-8325-4FF3-8BF4-E24907425ADE}" name="Notes" dataDxfId="48"/>
-    <tableColumn id="7" xr3:uid="{86983FC7-E843-4CB8-B776-1ACA5758C454}" name="Target_x000a_NS Prefix" dataDxfId="47"/>
-    <tableColumn id="8" xr3:uid="{F92DB840-CE8A-4128-8BB8-B8742F926D09}" name="Style" dataDxfId="46"/>
-    <tableColumn id="9" xr3:uid="{9202EAB5-4BBC-4DFA-8B29-56D32F2F95E2}" name="URI " dataDxfId="45"/>
-    <tableColumn id="10" xr3:uid="{BE82DF52-562E-40A7-B97A-C4017DCE324F}" name="Definition " dataDxfId="44"/>
-    <tableColumn id="11" xr3:uid="{834B3B3E-609B-4AA7-A013-2F95C8CA6ED1}" name="NDR Target" dataDxfId="43"/>
-    <tableColumn id="12" xr3:uid="{9C74517B-484A-41A5-B478-1107D7B7563E}" name="File Name" dataDxfId="42"/>
-    <tableColumn id="13" xr3:uid="{00E1E65A-D173-41FF-8A1D-F764DB3C85EB}" name="Relative Path" dataDxfId="41"/>
-    <tableColumn id="14" xr3:uid="{1A319080-CB5B-4F50-8EF6-DA7F3E87061A}" name="Draft Version" dataDxfId="40"/>
+    <tableColumn id="1" xr3:uid="{E1238927-B089-4D9E-8088-75D3EC35BFBA}" name="Source_x000a_NS Prefix" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{9410951A-EE35-4F3C-8F36-8BEE201CF8AF}" name="URI" dataDxfId="25"/>
+    <tableColumn id="3" xr3:uid="{2B517D23-941B-4B3E-A7DD-F7786E3924D5}" name="Definition" dataDxfId="24"/>
+    <tableColumn id="4" xr3:uid="{7DD55007-8311-4C82-A5D2-EBEDF474C65D}" name="Mapping_x000a_Code" dataDxfId="23"/>
+    <tableColumn id="5" xr3:uid="{0E949C96-18B4-4EB9-95F2-53DB84718832}" name="Description" dataDxfId="22"/>
+    <tableColumn id="6" xr3:uid="{E124F618-8325-4FF3-8BF4-E24907425ADE}" name="Notes" dataDxfId="21"/>
+    <tableColumn id="7" xr3:uid="{86983FC7-E843-4CB8-B776-1ACA5758C454}" name="Target_x000a_NS Prefix" dataDxfId="20"/>
+    <tableColumn id="8" xr3:uid="{F92DB840-CE8A-4128-8BB8-B8742F926D09}" name="Style" dataDxfId="19"/>
+    <tableColumn id="9" xr3:uid="{9202EAB5-4BBC-4DFA-8B29-56D32F2F95E2}" name="URI " dataDxfId="18"/>
+    <tableColumn id="10" xr3:uid="{BE82DF52-562E-40A7-B97A-C4017DCE324F}" name="Definition " dataDxfId="17"/>
+    <tableColumn id="11" xr3:uid="{834B3B3E-609B-4AA7-A013-2F95C8CA6ED1}" name="NDR Target" dataDxfId="16"/>
+    <tableColumn id="12" xr3:uid="{9C74517B-484A-41A5-B478-1107D7B7563E}" name="File Name" dataDxfId="15"/>
+    <tableColumn id="13" xr3:uid="{00E1E65A-D173-41FF-8A1D-F764DB3C85EB}" name="Relative Path" dataDxfId="14"/>
+    <tableColumn id="14" xr3:uid="{1A319080-CB5B-4F50-8EF6-DA7F3E87061A}" name="Draft Version" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{6A256153-0806-4BEE-936A-A12F0A0B7383}" name="Table11" displayName="Table11" ref="A1:K2" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38" headerRowCellStyle="Accent2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{6A256153-0806-4BEE-936A-A12F0A0B7383}" name="Table11" displayName="Table11" ref="A1:K2" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11" headerRowCellStyle="Accent2">
   <autoFilter ref="A1:K2" xr:uid="{79E81683-51FB-4FF9-9289-31DDA054DB7A}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{B23F336D-16B9-4C95-BE96-F5283EAE0F3C}" name="Source_x000a_NS Prefix" dataDxfId="37"/>
-    <tableColumn id="2" xr3:uid="{0D056408-CA8F-4336-AED7-3818011F9385}" name="Term" dataDxfId="36"/>
-    <tableColumn id="3" xr3:uid="{90A93FC4-10F0-4295-AC5C-E2A951CBA7BC}" name="Literal" dataDxfId="35"/>
-    <tableColumn id="4" xr3:uid="{A1AC1DB1-AA7D-48B2-9765-4E5BA52F23DE}" name="Definition" dataDxfId="34"/>
-    <tableColumn id="5" xr3:uid="{BD7B43BD-647B-4803-8F9F-0147C7FD23A4}" name="Mapping_x000a_Code" dataDxfId="33"/>
-    <tableColumn id="6" xr3:uid="{72609C76-FA3F-40C0-B5FF-60D4974FFD61}" name="Description" dataDxfId="32"/>
-    <tableColumn id="7" xr3:uid="{479204AB-0608-4CE8-8D22-F418523DDDA2}" name="Notes" dataDxfId="31"/>
-    <tableColumn id="8" xr3:uid="{2C9C9513-0007-44E3-8DFD-9FDD58431071}" name="Target_x000a_NS Prefix" dataDxfId="30"/>
-    <tableColumn id="9" xr3:uid="{1442C4F6-90A1-4765-A362-538E7A781367}" name="Term " dataDxfId="29"/>
-    <tableColumn id="10" xr3:uid="{92198433-569D-43D9-9243-453965C7540B}" name="Literal " dataDxfId="28"/>
-    <tableColumn id="11" xr3:uid="{38E45C62-D7D7-487A-BB8B-582528BBD31D}" name="Definition " dataDxfId="27"/>
+    <tableColumn id="1" xr3:uid="{B23F336D-16B9-4C95-BE96-F5283EAE0F3C}" name="Source_x000a_NS Prefix" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{0D056408-CA8F-4336-AED7-3818011F9385}" name="Term" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{90A93FC4-10F0-4295-AC5C-E2A951CBA7BC}" name="Literal" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{A1AC1DB1-AA7D-48B2-9765-4E5BA52F23DE}" name="Definition" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{BD7B43BD-647B-4803-8F9F-0147C7FD23A4}" name="Mapping_x000a_Code" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{72609C76-FA3F-40C0-B5FF-60D4974FFD61}" name="Description" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{479204AB-0608-4CE8-8D22-F418523DDDA2}" name="Notes" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{2C9C9513-0007-44E3-8DFD-9FDD58431071}" name="Target_x000a_NS Prefix" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{1442C4F6-90A1-4765-A362-538E7A781367}" name="Term " dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{92198433-569D-43D9-9243-453965C7540B}" name="Literal " dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{38E45C62-D7D7-487A-BB8B-582528BBD31D}" name="Definition " dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -4218,105 +4218,105 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table3" displayName="Table3" ref="A1:Y55" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25" headerRowCellStyle="Accent2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table3" displayName="Table3" ref="A1:Y55" totalsRowShown="0" headerRowDxfId="106" dataDxfId="105" headerRowCellStyle="Accent2">
   <autoFilter ref="A1:Y55" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="25">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Source_x000a_NS Prefix" dataDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Property Name" dataDxfId="23"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="Data Type" dataDxfId="22"/>
-    <tableColumn id="18" xr3:uid="{683B832A-0F1B-48CA-AA01-7512CABFD6B2}" name="Definition" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="Cardinality" dataDxfId="0"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="Mapping_x000a_Code" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="Description" dataDxfId="21"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0500-000007000000}" name="Notes" dataDxfId="20"/>
-    <tableColumn id="24" xr3:uid="{B256BE0E-1B95-49D2-BF5B-AD5320663854}" name="EDM Class" dataDxfId="19"/>
-    <tableColumn id="23" xr3:uid="{C5C0958E-E98B-4096-B70E-A6517F49A64D}" name="EDM Attribute" dataDxfId="18"/>
-    <tableColumn id="14" xr3:uid="{70B266EE-E89C-4B0F-ACFB-6BBC1BBE7978}" name="EDM Type" dataDxfId="17"/>
-    <tableColumn id="26" xr3:uid="{B613C991-CC70-4831-83C3-97449E0A59FB}" name="EDM Definition" dataDxfId="16"/>
-    <tableColumn id="27" xr3:uid="{9FF11716-702A-419A-91F2-858D4D3B16EE}" name="EDM Cardinality" dataDxfId="15"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0500-000008000000}" name="Target_x000a_NS Prefix" dataDxfId="14"/>
-    <tableColumn id="20" xr3:uid="{8CFFA3EE-5D28-4D5E-86E0-9F9851A3E676}" name="NIEM XPath" dataDxfId="13"/>
-    <tableColumn id="25" xr3:uid="{161AA4D8-B799-4722-BAB9-DA7BA3B360DA}" name="NIEM Type" dataDxfId="12"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0500-000009000000}" name="NIEM Property Name " dataDxfId="11"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0500-00000A000000}" name="NIEM Qualified Data Type" dataDxfId="10"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0500-00000B000000}" name="NIEM Definition " dataDxfId="9"/>
-    <tableColumn id="19" xr3:uid="{C2DBDA77-E9BC-497B-A1D8-611484B019B5}" name="Cardinality2" dataDxfId="8"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0500-00000C000000}" name="NIEM Qualified Substitution Group" dataDxfId="7"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0500-00000D000000}" name="Style_x000a_default=element" dataDxfId="6"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0500-00000F000000}" name="Keywords" dataDxfId="5"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0500-000010000000}" name="Example Content" dataDxfId="4"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0500-000011000000}" name="Usage Info" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Source_x000a_NS Prefix" dataDxfId="104"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Property Name" dataDxfId="103"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="Data Type" dataDxfId="102"/>
+    <tableColumn id="18" xr3:uid="{683B832A-0F1B-48CA-AA01-7512CABFD6B2}" name="Definition" dataDxfId="101"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="Cardinality" dataDxfId="100"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="Mapping_x000a_Code" dataDxfId="99"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="Description" dataDxfId="98"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0500-000007000000}" name="Notes" dataDxfId="97"/>
+    <tableColumn id="24" xr3:uid="{B256BE0E-1B95-49D2-BF5B-AD5320663854}" name="EDM Class" dataDxfId="96"/>
+    <tableColumn id="23" xr3:uid="{C5C0958E-E98B-4096-B70E-A6517F49A64D}" name="EDM Attribute" dataDxfId="95"/>
+    <tableColumn id="14" xr3:uid="{70B266EE-E89C-4B0F-ACFB-6BBC1BBE7978}" name="EDM Type" dataDxfId="94"/>
+    <tableColumn id="26" xr3:uid="{B613C991-CC70-4831-83C3-97449E0A59FB}" name="EDM Definition" dataDxfId="93"/>
+    <tableColumn id="27" xr3:uid="{9FF11716-702A-419A-91F2-858D4D3B16EE}" name="EDM Cardinality" dataDxfId="92"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0500-000008000000}" name="Target_x000a_NS Prefix" dataDxfId="91"/>
+    <tableColumn id="20" xr3:uid="{8CFFA3EE-5D28-4D5E-86E0-9F9851A3E676}" name="NIEM XPath" dataDxfId="90"/>
+    <tableColumn id="25" xr3:uid="{161AA4D8-B799-4722-BAB9-DA7BA3B360DA}" name="NIEM Type" dataDxfId="89"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0500-000009000000}" name="NIEM Property Name " dataDxfId="88"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0500-00000A000000}" name="NIEM Qualified Data Type" dataDxfId="87"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0500-00000B000000}" name="NIEM Definition " dataDxfId="86"/>
+    <tableColumn id="19" xr3:uid="{C2DBDA77-E9BC-497B-A1D8-611484B019B5}" name="Cardinality2" dataDxfId="85"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0500-00000C000000}" name="NIEM Qualified Substitution Group" dataDxfId="84"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0500-00000D000000}" name="Style_x000a_default=element" dataDxfId="83"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0500-00000F000000}" name="Keywords" dataDxfId="82"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0500-000010000000}" name="Example Content" dataDxfId="81"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0500-000011000000}" name="Usage Info" dataDxfId="80"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{8578AF98-37D1-469F-9DF8-407CA14E272E}" name="Table7" displayName="Table7" ref="A1:N2" insertRow="1" totalsRowShown="0" headerRowDxfId="106" dataDxfId="105" headerRowCellStyle="Accent2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{8578AF98-37D1-469F-9DF8-407CA14E272E}" name="Table7" displayName="Table7" ref="A1:N2" insertRow="1" totalsRowShown="0" headerRowDxfId="79" dataDxfId="78" headerRowCellStyle="Accent2">
   <autoFilter ref="A1:N2" xr:uid="{C7C77A82-0E27-43B2-B802-78C571058434}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{2DA18095-6134-4F51-B45C-1FD29868E9D3}" name="Source_x000a_NS Prefix" dataDxfId="104"/>
-    <tableColumn id="2" xr3:uid="{BB7222D3-DF23-4FB4-AACC-7074C8351301}" name="Type Name" dataDxfId="103"/>
-    <tableColumn id="3" xr3:uid="{3AFA1B4A-1B7D-4408-95C4-5D276F6AFCE8}" name="Parent / Base Type" dataDxfId="102"/>
-    <tableColumn id="4" xr3:uid="{DA420D7E-BF45-4DFA-A327-6F5816081658}" name="Definition" dataDxfId="101"/>
-    <tableColumn id="5" xr3:uid="{F0EC8E3B-3924-4431-8523-4FE53C5BC2F9}" name="Mapping_x000a_Code" dataDxfId="100"/>
-    <tableColumn id="6" xr3:uid="{529DD89A-D9F2-4643-B653-535C5D5260B2}" name="Description" dataDxfId="99"/>
-    <tableColumn id="7" xr3:uid="{6A865D88-3AC4-4546-981B-9A5A7EB8F351}" name="Notes" dataDxfId="98"/>
-    <tableColumn id="8" xr3:uid="{FF25761D-56AD-4BA0-8910-6C18CBA6D0CD}" name="Target_x000a_NS Prefix" dataDxfId="97"/>
-    <tableColumn id="9" xr3:uid="{B5902010-EF7D-4FA2-B2B6-B491046CA96D}" name="Type Name " dataDxfId="96"/>
-    <tableColumn id="10" xr3:uid="{422CF2D7-F9C5-4193-9DD3-943BF799ABB8}" name="Qualified Parent / Base Type " dataDxfId="95"/>
-    <tableColumn id="11" xr3:uid="{E69F557F-28BC-41CA-B77C-8F0F1781F3F8}" name="Definition " dataDxfId="94"/>
-    <tableColumn id="12" xr3:uid="{33FAD9D1-2E3A-4DD0-99A3-80B7DC1320DF}" name="Style _x000a_default=object" dataDxfId="93"/>
-    <tableColumn id="13" xr3:uid="{A3613263-4395-41B2-9149-1319C9DE1572}" name="Qualified Union Member Types_x000a_comma-separated list" dataDxfId="92"/>
-    <tableColumn id="14" xr3:uid="{DA9EC388-28FD-4FFC-9EB0-04AF1B5F2EBE}" name="Qualified Metadata Applies to Types_x000a_comma-separated list" dataDxfId="91"/>
+    <tableColumn id="1" xr3:uid="{2DA18095-6134-4F51-B45C-1FD29868E9D3}" name="Source_x000a_NS Prefix" dataDxfId="77"/>
+    <tableColumn id="2" xr3:uid="{BB7222D3-DF23-4FB4-AACC-7074C8351301}" name="Type Name" dataDxfId="76"/>
+    <tableColumn id="3" xr3:uid="{3AFA1B4A-1B7D-4408-95C4-5D276F6AFCE8}" name="Parent / Base Type" dataDxfId="75"/>
+    <tableColumn id="4" xr3:uid="{DA420D7E-BF45-4DFA-A327-6F5816081658}" name="Definition" dataDxfId="74"/>
+    <tableColumn id="5" xr3:uid="{F0EC8E3B-3924-4431-8523-4FE53C5BC2F9}" name="Mapping_x000a_Code" dataDxfId="73"/>
+    <tableColumn id="6" xr3:uid="{529DD89A-D9F2-4643-B653-535C5D5260B2}" name="Description" dataDxfId="72"/>
+    <tableColumn id="7" xr3:uid="{6A865D88-3AC4-4546-981B-9A5A7EB8F351}" name="Notes" dataDxfId="71"/>
+    <tableColumn id="8" xr3:uid="{FF25761D-56AD-4BA0-8910-6C18CBA6D0CD}" name="Target_x000a_NS Prefix" dataDxfId="70"/>
+    <tableColumn id="9" xr3:uid="{B5902010-EF7D-4FA2-B2B6-B491046CA96D}" name="Type Name " dataDxfId="69"/>
+    <tableColumn id="10" xr3:uid="{422CF2D7-F9C5-4193-9DD3-943BF799ABB8}" name="Qualified Parent / Base Type " dataDxfId="68"/>
+    <tableColumn id="11" xr3:uid="{E69F557F-28BC-41CA-B77C-8F0F1781F3F8}" name="Definition " dataDxfId="67"/>
+    <tableColumn id="12" xr3:uid="{33FAD9D1-2E3A-4DD0-99A3-80B7DC1320DF}" name="Style _x000a_default=object" dataDxfId="66"/>
+    <tableColumn id="13" xr3:uid="{A3613263-4395-41B2-9149-1319C9DE1572}" name="Qualified Union Member Types_x000a_comma-separated list" dataDxfId="65"/>
+    <tableColumn id="14" xr3:uid="{DA9EC388-28FD-4FFC-9EB0-04AF1B5F2EBE}" name="Qualified Metadata Applies to Types_x000a_comma-separated list" dataDxfId="64"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="Table8" displayName="Table8" ref="A1:Q2" insertRow="1" totalsRowShown="0" headerRowDxfId="90" dataDxfId="89">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="Table8" displayName="Table8" ref="A1:Q2" insertRow="1" totalsRowShown="0" headerRowDxfId="63" dataDxfId="62">
   <autoFilter ref="A1:Q2" xr:uid="{00000000-0009-0000-0100-000008000000}"/>
   <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="Source_x000a_Type NS" dataDxfId="88"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="Type Name" dataDxfId="87"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0600-000003000000}" name="Property NS" dataDxfId="86"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0600-000004000000}" name="Property Name" dataDxfId="85"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0600-000005000000}" name="Min" dataDxfId="84"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0600-000006000000}" name="Max" dataDxfId="83"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0600-000007000000}" name="Mapping_x000a_Code" dataDxfId="82"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0600-000008000000}" name="Description" dataDxfId="81"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0600-000009000000}" name="Notes" dataDxfId="80"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0600-00000A000000}" name="Target_x000a_Type NS" dataDxfId="79"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0600-00000B000000}" name="Type Name " dataDxfId="78"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0600-00000C000000}" name="Property NS " dataDxfId="77"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0600-00000D000000}" name="Property Name " dataDxfId="76"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0600-00000E000000}" name="Min_x000a_(default=0)" dataDxfId="75"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0600-00000F000000}" name="Max (default_x000a_=unbounded)" dataDxfId="74"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0600-000010000000}" name="Definition_x000a_For an external property in an adapter type" dataDxfId="73"/>
-    <tableColumn id="17" xr3:uid="{78D268D1-27FA-4E25-9781-8F942EC05BA0}" name="Sequence" dataDxfId="72"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="Source_x000a_Type NS" dataDxfId="61"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="Type Name" dataDxfId="60"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0600-000003000000}" name="Property NS" dataDxfId="59"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0600-000004000000}" name="Property Name" dataDxfId="58"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0600-000005000000}" name="Min" dataDxfId="57"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0600-000006000000}" name="Max" dataDxfId="56"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0600-000007000000}" name="Mapping_x000a_Code" dataDxfId="55"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0600-000008000000}" name="Description" dataDxfId="54"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0600-000009000000}" name="Notes" dataDxfId="53"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0600-00000A000000}" name="Target_x000a_Type NS" dataDxfId="52"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0600-00000B000000}" name="Type Name " dataDxfId="51"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0600-00000C000000}" name="Property NS " dataDxfId="50"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0600-00000D000000}" name="Property Name " dataDxfId="49"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0600-00000E000000}" name="Min_x000a_(default=0)" dataDxfId="48"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0600-00000F000000}" name="Max (default_x000a_=unbounded)" dataDxfId="47"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0600-000010000000}" name="Definition_x000a_For an external property in an adapter type" dataDxfId="46"/>
+    <tableColumn id="17" xr3:uid="{78D268D1-27FA-4E25-9781-8F942EC05BA0}" name="Sequence" dataDxfId="45"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="Table13" displayName="Table13" ref="A1:M2" totalsRowShown="0" headerRowDxfId="71" dataDxfId="70" headerRowCellStyle="Accent2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="Table13" displayName="Table13" ref="A1:M2" totalsRowShown="0" headerRowDxfId="44" dataDxfId="43" headerRowCellStyle="Accent2">
   <autoFilter ref="A1:M2" xr:uid="{00000000-0009-0000-0100-00000D000000}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="Source_x000a_NS Prefix" dataDxfId="69"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0700-000002000000}" name="Type Name" dataDxfId="68"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0700-000003000000}" name="Value" dataDxfId="67"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0700-000004000000}" name="Definition" dataDxfId="66"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0700-000005000000}" name="Style_x000a_default=enumeration" dataDxfId="65"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0700-000006000000}" name="Mapping_x000a_Code" dataDxfId="64"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0700-000007000000}" name="Description" dataDxfId="63"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0700-000008000000}" name="Notes" dataDxfId="62"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0700-000009000000}" name="Target_x000a_NS Prefix" dataDxfId="61"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0700-00000A000000}" name="Type Name " dataDxfId="60"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0700-00000B000000}" name="Value " dataDxfId="59"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0700-00000C000000}" name="Definition " dataDxfId="58"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0700-00000D000000}" name="Style_x000a_default=enumeration " dataDxfId="57"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="Source_x000a_NS Prefix" dataDxfId="42"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0700-000002000000}" name="Type Name" dataDxfId="41"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0700-000003000000}" name="Value" dataDxfId="40"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0700-000004000000}" name="Definition" dataDxfId="39"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0700-000005000000}" name="Style_x000a_default=enumeration" dataDxfId="38"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0700-000006000000}" name="Mapping_x000a_Code" dataDxfId="37"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0700-000007000000}" name="Description" dataDxfId="36"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0700-000008000000}" name="Notes" dataDxfId="35"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0700-000009000000}" name="Target_x000a_NS Prefix" dataDxfId="34"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0700-00000A000000}" name="Type Name " dataDxfId="33"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0700-00000B000000}" name="Value " dataDxfId="32"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0700-00000C000000}" name="Definition " dataDxfId="31"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0700-00000D000000}" name="Style_x000a_default=enumeration " dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -6871,13 +6871,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:AA56"/>
+  <dimension ref="A1:AA55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J33" sqref="J33"/>
+      <selection pane="bottomRight" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -6885,7 +6885,7 @@
     <col min="1" max="1" width="11.6640625" style="2" hidden="1" customWidth="1"/>
     <col min="2" max="2" width="16.59765625" style="2" customWidth="1"/>
     <col min="3" max="4" width="7.265625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="17.19921875" style="86" customWidth="1"/>
+    <col min="5" max="5" width="17.19921875" style="84" customWidth="1"/>
     <col min="6" max="6" width="4.9296875" style="2" hidden="1" customWidth="1"/>
     <col min="7" max="8" width="22.6640625" style="2" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="8.796875" style="2" customWidth="1"/>
@@ -6920,7 +6920,7 @@
       <c r="D1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="84" t="s">
+      <c r="E1" s="83" t="s">
         <v>448</v>
       </c>
       <c r="F1" s="9" t="s">
@@ -6988,2098 +6988,1108 @@
       </c>
     </row>
     <row r="2" spans="1:27" ht="99.75" x14ac:dyDescent="0.45">
-      <c r="B2" s="83" t="s">
+      <c r="B2" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="C2" s="83" t="s">
+      <c r="C2" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="D2" s="83"/>
-      <c r="E2" s="85">
+      <c r="E2" s="84">
         <v>1</v>
       </c>
-      <c r="F2" s="83"/>
-      <c r="G2" s="83"/>
-      <c r="H2" s="83"/>
-      <c r="I2" s="83" t="s">
+      <c r="I2" s="2" t="s">
         <v>364</v>
       </c>
-      <c r="J2" s="83" t="s">
+      <c r="J2" s="2" t="s">
         <v>358</v>
       </c>
-      <c r="K2" s="83" t="s">
+      <c r="K2" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="L2" s="83" t="s">
+      <c r="L2" s="2" t="s">
         <v>368</v>
       </c>
-      <c r="M2" s="83" t="s">
+      <c r="M2" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="N2" s="83"/>
-      <c r="O2" s="83"/>
-      <c r="P2" s="83"/>
-      <c r="Q2" s="83" t="s">
+      <c r="Q2" s="2" t="s">
         <v>369</v>
       </c>
-      <c r="R2" s="83" t="s">
+      <c r="R2" s="2" t="s">
         <v>468</v>
       </c>
-      <c r="S2" s="83"/>
-      <c r="T2" s="83"/>
-      <c r="U2" s="83"/>
-      <c r="V2" s="83"/>
-      <c r="W2" s="83"/>
-      <c r="X2" s="83"/>
-      <c r="Y2" s="83"/>
-      <c r="Z2" s="83"/>
-      <c r="AA2" s="83"/>
+      <c r="U2" s="2"/>
     </row>
     <row r="3" spans="1:27" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A3" s="83"/>
-      <c r="B3" s="83" t="s">
+      <c r="B3" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="C3" s="83" t="s">
+      <c r="C3" s="2" t="s">
         <v>406</v>
       </c>
-      <c r="D3" s="83" t="s">
+      <c r="D3" s="2" t="s">
         <v>423</v>
       </c>
-      <c r="E3" s="85" t="s">
+      <c r="E3" s="84" t="s">
         <v>366</v>
       </c>
-      <c r="F3" s="83"/>
-      <c r="G3" s="83"/>
-      <c r="H3" s="83"/>
       <c r="I3" s="82"/>
       <c r="J3" s="82"/>
       <c r="K3" s="82"/>
       <c r="L3" s="82"/>
       <c r="M3" s="82"/>
-      <c r="N3" s="83"/>
-      <c r="O3" s="83"/>
-      <c r="P3" s="83"/>
-      <c r="Q3" s="83"/>
-      <c r="R3" s="83"/>
-      <c r="S3" s="83"/>
-      <c r="T3" s="83"/>
-      <c r="U3" s="83"/>
-      <c r="V3" s="83"/>
-      <c r="W3" s="83"/>
-      <c r="X3" s="83"/>
-      <c r="Y3" s="83"/>
-      <c r="Z3" s="83"/>
-      <c r="AA3" s="83"/>
+      <c r="U3" s="2"/>
     </row>
     <row r="4" spans="1:27" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A4" s="83" t="s">
+      <c r="A4" s="2" t="s">
         <v>420</v>
       </c>
-      <c r="B4" s="83" t="s">
+      <c r="B4" s="2" t="s">
         <v>421</v>
       </c>
-      <c r="C4" s="83" t="s">
+      <c r="C4" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="D4" s="83" t="s">
+      <c r="D4" s="2" t="s">
         <v>423</v>
       </c>
-      <c r="E4" s="85" t="s">
+      <c r="E4" s="84" t="s">
         <v>366</v>
       </c>
-      <c r="F4" s="83"/>
-      <c r="G4" s="83"/>
-      <c r="H4" s="83"/>
       <c r="I4" s="82"/>
       <c r="J4" s="82"/>
       <c r="K4" s="82"/>
       <c r="L4" s="82"/>
       <c r="M4" s="82"/>
-      <c r="N4" s="83"/>
-      <c r="O4" s="83"/>
-      <c r="P4" s="83"/>
-      <c r="Q4" s="83"/>
-      <c r="R4" s="83"/>
-      <c r="S4" s="83"/>
-      <c r="T4" s="83"/>
-      <c r="U4" s="83"/>
-      <c r="V4" s="83"/>
-      <c r="W4" s="83"/>
-      <c r="X4" s="83"/>
-      <c r="Y4" s="83"/>
-      <c r="Z4" s="83"/>
-      <c r="AA4" s="83"/>
+      <c r="U4" s="2"/>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A5" s="83"/>
-      <c r="B5" s="83" t="s">
+      <c r="B5" s="2" t="s">
         <v>422</v>
       </c>
-      <c r="C5" s="83" t="s">
+      <c r="C5" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="D5" s="83" t="s">
+      <c r="D5" s="2" t="s">
         <v>423</v>
       </c>
-      <c r="E5" s="85" t="s">
+      <c r="E5" s="84" t="s">
         <v>366</v>
       </c>
-      <c r="F5" s="83"/>
-      <c r="G5" s="83"/>
-      <c r="H5" s="83"/>
       <c r="I5" s="82"/>
       <c r="J5" s="82"/>
       <c r="K5" s="82"/>
       <c r="L5" s="82"/>
       <c r="M5" s="82"/>
-      <c r="N5" s="83"/>
-      <c r="O5" s="83"/>
-      <c r="P5" s="83"/>
-      <c r="Q5" s="83"/>
-      <c r="R5" s="83"/>
-      <c r="S5" s="83"/>
-      <c r="T5" s="83"/>
-      <c r="U5" s="83"/>
-      <c r="V5" s="83"/>
-      <c r="W5" s="83"/>
-      <c r="X5" s="83"/>
-      <c r="Y5" s="83"/>
-      <c r="Z5" s="83"/>
-      <c r="AA5" s="83"/>
+      <c r="U5" s="2"/>
     </row>
     <row r="6" spans="1:27" ht="128.25" x14ac:dyDescent="0.45">
-      <c r="A6" s="83"/>
-      <c r="B6" s="83" t="s">
+      <c r="B6" s="2" t="s">
         <v>424</v>
       </c>
-      <c r="C6" s="83" t="s">
+      <c r="C6" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="D6" s="83"/>
-      <c r="E6" s="85">
+      <c r="E6" s="84">
         <v>1</v>
       </c>
-      <c r="F6" s="83"/>
-      <c r="G6" s="83"/>
-      <c r="H6" s="83"/>
-      <c r="I6" s="83" t="s">
+      <c r="I6" s="2" t="s">
         <v>365</v>
       </c>
-      <c r="J6" s="83" t="s">
+      <c r="J6" s="2" t="s">
         <v>469</v>
       </c>
-      <c r="K6" s="83" t="s">
+      <c r="K6" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="L6" s="83" t="s">
+      <c r="L6" s="2" t="s">
         <v>372</v>
       </c>
-      <c r="M6" s="83" t="s">
+      <c r="M6" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="N6" s="83"/>
-      <c r="O6" s="83"/>
-      <c r="P6" s="83"/>
-      <c r="Q6" s="83" t="s">
+      <c r="Q6" s="2" t="s">
         <v>375</v>
       </c>
-      <c r="R6" s="83" t="s">
+      <c r="R6" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="S6" s="83"/>
-      <c r="T6" s="83"/>
-      <c r="U6" s="83"/>
-      <c r="V6" s="83"/>
-      <c r="W6" s="83"/>
-      <c r="X6" s="83"/>
-      <c r="Y6" s="83"/>
-      <c r="Z6" s="83"/>
-      <c r="AA6" s="83"/>
+      <c r="U6" s="2"/>
     </row>
     <row r="7" spans="1:27" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B7" s="83" t="s">
+      <c r="B7" s="2" t="s">
         <v>409</v>
       </c>
-      <c r="C7" s="83" t="s">
+      <c r="C7" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="D7" s="83"/>
-      <c r="E7" s="85">
+      <c r="E7" s="84">
         <v>1</v>
       </c>
-      <c r="F7" s="83"/>
-      <c r="G7" s="83"/>
-      <c r="H7" s="83"/>
       <c r="I7" s="82"/>
       <c r="J7" s="82"/>
       <c r="K7" s="82"/>
       <c r="L7" s="82"/>
       <c r="M7" s="82"/>
-      <c r="N7" s="83"/>
-      <c r="O7" s="83"/>
-      <c r="P7" s="83"/>
-      <c r="Q7" s="83"/>
-      <c r="R7" s="83"/>
-      <c r="S7" s="83"/>
-      <c r="T7" s="83"/>
-      <c r="U7" s="83"/>
-      <c r="V7" s="83"/>
-      <c r="W7" s="83"/>
-      <c r="X7" s="83"/>
-      <c r="Y7" s="83"/>
-      <c r="Z7" s="83"/>
-      <c r="AA7" s="83"/>
+      <c r="U7" s="2"/>
     </row>
     <row r="8" spans="1:27" ht="57" x14ac:dyDescent="0.45">
-      <c r="B8" s="83" t="s">
+      <c r="B8" s="2" t="s">
         <v>410</v>
       </c>
-      <c r="C8" s="83" t="s">
+      <c r="C8" s="2" t="s">
         <v>406</v>
       </c>
-      <c r="D8" s="83" t="s">
+      <c r="D8" s="2" t="s">
         <v>411</v>
       </c>
-      <c r="E8" s="85" t="s">
+      <c r="E8" s="84" t="s">
         <v>366</v>
       </c>
-      <c r="F8" s="83"/>
-      <c r="G8" s="83"/>
-      <c r="H8" s="83"/>
       <c r="I8" s="82"/>
       <c r="J8" s="82"/>
       <c r="K8" s="82"/>
       <c r="L8" s="82"/>
       <c r="M8" s="82"/>
-      <c r="N8" s="83"/>
-      <c r="O8" s="83"/>
-      <c r="P8" s="83"/>
-      <c r="Q8" s="83"/>
-      <c r="R8" s="83"/>
-      <c r="S8" s="83"/>
-      <c r="T8" s="83"/>
-      <c r="U8" s="83"/>
-      <c r="V8" s="83"/>
-      <c r="W8" s="83"/>
-      <c r="X8" s="83"/>
-      <c r="Y8" s="83"/>
-      <c r="Z8" s="83"/>
-      <c r="AA8" s="83"/>
+      <c r="U8" s="2"/>
     </row>
     <row r="9" spans="1:27" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="B9" s="83" t="s">
+      <c r="B9" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="C9" s="83" t="s">
+      <c r="C9" s="2" t="s">
         <v>406</v>
       </c>
-      <c r="D9" s="83" t="s">
+      <c r="D9" s="2" t="s">
         <v>413</v>
       </c>
-      <c r="E9" s="85" t="s">
+      <c r="E9" s="84" t="s">
         <v>366</v>
       </c>
-      <c r="F9" s="83"/>
-      <c r="G9" s="83"/>
-      <c r="H9" s="83"/>
       <c r="I9" s="82"/>
       <c r="J9" s="82"/>
       <c r="K9" s="82"/>
       <c r="L9" s="82"/>
       <c r="M9" s="82"/>
-      <c r="N9" s="83"/>
-      <c r="O9" s="83"/>
-      <c r="P9" s="83"/>
-      <c r="Q9" s="83"/>
-      <c r="R9" s="83"/>
-      <c r="S9" s="83"/>
-      <c r="T9" s="83"/>
-      <c r="U9" s="83"/>
-      <c r="V9" s="83"/>
-      <c r="W9" s="83"/>
-      <c r="X9" s="83"/>
-      <c r="Y9" s="83"/>
-      <c r="Z9" s="83"/>
-      <c r="AA9" s="83"/>
+      <c r="U9" s="2"/>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="B10" s="83" t="s">
+      <c r="B10" s="2" t="s">
         <v>414</v>
       </c>
-      <c r="C10" s="83" t="s">
+      <c r="C10" s="2" t="s">
         <v>406</v>
       </c>
-      <c r="D10" s="83"/>
-      <c r="E10" s="85" t="s">
+      <c r="E10" s="84" t="s">
         <v>366</v>
       </c>
-      <c r="F10" s="83"/>
-      <c r="G10" s="83"/>
-      <c r="H10" s="83"/>
       <c r="I10" s="82"/>
       <c r="J10" s="82"/>
       <c r="K10" s="82"/>
       <c r="L10" s="82"/>
       <c r="M10" s="82"/>
-      <c r="N10" s="83"/>
-      <c r="O10" s="83"/>
-      <c r="P10" s="83"/>
-      <c r="Q10" s="83"/>
-      <c r="R10" s="83"/>
-      <c r="S10" s="83"/>
-      <c r="T10" s="83"/>
-      <c r="U10" s="83"/>
-      <c r="V10" s="83"/>
-      <c r="W10" s="83"/>
-      <c r="X10" s="83"/>
-      <c r="Y10" s="83"/>
-      <c r="Z10" s="83"/>
-      <c r="AA10" s="83"/>
+      <c r="U10" s="2"/>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A11" s="83" t="s">
+      <c r="A11" s="2" t="s">
         <v>418</v>
       </c>
-      <c r="B11" s="83" t="s">
+      <c r="B11" s="2" t="s">
         <v>418</v>
       </c>
-      <c r="C11" s="83" t="s">
+      <c r="C11" s="2" t="s">
         <v>406</v>
       </c>
-      <c r="D11" s="83"/>
-      <c r="E11" s="85" t="s">
+      <c r="E11" s="84" t="s">
         <v>366</v>
       </c>
-      <c r="F11" s="83"/>
-      <c r="G11" s="83"/>
-      <c r="H11" s="83"/>
-      <c r="I11" s="83"/>
-      <c r="J11" s="83"/>
-      <c r="K11" s="83"/>
-      <c r="L11" s="83"/>
-      <c r="M11" s="83"/>
-      <c r="N11" s="83"/>
-      <c r="O11" s="83"/>
-      <c r="P11" s="83"/>
-      <c r="Q11" s="83"/>
-      <c r="R11" s="83"/>
-      <c r="S11" s="83"/>
-      <c r="T11" s="83"/>
-      <c r="U11" s="83"/>
-      <c r="V11" s="83"/>
-      <c r="W11" s="83"/>
-      <c r="X11" s="83"/>
-      <c r="Y11" s="83"/>
-      <c r="Z11" s="83"/>
-      <c r="AA11" s="83"/>
+      <c r="U11" s="2"/>
     </row>
     <row r="12" spans="1:27" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B12" s="83" t="s">
+      <c r="B12" s="2" t="s">
         <v>415</v>
       </c>
-      <c r="C12" s="83" t="s">
+      <c r="C12" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="D12" s="83"/>
-      <c r="E12" s="85">
+      <c r="E12" s="84">
         <v>1</v>
       </c>
-      <c r="F12" s="83"/>
-      <c r="G12" s="83"/>
-      <c r="H12" s="83"/>
-      <c r="I12" s="83" t="s">
+      <c r="I12" s="2" t="s">
         <v>357</v>
       </c>
-      <c r="J12" s="83" t="s">
+      <c r="J12" s="2" t="s">
         <v>458</v>
       </c>
-      <c r="K12" s="83" t="s">
+      <c r="K12" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="L12" s="83" t="s">
+      <c r="L12" s="2" t="s">
         <v>452</v>
       </c>
-      <c r="M12" s="83" t="s">
+      <c r="M12" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="N12" s="83"/>
-      <c r="O12" s="83"/>
-      <c r="P12" s="83"/>
-      <c r="Q12" s="83" t="s">
+      <c r="Q12" s="2" t="s">
         <v>453</v>
       </c>
-      <c r="R12" s="83" t="s">
+      <c r="R12" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="S12" s="83"/>
-      <c r="T12" s="83"/>
-      <c r="U12" s="83"/>
-      <c r="V12" s="83"/>
-      <c r="W12" s="83"/>
-      <c r="X12" s="83"/>
-      <c r="Y12" s="83"/>
-      <c r="Z12" s="83"/>
-      <c r="AA12" s="83"/>
+      <c r="U12" s="2"/>
     </row>
     <row r="13" spans="1:27" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B13" s="83" t="s">
+      <c r="B13" s="2" t="s">
         <v>416</v>
       </c>
-      <c r="C13" s="83" t="s">
+      <c r="C13" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="D13" s="83"/>
-      <c r="E13" s="85">
+      <c r="E13" s="84">
         <v>1</v>
       </c>
-      <c r="F13" s="83"/>
-      <c r="G13" s="83"/>
-      <c r="H13" s="83"/>
-      <c r="I13" s="83" t="s">
+      <c r="I13" s="2" t="s">
         <v>357</v>
       </c>
-      <c r="J13" s="83" t="s">
+      <c r="J13" s="2" t="s">
         <v>459</v>
       </c>
-      <c r="K13" s="83" t="s">
+      <c r="K13" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="L13" s="83" t="s">
+      <c r="L13" s="2" t="s">
         <v>450</v>
       </c>
-      <c r="M13" s="83" t="s">
+      <c r="M13" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="N13" s="83"/>
-      <c r="O13" s="83"/>
-      <c r="P13" s="83"/>
-      <c r="Q13" s="83" t="s">
+      <c r="Q13" s="2" t="s">
         <v>451</v>
       </c>
-      <c r="R13" s="83" t="s">
+      <c r="R13" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="S13" s="83"/>
-      <c r="T13" s="83"/>
-      <c r="U13" s="83"/>
-      <c r="V13" s="83"/>
-      <c r="W13" s="83"/>
-      <c r="X13" s="83"/>
-      <c r="Y13" s="83"/>
-      <c r="Z13" s="83"/>
-      <c r="AA13" s="83"/>
+      <c r="U13" s="2"/>
     </row>
     <row r="14" spans="1:27" ht="57" x14ac:dyDescent="0.45">
-      <c r="B14" s="83" t="s">
+      <c r="B14" s="2" t="s">
         <v>417</v>
       </c>
-      <c r="C14" s="83" t="s">
+      <c r="C14" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="D14" s="83"/>
-      <c r="E14" s="85" t="s">
+      <c r="E14" s="84" t="s">
         <v>366</v>
       </c>
-      <c r="F14" s="83"/>
-      <c r="G14" s="83"/>
-      <c r="H14" s="83"/>
-      <c r="I14" s="83" t="s">
+      <c r="I14" s="2" t="s">
         <v>357</v>
       </c>
-      <c r="J14" s="83" t="s">
+      <c r="J14" s="2" t="s">
         <v>460</v>
       </c>
-      <c r="K14" s="83" t="s">
+      <c r="K14" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="L14" s="83" t="s">
+      <c r="L14" s="2" t="s">
         <v>454</v>
       </c>
-      <c r="M14" s="83" t="s">
+      <c r="M14" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="N14" s="83"/>
-      <c r="O14" s="83"/>
-      <c r="P14" s="83"/>
-      <c r="Q14" s="83" t="s">
+      <c r="Q14" s="2" t="s">
         <v>455</v>
       </c>
-      <c r="R14" s="83" t="s">
+      <c r="R14" s="2" t="s">
         <v>454</v>
       </c>
-      <c r="S14" s="83"/>
-      <c r="T14" s="83"/>
-      <c r="U14" s="83"/>
-      <c r="V14" s="83"/>
-      <c r="W14" s="83"/>
-      <c r="X14" s="83"/>
-      <c r="Y14" s="83"/>
-      <c r="Z14" s="83"/>
-      <c r="AA14" s="83"/>
+      <c r="U14" s="2"/>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="B15" s="83" t="s">
+      <c r="B15" s="2" t="s">
         <v>428</v>
       </c>
-      <c r="C15" s="83" t="s">
+      <c r="C15" s="2" t="s">
         <v>429</v>
       </c>
-      <c r="D15" s="83"/>
-      <c r="E15" s="85">
+      <c r="E15" s="84">
         <v>1</v>
       </c>
-      <c r="F15" s="83"/>
-      <c r="G15" s="83"/>
-      <c r="H15" s="83"/>
-      <c r="I15" s="83"/>
-      <c r="J15" s="83"/>
-      <c r="K15" s="83"/>
-      <c r="L15" s="83"/>
-      <c r="M15" s="83"/>
-      <c r="N15" s="83"/>
-      <c r="O15" s="83"/>
-      <c r="P15" s="83"/>
-      <c r="Q15" s="83"/>
-      <c r="R15" s="83"/>
-      <c r="S15" s="83"/>
-      <c r="T15" s="83"/>
-      <c r="U15" s="83"/>
-      <c r="V15" s="83"/>
-      <c r="W15" s="83"/>
-      <c r="X15" s="83"/>
-      <c r="Y15" s="83"/>
-      <c r="Z15" s="83"/>
-      <c r="AA15" s="83"/>
+      <c r="U15" s="2"/>
     </row>
     <row r="16" spans="1:27" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B16" s="83" t="s">
+      <c r="B16" s="2" t="s">
         <v>427</v>
       </c>
-      <c r="C16" s="83" t="s">
+      <c r="C16" s="2" t="s">
         <v>396</v>
       </c>
-      <c r="D16" s="83"/>
-      <c r="E16" s="85">
+      <c r="E16" s="84">
         <v>1</v>
       </c>
-      <c r="F16" s="83"/>
-      <c r="G16" s="83"/>
-      <c r="H16" s="83"/>
-      <c r="I16" s="83" t="s">
+      <c r="I16" s="2" t="s">
         <v>456</v>
       </c>
-      <c r="J16" s="83" t="s">
+      <c r="J16" s="2" t="s">
         <v>359</v>
       </c>
-      <c r="K16" s="83" t="s">
+      <c r="K16" s="2" t="s">
         <v>396</v>
       </c>
-      <c r="L16" s="83" t="s">
+      <c r="L16" s="2" t="s">
         <v>380</v>
       </c>
-      <c r="M16" s="83" t="s">
+      <c r="M16" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="N16" s="83"/>
-      <c r="O16" s="83"/>
-      <c r="P16" s="83"/>
-      <c r="Q16" s="83" t="s">
+      <c r="Q16" s="2" t="s">
         <v>381</v>
       </c>
-      <c r="R16" s="83" t="s">
+      <c r="R16" s="2" t="s">
         <v>382</v>
       </c>
-      <c r="S16" s="83"/>
-      <c r="T16" s="83"/>
-      <c r="U16" s="83"/>
-      <c r="V16" s="83"/>
-      <c r="W16" s="83"/>
-      <c r="X16" s="83"/>
-      <c r="Y16" s="83"/>
-      <c r="Z16" s="83"/>
-      <c r="AA16" s="83"/>
-    </row>
-    <row r="17" spans="1:27" ht="57" x14ac:dyDescent="0.45">
-      <c r="B17" s="83" t="s">
+      <c r="U16" s="2"/>
+    </row>
+    <row r="17" spans="2:21" ht="57" x14ac:dyDescent="0.45">
+      <c r="B17" s="2" t="s">
         <v>426</v>
       </c>
-      <c r="C17" s="83" t="s">
+      <c r="C17" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="D17" s="83" t="s">
+      <c r="D17" s="2" t="s">
         <v>425</v>
       </c>
-      <c r="E17" s="85" t="s">
+      <c r="E17" s="84" t="s">
         <v>366</v>
       </c>
-      <c r="F17" s="83"/>
-      <c r="G17" s="83"/>
-      <c r="H17" s="83"/>
-      <c r="I17" s="83" t="s">
+      <c r="I17" s="2" t="s">
         <v>457</v>
       </c>
-      <c r="J17" s="83" t="s">
+      <c r="J17" s="2" t="s">
         <v>361</v>
       </c>
-      <c r="K17" s="83" t="s">
+      <c r="K17" s="2" t="s">
         <v>397</v>
       </c>
-      <c r="L17" s="83" t="s">
+      <c r="L17" s="2" t="s">
         <v>376</v>
       </c>
-      <c r="M17" s="83" t="s">
+      <c r="M17" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="N17" s="83"/>
-      <c r="O17" s="83"/>
-      <c r="P17" s="83"/>
-      <c r="Q17" s="83" t="s">
+      <c r="Q17" s="2" t="s">
         <v>377</v>
       </c>
-      <c r="R17" s="83" t="s">
+      <c r="R17" s="2" t="s">
         <v>367</v>
       </c>
-      <c r="S17" s="83"/>
-      <c r="T17" s="83"/>
-      <c r="U17" s="83"/>
-      <c r="V17" s="83"/>
-      <c r="W17" s="83"/>
-      <c r="X17" s="83"/>
-      <c r="Y17" s="83"/>
-      <c r="Z17" s="83"/>
-      <c r="AA17" s="83"/>
-    </row>
-    <row r="18" spans="1:27" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A18" s="83"/>
-      <c r="B18" s="83" t="s">
+      <c r="U17" s="2"/>
+    </row>
+    <row r="18" spans="2:21" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="B18" s="2" t="s">
         <v>430</v>
       </c>
-      <c r="C18" s="83" t="s">
+      <c r="C18" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="D18" s="83" t="s">
+      <c r="D18" s="2" t="s">
         <v>431</v>
       </c>
-      <c r="E18" s="85" t="s">
+      <c r="E18" s="84" t="s">
         <v>366</v>
       </c>
-      <c r="F18" s="83"/>
-      <c r="G18" s="83"/>
-      <c r="H18" s="83"/>
-      <c r="I18" s="83" t="s">
+      <c r="I18" s="2" t="s">
         <v>457</v>
       </c>
-      <c r="J18" s="83" t="s">
+      <c r="J18" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="K18" s="83" t="s">
+      <c r="K18" s="2" t="s">
         <v>398</v>
       </c>
-      <c r="L18" s="83" t="s">
+      <c r="L18" s="2" t="s">
         <v>379</v>
       </c>
-      <c r="M18" s="83" t="s">
+      <c r="M18" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="N18" s="83"/>
-      <c r="O18" s="83"/>
-      <c r="P18" s="83"/>
-      <c r="Q18" s="83" t="s">
+      <c r="Q18" s="2" t="s">
         <v>378</v>
       </c>
-      <c r="R18" s="83" t="s">
+      <c r="R18" s="2" t="s">
         <v>367</v>
       </c>
-      <c r="S18" s="83"/>
-      <c r="T18" s="83"/>
-      <c r="U18" s="83"/>
-      <c r="V18" s="83"/>
-      <c r="W18" s="83"/>
-      <c r="X18" s="83"/>
-      <c r="Y18" s="83"/>
-      <c r="Z18" s="83"/>
-      <c r="AA18" s="83"/>
-    </row>
-    <row r="19" spans="1:27" ht="57" x14ac:dyDescent="0.45">
-      <c r="B19" s="83" t="s">
+      <c r="U18" s="2"/>
+    </row>
+    <row r="19" spans="2:21" ht="57" x14ac:dyDescent="0.45">
+      <c r="B19" s="2" t="s">
         <v>437</v>
       </c>
-      <c r="C19" s="83" t="s">
+      <c r="C19" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="D19" s="83"/>
-      <c r="E19" s="85" t="s">
+      <c r="E19" s="84" t="s">
         <v>366</v>
       </c>
-      <c r="F19" s="83"/>
-      <c r="G19" s="83"/>
-      <c r="H19" s="83"/>
-      <c r="I19" s="83" t="s">
+      <c r="I19" s="2" t="s">
         <v>456</v>
       </c>
-      <c r="J19" s="83" t="s">
+      <c r="J19" s="2" t="s">
         <v>360</v>
       </c>
-      <c r="K19" s="83" t="s">
+      <c r="K19" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="L19" s="83" t="s">
+      <c r="L19" s="2" t="s">
         <v>383</v>
       </c>
-      <c r="M19" s="83" t="s">
+      <c r="M19" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="N19" s="83"/>
-      <c r="O19" s="83"/>
-      <c r="P19" s="83"/>
-      <c r="Q19" s="83" t="s">
+      <c r="Q19" s="2" t="s">
         <v>384</v>
       </c>
-      <c r="R19" s="83" t="s">
+      <c r="R19" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="S19" s="83"/>
-      <c r="T19" s="83"/>
-      <c r="U19" s="83"/>
-      <c r="V19" s="83"/>
-      <c r="W19" s="83"/>
-      <c r="X19" s="83"/>
-      <c r="Y19" s="83"/>
-      <c r="Z19" s="83"/>
-      <c r="AA19" s="83"/>
-    </row>
-    <row r="20" spans="1:27" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A20" s="83"/>
-      <c r="B20" s="83" t="s">
+      <c r="U19" s="2"/>
+    </row>
+    <row r="20" spans="2:21" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B20" s="2" t="s">
         <v>437</v>
       </c>
-      <c r="C20" s="83" t="s">
+      <c r="C20" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="D20" s="83"/>
-      <c r="E20" s="85" t="s">
+      <c r="E20" s="84" t="s">
         <v>366</v>
       </c>
-      <c r="F20" s="83"/>
-      <c r="G20" s="83"/>
-      <c r="H20" s="83"/>
-      <c r="I20" s="83" t="s">
+      <c r="I20" s="2" t="s">
         <v>456</v>
       </c>
-      <c r="J20" s="83" t="s">
+      <c r="J20" s="2" t="s">
         <v>461</v>
       </c>
-      <c r="K20" s="83" t="s">
+      <c r="K20" s="2" t="s">
         <v>389</v>
       </c>
       <c r="L20" s="82"/>
-      <c r="M20" s="83" t="s">
+      <c r="M20" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="N20" s="83"/>
-      <c r="O20" s="83"/>
-      <c r="P20" s="83"/>
-      <c r="Q20" s="83" t="s">
+      <c r="Q20" s="2" t="s">
         <v>384</v>
       </c>
-      <c r="R20" s="83" t="s">
+      <c r="R20" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="S20" s="83"/>
-      <c r="T20" s="83"/>
-      <c r="U20" s="83"/>
-      <c r="V20" s="83"/>
-      <c r="W20" s="83"/>
-      <c r="X20" s="83"/>
-      <c r="Y20" s="83"/>
-      <c r="Z20" s="83"/>
-      <c r="AA20" s="83"/>
-    </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A21" s="83"/>
-      <c r="B21" s="83" t="s">
+      <c r="U20" s="2"/>
+    </row>
+    <row r="21" spans="2:21" x14ac:dyDescent="0.45">
+      <c r="B21" s="2" t="s">
         <v>432</v>
       </c>
-      <c r="C21" s="83" t="s">
+      <c r="C21" s="2" t="s">
         <v>433</v>
       </c>
-      <c r="D21" s="83" t="s">
+      <c r="D21" s="2" t="s">
         <v>423</v>
       </c>
-      <c r="E21" s="85" t="s">
+      <c r="E21" s="84" t="s">
         <v>366</v>
       </c>
-      <c r="F21" s="83"/>
-      <c r="G21" s="83"/>
-      <c r="H21" s="83"/>
       <c r="I21" s="82"/>
       <c r="J21" s="82"/>
       <c r="K21" s="82"/>
       <c r="L21" s="82"/>
       <c r="M21" s="82"/>
-      <c r="N21" s="83"/>
-      <c r="O21" s="83"/>
-      <c r="P21" s="83"/>
-      <c r="Q21" s="83"/>
-      <c r="R21" s="83"/>
-      <c r="S21" s="83"/>
-      <c r="T21" s="83"/>
-      <c r="U21" s="83"/>
-      <c r="V21" s="83"/>
-      <c r="W21" s="83"/>
-      <c r="X21" s="83"/>
-      <c r="Y21" s="83"/>
-      <c r="Z21" s="83"/>
-      <c r="AA21" s="83"/>
-    </row>
-    <row r="22" spans="1:27" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B22" s="83" t="s">
+      <c r="U21" s="2"/>
+    </row>
+    <row r="22" spans="2:21" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B22" s="2" t="s">
         <v>434</v>
       </c>
-      <c r="C22" s="83" t="s">
+      <c r="C22" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="D22" s="83" t="s">
+      <c r="D22" s="2" t="s">
         <v>423</v>
       </c>
-      <c r="E22" s="85" t="s">
+      <c r="E22" s="84" t="s">
         <v>366</v>
       </c>
-      <c r="F22" s="83"/>
-      <c r="G22" s="83"/>
-      <c r="H22" s="83"/>
       <c r="I22" s="82"/>
       <c r="J22" s="82"/>
       <c r="K22" s="82"/>
       <c r="L22" s="82"/>
       <c r="M22" s="82"/>
-      <c r="N22" s="83"/>
-      <c r="O22" s="83"/>
-      <c r="P22" s="83"/>
-      <c r="Q22" s="83"/>
-      <c r="R22" s="83"/>
-      <c r="S22" s="83"/>
-      <c r="T22" s="83"/>
-      <c r="U22" s="83"/>
-      <c r="V22" s="83"/>
-      <c r="W22" s="83"/>
-      <c r="X22" s="83"/>
-      <c r="Y22" s="83"/>
-      <c r="Z22" s="83"/>
-      <c r="AA22" s="83"/>
-    </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="B23" s="83" t="s">
+      <c r="U22" s="2"/>
+    </row>
+    <row r="23" spans="2:21" x14ac:dyDescent="0.45">
+      <c r="B23" s="2" t="s">
         <v>435</v>
       </c>
-      <c r="C23" s="83" t="s">
+      <c r="C23" s="2" t="s">
         <v>396</v>
       </c>
-      <c r="D23" s="83" t="s">
+      <c r="D23" s="2" t="s">
         <v>423</v>
       </c>
-      <c r="E23" s="85" t="s">
+      <c r="E23" s="84" t="s">
         <v>366</v>
       </c>
-      <c r="F23" s="83"/>
-      <c r="G23" s="83"/>
-      <c r="H23" s="83"/>
       <c r="I23" s="82"/>
       <c r="J23" s="82"/>
       <c r="K23" s="82"/>
       <c r="L23" s="82"/>
       <c r="M23" s="82"/>
-      <c r="N23" s="83"/>
-      <c r="O23" s="83"/>
-      <c r="P23" s="83"/>
-      <c r="Q23" s="83"/>
-      <c r="R23" s="83"/>
-      <c r="S23" s="83"/>
-      <c r="T23" s="83"/>
-      <c r="U23" s="83"/>
-      <c r="V23" s="83"/>
-      <c r="W23" s="83"/>
-      <c r="X23" s="83"/>
-      <c r="Y23" s="83"/>
-      <c r="Z23" s="83"/>
-      <c r="AA23" s="83"/>
-    </row>
-    <row r="24" spans="1:27" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B24" s="83" t="s">
+      <c r="U23" s="2"/>
+    </row>
+    <row r="24" spans="2:21" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B24" s="2" t="s">
         <v>436</v>
       </c>
-      <c r="C24" s="83" t="s">
+      <c r="C24" s="2" t="s">
         <v>357</v>
       </c>
-      <c r="D24" s="83" t="s">
+      <c r="D24" s="2" t="s">
         <v>423</v>
       </c>
-      <c r="E24" s="85" t="s">
+      <c r="E24" s="84" t="s">
         <v>366</v>
       </c>
-      <c r="F24" s="83"/>
-      <c r="G24" s="83"/>
-      <c r="H24" s="83"/>
       <c r="I24" s="82"/>
       <c r="J24" s="82"/>
       <c r="K24" s="82"/>
       <c r="L24" s="82"/>
       <c r="M24" s="82"/>
-      <c r="N24" s="83"/>
-      <c r="O24" s="83"/>
-      <c r="P24" s="83"/>
-      <c r="Q24" s="83"/>
-      <c r="R24" s="83"/>
-      <c r="S24" s="83"/>
-      <c r="T24" s="83"/>
-      <c r="U24" s="83"/>
-      <c r="V24" s="83"/>
-      <c r="W24" s="83"/>
-      <c r="X24" s="83"/>
-      <c r="Y24" s="83"/>
-      <c r="Z24" s="83"/>
-      <c r="AA24" s="83"/>
-    </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="B25" s="83" t="s">
+      <c r="U24" s="2"/>
+    </row>
+    <row r="25" spans="2:21" x14ac:dyDescent="0.45">
+      <c r="B25" s="2" t="s">
         <v>438</v>
       </c>
-      <c r="C25" s="83" t="s">
+      <c r="C25" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D25" s="83" t="s">
+      <c r="D25" s="2" t="s">
         <v>423</v>
       </c>
-      <c r="E25" s="85" t="s">
+      <c r="E25" s="84" t="s">
         <v>366</v>
       </c>
-      <c r="F25" s="83"/>
-      <c r="G25" s="83"/>
-      <c r="H25" s="83"/>
       <c r="I25" s="82"/>
       <c r="J25" s="82"/>
       <c r="K25" s="82"/>
       <c r="L25" s="82"/>
       <c r="M25" s="82"/>
-      <c r="N25" s="83"/>
-      <c r="O25" s="83"/>
-      <c r="P25" s="83"/>
-      <c r="Q25" s="83"/>
-      <c r="R25" s="83"/>
-      <c r="S25" s="83"/>
-      <c r="T25" s="83"/>
-      <c r="U25" s="83"/>
-      <c r="V25" s="83"/>
-      <c r="W25" s="83"/>
-      <c r="X25" s="83"/>
-      <c r="Y25" s="83"/>
-      <c r="Z25" s="83"/>
-      <c r="AA25" s="83"/>
-    </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="B26" s="83" t="s">
+      <c r="U25" s="2"/>
+    </row>
+    <row r="26" spans="2:21" x14ac:dyDescent="0.45">
+      <c r="B26" s="2" t="s">
         <v>439</v>
       </c>
-      <c r="C26" s="83" t="s">
+      <c r="C26" s="2" t="s">
         <v>433</v>
       </c>
-      <c r="D26" s="83"/>
-      <c r="E26" s="85" t="s">
+      <c r="E26" s="84" t="s">
         <v>366</v>
       </c>
-      <c r="F26" s="83"/>
-      <c r="G26" s="83"/>
-      <c r="H26" s="83"/>
       <c r="I26" s="82"/>
       <c r="J26" s="82"/>
       <c r="K26" s="82"/>
       <c r="L26" s="82"/>
       <c r="M26" s="82"/>
-      <c r="N26" s="83"/>
-      <c r="O26" s="83"/>
-      <c r="P26" s="83"/>
-      <c r="Q26" s="83"/>
-      <c r="R26" s="83"/>
-      <c r="S26" s="83"/>
-      <c r="T26" s="83"/>
-      <c r="U26" s="83"/>
-      <c r="V26" s="83"/>
-      <c r="W26" s="83"/>
-      <c r="X26" s="83"/>
-      <c r="Y26" s="83"/>
-      <c r="Z26" s="83"/>
-      <c r="AA26" s="83"/>
-    </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="B27" s="83" t="s">
+      <c r="U26" s="2"/>
+    </row>
+    <row r="27" spans="2:21" x14ac:dyDescent="0.45">
+      <c r="B27" s="2" t="s">
         <v>440</v>
       </c>
-      <c r="C27" s="83" t="s">
+      <c r="C27" s="2" t="s">
         <v>396</v>
       </c>
-      <c r="D27" s="83"/>
-      <c r="E27" s="85" t="s">
+      <c r="E27" s="84" t="s">
         <v>366</v>
       </c>
-      <c r="F27" s="83"/>
-      <c r="G27" s="83"/>
-      <c r="H27" s="83"/>
-      <c r="I27" s="83" t="s">
+      <c r="I27" s="2" t="s">
         <v>390</v>
       </c>
-      <c r="J27" s="83" t="s">
+      <c r="J27" s="2" t="s">
         <v>391</v>
       </c>
-      <c r="K27" s="83" t="s">
+      <c r="K27" s="2" t="s">
         <v>396</v>
       </c>
-      <c r="L27" s="83" t="s">
+      <c r="L27" s="2" t="s">
         <v>393</v>
       </c>
-      <c r="M27" s="83" t="s">
+      <c r="M27" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="N27" s="83"/>
-      <c r="O27" s="83"/>
-      <c r="P27" s="83"/>
-      <c r="Q27" s="83" t="s">
+      <c r="Q27" s="2" t="s">
         <v>381</v>
       </c>
-      <c r="R27" s="83" t="s">
+      <c r="R27" s="2" t="s">
         <v>382</v>
       </c>
-      <c r="S27" s="83"/>
-      <c r="T27" s="83"/>
-      <c r="U27" s="83"/>
-      <c r="V27" s="83"/>
-      <c r="W27" s="83"/>
-      <c r="X27" s="83"/>
-      <c r="Y27" s="83"/>
-      <c r="Z27" s="83"/>
-      <c r="AA27" s="83"/>
-    </row>
-    <row r="28" spans="1:27" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B28" s="83" t="s">
+      <c r="U27" s="2"/>
+    </row>
+    <row r="28" spans="2:21" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B28" s="2" t="s">
         <v>441</v>
       </c>
-      <c r="C28" s="83" t="s">
+      <c r="C28" s="2" t="s">
         <v>396</v>
       </c>
-      <c r="D28" s="83"/>
-      <c r="E28" s="85" t="s">
+      <c r="E28" s="84" t="s">
         <v>366</v>
       </c>
-      <c r="F28" s="83"/>
-      <c r="G28" s="83"/>
-      <c r="H28" s="83"/>
-      <c r="I28" s="83" t="s">
+      <c r="I28" s="2" t="s">
         <v>470</v>
       </c>
-      <c r="J28" s="83" t="s">
+      <c r="J28" s="2" t="s">
         <v>471</v>
       </c>
-      <c r="K28" s="83" t="s">
+      <c r="K28" s="2" t="s">
         <v>392</v>
       </c>
-      <c r="L28" s="83" t="s">
+      <c r="L28" s="2" t="s">
         <v>472</v>
       </c>
-      <c r="M28" s="83" t="s">
+      <c r="M28" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="N28" s="83"/>
-      <c r="O28" s="83"/>
-      <c r="P28" s="83"/>
-      <c r="Q28" s="83" t="s">
+      <c r="Q28" s="2" t="s">
         <v>394</v>
       </c>
-      <c r="R28" s="83" t="s">
+      <c r="R28" s="2" t="s">
         <v>395</v>
       </c>
-      <c r="S28" s="83"/>
-      <c r="T28" s="83"/>
-      <c r="U28" s="83"/>
-      <c r="V28" s="83"/>
-      <c r="W28" s="83"/>
-      <c r="X28" s="83"/>
-      <c r="Y28" s="83"/>
-      <c r="Z28" s="83"/>
-      <c r="AA28" s="83"/>
-    </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="B29" s="83" t="s">
+      <c r="U28" s="2"/>
+    </row>
+    <row r="29" spans="2:21" x14ac:dyDescent="0.45">
+      <c r="B29" s="2" t="s">
         <v>442</v>
       </c>
-      <c r="C29" s="83" t="s">
+      <c r="C29" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="D29" s="83" t="s">
+      <c r="D29" s="2" t="s">
         <v>423</v>
       </c>
-      <c r="E29" s="85" t="s">
+      <c r="E29" s="84" t="s">
         <v>366</v>
       </c>
-      <c r="F29" s="83"/>
-      <c r="G29" s="83"/>
-      <c r="H29" s="83"/>
       <c r="I29" s="82"/>
       <c r="J29" s="82"/>
       <c r="K29" s="82"/>
       <c r="L29" s="82"/>
       <c r="M29" s="82"/>
-      <c r="N29" s="83"/>
-      <c r="O29" s="83"/>
-      <c r="P29" s="83"/>
-      <c r="Q29" s="83"/>
-      <c r="R29" s="83"/>
-      <c r="S29" s="83"/>
-      <c r="T29" s="83"/>
-      <c r="U29" s="83"/>
-      <c r="V29" s="83"/>
-      <c r="W29" s="83"/>
-      <c r="X29" s="83"/>
-      <c r="Y29" s="83"/>
-      <c r="Z29" s="83"/>
-      <c r="AA29" s="83"/>
-    </row>
-    <row r="30" spans="1:27" ht="57" x14ac:dyDescent="0.45">
-      <c r="B30" s="83" t="s">
+      <c r="U29" s="2"/>
+    </row>
+    <row r="30" spans="2:21" ht="57" x14ac:dyDescent="0.45">
+      <c r="B30" s="2" t="s">
         <v>462</v>
       </c>
-      <c r="C30" s="83" t="s">
+      <c r="C30" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="D30" s="83"/>
-      <c r="E30" s="85" t="s">
+      <c r="E30" s="84" t="s">
         <v>449</v>
       </c>
-      <c r="F30" s="83"/>
-      <c r="G30" s="83"/>
-      <c r="H30" s="83"/>
-      <c r="I30" s="83" t="s">
+      <c r="I30" s="2" t="s">
         <v>385</v>
       </c>
-      <c r="J30" s="83" t="s">
+      <c r="J30" s="2" t="s">
         <v>476</v>
       </c>
-      <c r="K30" s="83" t="s">
+      <c r="K30" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="L30" s="83" t="s">
+      <c r="L30" s="2" t="s">
         <v>475</v>
       </c>
-      <c r="M30" s="83" t="s">
+      <c r="M30" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="N30" s="83"/>
-      <c r="O30" s="83"/>
-      <c r="P30" s="83"/>
-      <c r="Q30" s="83" t="s">
+      <c r="Q30" s="2" t="s">
         <v>384</v>
       </c>
-      <c r="R30" s="83" t="s">
+      <c r="R30" s="2" t="s">
         <v>477</v>
       </c>
-      <c r="S30" s="83"/>
-      <c r="T30" s="83"/>
-      <c r="U30" s="83"/>
-      <c r="V30" s="83"/>
-      <c r="W30" s="83"/>
-      <c r="X30" s="83"/>
-      <c r="Y30" s="83"/>
-      <c r="Z30" s="83"/>
-      <c r="AA30" s="83"/>
-    </row>
-    <row r="31" spans="1:27" ht="28.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B31" s="83" t="s">
+      <c r="U30" s="2"/>
+    </row>
+    <row r="31" spans="2:21" ht="28.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B31" s="2" t="s">
         <v>463</v>
       </c>
-      <c r="C31" s="83" t="s">
+      <c r="C31" s="2" t="s">
         <v>433</v>
       </c>
-      <c r="D31" s="83"/>
-      <c r="E31" s="85" t="s">
+      <c r="E31" s="84" t="s">
         <v>449</v>
       </c>
-      <c r="F31" s="83"/>
-      <c r="G31" s="83"/>
-      <c r="H31" s="83"/>
-      <c r="I31" s="83" t="s">
+      <c r="I31" s="2" t="s">
         <v>470</v>
       </c>
-      <c r="J31" s="83" t="s">
+      <c r="J31" s="2" t="s">
         <v>479</v>
       </c>
-      <c r="K31" s="83" t="s">
+      <c r="K31" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="L31" s="83" t="s">
+      <c r="L31" s="2" t="s">
         <v>478</v>
       </c>
-      <c r="M31" s="83" t="s">
+      <c r="M31" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="N31" s="83"/>
-      <c r="O31" s="83"/>
-      <c r="P31" s="83"/>
-      <c r="Q31" s="83" t="s">
+      <c r="Q31" s="2" t="s">
         <v>480</v>
       </c>
-      <c r="R31" s="83" t="s">
+      <c r="R31" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="S31" s="83"/>
-      <c r="T31" s="83"/>
-      <c r="U31" s="83"/>
-      <c r="V31" s="83"/>
-      <c r="W31" s="83"/>
-      <c r="X31" s="83"/>
-      <c r="Y31" s="83"/>
-      <c r="Z31" s="83"/>
-      <c r="AA31" s="83"/>
-    </row>
-    <row r="32" spans="1:27" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B32" s="83" t="s">
+      <c r="U31" s="2"/>
+    </row>
+    <row r="32" spans="2:21" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B32" s="2" t="s">
         <v>464</v>
       </c>
-      <c r="C32" s="83" t="s">
+      <c r="C32" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="D32" s="83"/>
-      <c r="E32" s="85" t="s">
+      <c r="E32" s="84" t="s">
         <v>449</v>
       </c>
-      <c r="F32" s="83"/>
-      <c r="G32" s="83"/>
-      <c r="H32" s="83"/>
-      <c r="I32" s="83" t="s">
+      <c r="I32" s="2" t="s">
         <v>385</v>
       </c>
-      <c r="J32" s="83" t="s">
+      <c r="J32" s="2" t="s">
         <v>474</v>
       </c>
-      <c r="K32" s="83"/>
-      <c r="L32" s="83" t="s">
+      <c r="L32" s="2" t="s">
         <v>473</v>
       </c>
-      <c r="M32" s="83" t="s">
+      <c r="M32" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="N32" s="83"/>
-      <c r="O32" s="83"/>
-      <c r="P32" s="83"/>
-      <c r="Q32" s="83" t="s">
+      <c r="Q32" s="2" t="s">
         <v>481</v>
       </c>
-      <c r="R32" s="83" t="s">
+      <c r="R32" s="2" t="s">
         <v>367</v>
       </c>
-      <c r="S32" s="83"/>
-      <c r="T32" s="83"/>
-      <c r="U32" s="83"/>
-      <c r="V32" s="83"/>
-      <c r="W32" s="83"/>
-      <c r="X32" s="83"/>
-      <c r="Y32" s="83"/>
-      <c r="Z32" s="83"/>
-      <c r="AA32" s="83"/>
-    </row>
-    <row r="33" spans="1:27" ht="128.25" x14ac:dyDescent="0.45">
-      <c r="B33" s="83" t="s">
+      <c r="U32" s="2"/>
+    </row>
+    <row r="33" spans="2:21" ht="128.25" x14ac:dyDescent="0.45">
+      <c r="B33" s="2" t="s">
         <v>465</v>
       </c>
-      <c r="C33" s="83" t="s">
+      <c r="C33" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="D33" s="83"/>
-      <c r="E33" s="85" t="s">
+      <c r="E33" s="84" t="s">
         <v>449</v>
       </c>
-      <c r="F33" s="83"/>
-      <c r="G33" s="83"/>
-      <c r="H33" s="83"/>
-      <c r="I33" s="83" t="s">
+      <c r="I33" s="2" t="s">
         <v>385</v>
       </c>
-      <c r="J33" s="83" t="s">
+      <c r="J33" s="2" t="s">
         <v>483</v>
       </c>
-      <c r="K33" s="83" t="s">
+      <c r="K33" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="L33" s="83" t="s">
+      <c r="L33" s="2" t="s">
         <v>484</v>
       </c>
-      <c r="M33" s="83" t="s">
+      <c r="M33" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="N33" s="83"/>
-      <c r="O33" s="83"/>
-      <c r="P33" s="83"/>
-      <c r="Q33" s="83" t="s">
+      <c r="Q33" s="2" t="s">
         <v>482</v>
       </c>
-      <c r="R33" s="83" t="s">
+      <c r="R33" s="2" t="s">
         <v>367</v>
       </c>
-      <c r="S33" s="83"/>
-      <c r="T33" s="83"/>
-      <c r="U33" s="83"/>
-      <c r="V33" s="83"/>
-      <c r="W33" s="83"/>
-      <c r="X33" s="83"/>
-      <c r="Y33" s="83"/>
-      <c r="Z33" s="83"/>
-      <c r="AA33" s="83"/>
-    </row>
-    <row r="34" spans="1:27" ht="71.25" x14ac:dyDescent="0.45">
-      <c r="B34" s="83" t="s">
+      <c r="U33" s="2"/>
+    </row>
+    <row r="34" spans="2:21" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="B34" s="2" t="s">
         <v>466</v>
       </c>
-      <c r="C34" s="83" t="s">
+      <c r="C34" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="D34" s="83"/>
-      <c r="E34" s="85" t="s">
+      <c r="E34" s="84" t="s">
         <v>449</v>
       </c>
-      <c r="F34" s="83"/>
-      <c r="G34" s="83"/>
-      <c r="H34" s="83"/>
-      <c r="I34" s="83" t="s">
+      <c r="I34" s="2" t="s">
         <v>385</v>
       </c>
-      <c r="J34" s="83" t="s">
+      <c r="J34" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="K34" s="83" t="s">
+      <c r="K34" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="L34" s="83" t="s">
+      <c r="L34" s="2" t="s">
         <v>485</v>
       </c>
-      <c r="M34" s="83" t="s">
+      <c r="M34" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="N34" s="83"/>
-      <c r="O34" s="83"/>
-      <c r="P34" s="83"/>
-      <c r="Q34" s="83" t="s">
+      <c r="Q34" s="2" t="s">
         <v>384</v>
       </c>
-      <c r="R34" s="83" t="s">
+      <c r="R34" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="S34" s="83"/>
-      <c r="T34" s="83"/>
-      <c r="U34" s="83"/>
-      <c r="V34" s="83"/>
-      <c r="W34" s="83"/>
-      <c r="X34" s="83"/>
-      <c r="Y34" s="83"/>
-      <c r="Z34" s="83"/>
-      <c r="AA34" s="83"/>
-    </row>
-    <row r="35" spans="1:27" ht="57" x14ac:dyDescent="0.45">
-      <c r="B35" s="83" t="s">
+      <c r="U34" s="2"/>
+    </row>
+    <row r="35" spans="2:21" ht="57" x14ac:dyDescent="0.45">
+      <c r="B35" s="2" t="s">
         <v>467</v>
       </c>
-      <c r="C35" s="83" t="s">
+      <c r="C35" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="D35" s="83"/>
-      <c r="E35" s="85" t="s">
+      <c r="E35" s="84" t="s">
         <v>449</v>
       </c>
-      <c r="F35" s="83"/>
-      <c r="G35" s="83"/>
-      <c r="H35" s="83"/>
-      <c r="I35" s="83" t="s">
+      <c r="I35" s="2" t="s">
         <v>385</v>
       </c>
-      <c r="J35" s="83" t="s">
+      <c r="J35" s="2" t="s">
         <v>476</v>
       </c>
-      <c r="K35" s="83" t="s">
+      <c r="K35" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="L35" s="83" t="s">
+      <c r="L35" s="2" t="s">
         <v>475</v>
       </c>
-      <c r="M35" s="83" t="s">
+      <c r="M35" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="N35" s="83"/>
-      <c r="O35" s="83"/>
-      <c r="P35" s="83"/>
-      <c r="Q35" s="83" t="s">
+      <c r="Q35" s="2" t="s">
         <v>384</v>
       </c>
-      <c r="R35" s="83" t="s">
+      <c r="R35" s="2" t="s">
         <v>477</v>
       </c>
-      <c r="S35" s="83"/>
-      <c r="T35" s="83"/>
-      <c r="U35" s="83"/>
-      <c r="V35" s="83"/>
-      <c r="W35" s="83"/>
-      <c r="X35" s="83"/>
-      <c r="Y35" s="83"/>
-      <c r="Z35" s="83"/>
-      <c r="AA35" s="83"/>
-    </row>
-    <row r="36" spans="1:27" ht="409.5" x14ac:dyDescent="0.45">
-      <c r="B36" s="83" t="s">
+      <c r="U35" s="2"/>
+    </row>
+    <row r="36" spans="2:21" ht="409.5" x14ac:dyDescent="0.45">
+      <c r="B36" s="2" t="s">
         <v>443</v>
       </c>
-      <c r="C36" s="83" t="s">
+      <c r="C36" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="D36" s="83"/>
-      <c r="E36" s="85" t="s">
+      <c r="E36" s="84" t="s">
         <v>449</v>
       </c>
-      <c r="F36" s="83"/>
-      <c r="G36" s="83"/>
-      <c r="H36" s="83"/>
-      <c r="I36" s="83" t="s">
+      <c r="I36" s="2" t="s">
         <v>470</v>
       </c>
-      <c r="J36" s="83" t="s">
+      <c r="J36" s="2" t="s">
         <v>479</v>
       </c>
-      <c r="K36" s="83" t="s">
+      <c r="K36" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="L36" s="83" t="s">
+      <c r="L36" s="2" t="s">
         <v>478</v>
       </c>
-      <c r="M36" s="83" t="s">
+      <c r="M36" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="N36" s="83"/>
-      <c r="O36" s="83"/>
-      <c r="P36" s="83"/>
-      <c r="Q36" s="83" t="s">
+      <c r="Q36" s="2" t="s">
         <v>480</v>
       </c>
-      <c r="R36" s="83" t="s">
+      <c r="R36" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="S36" s="83"/>
-      <c r="T36" s="83"/>
-      <c r="U36" s="83"/>
-      <c r="V36" s="83"/>
-      <c r="W36" s="83"/>
-      <c r="X36" s="83"/>
-      <c r="Y36" s="83"/>
-      <c r="Z36" s="83"/>
-      <c r="AA36" s="83"/>
-    </row>
-    <row r="37" spans="1:27" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B37" s="83" t="s">
+      <c r="U36" s="2"/>
+    </row>
+    <row r="37" spans="2:21" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B37" s="2" t="s">
         <v>444</v>
       </c>
-      <c r="C37" s="83" t="s">
+      <c r="C37" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="D37" s="83"/>
-      <c r="E37" s="85" t="s">
+      <c r="E37" s="84" t="s">
         <v>449</v>
       </c>
-      <c r="F37" s="83"/>
-      <c r="G37" s="83"/>
-      <c r="H37" s="83"/>
-      <c r="I37" s="83" t="s">
+      <c r="I37" s="2" t="s">
         <v>385</v>
       </c>
-      <c r="J37" s="83" t="s">
+      <c r="J37" s="2" t="s">
         <v>474</v>
       </c>
-      <c r="K37" s="83"/>
-      <c r="L37" s="83" t="s">
+      <c r="L37" s="2" t="s">
         <v>473</v>
       </c>
-      <c r="M37" s="83" t="s">
+      <c r="M37" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="N37" s="83"/>
-      <c r="O37" s="83"/>
-      <c r="P37" s="83"/>
-      <c r="Q37" s="83" t="s">
+      <c r="Q37" s="2" t="s">
         <v>481</v>
       </c>
-      <c r="R37" s="83" t="s">
+      <c r="R37" s="2" t="s">
         <v>367</v>
       </c>
-      <c r="S37" s="83"/>
-      <c r="T37" s="83"/>
-      <c r="U37" s="83"/>
-      <c r="V37" s="83"/>
-      <c r="W37" s="83"/>
-      <c r="X37" s="83"/>
-      <c r="Y37" s="83"/>
-      <c r="Z37" s="83"/>
-      <c r="AA37" s="83"/>
-    </row>
-    <row r="38" spans="1:27" ht="128.25" x14ac:dyDescent="0.45">
-      <c r="A38" s="83"/>
-      <c r="B38" s="83" t="s">
+      <c r="U37" s="2"/>
+    </row>
+    <row r="38" spans="2:21" ht="128.25" x14ac:dyDescent="0.45">
+      <c r="B38" s="2" t="s">
         <v>447</v>
       </c>
-      <c r="C38" s="83" t="s">
+      <c r="C38" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="D38" s="83"/>
-      <c r="E38" s="85" t="s">
+      <c r="E38" s="84" t="s">
         <v>449</v>
       </c>
-      <c r="F38" s="83"/>
-      <c r="G38" s="83"/>
-      <c r="H38" s="83"/>
-      <c r="I38" s="83" t="s">
+      <c r="I38" s="2" t="s">
         <v>385</v>
       </c>
-      <c r="J38" s="83" t="s">
+      <c r="J38" s="2" t="s">
         <v>483</v>
       </c>
-      <c r="K38" s="83" t="s">
+      <c r="K38" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="L38" s="83" t="s">
+      <c r="L38" s="2" t="s">
         <v>484</v>
       </c>
-      <c r="M38" s="83" t="s">
+      <c r="M38" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="N38" s="83"/>
-      <c r="O38" s="83"/>
-      <c r="P38" s="83"/>
-      <c r="Q38" s="83" t="s">
+      <c r="Q38" s="2" t="s">
         <v>482</v>
       </c>
-      <c r="R38" s="83" t="s">
+      <c r="R38" s="2" t="s">
         <v>367</v>
       </c>
-      <c r="S38" s="83"/>
-      <c r="T38" s="83"/>
-      <c r="U38" s="83"/>
-      <c r="V38" s="83"/>
-      <c r="W38" s="83"/>
-      <c r="X38" s="83"/>
-      <c r="Y38" s="83"/>
-      <c r="Z38" s="83"/>
-      <c r="AA38" s="83"/>
-    </row>
-    <row r="39" spans="1:27" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B39" s="83" t="s">
+      <c r="U38" s="2"/>
+    </row>
+    <row r="39" spans="2:21" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B39" s="2" t="s">
         <v>445</v>
       </c>
-      <c r="C39" s="83" t="s">
+      <c r="C39" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="D39" s="83"/>
-      <c r="E39" s="85" t="s">
+      <c r="E39" s="84" t="s">
         <v>449</v>
       </c>
-      <c r="F39" s="83"/>
-      <c r="G39" s="83"/>
-      <c r="H39" s="83"/>
       <c r="I39" s="82"/>
       <c r="J39" s="82"/>
       <c r="K39" s="82"/>
       <c r="L39" s="82"/>
       <c r="M39" s="82"/>
-      <c r="N39" s="83"/>
-      <c r="O39" s="83"/>
-      <c r="P39" s="83"/>
-      <c r="Q39" s="83"/>
-      <c r="R39" s="83"/>
-      <c r="S39" s="83"/>
-      <c r="T39" s="83"/>
-      <c r="U39" s="83"/>
-      <c r="V39" s="83"/>
-      <c r="W39" s="83"/>
-      <c r="X39" s="83"/>
-      <c r="Y39" s="83"/>
-      <c r="Z39" s="83"/>
-      <c r="AA39" s="83"/>
-    </row>
-    <row r="40" spans="1:27" ht="71.25" x14ac:dyDescent="0.45">
-      <c r="B40" s="83" t="s">
+      <c r="U39" s="2"/>
+    </row>
+    <row r="40" spans="2:21" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="B40" s="2" t="s">
         <v>446</v>
       </c>
-      <c r="C40" s="83" t="s">
+      <c r="C40" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="D40" s="83"/>
-      <c r="E40" s="85" t="s">
+      <c r="E40" s="84" t="s">
         <v>449</v>
       </c>
-      <c r="F40" s="83"/>
-      <c r="G40" s="83"/>
-      <c r="H40" s="83"/>
-      <c r="I40" s="83" t="s">
+      <c r="I40" s="2" t="s">
         <v>385</v>
       </c>
-      <c r="J40" s="83" t="s">
+      <c r="J40" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="K40" s="83" t="s">
+      <c r="K40" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="L40" s="83" t="s">
+      <c r="L40" s="2" t="s">
         <v>485</v>
       </c>
-      <c r="M40" s="83" t="s">
+      <c r="M40" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="N40" s="83"/>
-      <c r="O40" s="83"/>
-      <c r="P40" s="83"/>
-      <c r="Q40" s="83" t="s">
+      <c r="Q40" s="2" t="s">
         <v>384</v>
       </c>
-      <c r="R40" s="83" t="s">
+      <c r="R40" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="S40" s="83"/>
-      <c r="T40" s="83"/>
-      <c r="U40" s="83"/>
-      <c r="V40" s="83"/>
-      <c r="W40" s="83"/>
-      <c r="X40" s="83"/>
-      <c r="Y40" s="83"/>
-      <c r="Z40" s="83"/>
-      <c r="AA40" s="83"/>
-    </row>
-    <row r="41" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="B41" s="83"/>
-      <c r="C41" s="83"/>
-      <c r="D41" s="83"/>
-      <c r="E41" s="85"/>
-      <c r="F41" s="83"/>
-      <c r="G41" s="83"/>
-      <c r="H41" s="83"/>
-      <c r="I41" s="83"/>
-      <c r="J41" s="83"/>
-      <c r="K41" s="83"/>
-      <c r="L41" s="83"/>
-      <c r="M41" s="83"/>
-      <c r="N41" s="83"/>
-      <c r="O41" s="83"/>
-      <c r="P41" s="83"/>
-      <c r="Q41" s="83"/>
-      <c r="R41" s="83"/>
-      <c r="S41" s="83"/>
-      <c r="T41" s="83"/>
-      <c r="U41" s="83"/>
-      <c r="V41" s="83"/>
-      <c r="W41" s="83"/>
-      <c r="X41" s="83"/>
-      <c r="Y41" s="83"/>
-      <c r="Z41" s="83"/>
-      <c r="AA41" s="83"/>
-    </row>
-    <row r="42" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="B42" s="83"/>
-      <c r="C42" s="83"/>
-      <c r="D42" s="83"/>
-      <c r="E42" s="85"/>
-      <c r="F42" s="83"/>
-      <c r="G42" s="83"/>
-      <c r="H42" s="83"/>
-      <c r="I42" s="83"/>
-      <c r="J42" s="83"/>
-      <c r="K42" s="83"/>
-      <c r="L42" s="83"/>
-      <c r="M42" s="83"/>
-      <c r="N42" s="83"/>
-      <c r="O42" s="83"/>
-      <c r="P42" s="83"/>
-      <c r="Q42" s="83"/>
-      <c r="R42" s="83"/>
-      <c r="S42" s="83"/>
-      <c r="T42" s="83"/>
-      <c r="U42" s="83"/>
-      <c r="V42" s="83"/>
-      <c r="W42" s="83"/>
-      <c r="X42" s="83"/>
-      <c r="Y42" s="83"/>
-      <c r="Z42" s="83"/>
-      <c r="AA42" s="83"/>
-    </row>
-    <row r="43" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="B43" s="83"/>
-      <c r="C43" s="83"/>
-      <c r="D43" s="83"/>
-      <c r="E43" s="85"/>
-      <c r="F43" s="83"/>
-      <c r="G43" s="83"/>
-      <c r="H43" s="83"/>
-      <c r="I43" s="83"/>
-      <c r="J43" s="83"/>
-      <c r="K43" s="83"/>
-      <c r="L43" s="83"/>
-      <c r="M43" s="83"/>
-      <c r="N43" s="83"/>
-      <c r="O43" s="83"/>
-      <c r="P43" s="83"/>
-      <c r="Q43" s="83"/>
-      <c r="R43" s="83"/>
-      <c r="S43" s="83"/>
-      <c r="T43" s="83"/>
-      <c r="U43" s="83"/>
-      <c r="V43" s="83"/>
-      <c r="W43" s="83"/>
-      <c r="X43" s="83"/>
-      <c r="Y43" s="83"/>
-      <c r="Z43" s="83"/>
-      <c r="AA43" s="83"/>
-    </row>
-    <row r="44" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="B44" s="83"/>
-      <c r="C44" s="83"/>
-      <c r="D44" s="83"/>
-      <c r="E44" s="85"/>
-      <c r="F44" s="83"/>
-      <c r="G44" s="83"/>
-      <c r="H44" s="83"/>
-      <c r="I44" s="83"/>
-      <c r="J44" s="83"/>
-      <c r="K44" s="83"/>
-      <c r="L44" s="83"/>
-      <c r="M44" s="83"/>
-      <c r="N44" s="83"/>
-      <c r="O44" s="83"/>
-      <c r="P44" s="83"/>
-      <c r="Q44" s="83"/>
-      <c r="R44" s="83"/>
-      <c r="S44" s="83"/>
-      <c r="T44" s="83"/>
-      <c r="U44" s="83"/>
-      <c r="V44" s="83"/>
-      <c r="W44" s="83"/>
-      <c r="X44" s="83"/>
-      <c r="Y44" s="83"/>
-      <c r="Z44" s="83"/>
-      <c r="AA44" s="83"/>
-    </row>
-    <row r="45" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="B45" s="83"/>
-      <c r="C45" s="83"/>
-      <c r="D45" s="83"/>
-      <c r="E45" s="85"/>
-      <c r="F45" s="83"/>
-      <c r="G45" s="83"/>
-      <c r="H45" s="83"/>
-      <c r="I45" s="83"/>
-      <c r="J45" s="83"/>
-      <c r="K45" s="83"/>
-      <c r="L45" s="83"/>
-      <c r="M45" s="83"/>
-      <c r="N45" s="83"/>
-      <c r="O45" s="83"/>
-      <c r="P45" s="83"/>
-      <c r="Q45" s="83"/>
-      <c r="R45" s="83"/>
-      <c r="S45" s="83"/>
-      <c r="T45" s="83"/>
-      <c r="U45" s="83"/>
-      <c r="V45" s="83"/>
-      <c r="W45" s="83"/>
-      <c r="X45" s="83"/>
-      <c r="Y45" s="83"/>
-      <c r="Z45" s="83"/>
-      <c r="AA45" s="83"/>
-    </row>
-    <row r="46" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="B46" s="83"/>
-      <c r="C46" s="83"/>
-      <c r="D46" s="83"/>
-      <c r="E46" s="85"/>
-      <c r="F46" s="83"/>
-      <c r="G46" s="83"/>
-      <c r="H46" s="83"/>
-      <c r="I46" s="83"/>
-      <c r="J46" s="83"/>
-      <c r="K46" s="83"/>
-      <c r="L46" s="83"/>
-      <c r="M46" s="83"/>
-      <c r="N46" s="83"/>
-      <c r="O46" s="83"/>
-      <c r="P46" s="83"/>
-      <c r="Q46" s="83"/>
-      <c r="R46" s="83"/>
-      <c r="S46" s="83"/>
-      <c r="T46" s="83"/>
-      <c r="U46" s="83"/>
-      <c r="V46" s="83"/>
-      <c r="W46" s="83"/>
-      <c r="X46" s="83"/>
-      <c r="Y46" s="83"/>
-      <c r="Z46" s="83"/>
-      <c r="AA46" s="83"/>
-    </row>
-    <row r="47" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="B47" s="83"/>
-      <c r="C47" s="83"/>
-      <c r="D47" s="83"/>
-      <c r="E47" s="85"/>
-      <c r="F47" s="83"/>
-      <c r="G47" s="83"/>
-      <c r="H47" s="83"/>
-      <c r="I47" s="83"/>
-      <c r="J47" s="83"/>
-      <c r="K47" s="83"/>
-      <c r="L47" s="83"/>
-      <c r="M47" s="83"/>
-      <c r="N47" s="83"/>
-      <c r="O47" s="83"/>
-      <c r="P47" s="83"/>
-      <c r="Q47" s="83"/>
-      <c r="R47" s="83"/>
-      <c r="S47" s="83"/>
-      <c r="T47" s="83"/>
-      <c r="U47" s="83"/>
-      <c r="V47" s="83"/>
-      <c r="W47" s="83"/>
-      <c r="X47" s="83"/>
-      <c r="Y47" s="83"/>
-      <c r="Z47" s="83"/>
-      <c r="AA47" s="83"/>
-    </row>
-    <row r="48" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="B48" s="83"/>
-      <c r="C48" s="83"/>
-      <c r="D48" s="83"/>
-      <c r="E48" s="85"/>
-      <c r="F48" s="83"/>
-      <c r="G48" s="83"/>
-      <c r="H48" s="83"/>
-      <c r="I48" s="83"/>
-      <c r="J48" s="83"/>
-      <c r="K48" s="83"/>
-      <c r="L48" s="83"/>
-      <c r="M48" s="83"/>
-      <c r="N48" s="83"/>
-      <c r="O48" s="83"/>
-      <c r="P48" s="83"/>
-      <c r="Q48" s="83"/>
-      <c r="R48" s="83"/>
-      <c r="S48" s="83"/>
-      <c r="T48" s="83"/>
-      <c r="U48" s="83"/>
-      <c r="V48" s="83"/>
-      <c r="W48" s="83"/>
-      <c r="X48" s="83"/>
-      <c r="Y48" s="83"/>
-      <c r="Z48" s="83"/>
-      <c r="AA48" s="83"/>
-    </row>
-    <row r="49" spans="2:27" x14ac:dyDescent="0.45">
-      <c r="B49" s="83"/>
-      <c r="C49" s="83"/>
-      <c r="D49" s="83"/>
-      <c r="E49" s="85"/>
-      <c r="F49" s="83"/>
-      <c r="G49" s="83"/>
-      <c r="H49" s="83"/>
-      <c r="I49" s="83"/>
-      <c r="J49" s="83"/>
-      <c r="K49" s="83"/>
-      <c r="L49" s="83"/>
-      <c r="M49" s="83"/>
-      <c r="N49" s="83"/>
-      <c r="O49" s="83"/>
-      <c r="P49" s="83"/>
-      <c r="Q49" s="83"/>
-      <c r="R49" s="83"/>
-      <c r="S49" s="83"/>
-      <c r="T49" s="83"/>
-      <c r="U49" s="83"/>
-      <c r="V49" s="83"/>
-      <c r="W49" s="83"/>
-      <c r="X49" s="83"/>
-      <c r="Y49" s="83"/>
-      <c r="Z49" s="83"/>
-      <c r="AA49" s="83"/>
-    </row>
-    <row r="50" spans="2:27" x14ac:dyDescent="0.45">
-      <c r="B50" s="83"/>
-      <c r="C50" s="83"/>
-      <c r="D50" s="83"/>
-      <c r="E50" s="85"/>
-      <c r="F50" s="83"/>
-      <c r="G50" s="83"/>
-      <c r="H50" s="83"/>
-      <c r="I50" s="83"/>
-      <c r="J50" s="83"/>
-      <c r="K50" s="83"/>
-      <c r="L50" s="83"/>
-      <c r="M50" s="83"/>
-      <c r="N50" s="83"/>
-      <c r="O50" s="83"/>
-      <c r="P50" s="83"/>
-      <c r="Q50" s="83"/>
-      <c r="R50" s="83"/>
-      <c r="S50" s="83"/>
-      <c r="T50" s="83"/>
-      <c r="U50" s="83"/>
-      <c r="V50" s="83"/>
-      <c r="W50" s="83"/>
-      <c r="X50" s="83"/>
-      <c r="Y50" s="83"/>
-      <c r="Z50" s="83"/>
-      <c r="AA50" s="83"/>
-    </row>
-    <row r="51" spans="2:27" x14ac:dyDescent="0.45">
-      <c r="B51" s="83"/>
-      <c r="C51" s="83"/>
-      <c r="D51" s="83"/>
-      <c r="E51" s="85"/>
-      <c r="F51" s="83"/>
-      <c r="G51" s="83"/>
-      <c r="H51" s="83"/>
-      <c r="I51" s="83"/>
-      <c r="J51" s="83"/>
-      <c r="K51" s="83"/>
-      <c r="L51" s="83"/>
-      <c r="M51" s="83"/>
-      <c r="N51" s="83"/>
-      <c r="O51" s="83"/>
-      <c r="P51" s="83"/>
-      <c r="Q51" s="83"/>
-      <c r="R51" s="83"/>
-      <c r="S51" s="83"/>
-      <c r="T51" s="83"/>
-      <c r="U51" s="83"/>
-      <c r="V51" s="83"/>
-      <c r="W51" s="83"/>
-      <c r="X51" s="83"/>
-      <c r="Y51" s="83"/>
-      <c r="Z51" s="83"/>
-      <c r="AA51" s="83"/>
-    </row>
-    <row r="52" spans="2:27" x14ac:dyDescent="0.45">
-      <c r="B52" s="83"/>
-      <c r="C52" s="83"/>
-      <c r="D52" s="83"/>
-      <c r="E52" s="85"/>
-      <c r="F52" s="83"/>
-      <c r="G52" s="83"/>
-      <c r="H52" s="83"/>
-      <c r="I52" s="83"/>
-      <c r="J52" s="83"/>
-      <c r="K52" s="83"/>
-      <c r="L52" s="83"/>
-      <c r="M52" s="83"/>
-      <c r="N52" s="83"/>
-      <c r="O52" s="83"/>
-      <c r="P52" s="83"/>
-      <c r="Q52" s="83"/>
-      <c r="R52" s="83"/>
-      <c r="S52" s="83"/>
-      <c r="T52" s="83"/>
-      <c r="U52" s="83"/>
-      <c r="V52" s="83"/>
-      <c r="W52" s="83"/>
-      <c r="X52" s="83"/>
-      <c r="Y52" s="83"/>
-      <c r="Z52" s="83"/>
-      <c r="AA52" s="83"/>
-    </row>
-    <row r="53" spans="2:27" x14ac:dyDescent="0.45">
-      <c r="B53" s="83"/>
-      <c r="C53" s="83"/>
-      <c r="D53" s="83"/>
-      <c r="E53" s="85"/>
-      <c r="F53" s="83"/>
-      <c r="G53" s="83"/>
-      <c r="H53" s="83"/>
-      <c r="I53" s="83"/>
-      <c r="J53" s="83"/>
-      <c r="K53" s="83"/>
-      <c r="L53" s="83"/>
-      <c r="M53" s="83"/>
-      <c r="N53" s="83"/>
-      <c r="O53" s="83"/>
-      <c r="P53" s="83"/>
-      <c r="Q53" s="83"/>
-      <c r="R53" s="83"/>
-      <c r="S53" s="83"/>
-      <c r="T53" s="83"/>
-      <c r="U53" s="83"/>
-      <c r="V53" s="83"/>
-      <c r="W53" s="83"/>
-      <c r="X53" s="83"/>
-      <c r="Y53" s="83"/>
-      <c r="Z53" s="83"/>
-      <c r="AA53" s="83"/>
-    </row>
-    <row r="54" spans="2:27" x14ac:dyDescent="0.45">
-      <c r="B54" s="83"/>
-      <c r="C54" s="83"/>
-      <c r="D54" s="83"/>
-      <c r="E54" s="85"/>
-      <c r="F54" s="83"/>
-      <c r="G54" s="83"/>
-      <c r="H54" s="83"/>
-      <c r="I54" s="83"/>
-      <c r="J54" s="83"/>
-      <c r="K54" s="83"/>
-      <c r="L54" s="83"/>
-      <c r="M54" s="83"/>
-      <c r="N54" s="83"/>
-      <c r="O54" s="83"/>
-      <c r="P54" s="83"/>
-      <c r="Q54" s="83"/>
-      <c r="R54" s="83"/>
-      <c r="S54" s="83"/>
-      <c r="T54" s="83"/>
-      <c r="U54" s="83"/>
-      <c r="V54" s="83"/>
-      <c r="W54" s="83"/>
-      <c r="X54" s="83"/>
-      <c r="Y54" s="83"/>
-      <c r="Z54" s="83"/>
-      <c r="AA54" s="83"/>
-    </row>
-    <row r="55" spans="2:27" x14ac:dyDescent="0.45">
-      <c r="B55" s="83"/>
-      <c r="C55" s="83"/>
-      <c r="D55" s="83"/>
-      <c r="E55" s="85" t="s">
+      <c r="U40" s="2"/>
+    </row>
+    <row r="41" spans="2:21" ht="99.75" x14ac:dyDescent="0.45">
+      <c r="B41" s="2" t="s">
+        <v>486</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>487</v>
+      </c>
+      <c r="E41" s="84" t="s">
         <v>366</v>
       </c>
-      <c r="F55" s="83"/>
-      <c r="G55" s="83"/>
-      <c r="H55" s="83"/>
-      <c r="I55" s="83"/>
-      <c r="J55" s="83"/>
-      <c r="K55" s="83"/>
-      <c r="L55" s="83"/>
-      <c r="M55" s="83"/>
-      <c r="N55" s="83"/>
-      <c r="O55" s="83"/>
-      <c r="P55" s="83"/>
-      <c r="Q55" s="83"/>
-      <c r="R55" s="83"/>
-      <c r="S55" s="83"/>
-      <c r="T55" s="83"/>
-      <c r="U55" s="83"/>
-      <c r="V55" s="83"/>
-      <c r="W55" s="83"/>
-      <c r="X55" s="83"/>
-      <c r="Y55" s="83"/>
-      <c r="Z55" s="83"/>
-      <c r="AA55" s="83"/>
-    </row>
-    <row r="56" spans="2:27" x14ac:dyDescent="0.45">
-      <c r="E56" s="85" t="s">
-        <v>366</v>
-      </c>
+      <c r="I41" s="82"/>
+      <c r="J41" s="82"/>
+      <c r="K41" s="82"/>
+      <c r="L41" s="82"/>
+      <c r="M41" s="82"/>
+      <c r="U41" s="2"/>
+    </row>
+    <row r="42" spans="2:21" x14ac:dyDescent="0.45">
+      <c r="U42" s="2"/>
+    </row>
+    <row r="43" spans="2:21" x14ac:dyDescent="0.45">
+      <c r="U43" s="2"/>
+    </row>
+    <row r="44" spans="2:21" x14ac:dyDescent="0.45">
+      <c r="U44" s="2"/>
+    </row>
+    <row r="45" spans="2:21" x14ac:dyDescent="0.45">
+      <c r="U45" s="2"/>
+    </row>
+    <row r="46" spans="2:21" x14ac:dyDescent="0.45">
+      <c r="U46" s="2"/>
+    </row>
+    <row r="47" spans="2:21" x14ac:dyDescent="0.45">
+      <c r="U47" s="2"/>
+    </row>
+    <row r="48" spans="2:21" x14ac:dyDescent="0.45">
+      <c r="U48" s="2"/>
+    </row>
+    <row r="49" spans="21:21" x14ac:dyDescent="0.45">
+      <c r="U49" s="2"/>
+    </row>
+    <row r="50" spans="21:21" x14ac:dyDescent="0.45">
+      <c r="U50" s="2"/>
+    </row>
+    <row r="51" spans="21:21" x14ac:dyDescent="0.45">
+      <c r="U51" s="2"/>
+    </row>
+    <row r="52" spans="21:21" x14ac:dyDescent="0.45">
+      <c r="U52" s="2"/>
+    </row>
+    <row r="53" spans="21:21" x14ac:dyDescent="0.45">
+      <c r="U53" s="2"/>
+    </row>
+    <row r="54" spans="21:21" x14ac:dyDescent="0.45">
+      <c r="U54" s="2"/>
+    </row>
+    <row r="55" spans="21:21" x14ac:dyDescent="0.45">
+      <c r="U55" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="19" type="noConversion"/>

</xml_diff>

<commit_message>
Completed mapping and class diagram
</commit_message>
<xml_diff>
--- a/schemas/ChargeFiling_iepd/artifacts/ChargeFiling_MappingSpreadsheet.xlsx
+++ b/schemas/ChargeFiling_iepd/artifacts/ChargeFiling_MappingSpreadsheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JamesCabral\git\JTMP-Data-Exchange-Specs\schemas\ChargeFiling_iepd\artifacts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JamesCabral\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F52C61D3-B739-42DE-A29F-42FD5B75EEE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0821B922-D74E-4927-9424-542EDE59CD8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13335" yWindow="-21225" windowWidth="22755" windowHeight="19890" tabRatio="781" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21840" yWindow="-21600" windowWidth="25905" windowHeight="20985" tabRatio="781" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="9" state="hidden" r:id="rId1"/>
@@ -26,7 +26,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Codes | Facets'!$A$1:$M$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7">Namespace!$A$1:$N$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Property!$A$1:$V$55</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Property!$A$1:$W$35</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4">Type!$A$1:$L$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5">'Type-Has-Property'!$A$1:$P$1</definedName>
     <definedName name="CODES_NamespaceStyle">'Field Descriptions'!$B$165:$B$176</definedName>
@@ -107,22 +107,22 @@
     <definedName name="Namespace_Target_RelativePath">Namespace!$M$1</definedName>
     <definedName name="Namespace_Target_Style">Namespace!$H$1</definedName>
     <definedName name="Namespace_Target_URI">Namespace!$I$1</definedName>
-    <definedName name="Property_Mapping_Code">Property!$F$1</definedName>
-    <definedName name="Property_Mapping_Description">Property!$G$1</definedName>
-    <definedName name="Property_Mapping_Notes">Property!$H$1</definedName>
+    <definedName name="Property_Mapping_Code">Property!$G$1</definedName>
+    <definedName name="Property_Mapping_Description">Property!$H$1</definedName>
+    <definedName name="Property_Mapping_Notes">Property!$I$1</definedName>
     <definedName name="Property_Source_DataType">Property!$C$1</definedName>
     <definedName name="Property_Source_Definition">Property!$D$1</definedName>
     <definedName name="Property_Source_Name">Property!$B$1</definedName>
     <definedName name="Property_Source_NamespacePrefix">Property!$A$1</definedName>
-    <definedName name="Property_Target_DataType">Property!$R$1</definedName>
-    <definedName name="Property_Target_Definition">Property!$S$1</definedName>
-    <definedName name="Property_Target_ExampleContent">Property!$X$1</definedName>
-    <definedName name="Property_Target_Keywords">Property!$W$1</definedName>
-    <definedName name="Property_Target_Name">Property!$Q$1</definedName>
-    <definedName name="Property_Target_NamespacePrefix">Property!$N$1</definedName>
-    <definedName name="Property_Target_Style">Property!$V$1</definedName>
-    <definedName name="Property_Target_SubstitutionGroup">Property!$U$1</definedName>
-    <definedName name="Property_Target_UsageInfo">Property!$Y$1</definedName>
+    <definedName name="Property_Target_DataType">Property!$S$1</definedName>
+    <definedName name="Property_Target_Definition">Property!$T$1</definedName>
+    <definedName name="Property_Target_ExampleContent">Property!$Y$1</definedName>
+    <definedName name="Property_Target_Keywords">Property!$X$1</definedName>
+    <definedName name="Property_Target_Name">Property!$R$1</definedName>
+    <definedName name="Property_Target_NamespacePrefix">Property!$O$1</definedName>
+    <definedName name="Property_Target_Style">Property!$W$1</definedName>
+    <definedName name="Property_Target_SubstitutionGroup">Property!$V$1</definedName>
+    <definedName name="Property_Target_UsageInfo">Property!$Z$1</definedName>
     <definedName name="Type_Mapping_Code">Type!$E$1</definedName>
     <definedName name="Type_Mapping_Description">Type!$F$1</definedName>
     <definedName name="Type_Mapping_Notes">Type!$G$1</definedName>
@@ -149,7 +149,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="836" uniqueCount="488">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1008" uniqueCount="616">
   <si>
     <t>Definition</t>
   </si>
@@ -2114,9 +2114,6 @@
     <t>Follow case no</t>
   </si>
   <si>
-    <t>??</t>
-  </si>
-  <si>
     <t>Case number</t>
   </si>
   <si>
@@ -2147,9 +2144,6 @@
     <t>number</t>
   </si>
   <si>
-    <t>Number of Co-defendants</t>
-  </si>
-  <si>
     <t>Date screened</t>
   </si>
   <si>
@@ -2174,21 +2168,6 @@
     <t>Case type</t>
   </si>
   <si>
-    <t>Refused Charge Name</t>
-  </si>
-  <si>
-    <t>Refused Charge Class</t>
-  </si>
-  <si>
-    <t>Refused Charge Statute</t>
-  </si>
-  <si>
-    <t>Refused Charge Modifier</t>
-  </si>
-  <si>
-    <t>Refused Charge Disposition Refusal Code</t>
-  </si>
-  <si>
     <t>Cardinality</t>
   </si>
   <si>
@@ -2226,27 +2205,6 @@
   </si>
   <si>
     <t>MiddleName</t>
-  </si>
-  <si>
-    <t>BOINumber</t>
-  </si>
-  <si>
-    <t>Accepted Charge Item Number</t>
-  </si>
-  <si>
-    <t>Accepted Charge Arrest Number</t>
-  </si>
-  <si>
-    <t>Accepted Charge Name</t>
-  </si>
-  <si>
-    <t>Accepted Charge Class</t>
-  </si>
-  <si>
-    <t>Accepted Charge Statute</t>
-  </si>
-  <si>
-    <t>Accepted Charge Modifier</t>
   </si>
   <si>
     <t>nc:ProperNameTextType</t>
@@ -2306,10 +2264,436 @@
     <t>A unique identifier of a law, rule, or ordinance within a jurisdiction that a person is accused of violating.</t>
   </si>
   <si>
-    <t>Grand Jury Indicator</t>
-  </si>
-  <si>
-    <t>True if this filing is a grand jury indictment</t>
+    <t>Identifier in NOPD’s local criminal history system (nee “MOTION”, now “Castnet”) - equivalent to a local SID. </t>
+  </si>
+  <si>
+    <t>nc:CourtCase/j:CaseAugmentation/j:CaseCourt/nola-ext:CourtAugmentation/nc:AddressCountyName</t>
+  </si>
+  <si>
+    <t>nola-ext:CourtAugmentationType</t>
+  </si>
+  <si>
+    <t>A name of a county, parish, vicinage, or other such geopolitical subdivision of a state.</t>
+  </si>
+  <si>
+    <t>nc:CourtCase/nc:CaseDocketID</t>
+  </si>
+  <si>
+    <t>nc:CaseType</t>
+  </si>
+  <si>
+    <t>An identifier used to reference a case docket.</t>
+  </si>
+  <si>
+    <t>nc:CourtCase/j:CaseAugmentation/j:CaseDefendantParty/nc:EntityPerson/nc:PersonName/nc:PersonSurName</t>
+  </si>
+  <si>
+    <t>A last name or family name of a person.</t>
+  </si>
+  <si>
+    <t>nc:PersonNameType</t>
+  </si>
+  <si>
+    <t>nc:CourtCase/j:CaseAugmentation/j:CaseDefendantParty/nc:EntityPerson/nc:PersonName/nc:PersonGivenName</t>
+  </si>
+  <si>
+    <t>nc:CourtCase/j:CaseAugmentation/j:CaseDefendantParty/nc:EntityPerson/nc:PersonName/nc:PersonMiddleName</t>
+  </si>
+  <si>
+    <t>A first name of a person.</t>
+  </si>
+  <si>
+    <t>A middle name of a person.</t>
+  </si>
+  <si>
+    <t>ContactInformation</t>
+  </si>
+  <si>
+    <t>ContactAddress</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>nc:CourtCase/j:CaseAugmentation/j:CaseDefendantParty/nc:EntityPerson/nc:PersonContactInformation/nc:ContactMailingAddress/nc:AddressFullText</t>
+  </si>
+  <si>
+    <t>nc:AddressFullText</t>
+  </si>
+  <si>
+    <t>A postal address by which a person or organization may be contacted.</t>
+  </si>
+  <si>
+    <t>nc:CourtCase/j:CaseAugmentation/j:CaseDefendantParty/nc:EntityPerson/nc:PersonBirthDate/nc:Date</t>
+  </si>
+  <si>
+    <t>nc:DateType (nc:PersonBirthDate)</t>
+  </si>
+  <si>
+    <t>nc:AddressType (nc:MailingAddress)</t>
+  </si>
+  <si>
+    <t>nc:CourtCase/j:CaseAugmentation/j:CaseDefendantParty/nc:EntityPerson/nc:PersonRaceText</t>
+  </si>
+  <si>
+    <t>nc:PersonType</t>
+  </si>
+  <si>
+    <t>A physical location at which a person may be contacted.</t>
+  </si>
+  <si>
+    <t>nc:CourtCase/j:CaseAugmentation/j:CaseDefendantParty/nc:EntityPerson/nc:PersonSexText</t>
+  </si>
+  <si>
+    <t>nc:PersonStateIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>nc:IdentificationType (nc:PersonStateIdentification)</t>
+  </si>
+  <si>
+    <t>An identification of a person based on a state-issued ID card.</t>
+  </si>
+  <si>
+    <t>nc:DateType (nc:ActivityDate)</t>
+  </si>
+  <si>
+    <t>0..*</t>
+  </si>
+  <si>
+    <t>nc:DateType nola-ext:OffenseDate)</t>
+  </si>
+  <si>
+    <t>A date of an activity.</t>
+  </si>
+  <si>
+    <t>nc:IdentificationTyper (nola-ext:JMSChargeNumber)</t>
+  </si>
+  <si>
+    <t>j:ChargeType</t>
+  </si>
+  <si>
+    <t>nc:IdentificationType (j:StatuteCodeIdentification)</t>
+  </si>
+  <si>
+    <t>An identification number of a set of laws for a particular jurisdiction.</t>
+  </si>
+  <si>
+    <t>ChargeIncoate</t>
+  </si>
+  <si>
+    <t>The text of the offense identified in the State statute or section of a statute. A degree of involvement a person is being charged with committing in an offense.</t>
+  </si>
+  <si>
+    <t>j:ChargeApplicabilityText</t>
+  </si>
+  <si>
+    <t>A degree of involvement a person is being charged with committing in an offense.</t>
+  </si>
+  <si>
+    <t>ChargeDispositionCode</t>
+  </si>
+  <si>
+    <t>CodeList</t>
+  </si>
+  <si>
+    <t>A value that describes the type of disposition.</t>
+  </si>
+  <si>
+    <t>nola-ext:ChargeAugmentationType</t>
+  </si>
+  <si>
+    <t>Charge Item Number</t>
+  </si>
+  <si>
+    <t>Charge Arrest Number</t>
+  </si>
+  <si>
+    <t>Charge Name</t>
+  </si>
+  <si>
+    <t>Charge Class</t>
+  </si>
+  <si>
+    <t>Charge Statute</t>
+  </si>
+  <si>
+    <t>Charge Modifier</t>
+  </si>
+  <si>
+    <t>Resufed Charge Disposition RefusalCode</t>
+  </si>
+  <si>
+    <t>ChargeDisposiotion</t>
+  </si>
+  <si>
+    <t>nola-ext:ChargeDispositionCode</t>
+  </si>
+  <si>
+    <t>nola-ext:ChargeDispositionCodeType</t>
+  </si>
+  <si>
+    <t>j:Arrest/j:ArrestCharge/nola-ext:ArrestAugmentation/nola-ext:OffenseDate</t>
+  </si>
+  <si>
+    <t>j:Arrest/nc:ActivityDate/nc:DateTime</t>
+  </si>
+  <si>
+    <t>j:Arrest/j:ArrestCharge/nola-ext:ChargeAugmentation/nola-ext:JMSChargeNumber</t>
+  </si>
+  <si>
+    <t>/j:Arrest/j:ArrestCharge//nola-ext:ChargeAugmentation/nola-ext:StatewideArrestTrackingNumber</t>
+  </si>
+  <si>
+    <t>j:Arrest/j:ArrestCharge/j:ChargeDescriptionText</t>
+  </si>
+  <si>
+    <t>/j:Arrest/j:ArrestCharge/j:ChargeSeverityDescriptionText</t>
+  </si>
+  <si>
+    <t>j:Arrest/j:ArrestCharge/j:ChargeStatute/j:StatuteCodeIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>j:Arrest/j:ArrestCharge/j:ChargeApplicabilityText</t>
+  </si>
+  <si>
+    <t>j:Arrest/j:ArrestCharge/nola-ext:ChargeAugmentation/nola-ext:ChargeDispositionCode</t>
+  </si>
+  <si>
+    <t>ArrestDispositionCode</t>
+  </si>
+  <si>
+    <t>Indicates whether the arrest is accepted, refused, diverted, or referred.</t>
+  </si>
+  <si>
+    <t>j:Arrest/noa-ext:ArrestAugmentation/nola-ext:ArrestDispositionCode</t>
+  </si>
+  <si>
+    <t>nola-ext:ArrestDispositionCode</t>
+  </si>
+  <si>
+    <t>nola-ext:ArrestDispositionCodeType</t>
+  </si>
+  <si>
+    <t>nola-ext:ArrestAugmentationType</t>
+  </si>
+  <si>
+    <t>Indicates whether the arrest is accepted (any charge accepted), refused (all charges refused), diverted, or referred.</t>
+  </si>
+  <si>
+    <t>ArrestReceivedDate</t>
+  </si>
+  <si>
+    <t>The date the prosecutor received the arrest</t>
+  </si>
+  <si>
+    <t>j:Arrest/noa-ext:ArrestAugmentation/nola-ext:ArrestReceivedDate/nc:Date</t>
+  </si>
+  <si>
+    <t>nc:Date Type (nola-ext:ArrestReceivedDate)</t>
+  </si>
+  <si>
+    <t>nola-ext:CaseAugmentationType</t>
+  </si>
+  <si>
+    <t>niem-xs:boolean</t>
+  </si>
+  <si>
+    <t>Identifies the court section to transfer this case</t>
+  </si>
+  <si>
+    <t>Identifies an existing court case that this case should follow</t>
+  </si>
+  <si>
+    <t>Indicates whether the case is a standalone misdemeanor</t>
+  </si>
+  <si>
+    <t>nc:CourtCase/nola-ext:CaseAugmentation/nola-ext:CourtCaseStandaloneMisdemeanorIndicator</t>
+  </si>
+  <si>
+    <t>nola-ext:CourtCaseStandaloneMisdemeanorIndicator</t>
+  </si>
+  <si>
+    <t>nc:CourtCase/nola-ext:CaseAugmentation/nola-ext:CourtCaseTransferToSectionIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>nc:CourtCase/nola-ext:CaseAugmentation/nola-ext:CourtCaseFollowCaseIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>nc:IdentificationType (nola-ext:CourtCaseTransferToSectionID)</t>
+  </si>
+  <si>
+    <t>nc:IdentificationType (nola-ext:CourtCaseFollowCaseID)</t>
+  </si>
+  <si>
+    <t>CourtCaseStandaloneMisdemeanorIndicator</t>
+  </si>
+  <si>
+    <t>CourtCaseTransferToSectionID</t>
+  </si>
+  <si>
+    <t>CourtCaseFollowCaseID</t>
+  </si>
+  <si>
+    <t>Prosecutor System Magistrate Case Number</t>
+  </si>
+  <si>
+    <t>Co-defendants</t>
+  </si>
+  <si>
+    <t>Name of co-defendants</t>
+  </si>
+  <si>
+    <t>ProsecutorCaseNumber</t>
+  </si>
+  <si>
+    <t>ProsecutorCase</t>
+  </si>
+  <si>
+    <t>Date an ADA screened this case</t>
+  </si>
+  <si>
+    <t>ADA who screened this case</t>
+  </si>
+  <si>
+    <t>Date an ADA reviewed the screening of this case</t>
+  </si>
+  <si>
+    <t>Person</t>
+  </si>
+  <si>
+    <t>PersonName</t>
+  </si>
+  <si>
+    <t>nc:CourtCase/j:CaseAugmentation/j:CaseDefendantParty/nc:EntityPerson/nc:PersonName</t>
+  </si>
+  <si>
+    <t>nc:Person</t>
+  </si>
+  <si>
+    <t>nc:PersonName'</t>
+  </si>
+  <si>
+    <t>A combination of names and/or titles by which a person is known.</t>
+  </si>
+  <si>
+    <t>nc:IdentificationType (nola-ext:PersonLocalIdentification)</t>
+  </si>
+  <si>
+    <t>nc:CourtCase/j:CaseAugmentation/j:CaseDefendantParty/nc:EntityPerson/nola-ext:PersonAugmentation/nola-ext:PersonLocalIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>PersonIdentifiers</t>
+  </si>
+  <si>
+    <t>PersonLocalIdentification</t>
+  </si>
+  <si>
+    <t>ProsecutorCaseScreenedDate</t>
+  </si>
+  <si>
+    <t>ProsecutorCaseScreenedPerson</t>
+  </si>
+  <si>
+    <t>ProsecutorCaseReviewedPerson</t>
+  </si>
+  <si>
+    <t>Name of prosecutor who screened this case</t>
+  </si>
+  <si>
+    <t>Name of prosecutor who reviewed this case</t>
+  </si>
+  <si>
+    <t>A name of a unit of a court. CDC or MC</t>
+  </si>
+  <si>
+    <t>CaseType</t>
+  </si>
+  <si>
+    <t>nc:CourtCase/nc:CaseGeneralCategoryText</t>
+  </si>
+  <si>
+    <t>j:CaseType</t>
+  </si>
+  <si>
+    <t>nc:CaseGeneralCategoryText</t>
+  </si>
+  <si>
+    <t>A broadly defined kind of case.</t>
+  </si>
+  <si>
+    <t>nola-ext:ProsecutorCase/nc:CaseTrackingID</t>
+  </si>
+  <si>
+    <t>nc:CaseTrackingID</t>
+  </si>
+  <si>
+    <t>An identifier used to track a case.</t>
+  </si>
+  <si>
+    <t>nola-ext:ProsecutorCase/nola-ext:ProsecutorCaseScreenedDate/nc:Date</t>
+  </si>
+  <si>
+    <t>nc:DateType (nola-ext:ProsecutorCaseScreenedDate)</t>
+  </si>
+  <si>
+    <t>nola-ext:ProsecutorCase/nola-ext:ProsecutorCaseScreenedPerson/nc:PersonName</t>
+  </si>
+  <si>
+    <t>nola-ext:ProsecutorCase/nola-ext:ProsecutorCaseReviewedPerson/nc:PersonName</t>
+  </si>
+  <si>
+    <t>nc:PersonType (nola-ext:ProsecutorCaseScreenedPerson)</t>
+  </si>
+  <si>
+    <t>nc:PersonType (nola-ext:ProsecutorCaseReviewedPerson)</t>
+  </si>
+  <si>
+    <t>nc:PersonName</t>
+  </si>
+  <si>
+    <t>Example</t>
+  </si>
+  <si>
+    <t>Parish of Orleans</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>M999999</t>
+  </si>
+  <si>
+    <t>Doe</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>100 Main St, New Orleans, LA</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>James Smith</t>
+  </si>
+  <si>
+    <t>John Smith</t>
+  </si>
+  <si>
+    <t>6TH DISTRICT CASE</t>
+  </si>
+  <si>
+    <t>H-26560-24</t>
+  </si>
+  <si>
+    <t>CARNAL KNOWLEDGE</t>
+  </si>
+  <si>
+    <t>F/3</t>
   </si>
 </sst>
 </file>
@@ -2669,7 +3053,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2899,6 +3283,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="71">
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
@@ -2973,7 +3369,262 @@
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="124">
+  <dxfs count="125">
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -3660,258 +4311,6 @@
         <color theme="0"/>
         <name val="Calibri"/>
         <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -4122,66 +4521,66 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A5:D13" totalsRowShown="0" headerRowDxfId="123" dataDxfId="122">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A5:D13" totalsRowShown="0" headerRowDxfId="124" dataDxfId="123">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Document" dataDxfId="121"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Description" dataDxfId="120"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Source fields_x000a_(blue column headers)" dataDxfId="119"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Target fields_x000a_(red column headers)" dataDxfId="118"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Document" dataDxfId="122"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Description" dataDxfId="121"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Source fields_x000a_(blue column headers)" dataDxfId="120"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Target fields_x000a_(red column headers)" dataDxfId="119"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{733D753A-1A77-494A-B62C-0EC743EEA49A}" name="Table10" displayName="Table10" ref="A1:N2" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28" tableBorderDxfId="27" headerRowCellStyle="Accent2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{733D753A-1A77-494A-B62C-0EC743EEA49A}" name="Table10" displayName="Table10" ref="A1:N2" totalsRowShown="0" headerRowDxfId="57" dataDxfId="56" tableBorderDxfId="55" headerRowCellStyle="Accent2">
   <autoFilter ref="A1:N2" xr:uid="{E1E5EF99-DFA3-4734-B0F5-3FD6CA399E33}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{E1238927-B089-4D9E-8088-75D3EC35BFBA}" name="Source_x000a_NS Prefix" dataDxfId="26"/>
-    <tableColumn id="2" xr3:uid="{9410951A-EE35-4F3C-8F36-8BEE201CF8AF}" name="URI" dataDxfId="25"/>
-    <tableColumn id="3" xr3:uid="{2B517D23-941B-4B3E-A7DD-F7786E3924D5}" name="Definition" dataDxfId="24"/>
-    <tableColumn id="4" xr3:uid="{7DD55007-8311-4C82-A5D2-EBEDF474C65D}" name="Mapping_x000a_Code" dataDxfId="23"/>
-    <tableColumn id="5" xr3:uid="{0E949C96-18B4-4EB9-95F2-53DB84718832}" name="Description" dataDxfId="22"/>
-    <tableColumn id="6" xr3:uid="{E124F618-8325-4FF3-8BF4-E24907425ADE}" name="Notes" dataDxfId="21"/>
-    <tableColumn id="7" xr3:uid="{86983FC7-E843-4CB8-B776-1ACA5758C454}" name="Target_x000a_NS Prefix" dataDxfId="20"/>
-    <tableColumn id="8" xr3:uid="{F92DB840-CE8A-4128-8BB8-B8742F926D09}" name="Style" dataDxfId="19"/>
-    <tableColumn id="9" xr3:uid="{9202EAB5-4BBC-4DFA-8B29-56D32F2F95E2}" name="URI " dataDxfId="18"/>
-    <tableColumn id="10" xr3:uid="{BE82DF52-562E-40A7-B97A-C4017DCE324F}" name="Definition " dataDxfId="17"/>
-    <tableColumn id="11" xr3:uid="{834B3B3E-609B-4AA7-A013-2F95C8CA6ED1}" name="NDR Target" dataDxfId="16"/>
-    <tableColumn id="12" xr3:uid="{9C74517B-484A-41A5-B478-1107D7B7563E}" name="File Name" dataDxfId="15"/>
-    <tableColumn id="13" xr3:uid="{00E1E65A-D173-41FF-8A1D-F764DB3C85EB}" name="Relative Path" dataDxfId="14"/>
-    <tableColumn id="14" xr3:uid="{1A319080-CB5B-4F50-8EF6-DA7F3E87061A}" name="Draft Version" dataDxfId="13"/>
+    <tableColumn id="1" xr3:uid="{E1238927-B089-4D9E-8088-75D3EC35BFBA}" name="Source_x000a_NS Prefix" dataDxfId="54"/>
+    <tableColumn id="2" xr3:uid="{9410951A-EE35-4F3C-8F36-8BEE201CF8AF}" name="URI" dataDxfId="53"/>
+    <tableColumn id="3" xr3:uid="{2B517D23-941B-4B3E-A7DD-F7786E3924D5}" name="Definition" dataDxfId="52"/>
+    <tableColumn id="4" xr3:uid="{7DD55007-8311-4C82-A5D2-EBEDF474C65D}" name="Mapping_x000a_Code" dataDxfId="51"/>
+    <tableColumn id="5" xr3:uid="{0E949C96-18B4-4EB9-95F2-53DB84718832}" name="Description" dataDxfId="50"/>
+    <tableColumn id="6" xr3:uid="{E124F618-8325-4FF3-8BF4-E24907425ADE}" name="Notes" dataDxfId="49"/>
+    <tableColumn id="7" xr3:uid="{86983FC7-E843-4CB8-B776-1ACA5758C454}" name="Target_x000a_NS Prefix" dataDxfId="48"/>
+    <tableColumn id="8" xr3:uid="{F92DB840-CE8A-4128-8BB8-B8742F926D09}" name="Style" dataDxfId="47"/>
+    <tableColumn id="9" xr3:uid="{9202EAB5-4BBC-4DFA-8B29-56D32F2F95E2}" name="URI " dataDxfId="46"/>
+    <tableColumn id="10" xr3:uid="{BE82DF52-562E-40A7-B97A-C4017DCE324F}" name="Definition " dataDxfId="45"/>
+    <tableColumn id="11" xr3:uid="{834B3B3E-609B-4AA7-A013-2F95C8CA6ED1}" name="NDR Target" dataDxfId="44"/>
+    <tableColumn id="12" xr3:uid="{9C74517B-484A-41A5-B478-1107D7B7563E}" name="File Name" dataDxfId="43"/>
+    <tableColumn id="13" xr3:uid="{00E1E65A-D173-41FF-8A1D-F764DB3C85EB}" name="Relative Path" dataDxfId="42"/>
+    <tableColumn id="14" xr3:uid="{1A319080-CB5B-4F50-8EF6-DA7F3E87061A}" name="Draft Version" dataDxfId="41"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{6A256153-0806-4BEE-936A-A12F0A0B7383}" name="Table11" displayName="Table11" ref="A1:K2" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11" headerRowCellStyle="Accent2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{6A256153-0806-4BEE-936A-A12F0A0B7383}" name="Table11" displayName="Table11" ref="A1:K2" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39" headerRowCellStyle="Accent2">
   <autoFilter ref="A1:K2" xr:uid="{79E81683-51FB-4FF9-9289-31DDA054DB7A}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{B23F336D-16B9-4C95-BE96-F5283EAE0F3C}" name="Source_x000a_NS Prefix" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{0D056408-CA8F-4336-AED7-3818011F9385}" name="Term" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{90A93FC4-10F0-4295-AC5C-E2A951CBA7BC}" name="Literal" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{A1AC1DB1-AA7D-48B2-9765-4E5BA52F23DE}" name="Definition" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{BD7B43BD-647B-4803-8F9F-0147C7FD23A4}" name="Mapping_x000a_Code" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{72609C76-FA3F-40C0-B5FF-60D4974FFD61}" name="Description" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{479204AB-0608-4CE8-8D22-F418523DDDA2}" name="Notes" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{2C9C9513-0007-44E3-8DFD-9FDD58431071}" name="Target_x000a_NS Prefix" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{1442C4F6-90A1-4765-A362-538E7A781367}" name="Term " dataDxfId="2"/>
-    <tableColumn id="10" xr3:uid="{92198433-569D-43D9-9243-453965C7540B}" name="Literal " dataDxfId="1"/>
-    <tableColumn id="11" xr3:uid="{38E45C62-D7D7-487A-BB8B-582528BBD31D}" name="Definition " dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{B23F336D-16B9-4C95-BE96-F5283EAE0F3C}" name="Source_x000a_NS Prefix" dataDxfId="38"/>
+    <tableColumn id="2" xr3:uid="{0D056408-CA8F-4336-AED7-3818011F9385}" name="Term" dataDxfId="37"/>
+    <tableColumn id="3" xr3:uid="{90A93FC4-10F0-4295-AC5C-E2A951CBA7BC}" name="Literal" dataDxfId="36"/>
+    <tableColumn id="4" xr3:uid="{A1AC1DB1-AA7D-48B2-9765-4E5BA52F23DE}" name="Definition" dataDxfId="35"/>
+    <tableColumn id="5" xr3:uid="{BD7B43BD-647B-4803-8F9F-0147C7FD23A4}" name="Mapping_x000a_Code" dataDxfId="34"/>
+    <tableColumn id="6" xr3:uid="{72609C76-FA3F-40C0-B5FF-60D4974FFD61}" name="Description" dataDxfId="33"/>
+    <tableColumn id="7" xr3:uid="{479204AB-0608-4CE8-8D22-F418523DDDA2}" name="Notes" dataDxfId="32"/>
+    <tableColumn id="8" xr3:uid="{2C9C9513-0007-44E3-8DFD-9FDD58431071}" name="Target_x000a_NS Prefix" dataDxfId="31"/>
+    <tableColumn id="9" xr3:uid="{1442C4F6-90A1-4765-A362-538E7A781367}" name="Term " dataDxfId="30"/>
+    <tableColumn id="10" xr3:uid="{92198433-569D-43D9-9243-453965C7540B}" name="Literal " dataDxfId="29"/>
+    <tableColumn id="11" xr3:uid="{38E45C62-D7D7-487A-BB8B-582528BBD31D}" name="Definition " dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table1" displayName="Table1" ref="A31:B40" totalsRowShown="0" headerRowDxfId="117" dataDxfId="116" tableBorderDxfId="115" headerRowCellStyle="Neutral">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table1" displayName="Table1" ref="A31:B40" totalsRowShown="0" headerRowDxfId="118" dataDxfId="117" tableBorderDxfId="116" headerRowCellStyle="Neutral">
   <autoFilter ref="A31:B40" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Tips and tricks" dataDxfId="114"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Description" dataDxfId="113"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Tips and tricks" dataDxfId="115"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Description" dataDxfId="114"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4190,8 +4589,8 @@
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table4" displayName="Table4" ref="A2:B9" totalsRowShown="0">
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="SOURCE INFORMATION" dataDxfId="112"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name=" " dataDxfId="111"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="SOURCE INFORMATION" dataDxfId="113"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name=" " dataDxfId="112"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4200,8 +4599,8 @@
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table5" displayName="Table5" ref="A12:B17" totalsRowShown="0">
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="MAPPING INFORMATION" dataDxfId="110"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name=" " dataDxfId="109"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="MAPPING INFORMATION" dataDxfId="111"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name=" " dataDxfId="110"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4210,113 +4609,114 @@
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table6" displayName="Table6" ref="A20:B26" totalsRowShown="0">
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="TARGET INFORMATION" dataDxfId="108"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name=" " dataDxfId="107"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="TARGET INFORMATION" dataDxfId="109"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name=" " dataDxfId="108"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table3" displayName="Table3" ref="A1:Y55" totalsRowShown="0" headerRowDxfId="106" dataDxfId="105" headerRowCellStyle="Accent2">
-  <autoFilter ref="A1:Y55" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
-  <tableColumns count="25">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Source_x000a_NS Prefix" dataDxfId="104"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Property Name" dataDxfId="103"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="Data Type" dataDxfId="102"/>
-    <tableColumn id="18" xr3:uid="{683B832A-0F1B-48CA-AA01-7512CABFD6B2}" name="Definition" dataDxfId="101"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="Cardinality" dataDxfId="100"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="Mapping_x000a_Code" dataDxfId="99"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="Description" dataDxfId="98"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0500-000007000000}" name="Notes" dataDxfId="97"/>
-    <tableColumn id="24" xr3:uid="{B256BE0E-1B95-49D2-BF5B-AD5320663854}" name="EDM Class" dataDxfId="96"/>
-    <tableColumn id="23" xr3:uid="{C5C0958E-E98B-4096-B70E-A6517F49A64D}" name="EDM Attribute" dataDxfId="95"/>
-    <tableColumn id="14" xr3:uid="{70B266EE-E89C-4B0F-ACFB-6BBC1BBE7978}" name="EDM Type" dataDxfId="94"/>
-    <tableColumn id="26" xr3:uid="{B613C991-CC70-4831-83C3-97449E0A59FB}" name="EDM Definition" dataDxfId="93"/>
-    <tableColumn id="27" xr3:uid="{9FF11716-702A-419A-91F2-858D4D3B16EE}" name="EDM Cardinality" dataDxfId="92"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0500-000008000000}" name="Target_x000a_NS Prefix" dataDxfId="91"/>
-    <tableColumn id="20" xr3:uid="{8CFFA3EE-5D28-4D5E-86E0-9F9851A3E676}" name="NIEM XPath" dataDxfId="90"/>
-    <tableColumn id="25" xr3:uid="{161AA4D8-B799-4722-BAB9-DA7BA3B360DA}" name="NIEM Type" dataDxfId="89"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0500-000009000000}" name="NIEM Property Name " dataDxfId="88"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0500-00000A000000}" name="NIEM Qualified Data Type" dataDxfId="87"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0500-00000B000000}" name="NIEM Definition " dataDxfId="86"/>
-    <tableColumn id="19" xr3:uid="{C2DBDA77-E9BC-497B-A1D8-611484B019B5}" name="Cardinality2" dataDxfId="85"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0500-00000C000000}" name="NIEM Qualified Substitution Group" dataDxfId="84"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0500-00000D000000}" name="Style_x000a_default=element" dataDxfId="83"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0500-00000F000000}" name="Keywords" dataDxfId="82"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0500-000010000000}" name="Example Content" dataDxfId="81"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0500-000011000000}" name="Usage Info" dataDxfId="80"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table3" displayName="Table3" ref="A1:Z35" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26" headerRowCellStyle="Accent2">
+  <autoFilter ref="A1:Z35" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+  <tableColumns count="26">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Source_x000a_NS Prefix" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Property Name" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="Data Type" dataDxfId="23"/>
+    <tableColumn id="18" xr3:uid="{683B832A-0F1B-48CA-AA01-7512CABFD6B2}" name="Definition" dataDxfId="2"/>
+    <tableColumn id="21" xr3:uid="{42F421B2-5200-43B9-8173-69699FE1D709}" name="Example" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="Cardinality" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="Mapping_x000a_Code" dataDxfId="22"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="Description" dataDxfId="21"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0500-000007000000}" name="Notes" dataDxfId="20"/>
+    <tableColumn id="24" xr3:uid="{B256BE0E-1B95-49D2-BF5B-AD5320663854}" name="EDM Class" dataDxfId="19"/>
+    <tableColumn id="23" xr3:uid="{C5C0958E-E98B-4096-B70E-A6517F49A64D}" name="EDM Attribute" dataDxfId="18"/>
+    <tableColumn id="14" xr3:uid="{70B266EE-E89C-4B0F-ACFB-6BBC1BBE7978}" name="EDM Type" dataDxfId="17"/>
+    <tableColumn id="26" xr3:uid="{B613C991-CC70-4831-83C3-97449E0A59FB}" name="EDM Definition" dataDxfId="16"/>
+    <tableColumn id="27" xr3:uid="{9FF11716-702A-419A-91F2-858D4D3B16EE}" name="EDM Cardinality" dataDxfId="15"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0500-000008000000}" name="Target_x000a_NS Prefix" dataDxfId="14"/>
+    <tableColumn id="20" xr3:uid="{8CFFA3EE-5D28-4D5E-86E0-9F9851A3E676}" name="NIEM XPath" dataDxfId="13"/>
+    <tableColumn id="25" xr3:uid="{161AA4D8-B799-4722-BAB9-DA7BA3B360DA}" name="NIEM Type" dataDxfId="12"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0500-000009000000}" name="NIEM Property Name " dataDxfId="11"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0500-00000A000000}" name="NIEM Qualified Data Type" dataDxfId="10"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0500-00000B000000}" name="NIEM Definition " dataDxfId="9"/>
+    <tableColumn id="19" xr3:uid="{C2DBDA77-E9BC-497B-A1D8-611484B019B5}" name="Cardinality2" dataDxfId="8"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0500-00000C000000}" name="NIEM Qualified Substitution Group" dataDxfId="7"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0500-00000D000000}" name="Style_x000a_default=element" dataDxfId="6"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0500-00000F000000}" name="Keywords" dataDxfId="5"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0500-000010000000}" name="Example Content" dataDxfId="4"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0500-000011000000}" name="Usage Info" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{8578AF98-37D1-469F-9DF8-407CA14E272E}" name="Table7" displayName="Table7" ref="A1:N2" insertRow="1" totalsRowShown="0" headerRowDxfId="79" dataDxfId="78" headerRowCellStyle="Accent2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{8578AF98-37D1-469F-9DF8-407CA14E272E}" name="Table7" displayName="Table7" ref="A1:N2" insertRow="1" totalsRowShown="0" headerRowDxfId="107" dataDxfId="106" headerRowCellStyle="Accent2">
   <autoFilter ref="A1:N2" xr:uid="{C7C77A82-0E27-43B2-B802-78C571058434}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{2DA18095-6134-4F51-B45C-1FD29868E9D3}" name="Source_x000a_NS Prefix" dataDxfId="77"/>
-    <tableColumn id="2" xr3:uid="{BB7222D3-DF23-4FB4-AACC-7074C8351301}" name="Type Name" dataDxfId="76"/>
-    <tableColumn id="3" xr3:uid="{3AFA1B4A-1B7D-4408-95C4-5D276F6AFCE8}" name="Parent / Base Type" dataDxfId="75"/>
-    <tableColumn id="4" xr3:uid="{DA420D7E-BF45-4DFA-A327-6F5816081658}" name="Definition" dataDxfId="74"/>
-    <tableColumn id="5" xr3:uid="{F0EC8E3B-3924-4431-8523-4FE53C5BC2F9}" name="Mapping_x000a_Code" dataDxfId="73"/>
-    <tableColumn id="6" xr3:uid="{529DD89A-D9F2-4643-B653-535C5D5260B2}" name="Description" dataDxfId="72"/>
-    <tableColumn id="7" xr3:uid="{6A865D88-3AC4-4546-981B-9A5A7EB8F351}" name="Notes" dataDxfId="71"/>
-    <tableColumn id="8" xr3:uid="{FF25761D-56AD-4BA0-8910-6C18CBA6D0CD}" name="Target_x000a_NS Prefix" dataDxfId="70"/>
-    <tableColumn id="9" xr3:uid="{B5902010-EF7D-4FA2-B2B6-B491046CA96D}" name="Type Name " dataDxfId="69"/>
-    <tableColumn id="10" xr3:uid="{422CF2D7-F9C5-4193-9DD3-943BF799ABB8}" name="Qualified Parent / Base Type " dataDxfId="68"/>
-    <tableColumn id="11" xr3:uid="{E69F557F-28BC-41CA-B77C-8F0F1781F3F8}" name="Definition " dataDxfId="67"/>
-    <tableColumn id="12" xr3:uid="{33FAD9D1-2E3A-4DD0-99A3-80B7DC1320DF}" name="Style _x000a_default=object" dataDxfId="66"/>
-    <tableColumn id="13" xr3:uid="{A3613263-4395-41B2-9149-1319C9DE1572}" name="Qualified Union Member Types_x000a_comma-separated list" dataDxfId="65"/>
-    <tableColumn id="14" xr3:uid="{DA9EC388-28FD-4FFC-9EB0-04AF1B5F2EBE}" name="Qualified Metadata Applies to Types_x000a_comma-separated list" dataDxfId="64"/>
+    <tableColumn id="1" xr3:uid="{2DA18095-6134-4F51-B45C-1FD29868E9D3}" name="Source_x000a_NS Prefix" dataDxfId="105"/>
+    <tableColumn id="2" xr3:uid="{BB7222D3-DF23-4FB4-AACC-7074C8351301}" name="Type Name" dataDxfId="104"/>
+    <tableColumn id="3" xr3:uid="{3AFA1B4A-1B7D-4408-95C4-5D276F6AFCE8}" name="Parent / Base Type" dataDxfId="103"/>
+    <tableColumn id="4" xr3:uid="{DA420D7E-BF45-4DFA-A327-6F5816081658}" name="Definition" dataDxfId="102"/>
+    <tableColumn id="5" xr3:uid="{F0EC8E3B-3924-4431-8523-4FE53C5BC2F9}" name="Mapping_x000a_Code" dataDxfId="101"/>
+    <tableColumn id="6" xr3:uid="{529DD89A-D9F2-4643-B653-535C5D5260B2}" name="Description" dataDxfId="100"/>
+    <tableColumn id="7" xr3:uid="{6A865D88-3AC4-4546-981B-9A5A7EB8F351}" name="Notes" dataDxfId="99"/>
+    <tableColumn id="8" xr3:uid="{FF25761D-56AD-4BA0-8910-6C18CBA6D0CD}" name="Target_x000a_NS Prefix" dataDxfId="98"/>
+    <tableColumn id="9" xr3:uid="{B5902010-EF7D-4FA2-B2B6-B491046CA96D}" name="Type Name " dataDxfId="97"/>
+    <tableColumn id="10" xr3:uid="{422CF2D7-F9C5-4193-9DD3-943BF799ABB8}" name="Qualified Parent / Base Type " dataDxfId="96"/>
+    <tableColumn id="11" xr3:uid="{E69F557F-28BC-41CA-B77C-8F0F1781F3F8}" name="Definition " dataDxfId="95"/>
+    <tableColumn id="12" xr3:uid="{33FAD9D1-2E3A-4DD0-99A3-80B7DC1320DF}" name="Style _x000a_default=object" dataDxfId="94"/>
+    <tableColumn id="13" xr3:uid="{A3613263-4395-41B2-9149-1319C9DE1572}" name="Qualified Union Member Types_x000a_comma-separated list" dataDxfId="93"/>
+    <tableColumn id="14" xr3:uid="{DA9EC388-28FD-4FFC-9EB0-04AF1B5F2EBE}" name="Qualified Metadata Applies to Types_x000a_comma-separated list" dataDxfId="92"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="Table8" displayName="Table8" ref="A1:Q2" insertRow="1" totalsRowShown="0" headerRowDxfId="63" dataDxfId="62">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="Table8" displayName="Table8" ref="A1:Q2" insertRow="1" totalsRowShown="0" headerRowDxfId="91" dataDxfId="90">
   <autoFilter ref="A1:Q2" xr:uid="{00000000-0009-0000-0100-000008000000}"/>
   <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="Source_x000a_Type NS" dataDxfId="61"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="Type Name" dataDxfId="60"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0600-000003000000}" name="Property NS" dataDxfId="59"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0600-000004000000}" name="Property Name" dataDxfId="58"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0600-000005000000}" name="Min" dataDxfId="57"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0600-000006000000}" name="Max" dataDxfId="56"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0600-000007000000}" name="Mapping_x000a_Code" dataDxfId="55"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0600-000008000000}" name="Description" dataDxfId="54"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0600-000009000000}" name="Notes" dataDxfId="53"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0600-00000A000000}" name="Target_x000a_Type NS" dataDxfId="52"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0600-00000B000000}" name="Type Name " dataDxfId="51"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0600-00000C000000}" name="Property NS " dataDxfId="50"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0600-00000D000000}" name="Property Name " dataDxfId="49"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0600-00000E000000}" name="Min_x000a_(default=0)" dataDxfId="48"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0600-00000F000000}" name="Max (default_x000a_=unbounded)" dataDxfId="47"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0600-000010000000}" name="Definition_x000a_For an external property in an adapter type" dataDxfId="46"/>
-    <tableColumn id="17" xr3:uid="{78D268D1-27FA-4E25-9781-8F942EC05BA0}" name="Sequence" dataDxfId="45"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="Source_x000a_Type NS" dataDxfId="89"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="Type Name" dataDxfId="88"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0600-000003000000}" name="Property NS" dataDxfId="87"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0600-000004000000}" name="Property Name" dataDxfId="86"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0600-000005000000}" name="Min" dataDxfId="85"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0600-000006000000}" name="Max" dataDxfId="84"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0600-000007000000}" name="Mapping_x000a_Code" dataDxfId="83"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0600-000008000000}" name="Description" dataDxfId="82"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0600-000009000000}" name="Notes" dataDxfId="81"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0600-00000A000000}" name="Target_x000a_Type NS" dataDxfId="80"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0600-00000B000000}" name="Type Name " dataDxfId="79"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0600-00000C000000}" name="Property NS " dataDxfId="78"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0600-00000D000000}" name="Property Name " dataDxfId="77"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0600-00000E000000}" name="Min_x000a_(default=0)" dataDxfId="76"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0600-00000F000000}" name="Max (default_x000a_=unbounded)" dataDxfId="75"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0600-000010000000}" name="Definition_x000a_For an external property in an adapter type" dataDxfId="74"/>
+    <tableColumn id="17" xr3:uid="{78D268D1-27FA-4E25-9781-8F942EC05BA0}" name="Sequence" dataDxfId="73"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="Table13" displayName="Table13" ref="A1:M2" totalsRowShown="0" headerRowDxfId="44" dataDxfId="43" headerRowCellStyle="Accent2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="Table13" displayName="Table13" ref="A1:M2" totalsRowShown="0" headerRowDxfId="72" dataDxfId="71" headerRowCellStyle="Accent2">
   <autoFilter ref="A1:M2" xr:uid="{00000000-0009-0000-0100-00000D000000}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="Source_x000a_NS Prefix" dataDxfId="42"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0700-000002000000}" name="Type Name" dataDxfId="41"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0700-000003000000}" name="Value" dataDxfId="40"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0700-000004000000}" name="Definition" dataDxfId="39"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0700-000005000000}" name="Style_x000a_default=enumeration" dataDxfId="38"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0700-000006000000}" name="Mapping_x000a_Code" dataDxfId="37"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0700-000007000000}" name="Description" dataDxfId="36"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0700-000008000000}" name="Notes" dataDxfId="35"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0700-000009000000}" name="Target_x000a_NS Prefix" dataDxfId="34"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0700-00000A000000}" name="Type Name " dataDxfId="33"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0700-00000B000000}" name="Value " dataDxfId="32"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0700-00000C000000}" name="Definition " dataDxfId="31"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0700-00000D000000}" name="Style_x000a_default=enumeration " dataDxfId="30"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="Source_x000a_NS Prefix" dataDxfId="70"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0700-000002000000}" name="Type Name" dataDxfId="69"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0700-000003000000}" name="Value" dataDxfId="68"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0700-000004000000}" name="Definition" dataDxfId="67"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0700-000005000000}" name="Style_x000a_default=enumeration" dataDxfId="66"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0700-000006000000}" name="Mapping_x000a_Code" dataDxfId="65"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0700-000007000000}" name="Description" dataDxfId="64"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0700-000008000000}" name="Notes" dataDxfId="63"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0700-000009000000}" name="Target_x000a_NS Prefix" dataDxfId="62"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0700-00000A000000}" name="Type Name " dataDxfId="61"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0700-00000B000000}" name="Value " dataDxfId="60"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0700-00000C000000}" name="Definition " dataDxfId="59"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0700-00000D000000}" name="Style_x000a_default=enumeration " dataDxfId="58"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -6871,43 +7271,45 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:AA55"/>
+  <dimension ref="A1:AB47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B14" sqref="B14"/>
+      <selection pane="bottomRight" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="11.6640625" style="2" hidden="1" customWidth="1"/>
     <col min="2" max="2" width="16.59765625" style="2" customWidth="1"/>
-    <col min="3" max="4" width="7.265625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="17.19921875" style="84" customWidth="1"/>
-    <col min="6" max="6" width="4.9296875" style="2" hidden="1" customWidth="1"/>
-    <col min="7" max="8" width="22.6640625" style="2" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="8.796875" style="2" customWidth="1"/>
-    <col min="10" max="11" width="13.06640625" style="2" customWidth="1"/>
-    <col min="12" max="12" width="22.6640625" style="2" customWidth="1"/>
-    <col min="13" max="13" width="7.06640625" style="2" customWidth="1"/>
-    <col min="14" max="14" width="5.06640625" style="2" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="15.9296875" style="2" customWidth="1"/>
-    <col min="16" max="16" width="11.6640625" style="2" customWidth="1"/>
-    <col min="17" max="17" width="19.53125" style="2" customWidth="1"/>
-    <col min="18" max="18" width="11.53125" style="2" customWidth="1"/>
-    <col min="19" max="19" width="14.46484375" style="2" customWidth="1"/>
-    <col min="20" max="20" width="4.796875" style="2" hidden="1" customWidth="1"/>
-    <col min="22" max="22" width="29.6640625" style="2" hidden="1" customWidth="1"/>
-    <col min="23" max="23" width="17.33203125" style="2" hidden="1" customWidth="1"/>
-    <col min="24" max="24" width="31.33203125" style="2" hidden="1" customWidth="1"/>
-    <col min="25" max="26" width="31.86328125" style="2" hidden="1" customWidth="1"/>
-    <col min="27" max="27" width="31.86328125" style="2" customWidth="1"/>
-    <col min="28" max="16384" width="8.86328125" style="2"/>
+    <col min="3" max="3" width="7.265625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="12.46484375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="12.46484375" style="87" customWidth="1"/>
+    <col min="6" max="6" width="17.19921875" style="84" customWidth="1"/>
+    <col min="7" max="7" width="4.9296875" style="2" customWidth="1"/>
+    <col min="8" max="9" width="22.6640625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="8.796875" style="2" customWidth="1"/>
+    <col min="11" max="12" width="13.06640625" style="2" customWidth="1"/>
+    <col min="13" max="13" width="22.6640625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="7.06640625" style="2" customWidth="1"/>
+    <col min="15" max="15" width="5.06640625" style="2" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="15.9296875" style="2" customWidth="1"/>
+    <col min="17" max="17" width="11.6640625" style="2" customWidth="1"/>
+    <col min="18" max="18" width="19.53125" style="2" customWidth="1"/>
+    <col min="19" max="19" width="11.53125" style="2" customWidth="1"/>
+    <col min="20" max="20" width="14.46484375" style="2" customWidth="1"/>
+    <col min="21" max="21" width="4.796875" style="2" hidden="1" customWidth="1"/>
+    <col min="23" max="23" width="29.6640625" style="2" hidden="1" customWidth="1"/>
+    <col min="24" max="24" width="17.33203125" style="2" hidden="1" customWidth="1"/>
+    <col min="25" max="25" width="31.33203125" style="2" hidden="1" customWidth="1"/>
+    <col min="26" max="27" width="31.86328125" style="2" hidden="1" customWidth="1"/>
+    <col min="28" max="28" width="31.86328125" style="2" customWidth="1"/>
+    <col min="29" max="16384" width="8.86328125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="56" customFormat="1" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:28" s="56" customFormat="1" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>47</v>
       </c>
@@ -6920,127 +7322,162 @@
       <c r="D1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="83" t="s">
-        <v>448</v>
-      </c>
-      <c r="F1" s="9" t="s">
+      <c r="E1" s="86" t="s">
+        <v>601</v>
+      </c>
+      <c r="F1" s="83" t="s">
+        <v>441</v>
+      </c>
+      <c r="G1" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="H1" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="I1" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="J1" s="9" t="s">
         <v>370</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="K1" s="9" t="s">
         <v>371</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="L1" s="9" t="s">
         <v>386</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="M1" s="9" t="s">
         <v>387</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="N1" s="9" t="s">
         <v>388</v>
       </c>
-      <c r="N1" s="11" t="s">
+      <c r="O1" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>399</v>
       </c>
-      <c r="P1" s="11" t="s">
+      <c r="Q1" s="11" t="s">
         <v>400</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>401</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>402</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>403</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>373</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>404</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AA1" s="56" t="s">
+      <c r="AB1" s="56" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="2" spans="1:27" ht="99.75" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:28" ht="99.75" x14ac:dyDescent="0.45">
       <c r="B2" s="2" t="s">
         <v>408</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="E2" s="84">
+      <c r="E2" s="87" t="s">
+        <v>602</v>
+      </c>
+      <c r="F2" s="84">
         <v>1</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>364</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>358</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>368</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>366</v>
       </c>
+      <c r="P2" s="2" t="s">
+        <v>473</v>
+      </c>
       <c r="Q2" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="R2" s="2" t="s">
         <v>369</v>
       </c>
-      <c r="R2" s="2" t="s">
-        <v>468</v>
-      </c>
-      <c r="U2" s="2"/>
-    </row>
-    <row r="3" spans="1:27" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="S2" s="2" t="s">
+        <v>454</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>475</v>
+      </c>
+      <c r="V2" s="2"/>
+    </row>
+    <row r="3" spans="1:28" ht="85.5" x14ac:dyDescent="0.45">
       <c r="B3" s="2" t="s">
         <v>419</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>406</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>423</v>
-      </c>
-      <c r="E3" s="84" t="s">
+      <c r="F3" s="84" t="s">
         <v>366</v>
       </c>
-      <c r="I3" s="82"/>
-      <c r="J3" s="82"/>
-      <c r="K3" s="82"/>
-      <c r="L3" s="82"/>
-      <c r="M3" s="82"/>
-      <c r="U3" s="2"/>
-    </row>
-    <row r="4" spans="1:27" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="J3" s="82" t="s">
+        <v>365</v>
+      </c>
+      <c r="K3" s="82" t="s">
+        <v>559</v>
+      </c>
+      <c r="L3" s="82" t="s">
+        <v>406</v>
+      </c>
+      <c r="M3" s="82" t="s">
+        <v>552</v>
+      </c>
+      <c r="N3" s="82"/>
+      <c r="P3" s="82" t="s">
+        <v>553</v>
+      </c>
+      <c r="Q3" s="82" t="s">
+        <v>548</v>
+      </c>
+      <c r="R3" s="82" t="s">
+        <v>554</v>
+      </c>
+      <c r="S3" s="82" t="s">
+        <v>549</v>
+      </c>
+      <c r="T3" s="82" t="s">
+        <v>552</v>
+      </c>
+      <c r="V3" s="2"/>
+    </row>
+    <row r="4" spans="1:28" ht="99.75" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>420</v>
       </c>
@@ -7050,90 +7487,168 @@
       <c r="C4" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>423</v>
-      </c>
-      <c r="E4" s="84" t="s">
+      <c r="F4" s="84" t="s">
         <v>366</v>
       </c>
-      <c r="I4" s="82"/>
-      <c r="J4" s="82"/>
-      <c r="K4" s="82"/>
-      <c r="L4" s="82"/>
-      <c r="M4" s="82"/>
-      <c r="U4" s="2"/>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="J4" s="82" t="s">
+        <v>365</v>
+      </c>
+      <c r="K4" s="82" t="s">
+        <v>560</v>
+      </c>
+      <c r="L4" s="82" t="s">
+        <v>389</v>
+      </c>
+      <c r="M4" s="82" t="s">
+        <v>550</v>
+      </c>
+      <c r="N4" s="82"/>
+      <c r="P4" s="82" t="s">
+        <v>555</v>
+      </c>
+      <c r="Q4" s="82" t="s">
+        <v>557</v>
+      </c>
+      <c r="R4" s="82" t="s">
+        <v>384</v>
+      </c>
+      <c r="S4" s="82" t="s">
+        <v>374</v>
+      </c>
+      <c r="T4" s="82" t="s">
+        <v>550</v>
+      </c>
+      <c r="V4" s="2"/>
+    </row>
+    <row r="5" spans="1:28" ht="99.75" x14ac:dyDescent="0.45">
       <c r="B5" s="2" t="s">
         <v>422</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="F5" s="84" t="s">
+        <v>366</v>
+      </c>
+      <c r="J5" s="82" t="s">
+        <v>365</v>
+      </c>
+      <c r="K5" s="82" t="s">
+        <v>561</v>
+      </c>
+      <c r="L5" s="82" t="s">
+        <v>389</v>
+      </c>
+      <c r="M5" s="82" t="s">
+        <v>551</v>
+      </c>
+      <c r="N5" s="82"/>
+      <c r="P5" s="82" t="s">
+        <v>556</v>
+      </c>
+      <c r="Q5" s="82" t="s">
+        <v>558</v>
+      </c>
+      <c r="R5" s="82" t="s">
+        <v>384</v>
+      </c>
+      <c r="S5" s="82" t="s">
+        <v>374</v>
+      </c>
+      <c r="T5" s="82" t="s">
+        <v>551</v>
+      </c>
+      <c r="V5" s="2"/>
+    </row>
+    <row r="6" spans="1:28" ht="128.25" x14ac:dyDescent="0.45">
+      <c r="B6" s="2" t="s">
         <v>423</v>
-      </c>
-      <c r="E5" s="84" t="s">
-        <v>366</v>
-      </c>
-      <c r="I5" s="82"/>
-      <c r="J5" s="82"/>
-      <c r="K5" s="82"/>
-      <c r="L5" s="82"/>
-      <c r="M5" s="82"/>
-      <c r="U5" s="2"/>
-    </row>
-    <row r="6" spans="1:27" ht="128.25" x14ac:dyDescent="0.45">
-      <c r="B6" s="2" t="s">
-        <v>424</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="E6" s="84">
+      <c r="E6" s="87" t="s">
+        <v>604</v>
+      </c>
+      <c r="F6" s="84">
         <v>1</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="J6" s="2" t="s">
         <v>365</v>
       </c>
-      <c r="J6" s="2" t="s">
-        <v>469</v>
-      </c>
       <c r="K6" s="2" t="s">
+        <v>455</v>
+      </c>
+      <c r="L6" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="L6" s="2" t="s">
+      <c r="M6" s="2" t="s">
         <v>372</v>
       </c>
-      <c r="M6" s="2" t="s">
+      <c r="N6" s="2" t="s">
         <v>366</v>
       </c>
+      <c r="P6" s="2" t="s">
+        <v>476</v>
+      </c>
       <c r="Q6" s="2" t="s">
+        <v>477</v>
+      </c>
+      <c r="R6" s="2" t="s">
         <v>375</v>
       </c>
-      <c r="R6" s="2" t="s">
+      <c r="S6" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="U6" s="2"/>
-    </row>
-    <row r="7" spans="1:27" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="T6" s="2" t="s">
+        <v>478</v>
+      </c>
+      <c r="V6" s="2"/>
+    </row>
+    <row r="7" spans="1:28" ht="71.25" x14ac:dyDescent="0.45">
       <c r="B7" s="2" t="s">
         <v>409</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="E7" s="84">
+      <c r="E7" s="88">
+        <v>45505</v>
+      </c>
+      <c r="F7" s="84">
         <v>1</v>
       </c>
-      <c r="I7" s="82"/>
-      <c r="J7" s="82"/>
-      <c r="K7" s="82"/>
-      <c r="L7" s="82"/>
-      <c r="M7" s="82"/>
-      <c r="U7" s="2"/>
-    </row>
-    <row r="8" spans="1:27" ht="57" x14ac:dyDescent="0.45">
+      <c r="J7" s="82" t="s">
+        <v>456</v>
+      </c>
+      <c r="K7" s="82" t="s">
+        <v>544</v>
+      </c>
+      <c r="L7" s="82" t="s">
+        <v>396</v>
+      </c>
+      <c r="M7" s="82" t="s">
+        <v>545</v>
+      </c>
+      <c r="N7" s="82"/>
+      <c r="P7" s="82" t="s">
+        <v>546</v>
+      </c>
+      <c r="Q7" s="82" t="s">
+        <v>547</v>
+      </c>
+      <c r="R7" s="82" t="s">
+        <v>381</v>
+      </c>
+      <c r="S7" s="82" t="s">
+        <v>382</v>
+      </c>
+      <c r="T7" s="82" t="s">
+        <v>545</v>
+      </c>
+      <c r="V7" s="2"/>
+    </row>
+    <row r="8" spans="1:28" ht="99.75" x14ac:dyDescent="0.45">
       <c r="B8" s="2" t="s">
         <v>410</v>
       </c>
@@ -7143,17 +7658,45 @@
       <c r="D8" s="2" t="s">
         <v>411</v>
       </c>
-      <c r="E8" s="84" t="s">
+      <c r="E8" s="87" t="s">
+        <v>603</v>
+      </c>
+      <c r="F8" s="84" t="s">
         <v>366</v>
       </c>
-      <c r="I8" s="82"/>
-      <c r="J8" s="82"/>
-      <c r="K8" s="82"/>
-      <c r="L8" s="82"/>
-      <c r="M8" s="82"/>
-      <c r="U8" s="2"/>
-    </row>
-    <row r="9" spans="1:27" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="J8" s="82" t="s">
+        <v>456</v>
+      </c>
+      <c r="K8" s="82" t="s">
+        <v>537</v>
+      </c>
+      <c r="L8" s="82" t="s">
+        <v>515</v>
+      </c>
+      <c r="M8" s="82" t="s">
+        <v>543</v>
+      </c>
+      <c r="N8" s="82">
+        <v>1</v>
+      </c>
+      <c r="P8" s="82" t="s">
+        <v>539</v>
+      </c>
+      <c r="Q8" s="82" t="s">
+        <v>542</v>
+      </c>
+      <c r="R8" s="82" t="s">
+        <v>540</v>
+      </c>
+      <c r="S8" s="82" t="s">
+        <v>541</v>
+      </c>
+      <c r="T8" s="82" t="s">
+        <v>538</v>
+      </c>
+      <c r="V8" s="2"/>
+    </row>
+    <row r="9" spans="1:28" ht="99.75" x14ac:dyDescent="0.45">
       <c r="B9" s="2" t="s">
         <v>412</v>
       </c>
@@ -7163,34 +7706,84 @@
       <c r="D9" s="2" t="s">
         <v>413</v>
       </c>
-      <c r="E9" s="84" t="s">
+      <c r="F9" s="84" t="s">
         <v>366</v>
       </c>
-      <c r="I9" s="82"/>
-      <c r="J9" s="82"/>
-      <c r="K9" s="82"/>
-      <c r="L9" s="82"/>
-      <c r="M9" s="82"/>
-      <c r="U9" s="2"/>
-    </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="J9" s="82" t="s">
+        <v>456</v>
+      </c>
+      <c r="K9" s="82" t="s">
+        <v>537</v>
+      </c>
+      <c r="L9" s="82" t="s">
+        <v>515</v>
+      </c>
+      <c r="M9" s="82" t="s">
+        <v>543</v>
+      </c>
+      <c r="N9" s="82">
+        <v>1</v>
+      </c>
+      <c r="P9" s="82" t="s">
+        <v>539</v>
+      </c>
+      <c r="Q9" s="82" t="s">
+        <v>542</v>
+      </c>
+      <c r="R9" s="82" t="s">
+        <v>540</v>
+      </c>
+      <c r="S9" s="82" t="s">
+        <v>541</v>
+      </c>
+      <c r="T9" s="82" t="s">
+        <v>538</v>
+      </c>
+      <c r="V9" s="2"/>
+    </row>
+    <row r="10" spans="1:28" ht="99.75" x14ac:dyDescent="0.45">
       <c r="B10" s="2" t="s">
         <v>414</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>406</v>
       </c>
-      <c r="E10" s="84" t="s">
+      <c r="F10" s="84" t="s">
         <v>366</v>
       </c>
-      <c r="I10" s="82"/>
-      <c r="J10" s="82"/>
-      <c r="K10" s="82"/>
-      <c r="L10" s="82"/>
-      <c r="M10" s="82"/>
-      <c r="U10" s="2"/>
-    </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="J10" s="82" t="s">
+        <v>456</v>
+      </c>
+      <c r="K10" s="82" t="s">
+        <v>537</v>
+      </c>
+      <c r="L10" s="82" t="s">
+        <v>515</v>
+      </c>
+      <c r="M10" s="82" t="s">
+        <v>543</v>
+      </c>
+      <c r="N10" s="82">
+        <v>1</v>
+      </c>
+      <c r="P10" s="82" t="s">
+        <v>539</v>
+      </c>
+      <c r="Q10" s="82" t="s">
+        <v>542</v>
+      </c>
+      <c r="R10" s="82" t="s">
+        <v>540</v>
+      </c>
+      <c r="S10" s="82" t="s">
+        <v>541</v>
+      </c>
+      <c r="T10" s="82" t="s">
+        <v>538</v>
+      </c>
+      <c r="V10" s="2"/>
+    </row>
+    <row r="11" spans="1:28" ht="99.75" x14ac:dyDescent="0.45">
       <c r="A11" s="2" t="s">
         <v>418</v>
       </c>
@@ -7200,352 +7793,591 @@
       <c r="C11" s="2" t="s">
         <v>406</v>
       </c>
-      <c r="E11" s="84" t="s">
+      <c r="F11" s="84" t="s">
         <v>366</v>
       </c>
-      <c r="U11" s="2"/>
-    </row>
-    <row r="12" spans="1:27" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="J11" s="82" t="s">
+        <v>456</v>
+      </c>
+      <c r="K11" s="82" t="s">
+        <v>537</v>
+      </c>
+      <c r="L11" s="82" t="s">
+        <v>515</v>
+      </c>
+      <c r="M11" s="82" t="s">
+        <v>543</v>
+      </c>
+      <c r="N11" s="82">
+        <v>1</v>
+      </c>
+      <c r="P11" s="82" t="s">
+        <v>539</v>
+      </c>
+      <c r="Q11" s="82" t="s">
+        <v>542</v>
+      </c>
+      <c r="R11" s="82" t="s">
+        <v>540</v>
+      </c>
+      <c r="S11" s="82" t="s">
+        <v>541</v>
+      </c>
+      <c r="T11" s="82" t="s">
+        <v>538</v>
+      </c>
+      <c r="V11" s="2"/>
+    </row>
+    <row r="12" spans="1:28" ht="108.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B12" s="2" t="s">
         <v>415</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="E12" s="84">
+      <c r="E12" s="87" t="s">
+        <v>605</v>
+      </c>
+      <c r="F12" s="84">
         <v>1</v>
       </c>
-      <c r="I12" s="2" t="s">
+      <c r="J12" s="2" t="s">
         <v>357</v>
       </c>
-      <c r="J12" s="2" t="s">
-        <v>458</v>
-      </c>
       <c r="K12" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="L12" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="L12" s="2" t="s">
-        <v>452</v>
-      </c>
       <c r="M12" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="N12" s="2" t="s">
         <v>366</v>
       </c>
+      <c r="P12" s="2" t="s">
+        <v>479</v>
+      </c>
       <c r="Q12" s="2" t="s">
-        <v>453</v>
+        <v>481</v>
       </c>
       <c r="R12" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="S12" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="U12" s="2"/>
-    </row>
-    <row r="13" spans="1:27" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="T12" s="2" t="s">
+        <v>480</v>
+      </c>
+      <c r="V12" s="2"/>
+    </row>
+    <row r="13" spans="1:28" ht="85.5" x14ac:dyDescent="0.45">
       <c r="B13" s="2" t="s">
         <v>416</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="E13" s="84">
+      <c r="E13" s="87" t="s">
+        <v>606</v>
+      </c>
+      <c r="F13" s="84">
         <v>1</v>
       </c>
-      <c r="I13" s="2" t="s">
+      <c r="J13" s="2" t="s">
         <v>357</v>
       </c>
-      <c r="J13" s="2" t="s">
-        <v>459</v>
-      </c>
       <c r="K13" s="2" t="s">
+        <v>452</v>
+      </c>
+      <c r="L13" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="L13" s="2" t="s">
-        <v>450</v>
-      </c>
       <c r="M13" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="N13" s="2" t="s">
         <v>366</v>
       </c>
+      <c r="P13" s="2" t="s">
+        <v>482</v>
+      </c>
       <c r="Q13" s="2" t="s">
-        <v>451</v>
+        <v>481</v>
       </c>
       <c r="R13" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="S13" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="U13" s="2"/>
-    </row>
-    <row r="14" spans="1:27" ht="57" x14ac:dyDescent="0.45">
+      <c r="T13" s="2" t="s">
+        <v>484</v>
+      </c>
+      <c r="V13" s="2"/>
+    </row>
+    <row r="14" spans="1:28" ht="99.75" x14ac:dyDescent="0.45">
       <c r="B14" s="2" t="s">
         <v>417</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="E14" s="84" t="s">
+      <c r="F14" s="84" t="s">
         <v>366</v>
       </c>
-      <c r="I14" s="2" t="s">
+      <c r="J14" s="2" t="s">
         <v>357</v>
       </c>
-      <c r="J14" s="2" t="s">
-        <v>460</v>
-      </c>
       <c r="K14" s="2" t="s">
+        <v>453</v>
+      </c>
+      <c r="L14" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="L14" s="2" t="s">
-        <v>454</v>
-      </c>
       <c r="M14" s="2" t="s">
+        <v>447</v>
+      </c>
+      <c r="N14" s="2" t="s">
         <v>366</v>
       </c>
+      <c r="P14" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="Q14" s="2" t="s">
-        <v>455</v>
+        <v>481</v>
       </c>
       <c r="R14" s="2" t="s">
-        <v>454</v>
-      </c>
-      <c r="U14" s="2"/>
-    </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.45">
+        <v>448</v>
+      </c>
+      <c r="S14" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="T14" s="2" t="s">
+        <v>485</v>
+      </c>
+      <c r="V14" s="2"/>
+    </row>
+    <row r="15" spans="1:28" ht="114" x14ac:dyDescent="0.45">
       <c r="B15" s="2" t="s">
+        <v>427</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>428</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>429</v>
-      </c>
-      <c r="E15" s="84">
+      <c r="E15" s="87" t="s">
+        <v>607</v>
+      </c>
+      <c r="F15" s="84">
         <v>1</v>
       </c>
-      <c r="U15" s="2"/>
-    </row>
-    <row r="16" spans="1:27" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="J15" s="2" t="s">
+        <v>486</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>487</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>488</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>497</v>
+      </c>
+      <c r="N15" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="P15" s="2" t="s">
+        <v>489</v>
+      </c>
+      <c r="Q15" s="2" t="s">
+        <v>494</v>
+      </c>
+      <c r="R15" s="2" t="s">
+        <v>490</v>
+      </c>
+      <c r="S15" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="T15" s="2" t="s">
+        <v>491</v>
+      </c>
+      <c r="V15" s="2"/>
+    </row>
+    <row r="16" spans="1:28" ht="85.5" x14ac:dyDescent="0.45">
       <c r="B16" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>396</v>
       </c>
-      <c r="E16" s="84">
+      <c r="E16" s="88">
+        <v>25143</v>
+      </c>
+      <c r="F16" s="84">
         <v>1</v>
       </c>
-      <c r="I16" s="2" t="s">
-        <v>456</v>
-      </c>
       <c r="J16" s="2" t="s">
+        <v>449</v>
+      </c>
+      <c r="K16" s="2" t="s">
         <v>359</v>
       </c>
-      <c r="K16" s="2" t="s">
+      <c r="L16" s="2" t="s">
         <v>396</v>
       </c>
-      <c r="L16" s="2" t="s">
+      <c r="M16" s="2" t="s">
         <v>380</v>
       </c>
-      <c r="M16" s="2" t="s">
+      <c r="N16" s="2" t="s">
         <v>366</v>
       </c>
+      <c r="P16" s="2" t="s">
+        <v>492</v>
+      </c>
       <c r="Q16" s="2" t="s">
+        <v>493</v>
+      </c>
+      <c r="R16" s="2" t="s">
         <v>381</v>
       </c>
-      <c r="R16" s="2" t="s">
+      <c r="S16" s="2" t="s">
         <v>382</v>
       </c>
-      <c r="U16" s="2"/>
-    </row>
-    <row r="17" spans="2:21" ht="57" x14ac:dyDescent="0.45">
+      <c r="T16" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="V16" s="2"/>
+    </row>
+    <row r="17" spans="2:22" ht="99.75" x14ac:dyDescent="0.45">
       <c r="B17" s="2" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>389</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>425</v>
-      </c>
-      <c r="E17" s="84" t="s">
+        <v>424</v>
+      </c>
+      <c r="E17" s="87" t="s">
+        <v>608</v>
+      </c>
+      <c r="F17" s="84" t="s">
         <v>366</v>
       </c>
-      <c r="I17" s="2" t="s">
-        <v>457</v>
-      </c>
       <c r="J17" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="K17" s="2" t="s">
         <v>361</v>
       </c>
-      <c r="K17" s="2" t="s">
+      <c r="L17" s="2" t="s">
         <v>397</v>
       </c>
-      <c r="L17" s="2" t="s">
+      <c r="M17" s="2" t="s">
         <v>376</v>
       </c>
-      <c r="M17" s="2" t="s">
+      <c r="N17" s="2" t="s">
         <v>366</v>
       </c>
+      <c r="P17" s="2" t="s">
+        <v>495</v>
+      </c>
       <c r="Q17" s="2" t="s">
+        <v>496</v>
+      </c>
+      <c r="R17" s="2" t="s">
         <v>377</v>
       </c>
-      <c r="R17" s="2" t="s">
+      <c r="S17" s="2" t="s">
         <v>367</v>
       </c>
-      <c r="U17" s="2"/>
-    </row>
-    <row r="18" spans="2:21" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="T17" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="V17" s="2"/>
+    </row>
+    <row r="18" spans="2:22" ht="71.25" x14ac:dyDescent="0.45">
       <c r="B18" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>389</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>431</v>
-      </c>
-      <c r="E18" s="84" t="s">
+        <v>430</v>
+      </c>
+      <c r="E18" s="87" t="s">
+        <v>609</v>
+      </c>
+      <c r="F18" s="84" t="s">
         <v>366</v>
       </c>
-      <c r="I18" s="2" t="s">
-        <v>457</v>
-      </c>
       <c r="J18" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="K18" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="K18" s="2" t="s">
+      <c r="L18" s="2" t="s">
         <v>398</v>
       </c>
-      <c r="L18" s="2" t="s">
+      <c r="M18" s="2" t="s">
         <v>379</v>
       </c>
-      <c r="M18" s="2" t="s">
+      <c r="N18" s="2" t="s">
         <v>366</v>
       </c>
+      <c r="P18" s="2" t="s">
+        <v>498</v>
+      </c>
       <c r="Q18" s="2" t="s">
+        <v>496</v>
+      </c>
+      <c r="R18" s="2" t="s">
         <v>378</v>
       </c>
-      <c r="R18" s="2" t="s">
+      <c r="S18" s="2" t="s">
         <v>367</v>
       </c>
-      <c r="U18" s="2"/>
-    </row>
-    <row r="19" spans="2:21" ht="57" x14ac:dyDescent="0.45">
+      <c r="T18" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="V18" s="2"/>
+    </row>
+    <row r="19" spans="2:22" ht="71.25" x14ac:dyDescent="0.45">
       <c r="B19" s="2" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="E19" s="84" t="s">
+      <c r="F19" s="84" t="s">
         <v>366</v>
       </c>
-      <c r="I19" s="2" t="s">
-        <v>456</v>
-      </c>
       <c r="J19" s="2" t="s">
+        <v>449</v>
+      </c>
+      <c r="K19" s="2" t="s">
         <v>360</v>
       </c>
-      <c r="K19" s="2" t="s">
+      <c r="L19" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="L19" s="2" t="s">
+      <c r="M19" s="2" t="s">
         <v>383</v>
       </c>
-      <c r="M19" s="2" t="s">
+      <c r="N19" s="2" t="s">
         <v>366</v>
       </c>
+      <c r="P19" s="2" t="s">
+        <v>499</v>
+      </c>
       <c r="Q19" s="2" t="s">
+        <v>500</v>
+      </c>
+      <c r="R19" s="2" t="s">
         <v>384</v>
       </c>
-      <c r="R19" s="2" t="s">
+      <c r="S19" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="U19" s="2"/>
-    </row>
-    <row r="20" spans="2:21" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="T19" s="2" t="s">
+        <v>501</v>
+      </c>
+      <c r="V19" s="2"/>
+    </row>
+    <row r="20" spans="2:22" ht="57" x14ac:dyDescent="0.45">
       <c r="B20" s="2" t="s">
-        <v>437</v>
+        <v>431</v>
       </c>
       <c r="C20" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>562</v>
+      </c>
+      <c r="E20" s="87">
+        <v>9999999</v>
+      </c>
+      <c r="F20" s="84" t="s">
+        <v>366</v>
+      </c>
+      <c r="J20" s="82" t="s">
+        <v>566</v>
+      </c>
+      <c r="K20" s="82" t="s">
+        <v>565</v>
+      </c>
+      <c r="L20" s="82" t="s">
         <v>389</v>
       </c>
-      <c r="E20" s="84" t="s">
+      <c r="M20" s="82" t="s">
+        <v>562</v>
+      </c>
+      <c r="N20" s="85" t="s">
         <v>366</v>
       </c>
-      <c r="I20" s="2" t="s">
-        <v>456</v>
-      </c>
-      <c r="J20" s="2" t="s">
-        <v>461</v>
-      </c>
-      <c r="K20" s="2" t="s">
+      <c r="P20" s="82" t="s">
+        <v>591</v>
+      </c>
+      <c r="Q20" s="82" t="s">
+        <v>477</v>
+      </c>
+      <c r="R20" s="82" t="s">
+        <v>592</v>
+      </c>
+      <c r="S20" s="82" t="s">
+        <v>374</v>
+      </c>
+      <c r="T20" s="82" t="s">
+        <v>593</v>
+      </c>
+      <c r="V20" s="2"/>
+    </row>
+    <row r="21" spans="2:22" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="B21" s="2" t="s">
+        <v>563</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>564</v>
+      </c>
+      <c r="F21" s="84" t="s">
+        <v>503</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>570</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>571</v>
+      </c>
+      <c r="L21" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="L20" s="82"/>
-      <c r="M20" s="2" t="s">
+      <c r="M21" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="N21" s="84" t="s">
+        <v>503</v>
+      </c>
+      <c r="P21" s="2" t="s">
+        <v>572</v>
+      </c>
+      <c r="Q21" s="2" t="s">
+        <v>573</v>
+      </c>
+      <c r="R21" s="2" t="s">
+        <v>574</v>
+      </c>
+      <c r="S21" s="2" t="s">
+        <v>481</v>
+      </c>
+      <c r="T21" s="2" t="s">
+        <v>575</v>
+      </c>
+      <c r="V21" s="2"/>
+    </row>
+    <row r="22" spans="2:22" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="B22" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>567</v>
+      </c>
+      <c r="E22" s="88">
+        <v>45566</v>
+      </c>
+      <c r="F22" s="84" t="s">
         <v>366</v>
       </c>
-      <c r="Q20" s="2" t="s">
-        <v>384</v>
-      </c>
-      <c r="R20" s="2" t="s">
-        <v>374</v>
-      </c>
-      <c r="U20" s="2"/>
-    </row>
-    <row r="21" spans="2:21" x14ac:dyDescent="0.45">
-      <c r="B21" s="2" t="s">
-        <v>432</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>433</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>423</v>
-      </c>
-      <c r="E21" s="84" t="s">
+      <c r="J22" s="82" t="s">
+        <v>566</v>
+      </c>
+      <c r="K22" s="82" t="s">
+        <v>580</v>
+      </c>
+      <c r="L22" s="82" t="s">
+        <v>396</v>
+      </c>
+      <c r="M22" s="82" t="s">
+        <v>567</v>
+      </c>
+      <c r="N22" s="85" t="s">
         <v>366</v>
       </c>
-      <c r="I21" s="82"/>
-      <c r="J21" s="82"/>
-      <c r="K21" s="82"/>
-      <c r="L21" s="82"/>
-      <c r="M21" s="82"/>
-      <c r="U21" s="2"/>
-    </row>
-    <row r="22" spans="2:21" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B22" s="2" t="s">
+      <c r="P22" s="82" t="s">
+        <v>594</v>
+      </c>
+      <c r="Q22" s="82" t="s">
+        <v>595</v>
+      </c>
+      <c r="R22" s="82" t="s">
+        <v>381</v>
+      </c>
+      <c r="S22" s="82" t="s">
+        <v>382</v>
+      </c>
+      <c r="T22" s="82" t="s">
+        <v>567</v>
+      </c>
+      <c r="V22" s="2"/>
+    </row>
+    <row r="23" spans="2:22" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="B23" s="2" t="s">
         <v>434</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C23" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>568</v>
+      </c>
+      <c r="E23" s="87" t="s">
+        <v>610</v>
+      </c>
+      <c r="F23" s="84" t="s">
+        <v>366</v>
+      </c>
+      <c r="J23" s="82" t="s">
+        <v>566</v>
+      </c>
+      <c r="K23" s="82" t="s">
+        <v>581</v>
+      </c>
+      <c r="L23" s="82" t="s">
         <v>389</v>
       </c>
-      <c r="D22" s="2" t="s">
-        <v>423</v>
-      </c>
-      <c r="E22" s="84" t="s">
+      <c r="M23" s="82" t="s">
+        <v>583</v>
+      </c>
+      <c r="N23" s="85" t="s">
         <v>366</v>
       </c>
-      <c r="I22" s="82"/>
-      <c r="J22" s="82"/>
-      <c r="K22" s="82"/>
-      <c r="L22" s="82"/>
-      <c r="M22" s="82"/>
-      <c r="U22" s="2"/>
-    </row>
-    <row r="23" spans="2:21" x14ac:dyDescent="0.45">
-      <c r="B23" s="2" t="s">
-        <v>435</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>396</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>423</v>
-      </c>
-      <c r="E23" s="84" t="s">
-        <v>366</v>
-      </c>
-      <c r="I23" s="82"/>
-      <c r="J23" s="82"/>
-      <c r="K23" s="82"/>
-      <c r="L23" s="82"/>
-      <c r="M23" s="82"/>
-      <c r="U23" s="2"/>
-    </row>
-    <row r="24" spans="2:21" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="P23" s="82" t="s">
+        <v>596</v>
+      </c>
+      <c r="Q23" s="82" t="s">
+        <v>598</v>
+      </c>
+      <c r="R23" s="82" t="s">
+        <v>600</v>
+      </c>
+      <c r="S23" s="82" t="s">
+        <v>481</v>
+      </c>
+      <c r="T23" s="82" t="s">
+        <v>583</v>
+      </c>
+      <c r="V23" s="2"/>
+    </row>
+    <row r="24" spans="2:22" ht="85.5" x14ac:dyDescent="0.45">
       <c r="B24" s="2" t="s">
         <v>436</v>
       </c>
@@ -7553,552 +8385,580 @@
         <v>357</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>423</v>
-      </c>
-      <c r="E24" s="84" t="s">
+        <v>569</v>
+      </c>
+      <c r="E24" s="87" t="s">
+        <v>611</v>
+      </c>
+      <c r="F24" s="84" t="s">
         <v>366</v>
       </c>
-      <c r="I24" s="82"/>
-      <c r="J24" s="82"/>
-      <c r="K24" s="82"/>
-      <c r="L24" s="82"/>
-      <c r="M24" s="82"/>
-      <c r="U24" s="2"/>
-    </row>
-    <row r="25" spans="2:21" x14ac:dyDescent="0.45">
+      <c r="J24" s="82" t="s">
+        <v>566</v>
+      </c>
+      <c r="K24" s="82" t="s">
+        <v>582</v>
+      </c>
+      <c r="L24" s="82" t="s">
+        <v>389</v>
+      </c>
+      <c r="M24" s="82" t="s">
+        <v>584</v>
+      </c>
+      <c r="N24" s="85" t="s">
+        <v>366</v>
+      </c>
+      <c r="P24" s="82" t="s">
+        <v>597</v>
+      </c>
+      <c r="Q24" s="82" t="s">
+        <v>599</v>
+      </c>
+      <c r="R24" s="82" t="s">
+        <v>574</v>
+      </c>
+      <c r="S24" s="82" t="s">
+        <v>481</v>
+      </c>
+      <c r="T24" s="82" t="s">
+        <v>584</v>
+      </c>
+      <c r="V24" s="2"/>
+    </row>
+    <row r="25" spans="2:22" ht="127.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B25" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>472</v>
+      </c>
+      <c r="E25" s="87">
+        <v>999999</v>
+      </c>
+      <c r="F25" s="84" t="s">
+        <v>366</v>
+      </c>
+      <c r="J25" s="82" t="s">
+        <v>578</v>
+      </c>
+      <c r="K25" s="82" t="s">
+        <v>579</v>
+      </c>
+      <c r="L25" s="82" t="s">
+        <v>389</v>
+      </c>
+      <c r="M25" s="82" t="s">
+        <v>472</v>
+      </c>
+      <c r="N25" s="85" t="s">
+        <v>366</v>
+      </c>
+      <c r="P25" s="82" t="s">
+        <v>577</v>
+      </c>
+      <c r="Q25" s="82" t="s">
+        <v>576</v>
+      </c>
+      <c r="R25" s="82" t="s">
+        <v>384</v>
+      </c>
+      <c r="S25" s="82" t="s">
+        <v>374</v>
+      </c>
+      <c r="T25" s="82" t="s">
+        <v>472</v>
+      </c>
+      <c r="V25" s="2"/>
+    </row>
+    <row r="26" spans="2:22" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="B26" s="2" t="s">
         <v>438</v>
       </c>
-      <c r="C25" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>423</v>
-      </c>
-      <c r="E25" s="84" t="s">
+      <c r="C26" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="E26" s="88">
+        <v>45505</v>
+      </c>
+      <c r="F26" s="84" t="s">
         <v>366</v>
       </c>
-      <c r="I25" s="82"/>
-      <c r="J25" s="82"/>
-      <c r="K25" s="82"/>
-      <c r="L25" s="82"/>
-      <c r="M25" s="82"/>
-      <c r="U25" s="2"/>
-    </row>
-    <row r="26" spans="2:21" x14ac:dyDescent="0.45">
-      <c r="B26" s="2" t="s">
+      <c r="J26" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="L26" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="M26" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="N26" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="P26" s="82" t="s">
+        <v>528</v>
+      </c>
+      <c r="Q26" s="2" t="s">
+        <v>504</v>
+      </c>
+      <c r="R26" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="S26" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="T26" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="V26" s="2"/>
+    </row>
+    <row r="27" spans="2:22" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="B27" s="2" t="s">
         <v>439</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>433</v>
-      </c>
-      <c r="E26" s="84" t="s">
-        <v>366</v>
-      </c>
-      <c r="I26" s="82"/>
-      <c r="J26" s="82"/>
-      <c r="K26" s="82"/>
-      <c r="L26" s="82"/>
-      <c r="M26" s="82"/>
-      <c r="U26" s="2"/>
-    </row>
-    <row r="27" spans="2:21" x14ac:dyDescent="0.45">
-      <c r="B27" s="2" t="s">
-        <v>440</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>396</v>
       </c>
-      <c r="E27" s="84" t="s">
+      <c r="E27" s="88">
+        <v>45505</v>
+      </c>
+      <c r="F27" s="84" t="s">
         <v>366</v>
       </c>
-      <c r="I27" s="2" t="s">
-        <v>390</v>
-      </c>
       <c r="J27" s="2" t="s">
-        <v>391</v>
+        <v>456</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>396</v>
+        <v>457</v>
       </c>
       <c r="L27" s="2" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="M27" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="N27" s="2" t="s">
         <v>366</v>
       </c>
+      <c r="P27" s="82" t="s">
+        <v>529</v>
+      </c>
       <c r="Q27" s="2" t="s">
-        <v>381</v>
+        <v>502</v>
       </c>
       <c r="R27" s="2" t="s">
-        <v>382</v>
-      </c>
-      <c r="U27" s="2"/>
-    </row>
-    <row r="28" spans="2:21" ht="28.5" x14ac:dyDescent="0.45">
+        <v>394</v>
+      </c>
+      <c r="S27" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="T27" s="2" t="s">
+        <v>505</v>
+      </c>
+      <c r="V27" s="2"/>
+    </row>
+    <row r="28" spans="2:22" ht="42.75" x14ac:dyDescent="0.45">
       <c r="B28" s="2" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>396</v>
-      </c>
-      <c r="E28" s="84" t="s">
+        <v>389</v>
+      </c>
+      <c r="E28" s="87" t="s">
+        <v>612</v>
+      </c>
+      <c r="F28" s="84" t="s">
         <v>366</v>
       </c>
-      <c r="I28" s="2" t="s">
-        <v>470</v>
-      </c>
       <c r="J28" s="2" t="s">
-        <v>471</v>
+        <v>365</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>392</v>
+        <v>586</v>
       </c>
       <c r="L28" s="2" t="s">
-        <v>472</v>
+        <v>389</v>
       </c>
       <c r="M28" s="2" t="s">
+        <v>585</v>
+      </c>
+      <c r="N28" s="2" t="s">
         <v>366</v>
       </c>
+      <c r="P28" s="2" t="s">
+        <v>587</v>
+      </c>
       <c r="Q28" s="2" t="s">
-        <v>394</v>
+        <v>588</v>
       </c>
       <c r="R28" s="2" t="s">
-        <v>395</v>
-      </c>
-      <c r="U28" s="2"/>
-    </row>
-    <row r="29" spans="2:21" x14ac:dyDescent="0.45">
+        <v>589</v>
+      </c>
+      <c r="S28" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="T28" s="2" t="s">
+        <v>590</v>
+      </c>
+      <c r="V28" s="2"/>
+    </row>
+    <row r="29" spans="2:22" ht="85.5" x14ac:dyDescent="0.45">
       <c r="B29" s="2" t="s">
-        <v>442</v>
+        <v>518</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="D29" s="2" t="s">
-        <v>423</v>
-      </c>
-      <c r="E29" s="84" t="s">
+      <c r="E29" s="87" t="s">
+        <v>613</v>
+      </c>
+      <c r="F29" s="84" t="s">
+        <v>442</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="K29" s="2" t="s">
+        <v>462</v>
+      </c>
+      <c r="L29" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="M29" s="2" t="s">
+        <v>461</v>
+      </c>
+      <c r="N29" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="I29" s="82"/>
-      <c r="J29" s="82"/>
-      <c r="K29" s="82"/>
-      <c r="L29" s="82"/>
-      <c r="M29" s="82"/>
-      <c r="U29" s="2"/>
-    </row>
-    <row r="30" spans="2:21" ht="57" x14ac:dyDescent="0.45">
+      <c r="P29" s="2" t="s">
+        <v>530</v>
+      </c>
+      <c r="Q29" s="2" t="s">
+        <v>506</v>
+      </c>
+      <c r="R29" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="S29" s="2" t="s">
+        <v>463</v>
+      </c>
+      <c r="T29" s="2" t="s">
+        <v>461</v>
+      </c>
+      <c r="V29" s="2"/>
+    </row>
+    <row r="30" spans="2:22" ht="28.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B30" s="2" t="s">
-        <v>462</v>
+        <v>519</v>
       </c>
       <c r="C30" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="E30" s="87">
+        <v>12345678</v>
+      </c>
+      <c r="F30" s="84" t="s">
+        <v>442</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>456</v>
+      </c>
+      <c r="K30" s="2" t="s">
+        <v>465</v>
+      </c>
+      <c r="L30" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="E30" s="84" t="s">
-        <v>449</v>
-      </c>
-      <c r="I30" s="2" t="s">
+      <c r="M30" s="2" t="s">
+        <v>464</v>
+      </c>
+      <c r="N30" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="P30" s="2" t="s">
+        <v>531</v>
+      </c>
+      <c r="R30" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="S30" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="V30" s="2"/>
+    </row>
+    <row r="31" spans="2:22" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="B31" s="2" t="s">
+        <v>520</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="E31" s="87" t="s">
+        <v>614</v>
+      </c>
+      <c r="F31" s="84" t="s">
+        <v>442</v>
+      </c>
+      <c r="J31" s="2" t="s">
         <v>385</v>
       </c>
-      <c r="J30" s="2" t="s">
-        <v>476</v>
-      </c>
-      <c r="K30" s="2" t="s">
-        <v>389</v>
-      </c>
-      <c r="L30" s="2" t="s">
-        <v>475</v>
-      </c>
-      <c r="M30" s="2" t="s">
+      <c r="K31" s="2" t="s">
+        <v>460</v>
+      </c>
+      <c r="M31" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="N31" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="Q30" s="2" t="s">
-        <v>384</v>
-      </c>
-      <c r="R30" s="2" t="s">
-        <v>477</v>
-      </c>
-      <c r="U30" s="2"/>
-    </row>
-    <row r="31" spans="2:21" ht="28.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B31" s="2" t="s">
-        <v>463</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>433</v>
-      </c>
-      <c r="E31" s="84" t="s">
-        <v>449</v>
-      </c>
-      <c r="I31" s="2" t="s">
-        <v>470</v>
-      </c>
-      <c r="J31" s="2" t="s">
-        <v>479</v>
-      </c>
-      <c r="K31" s="2" t="s">
-        <v>389</v>
-      </c>
-      <c r="L31" s="2" t="s">
-        <v>478</v>
-      </c>
-      <c r="M31" s="2" t="s">
-        <v>366</v>
+      <c r="P31" s="2" t="s">
+        <v>532</v>
       </c>
       <c r="Q31" s="2" t="s">
-        <v>480</v>
+        <v>507</v>
       </c>
       <c r="R31" s="2" t="s">
-        <v>374</v>
-      </c>
-      <c r="U31" s="2"/>
-    </row>
-    <row r="32" spans="2:21" ht="28.5" x14ac:dyDescent="0.45">
+        <v>467</v>
+      </c>
+      <c r="S31" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="T31" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="V31" s="2"/>
+    </row>
+    <row r="32" spans="2:22" ht="228" x14ac:dyDescent="0.45">
       <c r="B32" s="2" t="s">
-        <v>464</v>
+        <v>521</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="E32" s="84" t="s">
-        <v>449</v>
-      </c>
-      <c r="I32" s="2" t="s">
+      <c r="E32" s="87" t="s">
+        <v>615</v>
+      </c>
+      <c r="F32" s="84" t="s">
+        <v>442</v>
+      </c>
+      <c r="J32" s="2" t="s">
         <v>385</v>
       </c>
-      <c r="J32" s="2" t="s">
-        <v>474</v>
+      <c r="K32" s="2" t="s">
+        <v>469</v>
       </c>
       <c r="L32" s="2" t="s">
-        <v>473</v>
+        <v>389</v>
       </c>
       <c r="M32" s="2" t="s">
+        <v>470</v>
+      </c>
+      <c r="N32" s="2" t="s">
         <v>366</v>
       </c>
+      <c r="P32" s="2" t="s">
+        <v>533</v>
+      </c>
       <c r="Q32" s="2" t="s">
-        <v>481</v>
+        <v>507</v>
       </c>
       <c r="R32" s="2" t="s">
+        <v>468</v>
+      </c>
+      <c r="S32" s="2" t="s">
         <v>367</v>
       </c>
-      <c r="U32" s="2"/>
-    </row>
-    <row r="33" spans="2:21" ht="128.25" x14ac:dyDescent="0.45">
+      <c r="T32" s="2" t="s">
+        <v>470</v>
+      </c>
+      <c r="V32" s="2"/>
+    </row>
+    <row r="33" spans="2:22" ht="71.25" x14ac:dyDescent="0.45">
       <c r="B33" s="2" t="s">
-        <v>465</v>
+        <v>522</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="E33" s="84" t="s">
-        <v>449</v>
-      </c>
-      <c r="I33" s="2" t="s">
+      <c r="E33" s="87">
+        <v>14.8</v>
+      </c>
+      <c r="F33" s="84" t="s">
+        <v>442</v>
+      </c>
+      <c r="J33" s="2" t="s">
         <v>385</v>
       </c>
-      <c r="J33" s="2" t="s">
-        <v>483</v>
-      </c>
       <c r="K33" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="L33" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="L33" s="2" t="s">
-        <v>484</v>
-      </c>
       <c r="M33" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="N33" s="2" t="s">
         <v>366</v>
       </c>
+      <c r="P33" s="2" t="s">
+        <v>534</v>
+      </c>
       <c r="Q33" s="2" t="s">
-        <v>482</v>
+        <v>508</v>
       </c>
       <c r="R33" s="2" t="s">
-        <v>367</v>
-      </c>
-      <c r="U33" s="2"/>
-    </row>
-    <row r="34" spans="2:21" ht="71.25" x14ac:dyDescent="0.45">
+        <v>384</v>
+      </c>
+      <c r="S33" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="T33" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="V33" s="2"/>
+    </row>
+    <row r="34" spans="2:22" ht="99.75" x14ac:dyDescent="0.45">
       <c r="B34" s="2" t="s">
-        <v>466</v>
+        <v>523</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="E34" s="84" t="s">
-        <v>449</v>
-      </c>
-      <c r="I34" s="2" t="s">
+      <c r="E34" s="87">
+        <v>0</v>
+      </c>
+      <c r="F34" s="84" t="s">
+        <v>442</v>
+      </c>
+      <c r="J34" s="2" t="s">
         <v>385</v>
       </c>
-      <c r="J34" s="2" t="s">
-        <v>363</v>
-      </c>
       <c r="K34" s="2" t="s">
+        <v>510</v>
+      </c>
+      <c r="L34" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="L34" s="2" t="s">
-        <v>485</v>
-      </c>
       <c r="M34" s="2" t="s">
+        <v>511</v>
+      </c>
+      <c r="N34" s="2" t="s">
         <v>366</v>
       </c>
+      <c r="P34" s="2" t="s">
+        <v>535</v>
+      </c>
       <c r="Q34" s="2" t="s">
-        <v>384</v>
+        <v>507</v>
       </c>
       <c r="R34" s="2" t="s">
-        <v>374</v>
-      </c>
-      <c r="U34" s="2"/>
-    </row>
-    <row r="35" spans="2:21" ht="57" x14ac:dyDescent="0.45">
+        <v>512</v>
+      </c>
+      <c r="S34" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="T34" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="V34" s="2"/>
+    </row>
+    <row r="35" spans="2:22" ht="85.5" x14ac:dyDescent="0.45">
       <c r="B35" s="2" t="s">
-        <v>467</v>
+        <v>524</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="E35" s="84" t="s">
-        <v>449</v>
-      </c>
-      <c r="I35" s="2" t="s">
-        <v>385</v>
-      </c>
-      <c r="J35" s="2" t="s">
-        <v>476</v>
-      </c>
-      <c r="K35" s="2" t="s">
+      <c r="E35" s="87" t="s">
+        <v>410</v>
+      </c>
+      <c r="F35" s="84" t="s">
+        <v>442</v>
+      </c>
+      <c r="J35" s="82" t="s">
+        <v>525</v>
+      </c>
+      <c r="K35" s="82" t="s">
+        <v>514</v>
+      </c>
+      <c r="L35" s="82" t="s">
         <v>389</v>
       </c>
-      <c r="L35" s="2" t="s">
-        <v>475</v>
-      </c>
-      <c r="M35" s="2" t="s">
+      <c r="M35" s="82" t="s">
+        <v>516</v>
+      </c>
+      <c r="N35" s="82" t="s">
         <v>366</v>
       </c>
-      <c r="Q35" s="2" t="s">
-        <v>384</v>
-      </c>
-      <c r="R35" s="2" t="s">
-        <v>477</v>
-      </c>
-      <c r="U35" s="2"/>
-    </row>
-    <row r="36" spans="2:21" ht="409.5" x14ac:dyDescent="0.45">
-      <c r="B36" s="2" t="s">
-        <v>443</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>389</v>
-      </c>
-      <c r="E36" s="84" t="s">
-        <v>449</v>
-      </c>
-      <c r="I36" s="2" t="s">
-        <v>470</v>
-      </c>
-      <c r="J36" s="2" t="s">
-        <v>479</v>
-      </c>
-      <c r="K36" s="2" t="s">
-        <v>389</v>
-      </c>
-      <c r="L36" s="2" t="s">
-        <v>478</v>
-      </c>
-      <c r="M36" s="2" t="s">
-        <v>366</v>
-      </c>
-      <c r="Q36" s="2" t="s">
-        <v>480</v>
-      </c>
-      <c r="R36" s="2" t="s">
-        <v>374</v>
-      </c>
-      <c r="U36" s="2"/>
-    </row>
-    <row r="37" spans="2:21" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B37" s="2" t="s">
-        <v>444</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>389</v>
-      </c>
-      <c r="E37" s="84" t="s">
-        <v>449</v>
-      </c>
-      <c r="I37" s="2" t="s">
-        <v>385</v>
-      </c>
-      <c r="J37" s="2" t="s">
-        <v>474</v>
-      </c>
-      <c r="L37" s="2" t="s">
-        <v>473</v>
-      </c>
-      <c r="M37" s="2" t="s">
-        <v>366</v>
-      </c>
-      <c r="Q37" s="2" t="s">
-        <v>481</v>
-      </c>
-      <c r="R37" s="2" t="s">
-        <v>367</v>
-      </c>
-      <c r="U37" s="2"/>
-    </row>
-    <row r="38" spans="2:21" ht="128.25" x14ac:dyDescent="0.45">
-      <c r="B38" s="2" t="s">
-        <v>447</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>389</v>
-      </c>
-      <c r="E38" s="84" t="s">
-        <v>449</v>
-      </c>
-      <c r="I38" s="2" t="s">
-        <v>385</v>
-      </c>
-      <c r="J38" s="2" t="s">
-        <v>483</v>
-      </c>
-      <c r="K38" s="2" t="s">
-        <v>389</v>
-      </c>
-      <c r="L38" s="2" t="s">
-        <v>484</v>
-      </c>
-      <c r="M38" s="2" t="s">
-        <v>366</v>
-      </c>
-      <c r="Q38" s="2" t="s">
-        <v>482</v>
-      </c>
-      <c r="R38" s="2" t="s">
-        <v>367</v>
-      </c>
-      <c r="U38" s="2"/>
-    </row>
-    <row r="39" spans="2:21" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B39" s="2" t="s">
-        <v>445</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>389</v>
-      </c>
-      <c r="E39" s="84" t="s">
-        <v>449</v>
-      </c>
-      <c r="I39" s="82"/>
-      <c r="J39" s="82"/>
-      <c r="K39" s="82"/>
-      <c r="L39" s="82"/>
-      <c r="M39" s="82"/>
-      <c r="U39" s="2"/>
-    </row>
-    <row r="40" spans="2:21" ht="71.25" x14ac:dyDescent="0.45">
-      <c r="B40" s="2" t="s">
-        <v>446</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>389</v>
-      </c>
-      <c r="E40" s="84" t="s">
-        <v>449</v>
-      </c>
-      <c r="I40" s="2" t="s">
-        <v>385</v>
-      </c>
-      <c r="J40" s="2" t="s">
-        <v>363</v>
-      </c>
-      <c r="K40" s="2" t="s">
-        <v>389</v>
-      </c>
-      <c r="L40" s="2" t="s">
-        <v>485</v>
-      </c>
-      <c r="M40" s="2" t="s">
-        <v>366</v>
-      </c>
-      <c r="Q40" s="2" t="s">
-        <v>384</v>
-      </c>
-      <c r="R40" s="2" t="s">
-        <v>374</v>
-      </c>
-      <c r="U40" s="2"/>
-    </row>
-    <row r="41" spans="2:21" ht="99.75" x14ac:dyDescent="0.45">
-      <c r="B41" s="2" t="s">
-        <v>486</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>406</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>487</v>
-      </c>
-      <c r="E41" s="84" t="s">
-        <v>366</v>
-      </c>
-      <c r="I41" s="82"/>
-      <c r="J41" s="82"/>
-      <c r="K41" s="82"/>
-      <c r="L41" s="82"/>
-      <c r="M41" s="82"/>
-      <c r="U41" s="2"/>
-    </row>
-    <row r="42" spans="2:21" x14ac:dyDescent="0.45">
-      <c r="U42" s="2"/>
-    </row>
-    <row r="43" spans="2:21" x14ac:dyDescent="0.45">
-      <c r="U43" s="2"/>
-    </row>
-    <row r="44" spans="2:21" x14ac:dyDescent="0.45">
-      <c r="U44" s="2"/>
-    </row>
-    <row r="45" spans="2:21" x14ac:dyDescent="0.45">
-      <c r="U45" s="2"/>
-    </row>
-    <row r="46" spans="2:21" x14ac:dyDescent="0.45">
-      <c r="U46" s="2"/>
-    </row>
-    <row r="47" spans="2:21" x14ac:dyDescent="0.45">
-      <c r="U47" s="2"/>
-    </row>
-    <row r="48" spans="2:21" x14ac:dyDescent="0.45">
-      <c r="U48" s="2"/>
-    </row>
-    <row r="49" spans="21:21" x14ac:dyDescent="0.45">
-      <c r="U49" s="2"/>
-    </row>
-    <row r="50" spans="21:21" x14ac:dyDescent="0.45">
-      <c r="U50" s="2"/>
-    </row>
-    <row r="51" spans="21:21" x14ac:dyDescent="0.45">
-      <c r="U51" s="2"/>
-    </row>
-    <row r="52" spans="21:21" x14ac:dyDescent="0.45">
-      <c r="U52" s="2"/>
-    </row>
-    <row r="53" spans="21:21" x14ac:dyDescent="0.45">
-      <c r="U53" s="2"/>
-    </row>
-    <row r="54" spans="21:21" x14ac:dyDescent="0.45">
-      <c r="U54" s="2"/>
-    </row>
-    <row r="55" spans="21:21" x14ac:dyDescent="0.45">
-      <c r="U55" s="2"/>
+      <c r="O35" s="82"/>
+      <c r="P35" s="82" t="s">
+        <v>536</v>
+      </c>
+      <c r="Q35" s="82" t="s">
+        <v>517</v>
+      </c>
+      <c r="R35" s="82" t="s">
+        <v>526</v>
+      </c>
+      <c r="S35" s="82" t="s">
+        <v>527</v>
+      </c>
+      <c r="T35" s="82" t="s">
+        <v>516</v>
+      </c>
+      <c r="V35" s="2"/>
+    </row>
+    <row r="36" spans="2:22" x14ac:dyDescent="0.45">
+      <c r="V36" s="2"/>
+    </row>
+    <row r="37" spans="2:22" x14ac:dyDescent="0.45">
+      <c r="V37" s="2"/>
+    </row>
+    <row r="38" spans="2:22" x14ac:dyDescent="0.45">
+      <c r="V38" s="2"/>
+    </row>
+    <row r="39" spans="2:22" x14ac:dyDescent="0.45">
+      <c r="V39" s="2"/>
+    </row>
+    <row r="40" spans="2:22" x14ac:dyDescent="0.45">
+      <c r="V40" s="2"/>
+    </row>
+    <row r="41" spans="2:22" x14ac:dyDescent="0.45">
+      <c r="V41" s="2"/>
+    </row>
+    <row r="42" spans="2:22" x14ac:dyDescent="0.45">
+      <c r="V42" s="2"/>
+    </row>
+    <row r="43" spans="2:22" x14ac:dyDescent="0.45">
+      <c r="V43" s="2"/>
+    </row>
+    <row r="44" spans="2:22" x14ac:dyDescent="0.45">
+      <c r="V44" s="2"/>
+    </row>
+    <row r="45" spans="2:22" x14ac:dyDescent="0.45">
+      <c r="V45" s="2"/>
+    </row>
+    <row r="46" spans="2:22" x14ac:dyDescent="0.45">
+      <c r="V46" s="2"/>
+    </row>
+    <row r="47" spans="2:22" x14ac:dyDescent="0.45">
+      <c r="V47" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="19" type="noConversion"/>
-  <dataValidations count="3">
-    <dataValidation errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1" xr:uid="{00000000-0002-0000-0300-000000000000}"/>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid value" error="Valid property styles are &quot;element&quot;, &quot;attribute&quot;, or &quot;abstract&quot;.  Leave the cell blank to use the default value &quot;element&quot;." promptTitle="Property Style" prompt="- &quot;element&quot; or blank (default) - Represents a typical NIEM property._x000a_- &quot;abstract&quot; - Used to create a substitution group_x000a_- &quot;attribute&quot; - Use sparingly, if at all; for values tightly-coupled to an element." sqref="W56:W1048576 V2:V55" xr:uid="{00000000-0002-0000-0300-000002000000}">
+  <dataValidations disablePrompts="1" count="3">
+    <dataValidation errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1" xr:uid="{00000000-0002-0000-0300-000000000000}"/>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid value" error="Valid property styles are &quot;element&quot;, &quot;attribute&quot;, or &quot;abstract&quot;.  Leave the cell blank to use the default value &quot;element&quot;." promptTitle="Property Style" prompt="- &quot;element&quot; or blank (default) - Represents a typical NIEM property._x000a_- &quot;abstract&quot; - Used to create a substitution group_x000a_- &quot;attribute&quot; - Use sparingly, if at all; for values tightly-coupled to an element." sqref="X48:X1048576 W2:W35" xr:uid="{00000000-0002-0000-0300-000002000000}">
       <formula1>"element,attribute,abstract"</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576" xr:uid="{00000000-0002-0000-0300-000001000000}">
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576" xr:uid="{00000000-0002-0000-0300-000001000000}">
       <formula1>MAPPING_CODES</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Hide unused columns in mapping
</commit_message>
<xml_diff>
--- a/schemas/ChargeFiling_iepd/artifacts/ChargeFiling_MappingSpreadsheet.xlsx
+++ b/schemas/ChargeFiling_iepd/artifacts/ChargeFiling_MappingSpreadsheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JamesCabral\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JamesCabral\git\JTMP-Data-Exchange-Specs\schemas\ChargeFiling_iepd\artifacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0821B922-D74E-4927-9424-542EDE59CD8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A85388D-5FDE-4B33-AA42-BD586786FCEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="21840" yWindow="-21600" windowWidth="25905" windowHeight="20985" tabRatio="781" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3371,261 +3371,6 @@
   </cellStyles>
   <dxfs count="125">
     <dxf>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -4311,6 +4056,261 @@
         <color theme="0"/>
         <name val="Calibri"/>
         <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -4533,43 +4533,43 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{733D753A-1A77-494A-B62C-0EC743EEA49A}" name="Table10" displayName="Table10" ref="A1:N2" totalsRowShown="0" headerRowDxfId="57" dataDxfId="56" tableBorderDxfId="55" headerRowCellStyle="Accent2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{733D753A-1A77-494A-B62C-0EC743EEA49A}" name="Table10" displayName="Table10" ref="A1:N2" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28" tableBorderDxfId="27" headerRowCellStyle="Accent2">
   <autoFilter ref="A1:N2" xr:uid="{E1E5EF99-DFA3-4734-B0F5-3FD6CA399E33}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{E1238927-B089-4D9E-8088-75D3EC35BFBA}" name="Source_x000a_NS Prefix" dataDxfId="54"/>
-    <tableColumn id="2" xr3:uid="{9410951A-EE35-4F3C-8F36-8BEE201CF8AF}" name="URI" dataDxfId="53"/>
-    <tableColumn id="3" xr3:uid="{2B517D23-941B-4B3E-A7DD-F7786E3924D5}" name="Definition" dataDxfId="52"/>
-    <tableColumn id="4" xr3:uid="{7DD55007-8311-4C82-A5D2-EBEDF474C65D}" name="Mapping_x000a_Code" dataDxfId="51"/>
-    <tableColumn id="5" xr3:uid="{0E949C96-18B4-4EB9-95F2-53DB84718832}" name="Description" dataDxfId="50"/>
-    <tableColumn id="6" xr3:uid="{E124F618-8325-4FF3-8BF4-E24907425ADE}" name="Notes" dataDxfId="49"/>
-    <tableColumn id="7" xr3:uid="{86983FC7-E843-4CB8-B776-1ACA5758C454}" name="Target_x000a_NS Prefix" dataDxfId="48"/>
-    <tableColumn id="8" xr3:uid="{F92DB840-CE8A-4128-8BB8-B8742F926D09}" name="Style" dataDxfId="47"/>
-    <tableColumn id="9" xr3:uid="{9202EAB5-4BBC-4DFA-8B29-56D32F2F95E2}" name="URI " dataDxfId="46"/>
-    <tableColumn id="10" xr3:uid="{BE82DF52-562E-40A7-B97A-C4017DCE324F}" name="Definition " dataDxfId="45"/>
-    <tableColumn id="11" xr3:uid="{834B3B3E-609B-4AA7-A013-2F95C8CA6ED1}" name="NDR Target" dataDxfId="44"/>
-    <tableColumn id="12" xr3:uid="{9C74517B-484A-41A5-B478-1107D7B7563E}" name="File Name" dataDxfId="43"/>
-    <tableColumn id="13" xr3:uid="{00E1E65A-D173-41FF-8A1D-F764DB3C85EB}" name="Relative Path" dataDxfId="42"/>
-    <tableColumn id="14" xr3:uid="{1A319080-CB5B-4F50-8EF6-DA7F3E87061A}" name="Draft Version" dataDxfId="41"/>
+    <tableColumn id="1" xr3:uid="{E1238927-B089-4D9E-8088-75D3EC35BFBA}" name="Source_x000a_NS Prefix" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{9410951A-EE35-4F3C-8F36-8BEE201CF8AF}" name="URI" dataDxfId="25"/>
+    <tableColumn id="3" xr3:uid="{2B517D23-941B-4B3E-A7DD-F7786E3924D5}" name="Definition" dataDxfId="24"/>
+    <tableColumn id="4" xr3:uid="{7DD55007-8311-4C82-A5D2-EBEDF474C65D}" name="Mapping_x000a_Code" dataDxfId="23"/>
+    <tableColumn id="5" xr3:uid="{0E949C96-18B4-4EB9-95F2-53DB84718832}" name="Description" dataDxfId="22"/>
+    <tableColumn id="6" xr3:uid="{E124F618-8325-4FF3-8BF4-E24907425ADE}" name="Notes" dataDxfId="21"/>
+    <tableColumn id="7" xr3:uid="{86983FC7-E843-4CB8-B776-1ACA5758C454}" name="Target_x000a_NS Prefix" dataDxfId="20"/>
+    <tableColumn id="8" xr3:uid="{F92DB840-CE8A-4128-8BB8-B8742F926D09}" name="Style" dataDxfId="19"/>
+    <tableColumn id="9" xr3:uid="{9202EAB5-4BBC-4DFA-8B29-56D32F2F95E2}" name="URI " dataDxfId="18"/>
+    <tableColumn id="10" xr3:uid="{BE82DF52-562E-40A7-B97A-C4017DCE324F}" name="Definition " dataDxfId="17"/>
+    <tableColumn id="11" xr3:uid="{834B3B3E-609B-4AA7-A013-2F95C8CA6ED1}" name="NDR Target" dataDxfId="16"/>
+    <tableColumn id="12" xr3:uid="{9C74517B-484A-41A5-B478-1107D7B7563E}" name="File Name" dataDxfId="15"/>
+    <tableColumn id="13" xr3:uid="{00E1E65A-D173-41FF-8A1D-F764DB3C85EB}" name="Relative Path" dataDxfId="14"/>
+    <tableColumn id="14" xr3:uid="{1A319080-CB5B-4F50-8EF6-DA7F3E87061A}" name="Draft Version" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{6A256153-0806-4BEE-936A-A12F0A0B7383}" name="Table11" displayName="Table11" ref="A1:K2" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39" headerRowCellStyle="Accent2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{6A256153-0806-4BEE-936A-A12F0A0B7383}" name="Table11" displayName="Table11" ref="A1:K2" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11" headerRowCellStyle="Accent2">
   <autoFilter ref="A1:K2" xr:uid="{79E81683-51FB-4FF9-9289-31DDA054DB7A}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{B23F336D-16B9-4C95-BE96-F5283EAE0F3C}" name="Source_x000a_NS Prefix" dataDxfId="38"/>
-    <tableColumn id="2" xr3:uid="{0D056408-CA8F-4336-AED7-3818011F9385}" name="Term" dataDxfId="37"/>
-    <tableColumn id="3" xr3:uid="{90A93FC4-10F0-4295-AC5C-E2A951CBA7BC}" name="Literal" dataDxfId="36"/>
-    <tableColumn id="4" xr3:uid="{A1AC1DB1-AA7D-48B2-9765-4E5BA52F23DE}" name="Definition" dataDxfId="35"/>
-    <tableColumn id="5" xr3:uid="{BD7B43BD-647B-4803-8F9F-0147C7FD23A4}" name="Mapping_x000a_Code" dataDxfId="34"/>
-    <tableColumn id="6" xr3:uid="{72609C76-FA3F-40C0-B5FF-60D4974FFD61}" name="Description" dataDxfId="33"/>
-    <tableColumn id="7" xr3:uid="{479204AB-0608-4CE8-8D22-F418523DDDA2}" name="Notes" dataDxfId="32"/>
-    <tableColumn id="8" xr3:uid="{2C9C9513-0007-44E3-8DFD-9FDD58431071}" name="Target_x000a_NS Prefix" dataDxfId="31"/>
-    <tableColumn id="9" xr3:uid="{1442C4F6-90A1-4765-A362-538E7A781367}" name="Term " dataDxfId="30"/>
-    <tableColumn id="10" xr3:uid="{92198433-569D-43D9-9243-453965C7540B}" name="Literal " dataDxfId="29"/>
-    <tableColumn id="11" xr3:uid="{38E45C62-D7D7-487A-BB8B-582528BBD31D}" name="Definition " dataDxfId="28"/>
+    <tableColumn id="1" xr3:uid="{B23F336D-16B9-4C95-BE96-F5283EAE0F3C}" name="Source_x000a_NS Prefix" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{0D056408-CA8F-4336-AED7-3818011F9385}" name="Term" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{90A93FC4-10F0-4295-AC5C-E2A951CBA7BC}" name="Literal" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{A1AC1DB1-AA7D-48B2-9765-4E5BA52F23DE}" name="Definition" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{BD7B43BD-647B-4803-8F9F-0147C7FD23A4}" name="Mapping_x000a_Code" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{72609C76-FA3F-40C0-B5FF-60D4974FFD61}" name="Description" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{479204AB-0608-4CE8-8D22-F418523DDDA2}" name="Notes" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{2C9C9513-0007-44E3-8DFD-9FDD58431071}" name="Target_x000a_NS Prefix" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{1442C4F6-90A1-4765-A362-538E7A781367}" name="Term " dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{92198433-569D-43D9-9243-453965C7540B}" name="Literal " dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{38E45C62-D7D7-487A-BB8B-582528BBD31D}" name="Definition " dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -4617,106 +4617,106 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table3" displayName="Table3" ref="A1:Z35" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26" headerRowCellStyle="Accent2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table3" displayName="Table3" ref="A1:Z35" totalsRowShown="0" headerRowDxfId="107" dataDxfId="106" headerRowCellStyle="Accent2">
   <autoFilter ref="A1:Z35" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="26">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Source_x000a_NS Prefix" dataDxfId="25"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Property Name" dataDxfId="24"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="Data Type" dataDxfId="23"/>
-    <tableColumn id="18" xr3:uid="{683B832A-0F1B-48CA-AA01-7512CABFD6B2}" name="Definition" dataDxfId="2"/>
-    <tableColumn id="21" xr3:uid="{42F421B2-5200-43B9-8173-69699FE1D709}" name="Example" dataDxfId="0"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="Cardinality" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="Mapping_x000a_Code" dataDxfId="22"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="Description" dataDxfId="21"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0500-000007000000}" name="Notes" dataDxfId="20"/>
-    <tableColumn id="24" xr3:uid="{B256BE0E-1B95-49D2-BF5B-AD5320663854}" name="EDM Class" dataDxfId="19"/>
-    <tableColumn id="23" xr3:uid="{C5C0958E-E98B-4096-B70E-A6517F49A64D}" name="EDM Attribute" dataDxfId="18"/>
-    <tableColumn id="14" xr3:uid="{70B266EE-E89C-4B0F-ACFB-6BBC1BBE7978}" name="EDM Type" dataDxfId="17"/>
-    <tableColumn id="26" xr3:uid="{B613C991-CC70-4831-83C3-97449E0A59FB}" name="EDM Definition" dataDxfId="16"/>
-    <tableColumn id="27" xr3:uid="{9FF11716-702A-419A-91F2-858D4D3B16EE}" name="EDM Cardinality" dataDxfId="15"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0500-000008000000}" name="Target_x000a_NS Prefix" dataDxfId="14"/>
-    <tableColumn id="20" xr3:uid="{8CFFA3EE-5D28-4D5E-86E0-9F9851A3E676}" name="NIEM XPath" dataDxfId="13"/>
-    <tableColumn id="25" xr3:uid="{161AA4D8-B799-4722-BAB9-DA7BA3B360DA}" name="NIEM Type" dataDxfId="12"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0500-000009000000}" name="NIEM Property Name " dataDxfId="11"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0500-00000A000000}" name="NIEM Qualified Data Type" dataDxfId="10"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0500-00000B000000}" name="NIEM Definition " dataDxfId="9"/>
-    <tableColumn id="19" xr3:uid="{C2DBDA77-E9BC-497B-A1D8-611484B019B5}" name="Cardinality2" dataDxfId="8"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0500-00000C000000}" name="NIEM Qualified Substitution Group" dataDxfId="7"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0500-00000D000000}" name="Style_x000a_default=element" dataDxfId="6"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0500-00000F000000}" name="Keywords" dataDxfId="5"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0500-000010000000}" name="Example Content" dataDxfId="4"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0500-000011000000}" name="Usage Info" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Source_x000a_NS Prefix" dataDxfId="105"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Property Name" dataDxfId="104"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="Data Type" dataDxfId="103"/>
+    <tableColumn id="18" xr3:uid="{683B832A-0F1B-48CA-AA01-7512CABFD6B2}" name="Definition" dataDxfId="102"/>
+    <tableColumn id="21" xr3:uid="{42F421B2-5200-43B9-8173-69699FE1D709}" name="Example" dataDxfId="101"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="Cardinality" dataDxfId="100"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="Mapping_x000a_Code" dataDxfId="99"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="Description" dataDxfId="98"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0500-000007000000}" name="Notes" dataDxfId="97"/>
+    <tableColumn id="24" xr3:uid="{B256BE0E-1B95-49D2-BF5B-AD5320663854}" name="EDM Class" dataDxfId="96"/>
+    <tableColumn id="23" xr3:uid="{C5C0958E-E98B-4096-B70E-A6517F49A64D}" name="EDM Attribute" dataDxfId="95"/>
+    <tableColumn id="14" xr3:uid="{70B266EE-E89C-4B0F-ACFB-6BBC1BBE7978}" name="EDM Type" dataDxfId="94"/>
+    <tableColumn id="26" xr3:uid="{B613C991-CC70-4831-83C3-97449E0A59FB}" name="EDM Definition" dataDxfId="93"/>
+    <tableColumn id="27" xr3:uid="{9FF11716-702A-419A-91F2-858D4D3B16EE}" name="EDM Cardinality" dataDxfId="92"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0500-000008000000}" name="Target_x000a_NS Prefix" dataDxfId="91"/>
+    <tableColumn id="20" xr3:uid="{8CFFA3EE-5D28-4D5E-86E0-9F9851A3E676}" name="NIEM XPath" dataDxfId="90"/>
+    <tableColumn id="25" xr3:uid="{161AA4D8-B799-4722-BAB9-DA7BA3B360DA}" name="NIEM Type" dataDxfId="89"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0500-000009000000}" name="NIEM Property Name " dataDxfId="88"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0500-00000A000000}" name="NIEM Qualified Data Type" dataDxfId="87"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0500-00000B000000}" name="NIEM Definition " dataDxfId="86"/>
+    <tableColumn id="19" xr3:uid="{C2DBDA77-E9BC-497B-A1D8-611484B019B5}" name="Cardinality2" dataDxfId="85"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0500-00000C000000}" name="NIEM Qualified Substitution Group" dataDxfId="84"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0500-00000D000000}" name="Style_x000a_default=element" dataDxfId="83"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0500-00000F000000}" name="Keywords" dataDxfId="82"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0500-000010000000}" name="Example Content" dataDxfId="81"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0500-000011000000}" name="Usage Info" dataDxfId="80"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{8578AF98-37D1-469F-9DF8-407CA14E272E}" name="Table7" displayName="Table7" ref="A1:N2" insertRow="1" totalsRowShown="0" headerRowDxfId="107" dataDxfId="106" headerRowCellStyle="Accent2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{8578AF98-37D1-469F-9DF8-407CA14E272E}" name="Table7" displayName="Table7" ref="A1:N2" insertRow="1" totalsRowShown="0" headerRowDxfId="79" dataDxfId="78" headerRowCellStyle="Accent2">
   <autoFilter ref="A1:N2" xr:uid="{C7C77A82-0E27-43B2-B802-78C571058434}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{2DA18095-6134-4F51-B45C-1FD29868E9D3}" name="Source_x000a_NS Prefix" dataDxfId="105"/>
-    <tableColumn id="2" xr3:uid="{BB7222D3-DF23-4FB4-AACC-7074C8351301}" name="Type Name" dataDxfId="104"/>
-    <tableColumn id="3" xr3:uid="{3AFA1B4A-1B7D-4408-95C4-5D276F6AFCE8}" name="Parent / Base Type" dataDxfId="103"/>
-    <tableColumn id="4" xr3:uid="{DA420D7E-BF45-4DFA-A327-6F5816081658}" name="Definition" dataDxfId="102"/>
-    <tableColumn id="5" xr3:uid="{F0EC8E3B-3924-4431-8523-4FE53C5BC2F9}" name="Mapping_x000a_Code" dataDxfId="101"/>
-    <tableColumn id="6" xr3:uid="{529DD89A-D9F2-4643-B653-535C5D5260B2}" name="Description" dataDxfId="100"/>
-    <tableColumn id="7" xr3:uid="{6A865D88-3AC4-4546-981B-9A5A7EB8F351}" name="Notes" dataDxfId="99"/>
-    <tableColumn id="8" xr3:uid="{FF25761D-56AD-4BA0-8910-6C18CBA6D0CD}" name="Target_x000a_NS Prefix" dataDxfId="98"/>
-    <tableColumn id="9" xr3:uid="{B5902010-EF7D-4FA2-B2B6-B491046CA96D}" name="Type Name " dataDxfId="97"/>
-    <tableColumn id="10" xr3:uid="{422CF2D7-F9C5-4193-9DD3-943BF799ABB8}" name="Qualified Parent / Base Type " dataDxfId="96"/>
-    <tableColumn id="11" xr3:uid="{E69F557F-28BC-41CA-B77C-8F0F1781F3F8}" name="Definition " dataDxfId="95"/>
-    <tableColumn id="12" xr3:uid="{33FAD9D1-2E3A-4DD0-99A3-80B7DC1320DF}" name="Style _x000a_default=object" dataDxfId="94"/>
-    <tableColumn id="13" xr3:uid="{A3613263-4395-41B2-9149-1319C9DE1572}" name="Qualified Union Member Types_x000a_comma-separated list" dataDxfId="93"/>
-    <tableColumn id="14" xr3:uid="{DA9EC388-28FD-4FFC-9EB0-04AF1B5F2EBE}" name="Qualified Metadata Applies to Types_x000a_comma-separated list" dataDxfId="92"/>
+    <tableColumn id="1" xr3:uid="{2DA18095-6134-4F51-B45C-1FD29868E9D3}" name="Source_x000a_NS Prefix" dataDxfId="77"/>
+    <tableColumn id="2" xr3:uid="{BB7222D3-DF23-4FB4-AACC-7074C8351301}" name="Type Name" dataDxfId="76"/>
+    <tableColumn id="3" xr3:uid="{3AFA1B4A-1B7D-4408-95C4-5D276F6AFCE8}" name="Parent / Base Type" dataDxfId="75"/>
+    <tableColumn id="4" xr3:uid="{DA420D7E-BF45-4DFA-A327-6F5816081658}" name="Definition" dataDxfId="74"/>
+    <tableColumn id="5" xr3:uid="{F0EC8E3B-3924-4431-8523-4FE53C5BC2F9}" name="Mapping_x000a_Code" dataDxfId="73"/>
+    <tableColumn id="6" xr3:uid="{529DD89A-D9F2-4643-B653-535C5D5260B2}" name="Description" dataDxfId="72"/>
+    <tableColumn id="7" xr3:uid="{6A865D88-3AC4-4546-981B-9A5A7EB8F351}" name="Notes" dataDxfId="71"/>
+    <tableColumn id="8" xr3:uid="{FF25761D-56AD-4BA0-8910-6C18CBA6D0CD}" name="Target_x000a_NS Prefix" dataDxfId="70"/>
+    <tableColumn id="9" xr3:uid="{B5902010-EF7D-4FA2-B2B6-B491046CA96D}" name="Type Name " dataDxfId="69"/>
+    <tableColumn id="10" xr3:uid="{422CF2D7-F9C5-4193-9DD3-943BF799ABB8}" name="Qualified Parent / Base Type " dataDxfId="68"/>
+    <tableColumn id="11" xr3:uid="{E69F557F-28BC-41CA-B77C-8F0F1781F3F8}" name="Definition " dataDxfId="67"/>
+    <tableColumn id="12" xr3:uid="{33FAD9D1-2E3A-4DD0-99A3-80B7DC1320DF}" name="Style _x000a_default=object" dataDxfId="66"/>
+    <tableColumn id="13" xr3:uid="{A3613263-4395-41B2-9149-1319C9DE1572}" name="Qualified Union Member Types_x000a_comma-separated list" dataDxfId="65"/>
+    <tableColumn id="14" xr3:uid="{DA9EC388-28FD-4FFC-9EB0-04AF1B5F2EBE}" name="Qualified Metadata Applies to Types_x000a_comma-separated list" dataDxfId="64"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="Table8" displayName="Table8" ref="A1:Q2" insertRow="1" totalsRowShown="0" headerRowDxfId="91" dataDxfId="90">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="Table8" displayName="Table8" ref="A1:Q2" insertRow="1" totalsRowShown="0" headerRowDxfId="63" dataDxfId="62">
   <autoFilter ref="A1:Q2" xr:uid="{00000000-0009-0000-0100-000008000000}"/>
   <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="Source_x000a_Type NS" dataDxfId="89"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="Type Name" dataDxfId="88"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0600-000003000000}" name="Property NS" dataDxfId="87"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0600-000004000000}" name="Property Name" dataDxfId="86"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0600-000005000000}" name="Min" dataDxfId="85"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0600-000006000000}" name="Max" dataDxfId="84"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0600-000007000000}" name="Mapping_x000a_Code" dataDxfId="83"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0600-000008000000}" name="Description" dataDxfId="82"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0600-000009000000}" name="Notes" dataDxfId="81"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0600-00000A000000}" name="Target_x000a_Type NS" dataDxfId="80"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0600-00000B000000}" name="Type Name " dataDxfId="79"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0600-00000C000000}" name="Property NS " dataDxfId="78"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0600-00000D000000}" name="Property Name " dataDxfId="77"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0600-00000E000000}" name="Min_x000a_(default=0)" dataDxfId="76"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0600-00000F000000}" name="Max (default_x000a_=unbounded)" dataDxfId="75"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0600-000010000000}" name="Definition_x000a_For an external property in an adapter type" dataDxfId="74"/>
-    <tableColumn id="17" xr3:uid="{78D268D1-27FA-4E25-9781-8F942EC05BA0}" name="Sequence" dataDxfId="73"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="Source_x000a_Type NS" dataDxfId="61"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="Type Name" dataDxfId="60"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0600-000003000000}" name="Property NS" dataDxfId="59"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0600-000004000000}" name="Property Name" dataDxfId="58"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0600-000005000000}" name="Min" dataDxfId="57"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0600-000006000000}" name="Max" dataDxfId="56"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0600-000007000000}" name="Mapping_x000a_Code" dataDxfId="55"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0600-000008000000}" name="Description" dataDxfId="54"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0600-000009000000}" name="Notes" dataDxfId="53"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0600-00000A000000}" name="Target_x000a_Type NS" dataDxfId="52"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0600-00000B000000}" name="Type Name " dataDxfId="51"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0600-00000C000000}" name="Property NS " dataDxfId="50"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0600-00000D000000}" name="Property Name " dataDxfId="49"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0600-00000E000000}" name="Min_x000a_(default=0)" dataDxfId="48"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0600-00000F000000}" name="Max (default_x000a_=unbounded)" dataDxfId="47"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0600-000010000000}" name="Definition_x000a_For an external property in an adapter type" dataDxfId="46"/>
+    <tableColumn id="17" xr3:uid="{78D268D1-27FA-4E25-9781-8F942EC05BA0}" name="Sequence" dataDxfId="45"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="Table13" displayName="Table13" ref="A1:M2" totalsRowShown="0" headerRowDxfId="72" dataDxfId="71" headerRowCellStyle="Accent2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="Table13" displayName="Table13" ref="A1:M2" totalsRowShown="0" headerRowDxfId="44" dataDxfId="43" headerRowCellStyle="Accent2">
   <autoFilter ref="A1:M2" xr:uid="{00000000-0009-0000-0100-00000D000000}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="Source_x000a_NS Prefix" dataDxfId="70"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0700-000002000000}" name="Type Name" dataDxfId="69"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0700-000003000000}" name="Value" dataDxfId="68"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0700-000004000000}" name="Definition" dataDxfId="67"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0700-000005000000}" name="Style_x000a_default=enumeration" dataDxfId="66"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0700-000006000000}" name="Mapping_x000a_Code" dataDxfId="65"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0700-000007000000}" name="Description" dataDxfId="64"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0700-000008000000}" name="Notes" dataDxfId="63"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0700-000009000000}" name="Target_x000a_NS Prefix" dataDxfId="62"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0700-00000A000000}" name="Type Name " dataDxfId="61"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0700-00000B000000}" name="Value " dataDxfId="60"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0700-00000C000000}" name="Definition " dataDxfId="59"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0700-00000D000000}" name="Style_x000a_default=enumeration " dataDxfId="58"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="Source_x000a_NS Prefix" dataDxfId="42"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0700-000002000000}" name="Type Name" dataDxfId="41"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0700-000003000000}" name="Value" dataDxfId="40"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0700-000004000000}" name="Definition" dataDxfId="39"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0700-000005000000}" name="Style_x000a_default=enumeration" dataDxfId="38"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0700-000006000000}" name="Mapping_x000a_Code" dataDxfId="37"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0700-000007000000}" name="Description" dataDxfId="36"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0700-000008000000}" name="Notes" dataDxfId="35"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0700-000009000000}" name="Target_x000a_NS Prefix" dataDxfId="34"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0700-00000A000000}" name="Type Name " dataDxfId="33"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0700-00000B000000}" name="Value " dataDxfId="32"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0700-00000C000000}" name="Definition " dataDxfId="31"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0700-00000D000000}" name="Style_x000a_default=enumeration " dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -7277,7 +7277,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E5" sqref="E5"/>
+      <selection pane="bottomRight" activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -7288,8 +7288,8 @@
     <col min="4" max="4" width="12.46484375" style="2" customWidth="1"/>
     <col min="5" max="5" width="12.46484375" style="87" customWidth="1"/>
     <col min="6" max="6" width="17.19921875" style="84" customWidth="1"/>
-    <col min="7" max="7" width="4.9296875" style="2" customWidth="1"/>
-    <col min="8" max="9" width="22.6640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="4.9296875" style="2" hidden="1" customWidth="1"/>
+    <col min="8" max="9" width="22.6640625" style="2" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="8.796875" style="2" customWidth="1"/>
     <col min="11" max="12" width="13.06640625" style="2" customWidth="1"/>
     <col min="13" max="13" width="22.6640625" style="2" customWidth="1"/>
@@ -8953,7 +8953,7 @@
     </row>
   </sheetData>
   <phoneticPr fontId="19" type="noConversion"/>
-  <dataValidations disablePrompts="1" count="3">
+  <dataValidations count="3">
     <dataValidation errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1" xr:uid="{00000000-0002-0000-0300-000000000000}"/>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid value" error="Valid property styles are &quot;element&quot;, &quot;attribute&quot;, or &quot;abstract&quot;.  Leave the cell blank to use the default value &quot;element&quot;." promptTitle="Property Style" prompt="- &quot;element&quot; or blank (default) - Represents a typical NIEM property._x000a_- &quot;abstract&quot; - Used to create a substitution group_x000a_- &quot;attribute&quot; - Use sparingly, if at all; for values tightly-coupled to an element." sqref="X48:X1048576 W2:W35" xr:uid="{00000000-0002-0000-0300-000002000000}">
       <formula1>"element,attribute,abstract"</formula1>

</xml_diff>

<commit_message>
Added ChargeKey, ChargeSequenceID, EmailAddress, PhoneNumner
</commit_message>
<xml_diff>
--- a/schemas/ChargeFiling_iepd/artifacts/ChargeFiling_MappingSpreadsheet.xlsx
+++ b/schemas/ChargeFiling_iepd/artifacts/ChargeFiling_MappingSpreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JamesCabral\git\JTMP-Data-Exchange-Specs\schemas\ChargeFiling_iepd\artifacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A85388D-5FDE-4B33-AA42-BD586786FCEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01AB4833-38DE-4EDC-A7F5-0AA934EA23FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="21840" yWindow="-21600" windowWidth="25905" windowHeight="20985" tabRatio="781" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Codes | Facets'!$A$1:$M$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7">Namespace!$A$1:$N$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Property!$A$1:$W$35</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Property!$A$1:$W$39</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4">Type!$A$1:$L$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5">'Type-Has-Property'!$A$1:$P$1</definedName>
     <definedName name="CODES_NamespaceStyle">'Field Descriptions'!$B$165:$B$176</definedName>
@@ -149,7 +149,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1008" uniqueCount="616">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1048" uniqueCount="637">
   <si>
     <t>Definition</t>
   </si>
@@ -2420,9 +2420,6 @@
     <t>Charge Modifier</t>
   </si>
   <si>
-    <t>Resufed Charge Disposition RefusalCode</t>
-  </si>
-  <si>
     <t>ChargeDisposiotion</t>
   </si>
   <si>
@@ -2694,6 +2691,72 @@
   </si>
   <si>
     <t>F/3</t>
+  </si>
+  <si>
+    <t>ChargeKey</t>
+  </si>
+  <si>
+    <t>ATNChargeSequenceID</t>
+  </si>
+  <si>
+    <t>Refused Charge Disposition RefusalCode</t>
+  </si>
+  <si>
+    <t>EmailAddress</t>
+  </si>
+  <si>
+    <t>PhoneNumber</t>
+  </si>
+  <si>
+    <t>TelephoneNumberType</t>
+  </si>
+  <si>
+    <t>A UCT Charge Key (Uniform Charge Table) is a shared key or identifier from a shared table that standardizes charge code definitions across the enterprise.</t>
+  </si>
+  <si>
+    <t>nola-ext:ChargeKey</t>
+  </si>
+  <si>
+    <t>j:Arrest/j:ArrestCharge/nola-ext:ChargeAugmentation/nola-ext:ChargeKey</t>
+  </si>
+  <si>
+    <t>nola-ext:StatewideATNChargeSequenceID</t>
+  </si>
+  <si>
+    <t>j:Arrest/j:ArrestCharge/nola-ext:ChargeAugmentation/nola-ext:ATNChargeSequenceNumber</t>
+  </si>
+  <si>
+    <t>A sequential identifier number assigned to the arrest of a subject i.e ATN. The State's Police Automated Fingerprint Inforamtion System (AFIS) generates an ATN to uniquely identify each booking event, often referred to as an Arrest Cycle. The ATN must be communicated from the Sheriff to the Court at a minimum, in order to effectively update the State computerized criminal history (CCH) with dispositions of arrest charges.</t>
+  </si>
+  <si>
+    <t>nc:ContactEmailID</t>
+  </si>
+  <si>
+    <t>An email address by which a case party will be notified electronically.</t>
+  </si>
+  <si>
+    <t>nc:CourtCase/j:CaseAugmentation/j:CaseDefendantParty/nc:EntityPerson/nc:PersonContactInformation/nc:ContactEmailID</t>
+  </si>
+  <si>
+    <t>nc:ContactInformationType</t>
+  </si>
+  <si>
+    <t>nc:ContactTelephoneNumber</t>
+  </si>
+  <si>
+    <t>nc:TelephoneNumberType</t>
+  </si>
+  <si>
+    <t>nc:CourtCase/j:CaseAugmentation/j:CaseDefendantParty/nc:EntityPerson/nc:PersonContactInformation/nc:ContactTelephoneNumber</t>
+  </si>
+  <si>
+    <t>A data concept for a telephone number.</t>
+  </si>
+  <si>
+    <t>An electronic mailing address by which a person or organization may be contacted.</t>
+  </si>
+  <si>
+    <t>A telephone number for a telecommunication device by which a person or organization may be contacted.</t>
   </si>
 </sst>
 </file>
@@ -3053,7 +3116,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3295,6 +3358,12 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="71">
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
@@ -4617,8 +4686,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table3" displayName="Table3" ref="A1:Z35" totalsRowShown="0" headerRowDxfId="107" dataDxfId="106" headerRowCellStyle="Accent2">
-  <autoFilter ref="A1:Z35" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table3" displayName="Table3" ref="A1:Z39" totalsRowShown="0" headerRowDxfId="107" dataDxfId="106" headerRowCellStyle="Accent2">
+  <autoFilter ref="A1:Z39" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="26">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Source_x000a_NS Prefix" dataDxfId="105"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Property Name" dataDxfId="104"/>
@@ -7273,11 +7342,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AB47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L4" sqref="L4"/>
+      <selection pane="bottomRight" activeCell="T45" sqref="T45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -7323,7 +7392,7 @@
         <v>0</v>
       </c>
       <c r="E1" s="86" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="F1" s="83" t="s">
         <v>441</v>
@@ -7400,7 +7469,7 @@
         <v>389</v>
       </c>
       <c r="E2" s="87" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="F2" s="84">
         <v>1</v>
@@ -7451,29 +7520,29 @@
         <v>365</v>
       </c>
       <c r="K3" s="82" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="L3" s="82" t="s">
         <v>406</v>
       </c>
       <c r="M3" s="82" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="N3" s="82"/>
       <c r="P3" s="82" t="s">
+        <v>552</v>
+      </c>
+      <c r="Q3" s="82" t="s">
+        <v>547</v>
+      </c>
+      <c r="R3" s="82" t="s">
         <v>553</v>
       </c>
-      <c r="Q3" s="82" t="s">
+      <c r="S3" s="82" t="s">
         <v>548</v>
       </c>
-      <c r="R3" s="82" t="s">
-        <v>554</v>
-      </c>
-      <c r="S3" s="82" t="s">
-        <v>549</v>
-      </c>
       <c r="T3" s="82" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="V3" s="2"/>
     </row>
@@ -7494,20 +7563,20 @@
         <v>365</v>
       </c>
       <c r="K4" s="82" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="L4" s="82" t="s">
         <v>389</v>
       </c>
       <c r="M4" s="82" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="N4" s="82"/>
       <c r="P4" s="82" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="Q4" s="82" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="R4" s="82" t="s">
         <v>384</v>
@@ -7516,7 +7585,7 @@
         <v>374</v>
       </c>
       <c r="T4" s="82" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="V4" s="2"/>
     </row>
@@ -7534,20 +7603,20 @@
         <v>365</v>
       </c>
       <c r="K5" s="82" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="L5" s="82" t="s">
         <v>389</v>
       </c>
       <c r="M5" s="82" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="N5" s="82"/>
       <c r="P5" s="82" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="Q5" s="82" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="R5" s="82" t="s">
         <v>384</v>
@@ -7556,7 +7625,7 @@
         <v>374</v>
       </c>
       <c r="T5" s="82" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="V5" s="2"/>
     </row>
@@ -7568,7 +7637,7 @@
         <v>389</v>
       </c>
       <c r="E6" s="87" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="F6" s="84">
         <v>1</v>
@@ -7622,20 +7691,20 @@
         <v>456</v>
       </c>
       <c r="K7" s="82" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="L7" s="82" t="s">
         <v>396</v>
       </c>
       <c r="M7" s="82" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="N7" s="82"/>
       <c r="P7" s="82" t="s">
+        <v>545</v>
+      </c>
+      <c r="Q7" s="82" t="s">
         <v>546</v>
-      </c>
-      <c r="Q7" s="82" t="s">
-        <v>547</v>
       </c>
       <c r="R7" s="82" t="s">
         <v>381</v>
@@ -7644,7 +7713,7 @@
         <v>382</v>
       </c>
       <c r="T7" s="82" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="V7" s="2"/>
     </row>
@@ -7659,7 +7728,7 @@
         <v>411</v>
       </c>
       <c r="E8" s="87" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="F8" s="84" t="s">
         <v>366</v>
@@ -7668,31 +7737,31 @@
         <v>456</v>
       </c>
       <c r="K8" s="82" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="L8" s="82" t="s">
         <v>515</v>
       </c>
       <c r="M8" s="82" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="N8" s="82">
         <v>1</v>
       </c>
       <c r="P8" s="82" t="s">
+        <v>538</v>
+      </c>
+      <c r="Q8" s="82" t="s">
+        <v>541</v>
+      </c>
+      <c r="R8" s="82" t="s">
         <v>539</v>
       </c>
-      <c r="Q8" s="82" t="s">
-        <v>542</v>
-      </c>
-      <c r="R8" s="82" t="s">
+      <c r="S8" s="82" t="s">
         <v>540</v>
       </c>
-      <c r="S8" s="82" t="s">
-        <v>541</v>
-      </c>
       <c r="T8" s="82" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="V8" s="2"/>
     </row>
@@ -7713,31 +7782,31 @@
         <v>456</v>
       </c>
       <c r="K9" s="82" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="L9" s="82" t="s">
         <v>515</v>
       </c>
       <c r="M9" s="82" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="N9" s="82">
         <v>1</v>
       </c>
       <c r="P9" s="82" t="s">
+        <v>538</v>
+      </c>
+      <c r="Q9" s="82" t="s">
+        <v>541</v>
+      </c>
+      <c r="R9" s="82" t="s">
         <v>539</v>
       </c>
-      <c r="Q9" s="82" t="s">
-        <v>542</v>
-      </c>
-      <c r="R9" s="82" t="s">
+      <c r="S9" s="82" t="s">
         <v>540</v>
       </c>
-      <c r="S9" s="82" t="s">
-        <v>541</v>
-      </c>
       <c r="T9" s="82" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="V9" s="2"/>
     </row>
@@ -7755,31 +7824,31 @@
         <v>456</v>
       </c>
       <c r="K10" s="82" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="L10" s="82" t="s">
         <v>515</v>
       </c>
       <c r="M10" s="82" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="N10" s="82">
         <v>1</v>
       </c>
       <c r="P10" s="82" t="s">
+        <v>538</v>
+      </c>
+      <c r="Q10" s="82" t="s">
+        <v>541</v>
+      </c>
+      <c r="R10" s="82" t="s">
         <v>539</v>
       </c>
-      <c r="Q10" s="82" t="s">
-        <v>542</v>
-      </c>
-      <c r="R10" s="82" t="s">
+      <c r="S10" s="82" t="s">
         <v>540</v>
       </c>
-      <c r="S10" s="82" t="s">
-        <v>541</v>
-      </c>
       <c r="T10" s="82" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="V10" s="2"/>
     </row>
@@ -7800,31 +7869,31 @@
         <v>456</v>
       </c>
       <c r="K11" s="82" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="L11" s="82" t="s">
         <v>515</v>
       </c>
       <c r="M11" s="82" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="N11" s="82">
         <v>1</v>
       </c>
       <c r="P11" s="82" t="s">
+        <v>538</v>
+      </c>
+      <c r="Q11" s="82" t="s">
+        <v>541</v>
+      </c>
+      <c r="R11" s="82" t="s">
         <v>539</v>
       </c>
-      <c r="Q11" s="82" t="s">
-        <v>542</v>
-      </c>
-      <c r="R11" s="82" t="s">
+      <c r="S11" s="82" t="s">
         <v>540</v>
       </c>
-      <c r="S11" s="82" t="s">
-        <v>541</v>
-      </c>
       <c r="T11" s="82" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="V11" s="2"/>
     </row>
@@ -7836,7 +7905,7 @@
         <v>389</v>
       </c>
       <c r="E12" s="87" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="F12" s="84">
         <v>1</v>
@@ -7881,7 +7950,7 @@
         <v>389</v>
       </c>
       <c r="E13" s="87" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="F13" s="84">
         <v>1</v>
@@ -7968,7 +8037,7 @@
         <v>428</v>
       </c>
       <c r="E15" s="87" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="F15" s="84">
         <v>1</v>
@@ -8061,7 +8130,7 @@
         <v>424</v>
       </c>
       <c r="E17" s="87" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="F17" s="84" t="s">
         <v>366</v>
@@ -8109,7 +8178,7 @@
         <v>430</v>
       </c>
       <c r="E18" s="87" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="F18" s="84" t="s">
         <v>366</v>
@@ -8196,7 +8265,7 @@
         <v>432</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="E20" s="87">
         <v>9999999</v>
@@ -8205,55 +8274,55 @@
         <v>366</v>
       </c>
       <c r="J20" s="82" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="K20" s="82" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L20" s="82" t="s">
         <v>389</v>
       </c>
       <c r="M20" s="82" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="N20" s="85" t="s">
         <v>366</v>
       </c>
       <c r="P20" s="82" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="Q20" s="82" t="s">
         <v>477</v>
       </c>
       <c r="R20" s="82" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="S20" s="82" t="s">
         <v>374</v>
       </c>
       <c r="T20" s="82" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="V20" s="2"/>
     </row>
     <row r="21" spans="2:22" ht="71.25" x14ac:dyDescent="0.45">
       <c r="B21" s="2" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>357</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="F21" s="84" t="s">
         <v>503</v>
       </c>
       <c r="J21" s="2" t="s">
+        <v>569</v>
+      </c>
+      <c r="K21" s="2" t="s">
         <v>570</v>
-      </c>
-      <c r="K21" s="2" t="s">
-        <v>571</v>
       </c>
       <c r="L21" s="2" t="s">
         <v>389</v>
@@ -8265,19 +8334,19 @@
         <v>503</v>
       </c>
       <c r="P21" s="2" t="s">
+        <v>571</v>
+      </c>
+      <c r="Q21" s="2" t="s">
         <v>572</v>
       </c>
-      <c r="Q21" s="2" t="s">
+      <c r="R21" s="2" t="s">
         <v>573</v>
-      </c>
-      <c r="R21" s="2" t="s">
-        <v>574</v>
       </c>
       <c r="S21" s="2" t="s">
         <v>481</v>
       </c>
       <c r="T21" s="2" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="V21" s="2"/>
     </row>
@@ -8289,7 +8358,7 @@
         <v>396</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="E22" s="88">
         <v>45566</v>
@@ -8298,25 +8367,25 @@
         <v>366</v>
       </c>
       <c r="J22" s="82" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="K22" s="82" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="L22" s="82" t="s">
         <v>396</v>
       </c>
       <c r="M22" s="82" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="N22" s="85" t="s">
         <v>366</v>
       </c>
       <c r="P22" s="82" t="s">
+        <v>593</v>
+      </c>
+      <c r="Q22" s="82" t="s">
         <v>594</v>
-      </c>
-      <c r="Q22" s="82" t="s">
-        <v>595</v>
       </c>
       <c r="R22" s="82" t="s">
         <v>381</v>
@@ -8325,7 +8394,7 @@
         <v>382</v>
       </c>
       <c r="T22" s="82" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="V22" s="2"/>
     </row>
@@ -8337,43 +8406,43 @@
         <v>357</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="E23" s="87" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="F23" s="84" t="s">
         <v>366</v>
       </c>
       <c r="J23" s="82" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="K23" s="82" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="L23" s="82" t="s">
         <v>389</v>
       </c>
       <c r="M23" s="82" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="N23" s="85" t="s">
         <v>366</v>
       </c>
       <c r="P23" s="82" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="Q23" s="82" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="R23" s="82" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="S23" s="82" t="s">
         <v>481</v>
       </c>
       <c r="T23" s="82" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="V23" s="2"/>
     </row>
@@ -8385,43 +8454,43 @@
         <v>357</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="E24" s="87" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="F24" s="84" t="s">
         <v>366</v>
       </c>
       <c r="J24" s="82" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="K24" s="82" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="L24" s="82" t="s">
         <v>389</v>
       </c>
       <c r="M24" s="82" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="N24" s="85" t="s">
         <v>366</v>
       </c>
       <c r="P24" s="82" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="Q24" s="82" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="R24" s="82" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="S24" s="82" t="s">
         <v>481</v>
       </c>
       <c r="T24" s="82" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="V24" s="2"/>
     </row>
@@ -8442,10 +8511,10 @@
         <v>366</v>
       </c>
       <c r="J25" s="82" t="s">
+        <v>577</v>
+      </c>
+      <c r="K25" s="82" t="s">
         <v>578</v>
-      </c>
-      <c r="K25" s="82" t="s">
-        <v>579</v>
       </c>
       <c r="L25" s="82" t="s">
         <v>389</v>
@@ -8457,10 +8526,10 @@
         <v>366</v>
       </c>
       <c r="P25" s="82" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="Q25" s="82" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="R25" s="82" t="s">
         <v>384</v>
@@ -8502,7 +8571,7 @@
         <v>366</v>
       </c>
       <c r="P26" s="82" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="Q26" s="2" t="s">
         <v>504</v>
@@ -8547,7 +8616,7 @@
         <v>366</v>
       </c>
       <c r="P27" s="82" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="Q27" s="2" t="s">
         <v>502</v>
@@ -8571,7 +8640,7 @@
         <v>389</v>
       </c>
       <c r="E28" s="87" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="F28" s="84" t="s">
         <v>366</v>
@@ -8580,31 +8649,31 @@
         <v>365</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="L28" s="2" t="s">
         <v>389</v>
       </c>
       <c r="M28" s="2" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="N28" s="2" t="s">
         <v>366</v>
       </c>
       <c r="P28" s="2" t="s">
+        <v>586</v>
+      </c>
+      <c r="Q28" s="2" t="s">
         <v>587</v>
       </c>
-      <c r="Q28" s="2" t="s">
+      <c r="R28" s="2" t="s">
         <v>588</v>
-      </c>
-      <c r="R28" s="2" t="s">
-        <v>589</v>
       </c>
       <c r="S28" s="2" t="s">
         <v>367</v>
       </c>
       <c r="T28" s="2" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="V28" s="2"/>
     </row>
@@ -8616,7 +8685,7 @@
         <v>389</v>
       </c>
       <c r="E29" s="87" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="F29" s="84" t="s">
         <v>442</v>
@@ -8637,7 +8706,7 @@
         <v>366</v>
       </c>
       <c r="P29" s="2" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="Q29" s="2" t="s">
         <v>506</v>
@@ -8682,7 +8751,7 @@
         <v>366</v>
       </c>
       <c r="P30" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="R30" s="2" t="s">
         <v>466</v>
@@ -8700,7 +8769,7 @@
         <v>389</v>
       </c>
       <c r="E31" s="87" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="F31" s="84" t="s">
         <v>442</v>
@@ -8718,7 +8787,7 @@
         <v>366</v>
       </c>
       <c r="P31" s="2" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="Q31" s="2" t="s">
         <v>507</v>
@@ -8742,7 +8811,7 @@
         <v>389</v>
       </c>
       <c r="E32" s="87" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F32" s="84" t="s">
         <v>442</v>
@@ -8763,7 +8832,7 @@
         <v>366</v>
       </c>
       <c r="P32" s="2" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="Q32" s="2" t="s">
         <v>507</v>
@@ -8779,7 +8848,7 @@
       </c>
       <c r="V32" s="2"/>
     </row>
-    <row r="33" spans="2:22" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:26" ht="71.25" x14ac:dyDescent="0.45">
       <c r="B33" s="2" t="s">
         <v>522</v>
       </c>
@@ -8808,7 +8877,7 @@
         <v>366</v>
       </c>
       <c r="P33" s="2" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="Q33" s="2" t="s">
         <v>508</v>
@@ -8824,7 +8893,7 @@
       </c>
       <c r="V33" s="2"/>
     </row>
-    <row r="34" spans="2:22" ht="99.75" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:26" ht="99.75" x14ac:dyDescent="0.45">
       <c r="B34" s="2" t="s">
         <v>523</v>
       </c>
@@ -8853,7 +8922,7 @@
         <v>366</v>
       </c>
       <c r="P34" s="2" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="Q34" s="2" t="s">
         <v>507</v>
@@ -8869,9 +8938,9 @@
       </c>
       <c r="V34" s="2"/>
     </row>
-    <row r="35" spans="2:22" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:26" ht="85.5" x14ac:dyDescent="0.45">
       <c r="B35" s="2" t="s">
-        <v>524</v>
+        <v>617</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>389</v>
@@ -8883,7 +8952,7 @@
         <v>442</v>
       </c>
       <c r="J35" s="82" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="K35" s="82" t="s">
         <v>514</v>
@@ -8899,63 +8968,239 @@
       </c>
       <c r="O35" s="82"/>
       <c r="P35" s="82" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="Q35" s="82" t="s">
         <v>517</v>
       </c>
       <c r="R35" s="82" t="s">
+        <v>525</v>
+      </c>
+      <c r="S35" s="82" t="s">
         <v>526</v>
-      </c>
-      <c r="S35" s="82" t="s">
-        <v>527</v>
       </c>
       <c r="T35" s="82" t="s">
         <v>516</v>
       </c>
       <c r="V35" s="2"/>
     </row>
-    <row r="36" spans="2:22" x14ac:dyDescent="0.45">
-      <c r="V36" s="2"/>
-    </row>
-    <row r="37" spans="2:22" x14ac:dyDescent="0.45">
-      <c r="V37" s="2"/>
-    </row>
-    <row r="38" spans="2:22" x14ac:dyDescent="0.45">
-      <c r="V38" s="2"/>
-    </row>
-    <row r="39" spans="2:22" x14ac:dyDescent="0.45">
-      <c r="V39" s="2"/>
-    </row>
-    <row r="40" spans="2:22" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:26" ht="142.5" x14ac:dyDescent="0.45">
+      <c r="A36" s="89"/>
+      <c r="B36" s="89"/>
+      <c r="C36" s="89"/>
+      <c r="D36" s="89"/>
+      <c r="F36" s="90"/>
+      <c r="G36" s="89"/>
+      <c r="H36" s="89"/>
+      <c r="I36" s="89"/>
+      <c r="J36" s="89" t="s">
+        <v>385</v>
+      </c>
+      <c r="K36" s="89" t="s">
+        <v>615</v>
+      </c>
+      <c r="L36" s="89" t="s">
+        <v>389</v>
+      </c>
+      <c r="M36" s="89" t="s">
+        <v>621</v>
+      </c>
+      <c r="N36" s="89" t="s">
+        <v>366</v>
+      </c>
+      <c r="O36" s="89"/>
+      <c r="P36" s="89" t="s">
+        <v>623</v>
+      </c>
+      <c r="Q36" s="89" t="s">
+        <v>517</v>
+      </c>
+      <c r="R36" s="89" t="s">
+        <v>622</v>
+      </c>
+      <c r="S36" s="89" t="s">
+        <v>374</v>
+      </c>
+      <c r="T36" s="89" t="s">
+        <v>621</v>
+      </c>
+      <c r="U36" s="89"/>
+      <c r="V36" s="89"/>
+      <c r="W36" s="89"/>
+      <c r="X36" s="89"/>
+      <c r="Y36" s="89"/>
+      <c r="Z36" s="89"/>
+    </row>
+    <row r="37" spans="1:26" ht="409.5" x14ac:dyDescent="0.45">
+      <c r="A37" s="89"/>
+      <c r="B37" s="89"/>
+      <c r="C37" s="89"/>
+      <c r="D37" s="89"/>
+      <c r="F37" s="90"/>
+      <c r="G37" s="89"/>
+      <c r="H37" s="89"/>
+      <c r="I37" s="89"/>
+      <c r="J37" s="89" t="s">
+        <v>456</v>
+      </c>
+      <c r="K37" s="89" t="s">
+        <v>616</v>
+      </c>
+      <c r="L37" s="89" t="s">
+        <v>389</v>
+      </c>
+      <c r="M37" s="89" t="s">
+        <v>626</v>
+      </c>
+      <c r="N37" s="89" t="s">
+        <v>503</v>
+      </c>
+      <c r="O37" s="89"/>
+      <c r="P37" s="89" t="s">
+        <v>625</v>
+      </c>
+      <c r="Q37" s="89" t="s">
+        <v>517</v>
+      </c>
+      <c r="R37" s="89" t="s">
+        <v>624</v>
+      </c>
+      <c r="S37" s="89" t="s">
+        <v>374</v>
+      </c>
+      <c r="T37" s="89" t="s">
+        <v>626</v>
+      </c>
+      <c r="U37" s="89"/>
+      <c r="V37" s="89"/>
+      <c r="W37" s="89"/>
+      <c r="X37" s="89"/>
+      <c r="Y37" s="89"/>
+      <c r="Z37" s="89"/>
+    </row>
+    <row r="38" spans="1:26" ht="99.75" x14ac:dyDescent="0.45">
+      <c r="A38" s="89"/>
+      <c r="B38" s="89"/>
+      <c r="C38" s="89"/>
+      <c r="D38" s="89"/>
+      <c r="F38" s="90"/>
+      <c r="G38" s="89"/>
+      <c r="H38" s="89"/>
+      <c r="I38" s="89"/>
+      <c r="J38" s="89" t="s">
+        <v>486</v>
+      </c>
+      <c r="K38" s="89" t="s">
+        <v>618</v>
+      </c>
+      <c r="L38" s="89" t="s">
+        <v>389</v>
+      </c>
+      <c r="M38" s="89" t="s">
+        <v>628</v>
+      </c>
+      <c r="N38" s="89" t="s">
+        <v>366</v>
+      </c>
+      <c r="O38" s="89"/>
+      <c r="P38" s="89" t="s">
+        <v>629</v>
+      </c>
+      <c r="Q38" s="89" t="s">
+        <v>630</v>
+      </c>
+      <c r="R38" s="89" t="s">
+        <v>627</v>
+      </c>
+      <c r="S38" s="89" t="s">
+        <v>374</v>
+      </c>
+      <c r="T38" s="89" t="s">
+        <v>635</v>
+      </c>
+      <c r="U38" s="89"/>
+      <c r="V38" s="89"/>
+      <c r="W38" s="89"/>
+      <c r="X38" s="89"/>
+      <c r="Y38" s="89"/>
+      <c r="Z38" s="89"/>
+    </row>
+    <row r="39" spans="1:26" ht="114" x14ac:dyDescent="0.45">
+      <c r="A39" s="89"/>
+      <c r="B39" s="89"/>
+      <c r="C39" s="89"/>
+      <c r="D39" s="89"/>
+      <c r="F39" s="90"/>
+      <c r="G39" s="89"/>
+      <c r="H39" s="89"/>
+      <c r="I39" s="89"/>
+      <c r="J39" s="89" t="s">
+        <v>486</v>
+      </c>
+      <c r="K39" s="89" t="s">
+        <v>619</v>
+      </c>
+      <c r="L39" s="89" t="s">
+        <v>620</v>
+      </c>
+      <c r="M39" s="89" t="s">
+        <v>634</v>
+      </c>
+      <c r="N39" s="89" t="s">
+        <v>503</v>
+      </c>
+      <c r="O39" s="89"/>
+      <c r="P39" s="89" t="s">
+        <v>633</v>
+      </c>
+      <c r="Q39" s="89" t="s">
+        <v>630</v>
+      </c>
+      <c r="R39" s="89" t="s">
+        <v>631</v>
+      </c>
+      <c r="S39" s="89" t="s">
+        <v>632</v>
+      </c>
+      <c r="T39" s="89" t="s">
+        <v>636</v>
+      </c>
+      <c r="U39" s="89"/>
+      <c r="V39" s="89"/>
+      <c r="W39" s="89"/>
+      <c r="X39" s="89"/>
+      <c r="Y39" s="89"/>
+      <c r="Z39" s="89"/>
+    </row>
+    <row r="40" spans="1:26" x14ac:dyDescent="0.45">
       <c r="V40" s="2"/>
     </row>
-    <row r="41" spans="2:22" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:26" x14ac:dyDescent="0.45">
       <c r="V41" s="2"/>
     </row>
-    <row r="42" spans="2:22" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:26" x14ac:dyDescent="0.45">
       <c r="V42" s="2"/>
     </row>
-    <row r="43" spans="2:22" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:26" x14ac:dyDescent="0.45">
       <c r="V43" s="2"/>
     </row>
-    <row r="44" spans="2:22" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:26" x14ac:dyDescent="0.45">
       <c r="V44" s="2"/>
     </row>
-    <row r="45" spans="2:22" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:26" x14ac:dyDescent="0.45">
       <c r="V45" s="2"/>
     </row>
-    <row r="46" spans="2:22" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:26" x14ac:dyDescent="0.45">
       <c r="V46" s="2"/>
     </row>
-    <row r="47" spans="2:22" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:26" x14ac:dyDescent="0.45">
       <c r="V47" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="19" type="noConversion"/>
   <dataValidations count="3">
     <dataValidation errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1" xr:uid="{00000000-0002-0000-0300-000000000000}"/>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid value" error="Valid property styles are &quot;element&quot;, &quot;attribute&quot;, or &quot;abstract&quot;.  Leave the cell blank to use the default value &quot;element&quot;." promptTitle="Property Style" prompt="- &quot;element&quot; or blank (default) - Represents a typical NIEM property._x000a_- &quot;abstract&quot; - Used to create a substitution group_x000a_- &quot;attribute&quot; - Use sparingly, if at all; for values tightly-coupled to an element." sqref="X48:X1048576 W2:W35" xr:uid="{00000000-0002-0000-0300-000002000000}">
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid value" error="Valid property styles are &quot;element&quot;, &quot;attribute&quot;, or &quot;abstract&quot;.  Leave the cell blank to use the default value &quot;element&quot;." promptTitle="Property Style" prompt="- &quot;element&quot; or blank (default) - Represents a typical NIEM property._x000a_- &quot;abstract&quot; - Used to create a substitution group_x000a_- &quot;attribute&quot; - Use sparingly, if at all; for values tightly-coupled to an element." sqref="X48:X1048576 W2:W39" xr:uid="{00000000-0002-0000-0300-000002000000}">
       <formula1>"element,attribute,abstract"</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576" xr:uid="{00000000-0002-0000-0300-000001000000}">

</xml_diff>

<commit_message>
Replaced person race and sex with NCIC codes
</commit_message>
<xml_diff>
--- a/schemas/ChargeFiling_iepd/artifacts/ChargeFiling_MappingSpreadsheet.xlsx
+++ b/schemas/ChargeFiling_iepd/artifacts/ChargeFiling_MappingSpreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JamesCabral\git\JTMP-Data-Exchange-Specs\schemas\ChargeFiling_iepd\artifacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFB4A685-7097-4956-ACBE-B41AA227960E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD94B943-C775-47C1-801F-ED1C95E5AA20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25815" yWindow="-21600" windowWidth="21930" windowHeight="20985" tabRatio="781" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16815" yWindow="-20985" windowWidth="16920" windowHeight="17730" tabRatio="781" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="9" state="hidden" r:id="rId1"/>
@@ -149,7 +149,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1076" uniqueCount="648">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1076" uniqueCount="650">
   <si>
     <t>Definition</t>
   </si>
@@ -1976,12 +1976,6 @@
     <t>A classification of a person based on factors such as geographical locations and genetics.</t>
   </si>
   <si>
-    <t>nc:PersonRaceText</t>
-  </si>
-  <si>
-    <t>nc:PersonSexText</t>
-  </si>
-  <si>
     <t>A gender or sex of a person.</t>
   </si>
   <si>
@@ -2333,16 +2327,10 @@
     <t>nc:AddressType (nc:MailingAddress)</t>
   </si>
   <si>
-    <t>nc:CourtCase/j:CaseAugmentation/j:CaseDefendantParty/nc:EntityPerson/nc:PersonRaceText</t>
-  </si>
-  <si>
     <t>nc:PersonType</t>
   </si>
   <si>
     <t>A physical location at which a person may be contacted.</t>
-  </si>
-  <si>
-    <t>nc:CourtCase/j:CaseAugmentation/j:CaseDefendantParty/nc:EntityPerson/nc:PersonSexText</t>
   </si>
   <si>
     <t>nc:PersonStateIdentification/nc:IdentificationID</t>
@@ -2791,6 +2779,24 @@
   </si>
   <si>
     <t>nola-ext:CourtCaseGrandJuryIndictmentIndicator</t>
+  </si>
+  <si>
+    <t>nc:CourtCase/j:CaseAugmentation/j:CaseDefendantParty/nc:EntityPerson/ncic:PersonRaceCode</t>
+  </si>
+  <si>
+    <t>ncic:PersonRaceCode</t>
+  </si>
+  <si>
+    <t>ncic:PersonSexCode</t>
+  </si>
+  <si>
+    <t>ncic:RACECodeType</t>
+  </si>
+  <si>
+    <t>ncic:SEXCodeType</t>
+  </si>
+  <si>
+    <t>nc:CourtCase/j:CaseAugmentation/j:CaseDefendantParty/nc:EntityPerson/ncic:PersonSexCode</t>
   </si>
 </sst>
 </file>
@@ -2934,6 +2940,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -3150,7 +3157,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3392,12 +3399,6 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="71">
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
@@ -4721,7 +4722,17 @@
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table3" displayName="Table3" ref="A1:Z41" totalsRowShown="0" headerRowDxfId="107" dataDxfId="106" headerRowCellStyle="Accent2">
-  <autoFilter ref="A1:Z41" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+  <autoFilter ref="A1:Z41" xr:uid="{00000000-0009-0000-0100-000003000000}">
+    <filterColumn colId="9">
+      <filters>
+        <filter val="Charge"/>
+        <filter val="Offense"/>
+        <filter val="Person Demographics"/>
+        <filter val="Person Identifiers"/>
+        <filter val="PersonIdentifiers"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="26">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Source_x000a_NS Prefix" dataDxfId="105"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Property Name" dataDxfId="104"/>
@@ -7377,10 +7388,10 @@
   <dimension ref="A1:AB49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C37" sqref="C37"/>
+      <selection pane="bottomRight" activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -7426,10 +7437,10 @@
         <v>0</v>
       </c>
       <c r="E1" s="86" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
       <c r="F1" s="83" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="G1" s="9" t="s">
         <v>49</v>
@@ -7447,37 +7458,37 @@
         <v>371</v>
       </c>
       <c r="L1" s="9" t="s">
+        <v>384</v>
+      </c>
+      <c r="M1" s="9" t="s">
+        <v>385</v>
+      </c>
+      <c r="N1" s="9" t="s">
         <v>386</v>
-      </c>
-      <c r="M1" s="9" t="s">
-        <v>387</v>
-      </c>
-      <c r="N1" s="9" t="s">
-        <v>388</v>
       </c>
       <c r="O1" s="11" t="s">
         <v>48</v>
       </c>
       <c r="P1" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="Q1" s="11" t="s">
+        <v>398</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>399</v>
       </c>
-      <c r="Q1" s="11" t="s">
+      <c r="S1" s="1" t="s">
         <v>400</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>401</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>402</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>403</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>373</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="W1" s="1" t="s">
         <v>223</v>
@@ -7492,18 +7503,18 @@
         <v>31</v>
       </c>
       <c r="AB1" s="56" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="2" spans="1:28" ht="99.75" x14ac:dyDescent="0.45">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" ht="99.75" hidden="1" x14ac:dyDescent="0.45">
       <c r="B2" s="2" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="E2" s="87" t="s">
-        <v>600</v>
+        <v>596</v>
       </c>
       <c r="F2" s="84">
         <v>1</v>
@@ -7515,7 +7526,7 @@
         <v>358</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>368</v>
@@ -7524,28 +7535,28 @@
         <v>366</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="R2" s="2" t="s">
         <v>369</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="V2" s="2"/>
     </row>
-    <row r="3" spans="1:28" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:28" ht="85.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="B3" s="2" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="F3" s="84" t="s">
         <v>366</v>
@@ -7554,41 +7565,41 @@
         <v>365</v>
       </c>
       <c r="K3" s="82" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
       <c r="L3" s="82" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="M3" s="82" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="N3" s="82"/>
       <c r="P3" s="82" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="Q3" s="82" t="s">
+        <v>542</v>
+      </c>
+      <c r="R3" s="82" t="s">
+        <v>548</v>
+      </c>
+      <c r="S3" s="82" t="s">
+        <v>543</v>
+      </c>
+      <c r="T3" s="82" t="s">
         <v>546</v>
       </c>
-      <c r="R3" s="82" t="s">
-        <v>552</v>
-      </c>
-      <c r="S3" s="82" t="s">
-        <v>547</v>
-      </c>
-      <c r="T3" s="82" t="s">
-        <v>550</v>
-      </c>
       <c r="V3" s="2"/>
     </row>
-    <row r="4" spans="1:28" ht="99.75" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:28" ht="99.75" hidden="1" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="F4" s="84" t="s">
         <v>366</v>
@@ -7597,38 +7608,38 @@
         <v>365</v>
       </c>
       <c r="K4" s="82" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
       <c r="L4" s="82" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="M4" s="82" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
       <c r="N4" s="82"/>
       <c r="P4" s="82" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="Q4" s="82" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="R4" s="82" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="S4" s="82" t="s">
         <v>374</v>
       </c>
       <c r="T4" s="82" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
       <c r="V4" s="2"/>
     </row>
-    <row r="5" spans="1:28" ht="99.75" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:28" ht="99.75" hidden="1" x14ac:dyDescent="0.45">
       <c r="B5" s="2" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="F5" s="84" t="s">
         <v>366</v>
@@ -7637,41 +7648,41 @@
         <v>365</v>
       </c>
       <c r="K5" s="82" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
       <c r="L5" s="82" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="M5" s="82" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
       <c r="N5" s="82"/>
       <c r="P5" s="82" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="Q5" s="82" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="R5" s="82" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="S5" s="82" t="s">
         <v>374</v>
       </c>
       <c r="T5" s="82" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
       <c r="V5" s="2"/>
     </row>
-    <row r="6" spans="1:28" ht="128.25" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:28" ht="128.25" hidden="1" x14ac:dyDescent="0.45">
       <c r="B6" s="2" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="E6" s="87" t="s">
-        <v>602</v>
+        <v>598</v>
       </c>
       <c r="F6" s="84">
         <v>1</v>
@@ -7680,10 +7691,10 @@
         <v>365</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="M6" s="2" t="s">
         <v>372</v>
@@ -7692,10 +7703,10 @@
         <v>366</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="R6" s="2" t="s">
         <v>375</v>
@@ -7704,13 +7715,13 @@
         <v>374</v>
       </c>
       <c r="T6" s="2" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="V6" s="2"/>
     </row>
-    <row r="7" spans="1:28" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:28" ht="71.25" hidden="1" x14ac:dyDescent="0.45">
       <c r="B7" s="2" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>220</v>
@@ -7722,224 +7733,224 @@
         <v>1</v>
       </c>
       <c r="J7" s="82" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="K7" s="82" t="s">
-        <v>542</v>
+        <v>538</v>
       </c>
       <c r="L7" s="82" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="M7" s="82" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
       <c r="N7" s="82"/>
       <c r="P7" s="82" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
       <c r="Q7" s="82" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="R7" s="82" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="S7" s="82" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="T7" s="82" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
       <c r="V7" s="2"/>
     </row>
-    <row r="8" spans="1:28" ht="99.75" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:28" ht="99.75" hidden="1" x14ac:dyDescent="0.45">
       <c r="B8" s="2" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="E8" s="87" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="F8" s="84" t="s">
         <v>366</v>
       </c>
       <c r="J8" s="82" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="K8" s="82" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
       <c r="L8" s="82" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="M8" s="82" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="N8" s="82">
         <v>1</v>
       </c>
       <c r="P8" s="82" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
       <c r="Q8" s="82" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
       <c r="R8" s="82" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="S8" s="82" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
       <c r="T8" s="82" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
       <c r="V8" s="2"/>
     </row>
-    <row r="9" spans="1:28" ht="99.75" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:28" ht="99.75" hidden="1" x14ac:dyDescent="0.45">
       <c r="B9" s="2" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="F9" s="84" t="s">
         <v>366</v>
       </c>
       <c r="J9" s="82" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="K9" s="82" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
       <c r="L9" s="82" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="M9" s="82" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="N9" s="82">
         <v>1</v>
       </c>
       <c r="P9" s="82" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
       <c r="Q9" s="82" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
       <c r="R9" s="82" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="S9" s="82" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
       <c r="T9" s="82" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
       <c r="V9" s="2"/>
     </row>
-    <row r="10" spans="1:28" ht="99.75" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:28" ht="99.75" hidden="1" x14ac:dyDescent="0.45">
       <c r="B10" s="2" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="F10" s="84" t="s">
         <v>366</v>
       </c>
       <c r="J10" s="82" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="K10" s="82" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
       <c r="L10" s="82" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="M10" s="82" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="N10" s="82">
         <v>1</v>
       </c>
       <c r="P10" s="82" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
       <c r="Q10" s="82" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
       <c r="R10" s="82" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="S10" s="82" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
       <c r="T10" s="82" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
       <c r="V10" s="2"/>
     </row>
-    <row r="11" spans="1:28" ht="99.75" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:28" ht="99.75" hidden="1" x14ac:dyDescent="0.45">
       <c r="A11" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="F11" s="84" t="s">
         <v>366</v>
       </c>
       <c r="J11" s="82" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="K11" s="82" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
       <c r="L11" s="82" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="M11" s="82" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="N11" s="82">
         <v>1</v>
       </c>
       <c r="P11" s="82" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
       <c r="Q11" s="82" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
       <c r="R11" s="82" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="S11" s="82" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
       <c r="T11" s="82" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
       <c r="V11" s="2"/>
     </row>
-    <row r="12" spans="1:28" ht="108.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:28" ht="108.75" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B12" s="2" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="E12" s="87" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="F12" s="84">
         <v>1</v>
@@ -7948,43 +7959,43 @@
         <v>357</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="N12" s="2" t="s">
         <v>366</v>
       </c>
       <c r="P12" s="2" t="s">
+        <v>477</v>
+      </c>
+      <c r="Q12" s="2" t="s">
         <v>479</v>
       </c>
-      <c r="Q12" s="2" t="s">
-        <v>481</v>
-      </c>
       <c r="R12" s="2" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="S12" s="2" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="T12" s="2" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="V12" s="2"/>
     </row>
-    <row r="13" spans="1:28" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:28" ht="85.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="B13" s="2" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="E13" s="87" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="F13" s="84">
         <v>1</v>
@@ -7993,40 +8004,40 @@
         <v>357</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="N13" s="2" t="s">
         <v>366</v>
       </c>
       <c r="P13" s="2" t="s">
+        <v>480</v>
+      </c>
+      <c r="Q13" s="2" t="s">
+        <v>479</v>
+      </c>
+      <c r="R13" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="S13" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="T13" s="2" t="s">
         <v>482</v>
       </c>
-      <c r="Q13" s="2" t="s">
-        <v>481</v>
-      </c>
-      <c r="R13" s="2" t="s">
-        <v>444</v>
-      </c>
-      <c r="S13" s="2" t="s">
-        <v>407</v>
-      </c>
-      <c r="T13" s="2" t="s">
-        <v>484</v>
-      </c>
       <c r="V13" s="2"/>
     </row>
-    <row r="14" spans="1:28" ht="99.75" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:28" ht="99.75" hidden="1" x14ac:dyDescent="0.45">
       <c r="B14" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="F14" s="84" t="s">
         <v>366</v>
@@ -8035,85 +8046,85 @@
         <v>357</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="N14" s="2" t="s">
         <v>366</v>
       </c>
       <c r="P14" s="2" t="s">
+        <v>481</v>
+      </c>
+      <c r="Q14" s="2" t="s">
+        <v>479</v>
+      </c>
+      <c r="R14" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="S14" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="T14" s="2" t="s">
         <v>483</v>
       </c>
-      <c r="Q14" s="2" t="s">
-        <v>481</v>
-      </c>
-      <c r="R14" s="2" t="s">
-        <v>448</v>
-      </c>
-      <c r="S14" s="2" t="s">
-        <v>407</v>
-      </c>
-      <c r="T14" s="2" t="s">
-        <v>485</v>
-      </c>
       <c r="V14" s="2"/>
     </row>
-    <row r="15" spans="1:28" ht="114" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:28" ht="114" hidden="1" x14ac:dyDescent="0.45">
       <c r="B15" s="2" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="E15" s="87" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="F15" s="84">
         <v>1</v>
       </c>
       <c r="J15" s="2" t="s">
+        <v>484</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>485</v>
+      </c>
+      <c r="L15" s="2" t="s">
         <v>486</v>
       </c>
-      <c r="K15" s="2" t="s">
-        <v>487</v>
-      </c>
-      <c r="L15" s="2" t="s">
-        <v>488</v>
-      </c>
       <c r="M15" s="2" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="N15" s="2" t="s">
         <v>366</v>
       </c>
       <c r="P15" s="2" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="Q15" s="2" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="R15" s="2" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="S15" s="2" t="s">
         <v>367</v>
       </c>
       <c r="T15" s="2" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="V15" s="2"/>
     </row>
     <row r="16" spans="1:28" ht="85.5" x14ac:dyDescent="0.45">
       <c r="B16" s="2" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="E16" s="88">
         <v>25143</v>
@@ -8122,61 +8133,61 @@
         <v>1</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="K16" s="2" t="s">
         <v>359</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="N16" s="2" t="s">
         <v>366</v>
       </c>
       <c r="P16" s="2" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="Q16" s="2" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="R16" s="2" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="S16" s="2" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="T16" s="2" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="V16" s="2"/>
     </row>
-    <row r="17" spans="1:26" ht="99.75" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:22" ht="99.75" x14ac:dyDescent="0.45">
       <c r="B17" s="2" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="E17" s="87" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
       <c r="F17" s="84" t="s">
         <v>366</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="K17" s="2" t="s">
         <v>361</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="M17" s="2" t="s">
         <v>376</v>
@@ -8185,121 +8196,121 @@
         <v>366</v>
       </c>
       <c r="P17" s="2" t="s">
-        <v>495</v>
+        <v>644</v>
       </c>
       <c r="Q17" s="2" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="R17" s="2" t="s">
-        <v>377</v>
+        <v>645</v>
       </c>
       <c r="S17" s="2" t="s">
-        <v>367</v>
+        <v>647</v>
       </c>
       <c r="T17" s="2" t="s">
         <v>376</v>
       </c>
       <c r="V17" s="2"/>
     </row>
-    <row r="18" spans="1:26" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:22" ht="71.25" x14ac:dyDescent="0.45">
       <c r="B18" s="2" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="E18" s="87" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="F18" s="84" t="s">
         <v>366</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="K18" s="2" t="s">
         <v>362</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="N18" s="2" t="s">
         <v>366</v>
       </c>
       <c r="P18" s="2" t="s">
-        <v>498</v>
+        <v>649</v>
       </c>
       <c r="Q18" s="2" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="R18" s="2" t="s">
-        <v>378</v>
+        <v>646</v>
       </c>
       <c r="S18" s="2" t="s">
-        <v>367</v>
+        <v>648</v>
       </c>
       <c r="T18" s="2" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="V18" s="2"/>
     </row>
-    <row r="19" spans="1:26" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:22" ht="71.25" x14ac:dyDescent="0.45">
       <c r="B19" s="2" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="F19" s="84" t="s">
         <v>366</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="K19" s="2" t="s">
         <v>360</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="N19" s="2" t="s">
         <v>366</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="Q19" s="2" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="R19" s="2" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="S19" s="2" t="s">
         <v>374</v>
       </c>
       <c r="T19" s="2" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="V19" s="2"/>
     </row>
-    <row r="20" spans="1:26" ht="57" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:22" ht="57" hidden="1" x14ac:dyDescent="0.45">
       <c r="B20" s="2" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
       <c r="E20" s="87">
         <v>9999999</v>
@@ -8308,91 +8319,91 @@
         <v>366</v>
       </c>
       <c r="J20" s="82" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="K20" s="82" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
       <c r="L20" s="82" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="M20" s="82" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
       <c r="N20" s="85" t="s">
         <v>366</v>
       </c>
       <c r="P20" s="82" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
       <c r="Q20" s="82" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="R20" s="82" t="s">
-        <v>590</v>
+        <v>586</v>
       </c>
       <c r="S20" s="82" t="s">
         <v>374</v>
       </c>
       <c r="T20" s="82" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
       <c r="V20" s="2"/>
     </row>
-    <row r="21" spans="1:26" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:22" ht="71.25" hidden="1" x14ac:dyDescent="0.45">
       <c r="B21" s="2" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>357</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
       <c r="F21" s="84" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="J21" s="2" t="s">
+        <v>564</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>565</v>
+      </c>
+      <c r="L21" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="M21" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="N21" s="84" t="s">
+        <v>499</v>
+      </c>
+      <c r="P21" s="2" t="s">
+        <v>566</v>
+      </c>
+      <c r="Q21" s="2" t="s">
+        <v>567</v>
+      </c>
+      <c r="R21" s="2" t="s">
         <v>568</v>
       </c>
-      <c r="K21" s="2" t="s">
+      <c r="S21" s="2" t="s">
+        <v>479</v>
+      </c>
+      <c r="T21" s="2" t="s">
         <v>569</v>
       </c>
-      <c r="L21" s="2" t="s">
-        <v>389</v>
-      </c>
-      <c r="M21" s="2" t="s">
-        <v>445</v>
-      </c>
-      <c r="N21" s="84" t="s">
-        <v>503</v>
-      </c>
-      <c r="P21" s="2" t="s">
-        <v>570</v>
-      </c>
-      <c r="Q21" s="2" t="s">
-        <v>571</v>
-      </c>
-      <c r="R21" s="2" t="s">
-        <v>572</v>
-      </c>
-      <c r="S21" s="2" t="s">
-        <v>481</v>
-      </c>
-      <c r="T21" s="2" t="s">
-        <v>573</v>
-      </c>
       <c r="V21" s="2"/>
     </row>
-    <row r="22" spans="1:26" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:22" ht="85.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="B22" s="2" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="E22" s="88">
         <v>45566</v>
@@ -8401,142 +8412,142 @@
         <v>366</v>
       </c>
       <c r="J22" s="82" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="K22" s="82" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
       <c r="L22" s="82" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="M22" s="82" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="N22" s="85" t="s">
         <v>366</v>
       </c>
       <c r="P22" s="82" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
       <c r="Q22" s="82" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
       <c r="R22" s="82" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="S22" s="82" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="T22" s="82" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="V22" s="2"/>
     </row>
-    <row r="23" spans="1:26" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:22" ht="85.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="B23" s="2" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>357</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
       <c r="E23" s="87" t="s">
-        <v>608</v>
+        <v>604</v>
       </c>
       <c r="F23" s="84" t="s">
         <v>366</v>
       </c>
       <c r="J23" s="82" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="K23" s="82" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="L23" s="82" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="M23" s="82" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
       <c r="N23" s="85" t="s">
         <v>366</v>
       </c>
       <c r="P23" s="82" t="s">
+        <v>590</v>
+      </c>
+      <c r="Q23" s="82" t="s">
+        <v>592</v>
+      </c>
+      <c r="R23" s="82" t="s">
         <v>594</v>
       </c>
-      <c r="Q23" s="82" t="s">
-        <v>596</v>
-      </c>
-      <c r="R23" s="82" t="s">
-        <v>598</v>
-      </c>
       <c r="S23" s="82" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="T23" s="82" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
       <c r="V23" s="2"/>
     </row>
-    <row r="24" spans="1:26" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:22" ht="85.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="B24" s="2" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>357</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
       <c r="E24" s="87" t="s">
-        <v>609</v>
+        <v>605</v>
       </c>
       <c r="F24" s="84" t="s">
         <v>366</v>
       </c>
       <c r="J24" s="82" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="K24" s="82" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
       <c r="L24" s="82" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="M24" s="82" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
       <c r="N24" s="85" t="s">
         <v>366</v>
       </c>
       <c r="P24" s="82" t="s">
-        <v>595</v>
+        <v>591</v>
       </c>
       <c r="Q24" s="82" t="s">
-        <v>597</v>
+        <v>593</v>
       </c>
       <c r="R24" s="82" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
       <c r="S24" s="82" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="T24" s="82" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
       <c r="V24" s="2"/>
     </row>
-    <row r="25" spans="1:26" ht="127.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:22" ht="127.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B25" s="2" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="E25" s="87">
         <v>999999</v>
@@ -8545,43 +8556,43 @@
         <v>366</v>
       </c>
       <c r="J25" s="82" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="K25" s="82" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
       <c r="L25" s="82" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="M25" s="82" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="N25" s="85" t="s">
         <v>366</v>
       </c>
       <c r="P25" s="82" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
       <c r="Q25" s="82" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
       <c r="R25" s="82" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="S25" s="82" t="s">
         <v>374</v>
       </c>
       <c r="T25" s="82" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="V25" s="2"/>
     </row>
-    <row r="26" spans="1:26" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:22" ht="71.25" x14ac:dyDescent="0.45">
       <c r="B26" s="2" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="E26" s="88">
         <v>45505</v>
@@ -8590,43 +8601,43 @@
         <v>366</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="K26" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="L26" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="M26" s="2" t="s">
         <v>391</v>
-      </c>
-      <c r="L26" s="2" t="s">
-        <v>396</v>
-      </c>
-      <c r="M26" s="2" t="s">
-        <v>393</v>
       </c>
       <c r="N26" s="2" t="s">
         <v>366</v>
       </c>
       <c r="P26" s="82" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
       <c r="Q26" s="2" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
       <c r="R26" s="2" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="S26" s="2" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="T26" s="2" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="V26" s="2"/>
     </row>
-    <row r="27" spans="1:26" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:22" ht="42.75" hidden="1" x14ac:dyDescent="0.45">
       <c r="B27" s="2" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="E27" s="88">
         <v>45505</v>
@@ -8635,46 +8646,46 @@
         <v>366</v>
       </c>
       <c r="J27" s="2" t="s">
+        <v>454</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>455</v>
+      </c>
+      <c r="L27" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="M27" s="2" t="s">
         <v>456</v>
-      </c>
-      <c r="K27" s="2" t="s">
-        <v>457</v>
-      </c>
-      <c r="L27" s="2" t="s">
-        <v>392</v>
-      </c>
-      <c r="M27" s="2" t="s">
-        <v>458</v>
       </c>
       <c r="N27" s="2" t="s">
         <v>366</v>
       </c>
       <c r="P27" s="82" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="Q27" s="2" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="R27" s="2" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="S27" s="2" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="T27" s="2" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="V27" s="2"/>
     </row>
-    <row r="28" spans="1:26" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="28" spans="2:22" ht="42.75" hidden="1" x14ac:dyDescent="0.45">
       <c r="B28" s="2" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="E28" s="87" t="s">
-        <v>610</v>
+        <v>606</v>
       </c>
       <c r="F28" s="84" t="s">
         <v>366</v>
@@ -8683,606 +8694,586 @@
         <v>365</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>584</v>
+        <v>580</v>
       </c>
       <c r="L28" s="2" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="M28" s="2" t="s">
-        <v>583</v>
+        <v>579</v>
       </c>
       <c r="N28" s="2" t="s">
         <v>366</v>
       </c>
       <c r="P28" s="2" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="Q28" s="2" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
       <c r="R28" s="2" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
       <c r="S28" s="2" t="s">
         <v>367</v>
       </c>
       <c r="T28" s="2" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
       <c r="V28" s="2"/>
     </row>
-    <row r="29" spans="1:26" ht="142.5" x14ac:dyDescent="0.45">
-      <c r="A29" s="89"/>
+    <row r="29" spans="2:22" ht="142.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="B29" s="2" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>389</v>
-      </c>
-      <c r="D29" s="89"/>
+        <v>387</v>
+      </c>
       <c r="E29" s="87" t="s">
-        <v>611</v>
+        <v>607</v>
       </c>
       <c r="F29" s="84" t="s">
-        <v>442</v>
-      </c>
-      <c r="G29" s="89"/>
-      <c r="H29" s="89"/>
-      <c r="I29" s="89"/>
-      <c r="J29" s="89" t="s">
+        <v>440</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>632</v>
+      </c>
+      <c r="K29" s="2" t="s">
+        <v>633</v>
+      </c>
+      <c r="L29" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="M29" s="2" t="s">
+        <v>637</v>
+      </c>
+      <c r="N29" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="P29" s="2" t="s">
+        <v>634</v>
+      </c>
+      <c r="Q29" s="2" t="s">
         <v>636</v>
       </c>
-      <c r="K29" s="89" t="s">
-        <v>637</v>
-      </c>
-      <c r="L29" s="89" t="s">
-        <v>389</v>
-      </c>
-      <c r="M29" s="89" t="s">
-        <v>641</v>
-      </c>
-      <c r="N29" s="89" t="s">
-        <v>366</v>
-      </c>
-      <c r="O29" s="89"/>
-      <c r="P29" s="89" t="s">
+      <c r="R29" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="S29" s="2" t="s">
+        <v>461</v>
+      </c>
+      <c r="T29" s="2" t="s">
         <v>638</v>
       </c>
-      <c r="Q29" s="2" t="s">
-        <v>640</v>
-      </c>
-      <c r="R29" s="2" t="s">
-        <v>384</v>
-      </c>
-      <c r="S29" s="2" t="s">
-        <v>463</v>
-      </c>
-      <c r="T29" s="89" t="s">
-        <v>642</v>
-      </c>
-      <c r="U29" s="89"/>
-      <c r="V29" s="89"/>
-      <c r="W29" s="89"/>
-      <c r="X29" s="89"/>
-      <c r="Y29" s="89"/>
-      <c r="Z29" s="89"/>
-    </row>
-    <row r="30" spans="1:26" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="V29" s="2"/>
+    </row>
+    <row r="30" spans="2:22" ht="85.5" x14ac:dyDescent="0.45">
       <c r="B30" s="2" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="E30" s="87" t="s">
-        <v>611</v>
+        <v>607</v>
       </c>
       <c r="F30" s="84" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="L30" s="2" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="M30" s="2" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="N30" s="2" t="s">
         <v>366</v>
       </c>
       <c r="P30" s="2" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="Q30" s="2" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
       <c r="R30" s="2" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="S30" s="2" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="T30" s="2" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="V30" s="2"/>
     </row>
-    <row r="31" spans="1:26" ht="28.9" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="31" spans="2:22" ht="28.9" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B31" s="2" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="E31" s="87">
         <v>12345678</v>
       </c>
       <c r="F31" s="84" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="L31" s="2" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="M31" s="2" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="N31" s="2" t="s">
         <v>366</v>
       </c>
       <c r="P31" s="2" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
       <c r="R31" s="2" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="S31" s="2" t="s">
         <v>374</v>
       </c>
       <c r="V31" s="2"/>
     </row>
-    <row r="32" spans="1:26" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="32" spans="2:22" ht="42.75" x14ac:dyDescent="0.45">
       <c r="B32" s="2" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="E32" s="87" t="s">
-        <v>612</v>
+        <v>608</v>
       </c>
       <c r="F32" s="84" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="M32" s="2" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="N32" s="2" t="s">
         <v>366</v>
       </c>
       <c r="P32" s="2" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
       <c r="Q32" s="2" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="R32" s="2" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="S32" s="2" t="s">
         <v>367</v>
       </c>
       <c r="T32" s="2" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="V32" s="2"/>
     </row>
-    <row r="33" spans="1:26" ht="228" x14ac:dyDescent="0.45">
+    <row r="33" spans="2:22" ht="228" x14ac:dyDescent="0.45">
       <c r="B33" s="2" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="E33" s="87" t="s">
-        <v>613</v>
+        <v>609</v>
       </c>
       <c r="F33" s="84" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="L33" s="2" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="M33" s="2" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="N33" s="2" t="s">
         <v>366</v>
       </c>
       <c r="P33" s="2" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
       <c r="Q33" s="2" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="R33" s="2" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="S33" s="2" t="s">
         <v>367</v>
       </c>
       <c r="T33" s="2" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="V33" s="2"/>
     </row>
-    <row r="34" spans="1:26" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="34" spans="2:22" ht="71.25" x14ac:dyDescent="0.45">
       <c r="B34" s="2" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="E34" s="87">
         <v>14.8</v>
       </c>
       <c r="F34" s="84" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="K34" s="2" t="s">
         <v>363</v>
       </c>
       <c r="L34" s="2" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="M34" s="2" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="N34" s="2" t="s">
         <v>366</v>
       </c>
       <c r="P34" s="2" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
       <c r="Q34" s="2" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="R34" s="2" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="S34" s="2" t="s">
         <v>374</v>
       </c>
       <c r="T34" s="2" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="V34" s="2"/>
     </row>
-    <row r="35" spans="1:26" ht="99.75" x14ac:dyDescent="0.45">
+    <row r="35" spans="2:22" ht="99.75" x14ac:dyDescent="0.45">
       <c r="B35" s="2" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="E35" s="87">
         <v>0</v>
       </c>
       <c r="F35" s="84" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="L35" s="2" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="M35" s="2" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="N35" s="2" t="s">
         <v>366</v>
       </c>
       <c r="P35" s="2" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="Q35" s="2" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="R35" s="2" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="S35" s="2" t="s">
         <v>367</v>
       </c>
       <c r="T35" s="2" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="V35" s="2"/>
     </row>
-    <row r="36" spans="1:26" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="36" spans="2:22" ht="85.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="B36" s="2" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="E36" s="87" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="F36" s="84" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="J36" s="82" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="K36" s="82" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="L36" s="82" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="M36" s="82" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="N36" s="82" t="s">
         <v>366</v>
       </c>
       <c r="O36" s="82"/>
       <c r="P36" s="82" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
       <c r="Q36" s="82" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
       <c r="R36" s="82" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
       <c r="S36" s="82" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="T36" s="82" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="V36" s="2"/>
     </row>
-    <row r="37" spans="1:26" ht="85.5" x14ac:dyDescent="0.45">
-      <c r="A37" s="89"/>
-      <c r="B37" s="89" t="s">
-        <v>643</v>
-      </c>
-      <c r="C37" s="89" t="s">
-        <v>406</v>
-      </c>
-      <c r="D37" s="89" t="s">
-        <v>644</v>
+    <row r="37" spans="2:22" ht="85.5" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B37" s="2" t="s">
+        <v>639</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>640</v>
       </c>
       <c r="E37" s="87" t="b">
         <v>0</v>
       </c>
-      <c r="F37" s="90" t="s">
+      <c r="F37" s="84" t="s">
         <v>366</v>
       </c>
-      <c r="G37" s="89"/>
-      <c r="H37" s="89"/>
-      <c r="I37" s="89"/>
       <c r="J37" s="82" t="s">
         <v>365</v>
       </c>
       <c r="K37" s="82" t="s">
-        <v>645</v>
+        <v>641</v>
       </c>
       <c r="L37" s="82" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="M37" s="82" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
       <c r="N37" s="82" t="s">
         <v>366</v>
       </c>
       <c r="O37" s="82"/>
       <c r="P37" s="82" t="s">
-        <v>646</v>
+        <v>642</v>
       </c>
       <c r="Q37" s="82" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="R37" s="82" t="s">
-        <v>647</v>
+        <v>643</v>
       </c>
       <c r="S37" s="82" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
       <c r="T37" s="82" t="s">
-        <v>644</v>
-      </c>
-      <c r="U37" s="89"/>
-      <c r="V37" s="89"/>
-      <c r="W37" s="89"/>
-      <c r="X37" s="89"/>
-      <c r="Y37" s="89"/>
-      <c r="Z37" s="89"/>
-    </row>
-    <row r="38" spans="1:26" ht="142.5" x14ac:dyDescent="0.45">
+        <v>640</v>
+      </c>
+      <c r="V37" s="2"/>
+    </row>
+    <row r="38" spans="2:22" ht="142.5" x14ac:dyDescent="0.45">
       <c r="J38" s="2" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>614</v>
+        <v>610</v>
       </c>
       <c r="L38" s="2" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="M38" s="2" t="s">
-        <v>620</v>
+        <v>616</v>
       </c>
       <c r="N38" s="2" t="s">
         <v>366</v>
       </c>
       <c r="P38" s="2" t="s">
-        <v>622</v>
+        <v>618</v>
       </c>
       <c r="Q38" s="2" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
       <c r="R38" s="2" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
       <c r="S38" s="2" t="s">
         <v>374</v>
       </c>
       <c r="T38" s="2" t="s">
+        <v>616</v>
+      </c>
+      <c r="V38" s="2"/>
+    </row>
+    <row r="39" spans="2:22" ht="409.5" hidden="1" x14ac:dyDescent="0.45">
+      <c r="J39" s="2" t="s">
+        <v>454</v>
+      </c>
+      <c r="K39" s="2" t="s">
+        <v>611</v>
+      </c>
+      <c r="L39" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="M39" s="2" t="s">
+        <v>621</v>
+      </c>
+      <c r="N39" s="2" t="s">
+        <v>499</v>
+      </c>
+      <c r="P39" s="2" t="s">
         <v>620</v>
       </c>
-      <c r="V38" s="2"/>
-    </row>
-    <row r="39" spans="1:26" ht="409.5" x14ac:dyDescent="0.45">
-      <c r="J39" s="2" t="s">
-        <v>456</v>
-      </c>
-      <c r="K39" s="2" t="s">
-        <v>615</v>
-      </c>
-      <c r="L39" s="2" t="s">
-        <v>389</v>
-      </c>
-      <c r="M39" s="2" t="s">
-        <v>625</v>
-      </c>
-      <c r="N39" s="2" t="s">
-        <v>503</v>
-      </c>
-      <c r="P39" s="2" t="s">
-        <v>624</v>
-      </c>
       <c r="Q39" s="2" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
       <c r="R39" s="2" t="s">
-        <v>623</v>
+        <v>619</v>
       </c>
       <c r="S39" s="2" t="s">
         <v>374</v>
       </c>
       <c r="T39" s="2" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
       <c r="V39" s="2"/>
     </row>
-    <row r="40" spans="1:26" ht="99.75" x14ac:dyDescent="0.45">
+    <row r="40" spans="2:22" ht="99.75" hidden="1" x14ac:dyDescent="0.45">
       <c r="J40" s="2" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="K40" s="2" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="L40" s="2" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="M40" s="2" t="s">
-        <v>627</v>
+        <v>623</v>
       </c>
       <c r="N40" s="2" t="s">
         <v>366</v>
       </c>
       <c r="P40" s="2" t="s">
-        <v>628</v>
+        <v>624</v>
       </c>
       <c r="Q40" s="2" t="s">
-        <v>629</v>
+        <v>625</v>
       </c>
       <c r="R40" s="2" t="s">
-        <v>626</v>
+        <v>622</v>
       </c>
       <c r="S40" s="2" t="s">
         <v>374</v>
       </c>
       <c r="T40" s="2" t="s">
-        <v>634</v>
+        <v>630</v>
       </c>
       <c r="V40" s="2"/>
     </row>
-    <row r="41" spans="1:26" ht="114" x14ac:dyDescent="0.45">
+    <row r="41" spans="2:22" ht="114" hidden="1" x14ac:dyDescent="0.45">
       <c r="J41" s="2" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="K41" s="2" t="s">
-        <v>618</v>
+        <v>614</v>
       </c>
       <c r="L41" s="2" t="s">
-        <v>619</v>
+        <v>615</v>
       </c>
       <c r="M41" s="2" t="s">
-        <v>633</v>
+        <v>629</v>
       </c>
       <c r="N41" s="2" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="P41" s="2" t="s">
-        <v>632</v>
+        <v>628</v>
       </c>
       <c r="Q41" s="2" t="s">
-        <v>629</v>
+        <v>625</v>
       </c>
       <c r="R41" s="2" t="s">
-        <v>630</v>
+        <v>626</v>
       </c>
       <c r="S41" s="2" t="s">
+        <v>627</v>
+      </c>
+      <c r="T41" s="2" t="s">
         <v>631</v>
       </c>
-      <c r="T41" s="2" t="s">
-        <v>635</v>
-      </c>
       <c r="V41" s="2"/>
     </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="42" spans="2:22" x14ac:dyDescent="0.45">
       <c r="V42" s="2"/>
     </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="43" spans="2:22" x14ac:dyDescent="0.45">
       <c r="V43" s="2"/>
     </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="44" spans="2:22" x14ac:dyDescent="0.45">
       <c r="V44" s="2"/>
     </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="45" spans="2:22" x14ac:dyDescent="0.45">
       <c r="V45" s="2"/>
     </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="46" spans="2:22" x14ac:dyDescent="0.45">
       <c r="V46" s="2"/>
     </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="47" spans="2:22" x14ac:dyDescent="0.45">
       <c r="V47" s="2"/>
     </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="48" spans="2:22" x14ac:dyDescent="0.45">
       <c r="V48" s="2"/>
     </row>
     <row r="49" spans="22:22" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
Added subset and iniital extension schemas
</commit_message>
<xml_diff>
--- a/schemas/ChargeFiling_iepd/artifacts/ChargeFiling_MappingSpreadsheet.xlsx
+++ b/schemas/ChargeFiling_iepd/artifacts/ChargeFiling_MappingSpreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JamesCabral\git\JTMP-Data-Exchange-Specs\schemas\ChargeFiling_iepd\artifacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD94B943-C775-47C1-801F-ED1C95E5AA20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0847D1D0-9D21-4EF6-9829-6AB3786F9AE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16815" yWindow="-20985" windowWidth="16920" windowHeight="17730" tabRatio="781" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10718" yWindow="0" windowWidth="10965" windowHeight="13763" tabRatio="781" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="9" state="hidden" r:id="rId1"/>
@@ -149,7 +149,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1076" uniqueCount="650">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1076" uniqueCount="651">
   <si>
     <t>Definition</t>
   </si>
@@ -2333,9 +2333,6 @@
     <t>A physical location at which a person may be contacted.</t>
   </si>
   <si>
-    <t>nc:PersonStateIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
     <t>nc:IdentificationType (nc:PersonStateIdentification)</t>
   </si>
   <si>
@@ -2414,24 +2411,15 @@
     <t>nola-ext:ChargeDispositionCodeType</t>
   </si>
   <si>
-    <t>j:Arrest/j:ArrestCharge/nola-ext:ArrestAugmentation/nola-ext:OffenseDate</t>
-  </si>
-  <si>
     <t>j:Arrest/nc:ActivityDate/nc:DateTime</t>
   </si>
   <si>
     <t>j:Arrest/j:ArrestCharge/nola-ext:ChargeAugmentation/nola-ext:JMSChargeNumber</t>
   </si>
   <si>
-    <t>/j:Arrest/j:ArrestCharge//nola-ext:ChargeAugmentation/nola-ext:StatewideArrestTrackingNumber</t>
-  </si>
-  <si>
     <t>j:Arrest/j:ArrestCharge/j:ChargeDescriptionText</t>
   </si>
   <si>
-    <t>/j:Arrest/j:ArrestCharge/j:ChargeSeverityDescriptionText</t>
-  </si>
-  <si>
     <t>j:Arrest/j:ArrestCharge/j:ChargeStatute/j:StatuteCodeIdentification/nc:IdentificationID</t>
   </si>
   <si>
@@ -2447,9 +2435,6 @@
     <t>Indicates whether the arrest is accepted, refused, diverted, or referred.</t>
   </si>
   <si>
-    <t>j:Arrest/noa-ext:ArrestAugmentation/nola-ext:ArrestDispositionCode</t>
-  </si>
-  <si>
     <t>nola-ext:ArrestDispositionCode</t>
   </si>
   <si>
@@ -2468,9 +2453,6 @@
     <t>The date the prosecutor received the arrest</t>
   </si>
   <si>
-    <t>j:Arrest/noa-ext:ArrestAugmentation/nola-ext:ArrestReceivedDate/nc:Date</t>
-  </si>
-  <si>
     <t>nc:Date Type (nola-ext:ArrestReceivedDate)</t>
   </si>
   <si>
@@ -2726,15 +2708,6 @@
     <t>nc:ContactInformationType</t>
   </si>
   <si>
-    <t>nc:ContactTelephoneNumber</t>
-  </si>
-  <si>
-    <t>nc:TelephoneNumberType</t>
-  </si>
-  <si>
-    <t>nc:CourtCase/j:CaseAugmentation/j:CaseDefendantParty/nc:EntityPerson/nc:PersonContactInformation/nc:ContactTelephoneNumber</t>
-  </si>
-  <si>
     <t>A data concept for a telephone number.</t>
   </si>
   <si>
@@ -2748,9 +2721,6 @@
   </si>
   <si>
     <t>IncidentItemNumber</t>
-  </si>
-  <si>
-    <t>j:Arrest/nola-ext:ArrestAugmentation/j:ArrestIncident/nc:ActivityIdentification/nc:IdentificationID</t>
   </si>
   <si>
     <t>nc:IdentificationType (nola-ext:JMSChargeNumber)</t>
@@ -2797,6 +2767,39 @@
   </si>
   <si>
     <t>nc:CourtCase/j:CaseAugmentation/j:CaseDefendantParty/nc:EntityPerson/ncic:PersonSexCode</t>
+  </si>
+  <si>
+    <t>j:Arrest/j:ArrestCharge/j:ChargeSeverityDescriptionText</t>
+  </si>
+  <si>
+    <t>j:Arrest/nola-ext:ArrestAugmentation/nola-ext:ArrestDispositionCode</t>
+  </si>
+  <si>
+    <t>j:Arrest/nola-ext:ArrestAugmentation/nola-ext:ArrestReceivedDate/nc:Date</t>
+  </si>
+  <si>
+    <t>j:Arrest/nola-ext:ArrestAugmentation/nola-ext:ArrestIncident/nc:ActivityIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>nc:CourtCase/j:CaseAugmentation/j:CaseDefendantParty/nc:EntityPerson/nc:PersonContactInformation/nc:ContactTelephoneNumber/nc:FullTelephoneNumber</t>
+  </si>
+  <si>
+    <t>nc:FullTelephoneNumber</t>
+  </si>
+  <si>
+    <t>nc:FullTelephoneNumberType</t>
+  </si>
+  <si>
+    <t>nc:TelephoneNumberType (nc:ContactTelephoneNumber)</t>
+  </si>
+  <si>
+    <t>nc:CourtCase/j:CaseAugmentation/j:CaseDefendantParty/nc:EntityPerson/nc:PersonStateIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>j:Arrest/j:ArrestCharge/nola-ext:ChargeAugmentation/nola-ext:StatewideArrestTrackingNumber</t>
+  </si>
+  <si>
+    <t>j:Arrest/nola-ext:ArrestAugmentation/nola-ext:OffenseDate</t>
   </si>
 </sst>
 </file>
@@ -4722,17 +4725,10 @@
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table3" displayName="Table3" ref="A1:Z41" totalsRowShown="0" headerRowDxfId="107" dataDxfId="106" headerRowCellStyle="Accent2">
-  <autoFilter ref="A1:Z41" xr:uid="{00000000-0009-0000-0100-000003000000}">
-    <filterColumn colId="9">
-      <filters>
-        <filter val="Charge"/>
-        <filter val="Offense"/>
-        <filter val="Person Demographics"/>
-        <filter val="Person Identifiers"/>
-        <filter val="PersonIdentifiers"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:Z41" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Z41">
+    <sortCondition ref="P1:P41"/>
+  </sortState>
   <tableColumns count="26">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Source_x000a_NS Prefix" dataDxfId="105"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Property Name" dataDxfId="104"/>
@@ -7388,10 +7384,10 @@
   <dimension ref="A1:AB49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C26" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="N5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K33" sqref="K33"/>
+      <selection pane="bottomRight" activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -7437,7 +7433,7 @@
         <v>0</v>
       </c>
       <c r="E1" s="86" t="s">
-        <v>595</v>
+        <v>589</v>
       </c>
       <c r="F1" s="83" t="s">
         <v>439</v>
@@ -7506,1774 +7502,1774 @@
         <v>403</v>
       </c>
     </row>
-    <row r="2" spans="1:28" ht="99.75" hidden="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:28" ht="409.5" x14ac:dyDescent="0.45">
       <c r="B2" s="2" t="s">
-        <v>406</v>
+        <v>513</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>387</v>
-      </c>
-      <c r="E2" s="87" t="s">
-        <v>596</v>
-      </c>
-      <c r="F2" s="84">
-        <v>1</v>
+        <v>430</v>
+      </c>
+      <c r="E2" s="87">
+        <v>12345678</v>
+      </c>
+      <c r="F2" s="84" t="s">
+        <v>440</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>364</v>
+        <v>454</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>358</v>
+        <v>463</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>387</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>368</v>
+        <v>462</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>366</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>471</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>472</v>
+        <v>649</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>369</v>
+        <v>464</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>452</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>473</v>
+        <v>374</v>
       </c>
       <c r="V2" s="2"/>
     </row>
-    <row r="3" spans="1:28" ht="85.5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:28" ht="99.75" x14ac:dyDescent="0.45">
       <c r="B3" s="2" t="s">
-        <v>417</v>
+        <v>517</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>404</v>
+        <v>387</v>
+      </c>
+      <c r="E3" s="87">
+        <v>0</v>
       </c>
       <c r="F3" s="84" t="s">
+        <v>440</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>504</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>505</v>
+      </c>
+      <c r="N3" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="J3" s="82" t="s">
-        <v>365</v>
-      </c>
-      <c r="K3" s="82" t="s">
-        <v>553</v>
-      </c>
-      <c r="L3" s="82" t="s">
-        <v>404</v>
-      </c>
-      <c r="M3" s="82" t="s">
-        <v>546</v>
-      </c>
-      <c r="N3" s="82"/>
-      <c r="P3" s="82" t="s">
-        <v>547</v>
-      </c>
-      <c r="Q3" s="82" t="s">
-        <v>542</v>
-      </c>
-      <c r="R3" s="82" t="s">
-        <v>548</v>
-      </c>
-      <c r="S3" s="82" t="s">
-        <v>543</v>
-      </c>
-      <c r="T3" s="82" t="s">
-        <v>546</v>
+      <c r="P3" s="2" t="s">
+        <v>525</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>501</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>506</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>507</v>
       </c>
       <c r="V3" s="2"/>
     </row>
-    <row r="4" spans="1:28" ht="99.75" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="2" t="s">
-        <v>418</v>
-      </c>
+    <row r="4" spans="1:28" ht="42.75" x14ac:dyDescent="0.45">
       <c r="B4" s="2" t="s">
-        <v>419</v>
+        <v>514</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>387</v>
       </c>
+      <c r="E4" s="87" t="s">
+        <v>602</v>
+      </c>
       <c r="F4" s="84" t="s">
+        <v>440</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>457</v>
+      </c>
+      <c r="N4" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="J4" s="82" t="s">
-        <v>365</v>
-      </c>
-      <c r="K4" s="82" t="s">
-        <v>554</v>
-      </c>
-      <c r="L4" s="82" t="s">
-        <v>387</v>
-      </c>
-      <c r="M4" s="82" t="s">
-        <v>544</v>
-      </c>
-      <c r="N4" s="82"/>
-      <c r="P4" s="82" t="s">
-        <v>549</v>
-      </c>
-      <c r="Q4" s="82" t="s">
-        <v>551</v>
-      </c>
-      <c r="R4" s="82" t="s">
-        <v>382</v>
-      </c>
-      <c r="S4" s="82" t="s">
-        <v>374</v>
-      </c>
-      <c r="T4" s="82" t="s">
-        <v>544</v>
+      <c r="P4" s="2" t="s">
+        <v>523</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>501</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>465</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="T4" s="2" t="s">
+        <v>457</v>
       </c>
       <c r="V4" s="2"/>
     </row>
-    <row r="5" spans="1:28" ht="99.75" hidden="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:28" ht="228" x14ac:dyDescent="0.45">
       <c r="B5" s="2" t="s">
-        <v>420</v>
+        <v>515</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>387</v>
       </c>
+      <c r="E5" s="87" t="s">
+        <v>603</v>
+      </c>
       <c r="F5" s="84" t="s">
+        <v>440</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>467</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>468</v>
+      </c>
+      <c r="N5" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="J5" s="82" t="s">
-        <v>365</v>
-      </c>
-      <c r="K5" s="82" t="s">
-        <v>555</v>
-      </c>
-      <c r="L5" s="82" t="s">
-        <v>387</v>
-      </c>
-      <c r="M5" s="82" t="s">
-        <v>545</v>
-      </c>
-      <c r="N5" s="82"/>
-      <c r="P5" s="82" t="s">
-        <v>550</v>
-      </c>
-      <c r="Q5" s="82" t="s">
-        <v>552</v>
-      </c>
-      <c r="R5" s="82" t="s">
-        <v>382</v>
-      </c>
-      <c r="S5" s="82" t="s">
-        <v>374</v>
-      </c>
-      <c r="T5" s="82" t="s">
-        <v>545</v>
+      <c r="P5" s="2" t="s">
+        <v>640</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>501</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="T5" s="2" t="s">
+        <v>468</v>
       </c>
       <c r="V5" s="2"/>
     </row>
-    <row r="6" spans="1:28" ht="128.25" hidden="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:28" ht="71.25" x14ac:dyDescent="0.45">
       <c r="B6" s="2" t="s">
-        <v>421</v>
+        <v>516</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>387</v>
       </c>
-      <c r="E6" s="87" t="s">
-        <v>598</v>
-      </c>
-      <c r="F6" s="84">
-        <v>1</v>
+      <c r="E6" s="87">
+        <v>14.8</v>
+      </c>
+      <c r="F6" s="84" t="s">
+        <v>440</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>365</v>
+        <v>383</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>453</v>
+        <v>363</v>
       </c>
       <c r="L6" s="2" t="s">
         <v>387</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>372</v>
+        <v>469</v>
       </c>
       <c r="N6" s="2" t="s">
         <v>366</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>474</v>
+        <v>524</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>475</v>
+        <v>502</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>375</v>
+        <v>382</v>
       </c>
       <c r="S6" s="2" t="s">
         <v>374</v>
       </c>
       <c r="T6" s="2" t="s">
-        <v>476</v>
+        <v>503</v>
       </c>
       <c r="V6" s="2"/>
     </row>
-    <row r="7" spans="1:28" ht="71.25" hidden="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:28" ht="57" x14ac:dyDescent="0.45">
       <c r="B7" s="2" t="s">
-        <v>407</v>
+        <v>436</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>220</v>
+        <v>394</v>
       </c>
       <c r="E7" s="88">
         <v>45505</v>
       </c>
-      <c r="F7" s="84">
-        <v>1</v>
-      </c>
-      <c r="J7" s="82" t="s">
+      <c r="F7" s="84" t="s">
+        <v>366</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="P7" s="82" t="s">
+        <v>650</v>
+      </c>
+      <c r="Q7" s="2" t="s">
+        <v>499</v>
+      </c>
+      <c r="R7" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="S7" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="T7" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="V7" s="2"/>
+    </row>
+    <row r="8" spans="1:28" ht="409.5" x14ac:dyDescent="0.45">
+      <c r="J8" s="2" t="s">
         <v>454</v>
       </c>
-      <c r="K7" s="82" t="s">
-        <v>538</v>
-      </c>
-      <c r="L7" s="82" t="s">
+      <c r="K8" s="2" t="s">
+        <v>605</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>615</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>498</v>
+      </c>
+      <c r="P8" s="2" t="s">
+        <v>614</v>
+      </c>
+      <c r="Q8" s="2" t="s">
+        <v>511</v>
+      </c>
+      <c r="R8" s="2" t="s">
+        <v>613</v>
+      </c>
+      <c r="S8" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="T8" s="2" t="s">
+        <v>615</v>
+      </c>
+      <c r="V8" s="2"/>
+    </row>
+    <row r="9" spans="1:28" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="B9" s="2" t="s">
+        <v>606</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="E9" s="87" t="s">
+        <v>408</v>
+      </c>
+      <c r="F9" s="84" t="s">
+        <v>440</v>
+      </c>
+      <c r="J9" s="82" t="s">
+        <v>518</v>
+      </c>
+      <c r="K9" s="82" t="s">
+        <v>508</v>
+      </c>
+      <c r="L9" s="82" t="s">
+        <v>387</v>
+      </c>
+      <c r="M9" s="82" t="s">
+        <v>510</v>
+      </c>
+      <c r="N9" s="82" t="s">
+        <v>366</v>
+      </c>
+      <c r="O9" s="82"/>
+      <c r="P9" s="82" t="s">
+        <v>526</v>
+      </c>
+      <c r="Q9" s="82" t="s">
+        <v>511</v>
+      </c>
+      <c r="R9" s="82" t="s">
+        <v>519</v>
+      </c>
+      <c r="S9" s="82" t="s">
+        <v>520</v>
+      </c>
+      <c r="T9" s="82" t="s">
+        <v>510</v>
+      </c>
+      <c r="V9" s="2"/>
+    </row>
+    <row r="10" spans="1:28" ht="142.5" x14ac:dyDescent="0.45">
+      <c r="J10" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>604</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>610</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="P10" s="2" t="s">
+        <v>612</v>
+      </c>
+      <c r="Q10" s="2" t="s">
+        <v>511</v>
+      </c>
+      <c r="R10" s="2" t="s">
+        <v>611</v>
+      </c>
+      <c r="S10" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="T10" s="2" t="s">
+        <v>610</v>
+      </c>
+      <c r="V10" s="2"/>
+    </row>
+    <row r="11" spans="1:28" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="B11" s="2" t="s">
+        <v>512</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="E11" s="87" t="s">
+        <v>601</v>
+      </c>
+      <c r="F11" s="84" t="s">
+        <v>440</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>460</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="P11" s="2" t="s">
+        <v>522</v>
+      </c>
+      <c r="Q11" s="2" t="s">
+        <v>625</v>
+      </c>
+      <c r="R11" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="S11" s="2" t="s">
+        <v>461</v>
+      </c>
+      <c r="T11" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="V11" s="2"/>
+    </row>
+    <row r="12" spans="1:28" ht="108.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B12" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>394</v>
       </c>
-      <c r="M7" s="82" t="s">
-        <v>539</v>
-      </c>
-      <c r="N7" s="82"/>
-      <c r="P7" s="82" t="s">
-        <v>540</v>
-      </c>
-      <c r="Q7" s="82" t="s">
-        <v>541</v>
-      </c>
-      <c r="R7" s="82" t="s">
-        <v>379</v>
-      </c>
-      <c r="S7" s="82" t="s">
-        <v>380</v>
-      </c>
-      <c r="T7" s="82" t="s">
-        <v>539</v>
-      </c>
-      <c r="V7" s="2"/>
-    </row>
-    <row r="8" spans="1:28" ht="99.75" hidden="1" x14ac:dyDescent="0.45">
-      <c r="B8" s="2" t="s">
-        <v>408</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>404</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>409</v>
-      </c>
-      <c r="E8" s="87" t="s">
-        <v>597</v>
-      </c>
-      <c r="F8" s="84" t="s">
+      <c r="E12" s="88">
+        <v>45505</v>
+      </c>
+      <c r="F12" s="84" t="s">
         <v>366</v>
       </c>
-      <c r="J8" s="82" t="s">
+      <c r="J12" s="2" t="s">
         <v>454</v>
       </c>
-      <c r="K8" s="82" t="s">
-        <v>531</v>
-      </c>
-      <c r="L8" s="82" t="s">
-        <v>510</v>
-      </c>
-      <c r="M8" s="82" t="s">
-        <v>537</v>
-      </c>
-      <c r="N8" s="82">
-        <v>1</v>
-      </c>
-      <c r="P8" s="82" t="s">
-        <v>533</v>
-      </c>
-      <c r="Q8" s="82" t="s">
-        <v>536</v>
-      </c>
-      <c r="R8" s="82" t="s">
-        <v>534</v>
-      </c>
-      <c r="S8" s="82" t="s">
-        <v>535</v>
-      </c>
-      <c r="T8" s="82" t="s">
-        <v>532</v>
-      </c>
-      <c r="V8" s="2"/>
-    </row>
-    <row r="9" spans="1:28" ht="99.75" hidden="1" x14ac:dyDescent="0.45">
-      <c r="B9" s="2" t="s">
-        <v>410</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>404</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>411</v>
-      </c>
-      <c r="F9" s="84" t="s">
-        <v>366</v>
-      </c>
-      <c r="J9" s="82" t="s">
-        <v>454</v>
-      </c>
-      <c r="K9" s="82" t="s">
-        <v>531</v>
-      </c>
-      <c r="L9" s="82" t="s">
-        <v>510</v>
-      </c>
-      <c r="M9" s="82" t="s">
-        <v>537</v>
-      </c>
-      <c r="N9" s="82">
-        <v>1</v>
-      </c>
-      <c r="P9" s="82" t="s">
-        <v>533</v>
-      </c>
-      <c r="Q9" s="82" t="s">
-        <v>536</v>
-      </c>
-      <c r="R9" s="82" t="s">
-        <v>534</v>
-      </c>
-      <c r="S9" s="82" t="s">
-        <v>535</v>
-      </c>
-      <c r="T9" s="82" t="s">
-        <v>532</v>
-      </c>
-      <c r="V9" s="2"/>
-    </row>
-    <row r="10" spans="1:28" ht="99.75" hidden="1" x14ac:dyDescent="0.45">
-      <c r="B10" s="2" t="s">
-        <v>412</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>404</v>
-      </c>
-      <c r="F10" s="84" t="s">
-        <v>366</v>
-      </c>
-      <c r="J10" s="82" t="s">
-        <v>454</v>
-      </c>
-      <c r="K10" s="82" t="s">
-        <v>531</v>
-      </c>
-      <c r="L10" s="82" t="s">
-        <v>510</v>
-      </c>
-      <c r="M10" s="82" t="s">
-        <v>537</v>
-      </c>
-      <c r="N10" s="82">
-        <v>1</v>
-      </c>
-      <c r="P10" s="82" t="s">
-        <v>533</v>
-      </c>
-      <c r="Q10" s="82" t="s">
-        <v>536</v>
-      </c>
-      <c r="R10" s="82" t="s">
-        <v>534</v>
-      </c>
-      <c r="S10" s="82" t="s">
-        <v>535</v>
-      </c>
-      <c r="T10" s="82" t="s">
-        <v>532</v>
-      </c>
-      <c r="V10" s="2"/>
-    </row>
-    <row r="11" spans="1:28" ht="99.75" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="2" t="s">
-        <v>416</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>416</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>404</v>
-      </c>
-      <c r="F11" s="84" t="s">
-        <v>366</v>
-      </c>
-      <c r="J11" s="82" t="s">
-        <v>454</v>
-      </c>
-      <c r="K11" s="82" t="s">
-        <v>531</v>
-      </c>
-      <c r="L11" s="82" t="s">
-        <v>510</v>
-      </c>
-      <c r="M11" s="82" t="s">
-        <v>537</v>
-      </c>
-      <c r="N11" s="82">
-        <v>1</v>
-      </c>
-      <c r="P11" s="82" t="s">
-        <v>533</v>
-      </c>
-      <c r="Q11" s="82" t="s">
-        <v>536</v>
-      </c>
-      <c r="R11" s="82" t="s">
-        <v>534</v>
-      </c>
-      <c r="S11" s="82" t="s">
-        <v>535</v>
-      </c>
-      <c r="T11" s="82" t="s">
-        <v>532</v>
-      </c>
-      <c r="V11" s="2"/>
-    </row>
-    <row r="12" spans="1:28" ht="108.75" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B12" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>387</v>
-      </c>
-      <c r="E12" s="87" t="s">
-        <v>599</v>
-      </c>
-      <c r="F12" s="84">
-        <v>1</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>357</v>
-      </c>
       <c r="K12" s="2" t="s">
-        <v>449</v>
+        <v>455</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>387</v>
+        <v>390</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>443</v>
+        <v>456</v>
       </c>
       <c r="N12" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="P12" s="2" t="s">
-        <v>477</v>
+      <c r="P12" s="82" t="s">
+        <v>521</v>
       </c>
       <c r="Q12" s="2" t="s">
-        <v>479</v>
+        <v>497</v>
       </c>
       <c r="R12" s="2" t="s">
-        <v>444</v>
+        <v>392</v>
       </c>
       <c r="S12" s="2" t="s">
-        <v>405</v>
+        <v>393</v>
       </c>
       <c r="T12" s="2" t="s">
-        <v>478</v>
+        <v>500</v>
       </c>
       <c r="V12" s="2"/>
     </row>
-    <row r="13" spans="1:28" ht="85.5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:28" ht="99.75" x14ac:dyDescent="0.45">
       <c r="B13" s="2" t="s">
-        <v>414</v>
+        <v>408</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>387</v>
+        <v>404</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>409</v>
       </c>
       <c r="E13" s="87" t="s">
-        <v>600</v>
-      </c>
-      <c r="F13" s="84">
+        <v>591</v>
+      </c>
+      <c r="F13" s="84" t="s">
+        <v>366</v>
+      </c>
+      <c r="J13" s="82" t="s">
+        <v>454</v>
+      </c>
+      <c r="K13" s="82" t="s">
+        <v>527</v>
+      </c>
+      <c r="L13" s="82" t="s">
+        <v>509</v>
+      </c>
+      <c r="M13" s="82" t="s">
+        <v>532</v>
+      </c>
+      <c r="N13" s="82">
         <v>1</v>
       </c>
-      <c r="J13" s="2" t="s">
-        <v>357</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>450</v>
-      </c>
-      <c r="L13" s="2" t="s">
-        <v>387</v>
-      </c>
-      <c r="M13" s="2" t="s">
-        <v>441</v>
-      </c>
-      <c r="N13" s="2" t="s">
-        <v>366</v>
-      </c>
-      <c r="P13" s="2" t="s">
-        <v>480</v>
-      </c>
-      <c r="Q13" s="2" t="s">
-        <v>479</v>
-      </c>
-      <c r="R13" s="2" t="s">
-        <v>442</v>
-      </c>
-      <c r="S13" s="2" t="s">
-        <v>405</v>
-      </c>
-      <c r="T13" s="2" t="s">
-        <v>482</v>
+      <c r="P13" s="82" t="s">
+        <v>641</v>
+      </c>
+      <c r="Q13" s="82" t="s">
+        <v>531</v>
+      </c>
+      <c r="R13" s="82" t="s">
+        <v>529</v>
+      </c>
+      <c r="S13" s="82" t="s">
+        <v>530</v>
+      </c>
+      <c r="T13" s="82" t="s">
+        <v>528</v>
       </c>
       <c r="V13" s="2"/>
     </row>
-    <row r="14" spans="1:28" ht="99.75" hidden="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:28" ht="99.75" x14ac:dyDescent="0.45">
       <c r="B14" s="2" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>387</v>
+        <v>404</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>411</v>
       </c>
       <c r="F14" s="84" t="s">
         <v>366</v>
       </c>
-      <c r="J14" s="2" t="s">
-        <v>357</v>
-      </c>
-      <c r="K14" s="2" t="s">
-        <v>451</v>
-      </c>
-      <c r="L14" s="2" t="s">
-        <v>387</v>
-      </c>
-      <c r="M14" s="2" t="s">
-        <v>445</v>
-      </c>
-      <c r="N14" s="2" t="s">
+      <c r="J14" s="82" t="s">
+        <v>454</v>
+      </c>
+      <c r="K14" s="82" t="s">
+        <v>527</v>
+      </c>
+      <c r="L14" s="82" t="s">
+        <v>509</v>
+      </c>
+      <c r="M14" s="82" t="s">
+        <v>532</v>
+      </c>
+      <c r="N14" s="82">
+        <v>1</v>
+      </c>
+      <c r="P14" s="82" t="s">
+        <v>641</v>
+      </c>
+      <c r="Q14" s="82" t="s">
+        <v>531</v>
+      </c>
+      <c r="R14" s="82" t="s">
+        <v>529</v>
+      </c>
+      <c r="S14" s="82" t="s">
+        <v>530</v>
+      </c>
+      <c r="T14" s="82" t="s">
+        <v>528</v>
+      </c>
+      <c r="V14" s="2"/>
+    </row>
+    <row r="15" spans="1:28" ht="99.75" x14ac:dyDescent="0.45">
+      <c r="B15" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="F15" s="84" t="s">
         <v>366</v>
       </c>
-      <c r="P14" s="2" t="s">
-        <v>481</v>
-      </c>
-      <c r="Q14" s="2" t="s">
-        <v>479</v>
-      </c>
-      <c r="R14" s="2" t="s">
-        <v>446</v>
-      </c>
-      <c r="S14" s="2" t="s">
-        <v>405</v>
-      </c>
-      <c r="T14" s="2" t="s">
-        <v>483</v>
-      </c>
-      <c r="V14" s="2"/>
-    </row>
-    <row r="15" spans="1:28" ht="114" hidden="1" x14ac:dyDescent="0.45">
-      <c r="B15" s="2" t="s">
-        <v>425</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>426</v>
-      </c>
-      <c r="E15" s="87" t="s">
-        <v>601</v>
-      </c>
-      <c r="F15" s="84">
+      <c r="J15" s="82" t="s">
+        <v>454</v>
+      </c>
+      <c r="K15" s="82" t="s">
+        <v>527</v>
+      </c>
+      <c r="L15" s="82" t="s">
+        <v>509</v>
+      </c>
+      <c r="M15" s="82" t="s">
+        <v>532</v>
+      </c>
+      <c r="N15" s="82">
         <v>1</v>
       </c>
-      <c r="J15" s="2" t="s">
-        <v>484</v>
-      </c>
-      <c r="K15" s="2" t="s">
-        <v>485</v>
-      </c>
-      <c r="L15" s="2" t="s">
-        <v>486</v>
-      </c>
-      <c r="M15" s="2" t="s">
-        <v>494</v>
-      </c>
-      <c r="N15" s="2" t="s">
+      <c r="P15" s="82" t="s">
+        <v>641</v>
+      </c>
+      <c r="Q15" s="82" t="s">
+        <v>531</v>
+      </c>
+      <c r="R15" s="82" t="s">
+        <v>529</v>
+      </c>
+      <c r="S15" s="82" t="s">
+        <v>530</v>
+      </c>
+      <c r="T15" s="82" t="s">
+        <v>528</v>
+      </c>
+      <c r="V15" s="2"/>
+    </row>
+    <row r="16" spans="1:28" ht="99.75" x14ac:dyDescent="0.45">
+      <c r="A16" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="F16" s="84" t="s">
         <v>366</v>
       </c>
-      <c r="P15" s="2" t="s">
-        <v>487</v>
-      </c>
-      <c r="Q15" s="2" t="s">
-        <v>492</v>
-      </c>
-      <c r="R15" s="2" t="s">
-        <v>488</v>
-      </c>
-      <c r="S15" s="2" t="s">
-        <v>367</v>
-      </c>
-      <c r="T15" s="2" t="s">
-        <v>489</v>
-      </c>
-      <c r="V15" s="2"/>
-    </row>
-    <row r="16" spans="1:28" ht="85.5" x14ac:dyDescent="0.45">
-      <c r="B16" s="2" t="s">
-        <v>424</v>
-      </c>
-      <c r="C16" s="2" t="s">
+      <c r="J16" s="82" t="s">
+        <v>454</v>
+      </c>
+      <c r="K16" s="82" t="s">
+        <v>527</v>
+      </c>
+      <c r="L16" s="82" t="s">
+        <v>509</v>
+      </c>
+      <c r="M16" s="82" t="s">
+        <v>532</v>
+      </c>
+      <c r="N16" s="82">
+        <v>1</v>
+      </c>
+      <c r="P16" s="82" t="s">
+        <v>641</v>
+      </c>
+      <c r="Q16" s="82" t="s">
+        <v>531</v>
+      </c>
+      <c r="R16" s="82" t="s">
+        <v>529</v>
+      </c>
+      <c r="S16" s="82" t="s">
+        <v>530</v>
+      </c>
+      <c r="T16" s="82" t="s">
+        <v>528</v>
+      </c>
+      <c r="V16" s="2"/>
+    </row>
+    <row r="17" spans="2:22" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="B17" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="E17" s="88">
+        <v>45505</v>
+      </c>
+      <c r="F17" s="84">
+        <v>1</v>
+      </c>
+      <c r="J17" s="82" t="s">
+        <v>454</v>
+      </c>
+      <c r="K17" s="82" t="s">
+        <v>533</v>
+      </c>
+      <c r="L17" s="82" t="s">
         <v>394</v>
       </c>
-      <c r="E16" s="88">
-        <v>25143</v>
-      </c>
-      <c r="F16" s="84">
-        <v>1</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>447</v>
-      </c>
-      <c r="K16" s="2" t="s">
-        <v>359</v>
-      </c>
-      <c r="L16" s="2" t="s">
-        <v>394</v>
-      </c>
-      <c r="M16" s="2" t="s">
-        <v>378</v>
-      </c>
-      <c r="N16" s="2" t="s">
-        <v>366</v>
-      </c>
-      <c r="P16" s="2" t="s">
-        <v>490</v>
-      </c>
-      <c r="Q16" s="2" t="s">
-        <v>491</v>
-      </c>
-      <c r="R16" s="2" t="s">
+      <c r="M17" s="82" t="s">
+        <v>534</v>
+      </c>
+      <c r="N17" s="82"/>
+      <c r="P17" s="82" t="s">
+        <v>642</v>
+      </c>
+      <c r="Q17" s="82" t="s">
+        <v>535</v>
+      </c>
+      <c r="R17" s="82" t="s">
         <v>379</v>
       </c>
-      <c r="S16" s="2" t="s">
+      <c r="S17" s="82" t="s">
         <v>380</v>
       </c>
-      <c r="T16" s="2" t="s">
-        <v>378</v>
-      </c>
-      <c r="V16" s="2"/>
-    </row>
-    <row r="17" spans="2:22" ht="99.75" x14ac:dyDescent="0.45">
-      <c r="B17" s="2" t="s">
-        <v>423</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>387</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>422</v>
-      </c>
-      <c r="E17" s="87" t="s">
-        <v>602</v>
-      </c>
-      <c r="F17" s="84" t="s">
-        <v>366</v>
-      </c>
-      <c r="J17" s="2" t="s">
-        <v>448</v>
-      </c>
-      <c r="K17" s="2" t="s">
-        <v>361</v>
-      </c>
-      <c r="L17" s="2" t="s">
-        <v>395</v>
-      </c>
-      <c r="M17" s="2" t="s">
-        <v>376</v>
-      </c>
-      <c r="N17" s="2" t="s">
-        <v>366</v>
-      </c>
-      <c r="P17" s="2" t="s">
-        <v>644</v>
-      </c>
-      <c r="Q17" s="2" t="s">
-        <v>493</v>
-      </c>
-      <c r="R17" s="2" t="s">
-        <v>645</v>
-      </c>
-      <c r="S17" s="2" t="s">
-        <v>647</v>
-      </c>
-      <c r="T17" s="2" t="s">
-        <v>376</v>
+      <c r="T17" s="82" t="s">
+        <v>534</v>
       </c>
       <c r="V17" s="2"/>
     </row>
-    <row r="18" spans="2:22" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:22" ht="142.5" x14ac:dyDescent="0.45">
       <c r="B18" s="2" t="s">
-        <v>427</v>
+        <v>512</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>387</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>428</v>
-      </c>
       <c r="E18" s="87" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="F18" s="84" t="s">
-        <v>366</v>
+        <v>440</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>448</v>
+        <v>623</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>362</v>
+        <v>624</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>396</v>
+        <v>387</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>377</v>
+        <v>627</v>
       </c>
       <c r="N18" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="P18" s="2" t="s">
-        <v>649</v>
-      </c>
-      <c r="Q18" s="2" t="s">
-        <v>493</v>
-      </c>
-      <c r="R18" s="2" t="s">
-        <v>646</v>
-      </c>
-      <c r="S18" s="2" t="s">
-        <v>648</v>
-      </c>
-      <c r="T18" s="2" t="s">
-        <v>377</v>
+      <c r="P18" s="82" t="s">
+        <v>643</v>
+      </c>
+      <c r="Q18" s="82" t="s">
+        <v>626</v>
+      </c>
+      <c r="R18" s="82" t="s">
+        <v>382</v>
+      </c>
+      <c r="S18" s="82" t="s">
+        <v>461</v>
+      </c>
+      <c r="T18" s="82" t="s">
+        <v>628</v>
       </c>
       <c r="V18" s="2"/>
     </row>
-    <row r="19" spans="2:22" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:22" ht="99.75" x14ac:dyDescent="0.45">
       <c r="B19" s="2" t="s">
-        <v>433</v>
+        <v>406</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>387</v>
       </c>
-      <c r="F19" s="84" t="s">
-        <v>366</v>
+      <c r="E19" s="87" t="s">
+        <v>590</v>
+      </c>
+      <c r="F19" s="84">
+        <v>1</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>447</v>
+        <v>364</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="L19" s="2" t="s">
         <v>387</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>381</v>
+        <v>368</v>
       </c>
       <c r="N19" s="2" t="s">
         <v>366</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>495</v>
+        <v>471</v>
       </c>
       <c r="Q19" s="2" t="s">
-        <v>496</v>
+        <v>472</v>
       </c>
       <c r="R19" s="2" t="s">
-        <v>382</v>
+        <v>369</v>
       </c>
       <c r="S19" s="2" t="s">
-        <v>374</v>
+        <v>452</v>
       </c>
       <c r="T19" s="2" t="s">
-        <v>497</v>
+        <v>473</v>
       </c>
       <c r="V19" s="2"/>
     </row>
-    <row r="20" spans="2:22" ht="57" hidden="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:22" ht="85.5" x14ac:dyDescent="0.45">
       <c r="B20" s="2" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>430</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>556</v>
-      </c>
-      <c r="E20" s="87">
-        <v>9999999</v>
-      </c>
-      <c r="F20" s="84" t="s">
+        <v>394</v>
+      </c>
+      <c r="E20" s="88">
+        <v>25143</v>
+      </c>
+      <c r="F20" s="84">
+        <v>1</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>447</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="L20" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="M20" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="N20" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="J20" s="82" t="s">
-        <v>560</v>
-      </c>
-      <c r="K20" s="82" t="s">
-        <v>559</v>
-      </c>
-      <c r="L20" s="82" t="s">
-        <v>387</v>
-      </c>
-      <c r="M20" s="82" t="s">
-        <v>556</v>
-      </c>
-      <c r="N20" s="85" t="s">
-        <v>366</v>
-      </c>
-      <c r="P20" s="82" t="s">
-        <v>585</v>
-      </c>
-      <c r="Q20" s="82" t="s">
-        <v>475</v>
-      </c>
-      <c r="R20" s="82" t="s">
-        <v>586</v>
-      </c>
-      <c r="S20" s="82" t="s">
-        <v>374</v>
-      </c>
-      <c r="T20" s="82" t="s">
-        <v>587</v>
+      <c r="P20" s="2" t="s">
+        <v>490</v>
+      </c>
+      <c r="Q20" s="2" t="s">
+        <v>491</v>
+      </c>
+      <c r="R20" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="S20" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="T20" s="2" t="s">
+        <v>378</v>
       </c>
       <c r="V20" s="2"/>
     </row>
-    <row r="21" spans="2:22" ht="71.25" hidden="1" x14ac:dyDescent="0.45">
-      <c r="B21" s="2" t="s">
-        <v>557</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>357</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>558</v>
-      </c>
-      <c r="F21" s="84" t="s">
-        <v>499</v>
-      </c>
+    <row r="21" spans="2:22" ht="99.75" x14ac:dyDescent="0.45">
       <c r="J21" s="2" t="s">
-        <v>564</v>
+        <v>484</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>565</v>
+        <v>607</v>
       </c>
       <c r="L21" s="2" t="s">
         <v>387</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>443</v>
-      </c>
-      <c r="N21" s="84" t="s">
-        <v>499</v>
+        <v>617</v>
+      </c>
+      <c r="N21" s="2" t="s">
+        <v>366</v>
       </c>
       <c r="P21" s="2" t="s">
-        <v>566</v>
+        <v>618</v>
       </c>
       <c r="Q21" s="2" t="s">
-        <v>567</v>
+        <v>619</v>
       </c>
       <c r="R21" s="2" t="s">
-        <v>568</v>
+        <v>616</v>
       </c>
       <c r="S21" s="2" t="s">
-        <v>479</v>
+        <v>374</v>
       </c>
       <c r="T21" s="2" t="s">
-        <v>569</v>
+        <v>621</v>
       </c>
       <c r="V21" s="2"/>
     </row>
-    <row r="22" spans="2:22" ht="85.5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:22" ht="114" x14ac:dyDescent="0.45">
       <c r="B22" s="2" t="s">
-        <v>431</v>
+        <v>425</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>394</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>561</v>
-      </c>
-      <c r="E22" s="88">
-        <v>45566</v>
-      </c>
-      <c r="F22" s="84" t="s">
+        <v>426</v>
+      </c>
+      <c r="E22" s="87" t="s">
+        <v>595</v>
+      </c>
+      <c r="F22" s="84">
+        <v>1</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>484</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>485</v>
+      </c>
+      <c r="L22" s="2" t="s">
+        <v>486</v>
+      </c>
+      <c r="M22" s="2" t="s">
+        <v>494</v>
+      </c>
+      <c r="N22" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="J22" s="82" t="s">
-        <v>560</v>
-      </c>
-      <c r="K22" s="82" t="s">
-        <v>574</v>
-      </c>
-      <c r="L22" s="82" t="s">
-        <v>394</v>
-      </c>
-      <c r="M22" s="82" t="s">
-        <v>561</v>
-      </c>
-      <c r="N22" s="85" t="s">
-        <v>366</v>
-      </c>
-      <c r="P22" s="82" t="s">
-        <v>588</v>
-      </c>
-      <c r="Q22" s="82" t="s">
-        <v>589</v>
-      </c>
-      <c r="R22" s="82" t="s">
-        <v>379</v>
-      </c>
-      <c r="S22" s="82" t="s">
-        <v>380</v>
-      </c>
-      <c r="T22" s="82" t="s">
-        <v>561</v>
+      <c r="P22" s="2" t="s">
+        <v>487</v>
+      </c>
+      <c r="Q22" s="2" t="s">
+        <v>492</v>
+      </c>
+      <c r="R22" s="2" t="s">
+        <v>488</v>
+      </c>
+      <c r="S22" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="T22" s="2" t="s">
+        <v>489</v>
       </c>
       <c r="V22" s="2"/>
     </row>
-    <row r="23" spans="2:22" ht="85.5" hidden="1" x14ac:dyDescent="0.45">
-      <c r="B23" s="2" t="s">
-        <v>432</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>357</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>562</v>
-      </c>
-      <c r="E23" s="87" t="s">
-        <v>604</v>
-      </c>
-      <c r="F23" s="84" t="s">
-        <v>366</v>
-      </c>
-      <c r="J23" s="82" t="s">
-        <v>560</v>
-      </c>
-      <c r="K23" s="82" t="s">
-        <v>575</v>
-      </c>
-      <c r="L23" s="82" t="s">
-        <v>387</v>
-      </c>
-      <c r="M23" s="82" t="s">
-        <v>577</v>
-      </c>
-      <c r="N23" s="85" t="s">
-        <v>366</v>
-      </c>
-      <c r="P23" s="82" t="s">
-        <v>590</v>
-      </c>
-      <c r="Q23" s="82" t="s">
-        <v>592</v>
-      </c>
-      <c r="R23" s="82" t="s">
-        <v>594</v>
-      </c>
-      <c r="S23" s="82" t="s">
-        <v>479</v>
-      </c>
-      <c r="T23" s="82" t="s">
-        <v>577</v>
+    <row r="23" spans="2:22" ht="128.25" x14ac:dyDescent="0.45">
+      <c r="J23" s="2" t="s">
+        <v>484</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>608</v>
+      </c>
+      <c r="L23" s="2" t="s">
+        <v>609</v>
+      </c>
+      <c r="M23" s="2" t="s">
+        <v>620</v>
+      </c>
+      <c r="N23" s="2" t="s">
+        <v>498</v>
+      </c>
+      <c r="P23" s="2" t="s">
+        <v>644</v>
+      </c>
+      <c r="Q23" s="2" t="s">
+        <v>647</v>
+      </c>
+      <c r="R23" s="2" t="s">
+        <v>645</v>
+      </c>
+      <c r="S23" s="2" t="s">
+        <v>646</v>
+      </c>
+      <c r="T23" s="2" t="s">
+        <v>622</v>
       </c>
       <c r="V23" s="2"/>
     </row>
-    <row r="24" spans="2:22" ht="85.5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:22" ht="71.25" x14ac:dyDescent="0.45">
       <c r="B24" s="2" t="s">
-        <v>434</v>
+        <v>551</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>357</v>
       </c>
       <c r="D24" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="F24" s="84" t="s">
+        <v>498</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>558</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>559</v>
+      </c>
+      <c r="L24" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="M24" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="N24" s="84" t="s">
+        <v>498</v>
+      </c>
+      <c r="P24" s="2" t="s">
+        <v>560</v>
+      </c>
+      <c r="Q24" s="2" t="s">
+        <v>561</v>
+      </c>
+      <c r="R24" s="2" t="s">
+        <v>588</v>
+      </c>
+      <c r="S24" s="2" t="s">
+        <v>479</v>
+      </c>
+      <c r="T24" s="2" t="s">
         <v>563</v>
-      </c>
-      <c r="E24" s="87" t="s">
-        <v>605</v>
-      </c>
-      <c r="F24" s="84" t="s">
-        <v>366</v>
-      </c>
-      <c r="J24" s="82" t="s">
-        <v>560</v>
-      </c>
-      <c r="K24" s="82" t="s">
-        <v>576</v>
-      </c>
-      <c r="L24" s="82" t="s">
-        <v>387</v>
-      </c>
-      <c r="M24" s="82" t="s">
-        <v>578</v>
-      </c>
-      <c r="N24" s="85" t="s">
-        <v>366</v>
-      </c>
-      <c r="P24" s="82" t="s">
-        <v>591</v>
-      </c>
-      <c r="Q24" s="82" t="s">
-        <v>593</v>
-      </c>
-      <c r="R24" s="82" t="s">
-        <v>568</v>
-      </c>
-      <c r="S24" s="82" t="s">
-        <v>479</v>
-      </c>
-      <c r="T24" s="82" t="s">
-        <v>578</v>
       </c>
       <c r="V24" s="2"/>
     </row>
     <row r="25" spans="2:22" ht="127.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B25" s="2" t="s">
-        <v>435</v>
+        <v>414</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>430</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>470</v>
-      </c>
-      <c r="E25" s="87">
-        <v>999999</v>
-      </c>
-      <c r="F25" s="84" t="s">
+        <v>387</v>
+      </c>
+      <c r="E25" s="87" t="s">
+        <v>594</v>
+      </c>
+      <c r="F25" s="84">
+        <v>1</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="L25" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="M25" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="N25" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="J25" s="82" t="s">
-        <v>572</v>
-      </c>
-      <c r="K25" s="82" t="s">
-        <v>573</v>
-      </c>
-      <c r="L25" s="82" t="s">
+      <c r="P25" s="2" t="s">
+        <v>480</v>
+      </c>
+      <c r="Q25" s="2" t="s">
+        <v>479</v>
+      </c>
+      <c r="R25" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="S25" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="T25" s="2" t="s">
+        <v>482</v>
+      </c>
+      <c r="V25" s="2"/>
+    </row>
+    <row r="26" spans="2:22" ht="99.75" x14ac:dyDescent="0.45">
+      <c r="B26" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>387</v>
-      </c>
-      <c r="M25" s="82" t="s">
-        <v>470</v>
-      </c>
-      <c r="N25" s="85" t="s">
-        <v>366</v>
-      </c>
-      <c r="P25" s="82" t="s">
-        <v>571</v>
-      </c>
-      <c r="Q25" s="82" t="s">
-        <v>570</v>
-      </c>
-      <c r="R25" s="82" t="s">
-        <v>382</v>
-      </c>
-      <c r="S25" s="82" t="s">
-        <v>374</v>
-      </c>
-      <c r="T25" s="82" t="s">
-        <v>470</v>
-      </c>
-      <c r="V25" s="2"/>
-    </row>
-    <row r="26" spans="2:22" ht="71.25" x14ac:dyDescent="0.45">
-      <c r="B26" s="2" t="s">
-        <v>436</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>394</v>
-      </c>
-      <c r="E26" s="88">
-        <v>45505</v>
       </c>
       <c r="F26" s="84" t="s">
         <v>366</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>388</v>
+        <v>357</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>389</v>
+        <v>451</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>394</v>
+        <v>387</v>
       </c>
       <c r="M26" s="2" t="s">
-        <v>391</v>
+        <v>445</v>
       </c>
       <c r="N26" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="P26" s="82" t="s">
-        <v>522</v>
+      <c r="P26" s="2" t="s">
+        <v>481</v>
       </c>
       <c r="Q26" s="2" t="s">
-        <v>500</v>
+        <v>479</v>
       </c>
       <c r="R26" s="2" t="s">
-        <v>379</v>
+        <v>446</v>
       </c>
       <c r="S26" s="2" t="s">
-        <v>380</v>
+        <v>405</v>
       </c>
       <c r="T26" s="2" t="s">
-        <v>391</v>
+        <v>483</v>
       </c>
       <c r="V26" s="2"/>
     </row>
-    <row r="27" spans="2:22" ht="42.75" hidden="1" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:22" ht="85.5" x14ac:dyDescent="0.45">
       <c r="B27" s="2" t="s">
-        <v>437</v>
+        <v>413</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>394</v>
-      </c>
-      <c r="E27" s="88">
-        <v>45505</v>
-      </c>
-      <c r="F27" s="84" t="s">
-        <v>366</v>
+        <v>387</v>
+      </c>
+      <c r="E27" s="87" t="s">
+        <v>593</v>
+      </c>
+      <c r="F27" s="84">
+        <v>1</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>454</v>
+        <v>357</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>455</v>
+        <v>449</v>
       </c>
       <c r="L27" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="M27" s="2" t="s">
-        <v>456</v>
+        <v>443</v>
       </c>
       <c r="N27" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="P27" s="82" t="s">
-        <v>523</v>
+      <c r="P27" s="2" t="s">
+        <v>477</v>
       </c>
       <c r="Q27" s="2" t="s">
-        <v>498</v>
+        <v>479</v>
       </c>
       <c r="R27" s="2" t="s">
-        <v>392</v>
+        <v>444</v>
       </c>
       <c r="S27" s="2" t="s">
-        <v>393</v>
+        <v>405</v>
       </c>
       <c r="T27" s="2" t="s">
-        <v>501</v>
+        <v>478</v>
       </c>
       <c r="V27" s="2"/>
     </row>
-    <row r="28" spans="2:22" ht="42.75" hidden="1" x14ac:dyDescent="0.45">
+    <row r="28" spans="2:22" ht="99.75" x14ac:dyDescent="0.45">
       <c r="B28" s="2" t="s">
-        <v>438</v>
+        <v>423</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>387</v>
       </c>
+      <c r="D28" s="2" t="s">
+        <v>422</v>
+      </c>
       <c r="E28" s="87" t="s">
-        <v>606</v>
+        <v>596</v>
       </c>
       <c r="F28" s="84" t="s">
         <v>366</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>365</v>
+        <v>448</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>580</v>
+        <v>361</v>
       </c>
       <c r="L28" s="2" t="s">
-        <v>387</v>
+        <v>395</v>
       </c>
       <c r="M28" s="2" t="s">
-        <v>579</v>
+        <v>376</v>
       </c>
       <c r="N28" s="2" t="s">
         <v>366</v>
       </c>
       <c r="P28" s="2" t="s">
-        <v>581</v>
+        <v>634</v>
       </c>
       <c r="Q28" s="2" t="s">
-        <v>582</v>
+        <v>493</v>
       </c>
       <c r="R28" s="2" t="s">
-        <v>583</v>
+        <v>635</v>
       </c>
       <c r="S28" s="2" t="s">
-        <v>367</v>
+        <v>637</v>
       </c>
       <c r="T28" s="2" t="s">
-        <v>584</v>
+        <v>376</v>
       </c>
       <c r="V28" s="2"/>
     </row>
-    <row r="29" spans="2:22" ht="142.5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:22" ht="71.25" x14ac:dyDescent="0.45">
       <c r="B29" s="2" t="s">
-        <v>513</v>
+        <v>427</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>387</v>
       </c>
+      <c r="D29" s="2" t="s">
+        <v>428</v>
+      </c>
       <c r="E29" s="87" t="s">
-        <v>607</v>
+        <v>597</v>
       </c>
       <c r="F29" s="84" t="s">
-        <v>440</v>
+        <v>366</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>632</v>
+        <v>448</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>633</v>
+        <v>362</v>
       </c>
       <c r="L29" s="2" t="s">
-        <v>387</v>
+        <v>396</v>
       </c>
       <c r="M29" s="2" t="s">
-        <v>637</v>
+        <v>377</v>
       </c>
       <c r="N29" s="2" t="s">
         <v>366</v>
       </c>
       <c r="P29" s="2" t="s">
-        <v>634</v>
+        <v>639</v>
       </c>
       <c r="Q29" s="2" t="s">
+        <v>493</v>
+      </c>
+      <c r="R29" s="2" t="s">
         <v>636</v>
       </c>
-      <c r="R29" s="2" t="s">
+      <c r="S29" s="2" t="s">
+        <v>638</v>
+      </c>
+      <c r="T29" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="V29" s="2"/>
+    </row>
+    <row r="30" spans="2:22" ht="142.5" x14ac:dyDescent="0.45">
+      <c r="B30" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>470</v>
+      </c>
+      <c r="E30" s="87">
+        <v>999999</v>
+      </c>
+      <c r="F30" s="84" t="s">
+        <v>366</v>
+      </c>
+      <c r="J30" s="82" t="s">
+        <v>566</v>
+      </c>
+      <c r="K30" s="82" t="s">
+        <v>567</v>
+      </c>
+      <c r="L30" s="82" t="s">
+        <v>387</v>
+      </c>
+      <c r="M30" s="82" t="s">
+        <v>470</v>
+      </c>
+      <c r="N30" s="85" t="s">
+        <v>366</v>
+      </c>
+      <c r="P30" s="82" t="s">
+        <v>565</v>
+      </c>
+      <c r="Q30" s="82" t="s">
+        <v>564</v>
+      </c>
+      <c r="R30" s="82" t="s">
         <v>382</v>
       </c>
-      <c r="S29" s="2" t="s">
-        <v>461</v>
-      </c>
-      <c r="T29" s="2" t="s">
-        <v>638</v>
-      </c>
-      <c r="V29" s="2"/>
-    </row>
-    <row r="30" spans="2:22" ht="85.5" x14ac:dyDescent="0.45">
-      <c r="B30" s="2" t="s">
-        <v>513</v>
-      </c>
-      <c r="C30" s="2" t="s">
+      <c r="S30" s="82" t="s">
+        <v>374</v>
+      </c>
+      <c r="T30" s="82" t="s">
+        <v>470</v>
+      </c>
+      <c r="V30" s="2"/>
+    </row>
+    <row r="31" spans="2:22" ht="28.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B31" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="C31" s="2" t="s">
         <v>387</v>
       </c>
-      <c r="E30" s="87" t="s">
-        <v>607</v>
-      </c>
-      <c r="F30" s="84" t="s">
-        <v>440</v>
-      </c>
-      <c r="J30" s="2" t="s">
-        <v>383</v>
-      </c>
-      <c r="K30" s="2" t="s">
-        <v>460</v>
-      </c>
-      <c r="L30" s="2" t="s">
-        <v>387</v>
-      </c>
-      <c r="M30" s="2" t="s">
-        <v>459</v>
-      </c>
-      <c r="N30" s="2" t="s">
-        <v>366</v>
-      </c>
-      <c r="P30" s="2" t="s">
-        <v>524</v>
-      </c>
-      <c r="Q30" s="2" t="s">
-        <v>635</v>
-      </c>
-      <c r="R30" s="2" t="s">
-        <v>382</v>
-      </c>
-      <c r="S30" s="2" t="s">
-        <v>461</v>
-      </c>
-      <c r="T30" s="2" t="s">
-        <v>459</v>
-      </c>
-      <c r="V30" s="2"/>
-    </row>
-    <row r="31" spans="2:22" ht="28.9" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B31" s="2" t="s">
-        <v>514</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>430</v>
-      </c>
-      <c r="E31" s="87">
-        <v>12345678</v>
-      </c>
-      <c r="F31" s="84" t="s">
-        <v>440</v>
+      <c r="E31" s="87" t="s">
+        <v>592</v>
+      </c>
+      <c r="F31" s="84">
+        <v>1</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>454</v>
+        <v>365</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>463</v>
+        <v>453</v>
       </c>
       <c r="L31" s="2" t="s">
         <v>387</v>
       </c>
       <c r="M31" s="2" t="s">
-        <v>462</v>
+        <v>372</v>
       </c>
       <c r="N31" s="2" t="s">
         <v>366</v>
       </c>
       <c r="P31" s="2" t="s">
-        <v>525</v>
+        <v>474</v>
+      </c>
+      <c r="Q31" s="2" t="s">
+        <v>475</v>
       </c>
       <c r="R31" s="2" t="s">
-        <v>464</v>
+        <v>375</v>
       </c>
       <c r="S31" s="2" t="s">
         <v>374</v>
       </c>
+      <c r="T31" s="2" t="s">
+        <v>476</v>
+      </c>
       <c r="V31" s="2"/>
     </row>
     <row r="32" spans="2:22" ht="42.75" x14ac:dyDescent="0.45">
       <c r="B32" s="2" t="s">
-        <v>515</v>
+        <v>438</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>387</v>
       </c>
       <c r="E32" s="87" t="s">
-        <v>608</v>
+        <v>600</v>
       </c>
       <c r="F32" s="84" t="s">
-        <v>440</v>
+        <v>366</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>383</v>
+        <v>365</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>458</v>
+        <v>574</v>
+      </c>
+      <c r="L32" s="2" t="s">
+        <v>387</v>
       </c>
       <c r="M32" s="2" t="s">
-        <v>457</v>
+        <v>573</v>
       </c>
       <c r="N32" s="2" t="s">
         <v>366</v>
       </c>
       <c r="P32" s="2" t="s">
-        <v>526</v>
+        <v>575</v>
       </c>
       <c r="Q32" s="2" t="s">
-        <v>502</v>
+        <v>576</v>
       </c>
       <c r="R32" s="2" t="s">
-        <v>465</v>
+        <v>577</v>
       </c>
       <c r="S32" s="2" t="s">
         <v>367</v>
       </c>
       <c r="T32" s="2" t="s">
-        <v>457</v>
+        <v>578</v>
       </c>
       <c r="V32" s="2"/>
     </row>
-    <row r="33" spans="2:22" ht="228" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:22" ht="99.75" x14ac:dyDescent="0.45">
       <c r="B33" s="2" t="s">
-        <v>516</v>
+        <v>420</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>387</v>
       </c>
-      <c r="E33" s="87" t="s">
-        <v>609</v>
-      </c>
       <c r="F33" s="84" t="s">
-        <v>440</v>
-      </c>
-      <c r="J33" s="2" t="s">
-        <v>383</v>
-      </c>
-      <c r="K33" s="2" t="s">
-        <v>467</v>
-      </c>
-      <c r="L33" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="J33" s="82" t="s">
+        <v>365</v>
+      </c>
+      <c r="K33" s="82" t="s">
+        <v>549</v>
+      </c>
+      <c r="L33" s="82" t="s">
         <v>387</v>
       </c>
-      <c r="M33" s="2" t="s">
-        <v>468</v>
-      </c>
-      <c r="N33" s="2" t="s">
+      <c r="M33" s="82" t="s">
+        <v>539</v>
+      </c>
+      <c r="N33" s="82"/>
+      <c r="P33" s="82" t="s">
+        <v>544</v>
+      </c>
+      <c r="Q33" s="82" t="s">
+        <v>546</v>
+      </c>
+      <c r="R33" s="82" t="s">
+        <v>382</v>
+      </c>
+      <c r="S33" s="82" t="s">
+        <v>374</v>
+      </c>
+      <c r="T33" s="82" t="s">
+        <v>539</v>
+      </c>
+      <c r="V33" s="2"/>
+    </row>
+    <row r="34" spans="1:22" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="B34" s="2" t="s">
+        <v>629</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>630</v>
+      </c>
+      <c r="E34" s="87" t="b">
+        <v>0</v>
+      </c>
+      <c r="F34" s="84" t="s">
         <v>366</v>
       </c>
-      <c r="P33" s="2" t="s">
-        <v>527</v>
-      </c>
-      <c r="Q33" s="2" t="s">
-        <v>502</v>
-      </c>
-      <c r="R33" s="2" t="s">
-        <v>466</v>
-      </c>
-      <c r="S33" s="2" t="s">
-        <v>367</v>
-      </c>
-      <c r="T33" s="2" t="s">
-        <v>468</v>
-      </c>
-      <c r="V33" s="2"/>
-    </row>
-    <row r="34" spans="2:22" ht="71.25" x14ac:dyDescent="0.45">
-      <c r="B34" s="2" t="s">
-        <v>517</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>387</v>
-      </c>
-      <c r="E34" s="87">
-        <v>14.8</v>
-      </c>
-      <c r="F34" s="84" t="s">
-        <v>440</v>
-      </c>
-      <c r="J34" s="2" t="s">
-        <v>383</v>
-      </c>
-      <c r="K34" s="2" t="s">
-        <v>363</v>
-      </c>
-      <c r="L34" s="2" t="s">
-        <v>387</v>
-      </c>
-      <c r="M34" s="2" t="s">
-        <v>469</v>
-      </c>
-      <c r="N34" s="2" t="s">
+      <c r="J34" s="82" t="s">
+        <v>365</v>
+      </c>
+      <c r="K34" s="82" t="s">
+        <v>631</v>
+      </c>
+      <c r="L34" s="82" t="s">
+        <v>404</v>
+      </c>
+      <c r="M34" s="82" t="s">
+        <v>630</v>
+      </c>
+      <c r="N34" s="82" t="s">
         <v>366</v>
       </c>
-      <c r="P34" s="2" t="s">
-        <v>528</v>
-      </c>
-      <c r="Q34" s="2" t="s">
-        <v>503</v>
-      </c>
-      <c r="R34" s="2" t="s">
-        <v>382</v>
-      </c>
-      <c r="S34" s="2" t="s">
-        <v>374</v>
-      </c>
-      <c r="T34" s="2" t="s">
-        <v>504</v>
+      <c r="O34" s="82"/>
+      <c r="P34" s="82" t="s">
+        <v>632</v>
+      </c>
+      <c r="Q34" s="82" t="s">
+        <v>536</v>
+      </c>
+      <c r="R34" s="82" t="s">
+        <v>633</v>
+      </c>
+      <c r="S34" s="82" t="s">
+        <v>537</v>
+      </c>
+      <c r="T34" s="82" t="s">
+        <v>630</v>
       </c>
       <c r="V34" s="2"/>
     </row>
-    <row r="35" spans="2:22" ht="99.75" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:22" ht="85.5" x14ac:dyDescent="0.45">
       <c r="B35" s="2" t="s">
-        <v>518</v>
+        <v>417</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>387</v>
-      </c>
-      <c r="E35" s="87">
-        <v>0</v>
+        <v>404</v>
       </c>
       <c r="F35" s="84" t="s">
-        <v>440</v>
-      </c>
-      <c r="J35" s="2" t="s">
-        <v>383</v>
-      </c>
-      <c r="K35" s="2" t="s">
-        <v>505</v>
-      </c>
-      <c r="L35" s="2" t="s">
-        <v>387</v>
-      </c>
-      <c r="M35" s="2" t="s">
-        <v>506</v>
-      </c>
-      <c r="N35" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="P35" s="2" t="s">
-        <v>529</v>
-      </c>
-      <c r="Q35" s="2" t="s">
-        <v>502</v>
-      </c>
-      <c r="R35" s="2" t="s">
-        <v>507</v>
-      </c>
-      <c r="S35" s="2" t="s">
-        <v>367</v>
-      </c>
-      <c r="T35" s="2" t="s">
-        <v>508</v>
+      <c r="J35" s="82" t="s">
+        <v>365</v>
+      </c>
+      <c r="K35" s="82" t="s">
+        <v>547</v>
+      </c>
+      <c r="L35" s="82" t="s">
+        <v>404</v>
+      </c>
+      <c r="M35" s="82" t="s">
+        <v>540</v>
+      </c>
+      <c r="N35" s="82"/>
+      <c r="P35" s="82" t="s">
+        <v>541</v>
+      </c>
+      <c r="Q35" s="82" t="s">
+        <v>536</v>
+      </c>
+      <c r="R35" s="82" t="s">
+        <v>542</v>
+      </c>
+      <c r="S35" s="82" t="s">
+        <v>537</v>
+      </c>
+      <c r="T35" s="82" t="s">
+        <v>540</v>
       </c>
       <c r="V35" s="2"/>
     </row>
-    <row r="36" spans="2:22" ht="85.5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:22" ht="99.75" x14ac:dyDescent="0.45">
+      <c r="A36" s="2" t="s">
+        <v>418</v>
+      </c>
       <c r="B36" s="2" t="s">
-        <v>612</v>
+        <v>419</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>387</v>
       </c>
-      <c r="E36" s="87" t="s">
-        <v>408</v>
-      </c>
       <c r="F36" s="84" t="s">
-        <v>440</v>
+        <v>366</v>
       </c>
       <c r="J36" s="82" t="s">
-        <v>519</v>
+        <v>365</v>
       </c>
       <c r="K36" s="82" t="s">
-        <v>509</v>
+        <v>548</v>
       </c>
       <c r="L36" s="82" t="s">
         <v>387</v>
       </c>
       <c r="M36" s="82" t="s">
-        <v>511</v>
-      </c>
-      <c r="N36" s="82" t="s">
-        <v>366</v>
-      </c>
-      <c r="O36" s="82"/>
+        <v>538</v>
+      </c>
+      <c r="N36" s="82"/>
       <c r="P36" s="82" t="s">
-        <v>530</v>
+        <v>543</v>
       </c>
       <c r="Q36" s="82" t="s">
-        <v>512</v>
+        <v>545</v>
       </c>
       <c r="R36" s="82" t="s">
-        <v>520</v>
+        <v>382</v>
       </c>
       <c r="S36" s="82" t="s">
-        <v>521</v>
+        <v>374</v>
       </c>
       <c r="T36" s="82" t="s">
-        <v>511</v>
+        <v>538</v>
       </c>
       <c r="V36" s="2"/>
     </row>
-    <row r="37" spans="2:22" ht="85.5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:22" ht="99.75" x14ac:dyDescent="0.45">
       <c r="B37" s="2" t="s">
-        <v>639</v>
+        <v>433</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>404</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>640</v>
-      </c>
-      <c r="E37" s="87" t="b">
-        <v>0</v>
+        <v>387</v>
       </c>
       <c r="F37" s="84" t="s">
         <v>366</v>
       </c>
-      <c r="J37" s="82" t="s">
-        <v>365</v>
-      </c>
-      <c r="K37" s="82" t="s">
-        <v>641</v>
-      </c>
-      <c r="L37" s="82" t="s">
-        <v>404</v>
-      </c>
-      <c r="M37" s="82" t="s">
-        <v>640</v>
-      </c>
-      <c r="N37" s="82" t="s">
+      <c r="J37" s="2" t="s">
+        <v>447</v>
+      </c>
+      <c r="K37" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="L37" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="M37" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="N37" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="O37" s="82"/>
-      <c r="P37" s="82" t="s">
-        <v>642</v>
-      </c>
-      <c r="Q37" s="82" t="s">
-        <v>542</v>
-      </c>
-      <c r="R37" s="82" t="s">
-        <v>643</v>
-      </c>
-      <c r="S37" s="82" t="s">
-        <v>543</v>
-      </c>
-      <c r="T37" s="82" t="s">
-        <v>640</v>
+      <c r="P37" s="2" t="s">
+        <v>648</v>
+      </c>
+      <c r="Q37" s="2" t="s">
+        <v>495</v>
+      </c>
+      <c r="R37" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="S37" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="T37" s="2" t="s">
+        <v>496</v>
       </c>
       <c r="V37" s="2"/>
     </row>
-    <row r="38" spans="2:22" ht="142.5" x14ac:dyDescent="0.45">
-      <c r="J38" s="2" t="s">
-        <v>383</v>
-      </c>
-      <c r="K38" s="2" t="s">
-        <v>610</v>
-      </c>
-      <c r="L38" s="2" t="s">
+    <row r="38" spans="1:22" ht="57" x14ac:dyDescent="0.45">
+      <c r="B38" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="E38" s="87">
+        <v>9999999</v>
+      </c>
+      <c r="F38" s="84" t="s">
+        <v>366</v>
+      </c>
+      <c r="J38" s="82" t="s">
+        <v>554</v>
+      </c>
+      <c r="K38" s="82" t="s">
+        <v>553</v>
+      </c>
+      <c r="L38" s="82" t="s">
         <v>387</v>
       </c>
-      <c r="M38" s="2" t="s">
-        <v>616</v>
-      </c>
-      <c r="N38" s="2" t="s">
+      <c r="M38" s="82" t="s">
+        <v>550</v>
+      </c>
+      <c r="N38" s="85" t="s">
         <v>366</v>
       </c>
-      <c r="P38" s="2" t="s">
-        <v>618</v>
-      </c>
-      <c r="Q38" s="2" t="s">
-        <v>512</v>
-      </c>
-      <c r="R38" s="2" t="s">
-        <v>617</v>
-      </c>
-      <c r="S38" s="2" t="s">
+      <c r="P38" s="82" t="s">
+        <v>579</v>
+      </c>
+      <c r="Q38" s="82" t="s">
+        <v>475</v>
+      </c>
+      <c r="R38" s="82" t="s">
+        <v>580</v>
+      </c>
+      <c r="S38" s="82" t="s">
         <v>374</v>
       </c>
-      <c r="T38" s="2" t="s">
-        <v>616</v>
+      <c r="T38" s="82" t="s">
+        <v>581</v>
       </c>
       <c r="V38" s="2"/>
     </row>
-    <row r="39" spans="2:22" ht="409.5" hidden="1" x14ac:dyDescent="0.45">
-      <c r="J39" s="2" t="s">
-        <v>454</v>
-      </c>
-      <c r="K39" s="2" t="s">
-        <v>611</v>
-      </c>
-      <c r="L39" s="2" t="s">
+    <row r="39" spans="1:22" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="B39" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>557</v>
+      </c>
+      <c r="E39" s="87" t="s">
+        <v>599</v>
+      </c>
+      <c r="F39" s="84" t="s">
+        <v>366</v>
+      </c>
+      <c r="J39" s="82" t="s">
+        <v>554</v>
+      </c>
+      <c r="K39" s="82" t="s">
+        <v>570</v>
+      </c>
+      <c r="L39" s="82" t="s">
         <v>387</v>
       </c>
-      <c r="M39" s="2" t="s">
-        <v>621</v>
-      </c>
-      <c r="N39" s="2" t="s">
-        <v>499</v>
-      </c>
-      <c r="P39" s="2" t="s">
-        <v>620</v>
-      </c>
-      <c r="Q39" s="2" t="s">
-        <v>512</v>
-      </c>
-      <c r="R39" s="2" t="s">
-        <v>619</v>
-      </c>
-      <c r="S39" s="2" t="s">
-        <v>374</v>
-      </c>
-      <c r="T39" s="2" t="s">
-        <v>621</v>
+      <c r="M39" s="82" t="s">
+        <v>572</v>
+      </c>
+      <c r="N39" s="85" t="s">
+        <v>366</v>
+      </c>
+      <c r="P39" s="82" t="s">
+        <v>585</v>
+      </c>
+      <c r="Q39" s="82" t="s">
+        <v>587</v>
+      </c>
+      <c r="R39" s="82" t="s">
+        <v>562</v>
+      </c>
+      <c r="S39" s="82" t="s">
+        <v>479</v>
+      </c>
+      <c r="T39" s="82" t="s">
+        <v>572</v>
       </c>
       <c r="V39" s="2"/>
     </row>
-    <row r="40" spans="2:22" ht="99.75" hidden="1" x14ac:dyDescent="0.45">
-      <c r="J40" s="2" t="s">
-        <v>484</v>
-      </c>
-      <c r="K40" s="2" t="s">
-        <v>613</v>
-      </c>
-      <c r="L40" s="2" t="s">
+    <row r="40" spans="1:22" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="B40" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>555</v>
+      </c>
+      <c r="E40" s="88">
+        <v>45566</v>
+      </c>
+      <c r="F40" s="84" t="s">
+        <v>366</v>
+      </c>
+      <c r="J40" s="82" t="s">
+        <v>554</v>
+      </c>
+      <c r="K40" s="82" t="s">
+        <v>568</v>
+      </c>
+      <c r="L40" s="82" t="s">
+        <v>394</v>
+      </c>
+      <c r="M40" s="82" t="s">
+        <v>555</v>
+      </c>
+      <c r="N40" s="85" t="s">
+        <v>366</v>
+      </c>
+      <c r="P40" s="82" t="s">
+        <v>582</v>
+      </c>
+      <c r="Q40" s="82" t="s">
+        <v>583</v>
+      </c>
+      <c r="R40" s="82" t="s">
+        <v>379</v>
+      </c>
+      <c r="S40" s="82" t="s">
+        <v>380</v>
+      </c>
+      <c r="T40" s="82" t="s">
+        <v>555</v>
+      </c>
+      <c r="V40" s="2"/>
+    </row>
+    <row r="41" spans="1:22" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="B41" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>556</v>
+      </c>
+      <c r="E41" s="87" t="s">
+        <v>598</v>
+      </c>
+      <c r="F41" s="84" t="s">
+        <v>366</v>
+      </c>
+      <c r="J41" s="82" t="s">
+        <v>554</v>
+      </c>
+      <c r="K41" s="82" t="s">
+        <v>569</v>
+      </c>
+      <c r="L41" s="82" t="s">
         <v>387</v>
       </c>
-      <c r="M40" s="2" t="s">
-        <v>623</v>
-      </c>
-      <c r="N40" s="2" t="s">
+      <c r="M41" s="82" t="s">
+        <v>571</v>
+      </c>
+      <c r="N41" s="85" t="s">
         <v>366</v>
       </c>
-      <c r="P40" s="2" t="s">
-        <v>624</v>
-      </c>
-      <c r="Q40" s="2" t="s">
-        <v>625</v>
-      </c>
-      <c r="R40" s="2" t="s">
-        <v>622</v>
-      </c>
-      <c r="S40" s="2" t="s">
-        <v>374</v>
-      </c>
-      <c r="T40" s="2" t="s">
-        <v>630</v>
-      </c>
-      <c r="V40" s="2"/>
-    </row>
-    <row r="41" spans="2:22" ht="114" hidden="1" x14ac:dyDescent="0.45">
-      <c r="J41" s="2" t="s">
-        <v>484</v>
-      </c>
-      <c r="K41" s="2" t="s">
-        <v>614</v>
-      </c>
-      <c r="L41" s="2" t="s">
-        <v>615</v>
-      </c>
-      <c r="M41" s="2" t="s">
-        <v>629</v>
-      </c>
-      <c r="N41" s="2" t="s">
-        <v>499</v>
-      </c>
-      <c r="P41" s="2" t="s">
-        <v>628</v>
-      </c>
-      <c r="Q41" s="2" t="s">
-        <v>625</v>
-      </c>
-      <c r="R41" s="2" t="s">
-        <v>626</v>
-      </c>
-      <c r="S41" s="2" t="s">
-        <v>627</v>
-      </c>
-      <c r="T41" s="2" t="s">
-        <v>631</v>
+      <c r="P41" s="82" t="s">
+        <v>584</v>
+      </c>
+      <c r="Q41" s="82" t="s">
+        <v>586</v>
+      </c>
+      <c r="R41" s="82" t="s">
+        <v>588</v>
+      </c>
+      <c r="S41" s="82" t="s">
+        <v>479</v>
+      </c>
+      <c r="T41" s="82" t="s">
+        <v>571</v>
       </c>
       <c r="V41" s="2"/>
     </row>
-    <row r="42" spans="2:22" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:22" x14ac:dyDescent="0.45">
       <c r="V42" s="2"/>
     </row>
-    <row r="43" spans="2:22" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:22" x14ac:dyDescent="0.45">
       <c r="V43" s="2"/>
     </row>
-    <row r="44" spans="2:22" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:22" x14ac:dyDescent="0.45">
       <c r="V44" s="2"/>
     </row>
-    <row r="45" spans="2:22" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:22" x14ac:dyDescent="0.45">
       <c r="V45" s="2"/>
     </row>
-    <row r="46" spans="2:22" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:22" x14ac:dyDescent="0.45">
       <c r="V46" s="2"/>
     </row>
-    <row r="47" spans="2:22" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:22" x14ac:dyDescent="0.45">
       <c r="V47" s="2"/>
     </row>
-    <row r="48" spans="2:22" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:22" x14ac:dyDescent="0.45">
       <c r="V48" s="2"/>
     </row>
     <row r="49" spans="22:22" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
Complete schemas and instance
</commit_message>
<xml_diff>
--- a/schemas/ChargeFiling_iepd/artifacts/ChargeFiling_MappingSpreadsheet.xlsx
+++ b/schemas/ChargeFiling_iepd/artifacts/ChargeFiling_MappingSpreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JamesCabral\git\JTMP-Data-Exchange-Specs\schemas\ChargeFiling_iepd\artifacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0847D1D0-9D21-4EF6-9829-6AB3786F9AE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD75C440-E7A6-46B9-A2FB-5025BB798305}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10718" yWindow="0" windowWidth="10965" windowHeight="13763" tabRatio="781" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" tabRatio="781" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="9" state="hidden" r:id="rId1"/>
@@ -149,7 +149,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1076" uniqueCount="651">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1088" uniqueCount="655">
   <si>
     <t>Definition</t>
   </si>
@@ -2408,9 +2408,6 @@
     <t>nola-ext:ChargeDispositionCode</t>
   </si>
   <si>
-    <t>nola-ext:ChargeDispositionCodeType</t>
-  </si>
-  <si>
     <t>j:Arrest/nc:ActivityDate/nc:DateTime</t>
   </si>
   <si>
@@ -2600,36 +2597,15 @@
     <t>nc:DateType (nola-ext:ProsecutorCaseScreenedDate)</t>
   </si>
   <si>
-    <t>nola-ext:ProsecutorCase/nola-ext:ProsecutorCaseScreenedPerson/nc:PersonName</t>
-  </si>
-  <si>
-    <t>nola-ext:ProsecutorCase/nola-ext:ProsecutorCaseReviewedPerson/nc:PersonName</t>
-  </si>
-  <si>
-    <t>nc:PersonType (nola-ext:ProsecutorCaseScreenedPerson)</t>
-  </si>
-  <si>
-    <t>nc:PersonType (nola-ext:ProsecutorCaseReviewedPerson)</t>
-  </si>
-  <si>
     <t>nc:PersonName</t>
   </si>
   <si>
     <t>Example</t>
   </si>
   <si>
-    <t>Parish of Orleans</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
     <t>M999999</t>
   </si>
   <si>
-    <t>Doe</t>
-  </si>
-  <si>
     <t>John</t>
   </si>
   <si>
@@ -2642,12 +2618,6 @@
     <t>M</t>
   </si>
   <si>
-    <t>James Smith</t>
-  </si>
-  <si>
-    <t>John Smith</t>
-  </si>
-  <si>
     <t>6TH DISTRICT CASE</t>
   </si>
   <si>
@@ -2688,9 +2658,6 @@
   </si>
   <si>
     <t>nola-ext:StatewideATNChargeSequenceID</t>
-  </si>
-  <si>
-    <t>j:Arrest/j:ArrestCharge/nola-ext:ChargeAugmentation/nola-ext:ATNChargeSequenceNumber</t>
   </si>
   <si>
     <t>A sequential identifier number assigned to the arrest of a subject i.e ATN. The State's Police Automated Fingerprint Inforamtion System (AFIS) generates an ATN to uniquely identify each booking event, often referred to as an Arrest Cycle. The ATN must be communicated from the Sheriff to the Court at a minimum, in order to effectively update the State computerized criminal history (CCH) with dispositions of arrest charges.</t>
@@ -2799,7 +2766,52 @@
     <t>j:Arrest/j:ArrestCharge/nola-ext:ChargeAugmentation/nola-ext:StatewideArrestTrackingNumber</t>
   </si>
   <si>
-    <t>j:Arrest/nola-ext:ArrestAugmentation/nola-ext:OffenseDate</t>
+    <t>j:Arrest/j:ArrestCharge/nola-ext:ChargeAugmentation/nola-ext:StatewideATNChargeSequenceNumber</t>
+  </si>
+  <si>
+    <t>j:Arrest/j:ArrestCharge/nola-ext:ChargeAugmentation/nola-ext:OffenseDate</t>
+  </si>
+  <si>
+    <t>nola-ext:ProsecutorCase/nola-ext:ProsecutorCaseReviewedByPerson/nc:PersonName</t>
+  </si>
+  <si>
+    <t>nola-ext:ProsecutorCase/nola-ext:ProsecutorCaseScreenedByPerson/nc:PersonName</t>
+  </si>
+  <si>
+    <t>nc:PersonType (nola-ext:ProsecutorCaseScreenedByPerson)</t>
+  </si>
+  <si>
+    <t>nc:PersonType (nola-ext:ProsecutorCaseReviewedByPerson)</t>
+  </si>
+  <si>
+    <t>accepted</t>
+  </si>
+  <si>
+    <t>Charge Key</t>
+  </si>
+  <si>
+    <t>Orleans</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>Smith</t>
+  </si>
+  <si>
+    <t>James</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Brown</t>
+  </si>
+  <si>
+    <t>John Q Smith</t>
+  </si>
+  <si>
+    <t>James T Smith</t>
   </si>
 </sst>
 </file>
@@ -7384,10 +7396,10 @@
   <dimension ref="A1:AB49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="N5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C29" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P7" sqref="P7"/>
+      <selection pane="bottomRight" activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -7433,7 +7445,7 @@
         <v>0</v>
       </c>
       <c r="E1" s="86" t="s">
-        <v>589</v>
+        <v>584</v>
       </c>
       <c r="F1" s="83" t="s">
         <v>439</v>
@@ -7502,54 +7514,60 @@
         <v>403</v>
       </c>
     </row>
-    <row r="2" spans="1:28" ht="409.5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:28" ht="99.75" x14ac:dyDescent="0.45">
       <c r="B2" s="2" t="s">
-        <v>513</v>
+        <v>517</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>430</v>
+        <v>387</v>
       </c>
       <c r="E2" s="87">
-        <v>12345678</v>
+        <v>0</v>
       </c>
       <c r="F2" s="84" t="s">
         <v>440</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>454</v>
+        <v>383</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>463</v>
+        <v>504</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>387</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>462</v>
+        <v>505</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>366</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>649</v>
+        <v>524</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>501</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>464</v>
+        <v>506</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>374</v>
+        <v>367</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>507</v>
       </c>
       <c r="V2" s="2"/>
     </row>
-    <row r="3" spans="1:28" ht="99.75" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:28" ht="42.75" x14ac:dyDescent="0.45">
       <c r="B3" s="2" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>387</v>
       </c>
-      <c r="E3" s="87">
-        <v>0</v>
+      <c r="E3" s="87" t="s">
+        <v>592</v>
       </c>
       <c r="F3" s="84" t="s">
         <v>440</v>
@@ -7558,43 +7576,40 @@
         <v>383</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>504</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>387</v>
+        <v>458</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>505</v>
+        <v>457</v>
       </c>
       <c r="N3" s="2" t="s">
         <v>366</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="Q3" s="2" t="s">
         <v>501</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>506</v>
+        <v>465</v>
       </c>
       <c r="S3" s="2" t="s">
         <v>367</v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>507</v>
+        <v>457</v>
       </c>
       <c r="V3" s="2"/>
     </row>
-    <row r="4" spans="1:28" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:28" ht="228" x14ac:dyDescent="0.45">
       <c r="B4" s="2" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>387</v>
       </c>
       <c r="E4" s="87" t="s">
-        <v>602</v>
+        <v>593</v>
       </c>
       <c r="F4" s="84" t="s">
         <v>440</v>
@@ -7603,40 +7618,43 @@
         <v>383</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>458</v>
+        <v>467</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>387</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>457</v>
+        <v>468</v>
       </c>
       <c r="N4" s="2" t="s">
         <v>366</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>523</v>
+        <v>629</v>
       </c>
       <c r="Q4" s="2" t="s">
         <v>501</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="S4" s="2" t="s">
         <v>367</v>
       </c>
       <c r="T4" s="2" t="s">
-        <v>457</v>
+        <v>468</v>
       </c>
       <c r="V4" s="2"/>
     </row>
-    <row r="5" spans="1:28" ht="228" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:28" ht="71.25" x14ac:dyDescent="0.45">
       <c r="B5" s="2" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>387</v>
       </c>
-      <c r="E5" s="87" t="s">
-        <v>603</v>
+      <c r="E5" s="87">
+        <v>14.8</v>
       </c>
       <c r="F5" s="84" t="s">
         <v>440</v>
@@ -7645,278 +7663,278 @@
         <v>383</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>467</v>
+        <v>363</v>
       </c>
       <c r="L5" s="2" t="s">
         <v>387</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="N5" s="2" t="s">
         <v>366</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>640</v>
+        <v>523</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>466</v>
+        <v>382</v>
       </c>
       <c r="S5" s="2" t="s">
-        <v>367</v>
+        <v>374</v>
       </c>
       <c r="T5" s="2" t="s">
-        <v>468</v>
+        <v>503</v>
       </c>
       <c r="V5" s="2"/>
     </row>
-    <row r="6" spans="1:28" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:28" ht="85.5" x14ac:dyDescent="0.45">
       <c r="B6" s="2" t="s">
-        <v>516</v>
+        <v>596</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>387</v>
       </c>
-      <c r="E6" s="87">
-        <v>14.8</v>
+      <c r="E6" s="87" t="s">
+        <v>645</v>
       </c>
       <c r="F6" s="84" t="s">
         <v>440</v>
       </c>
-      <c r="J6" s="2" t="s">
-        <v>383</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>363</v>
-      </c>
-      <c r="L6" s="2" t="s">
+      <c r="J6" s="82" t="s">
+        <v>518</v>
+      </c>
+      <c r="K6" s="82" t="s">
+        <v>508</v>
+      </c>
+      <c r="L6" s="82" t="s">
         <v>387</v>
       </c>
-      <c r="M6" s="2" t="s">
-        <v>469</v>
-      </c>
-      <c r="N6" s="2" t="s">
+      <c r="M6" s="82" t="s">
+        <v>510</v>
+      </c>
+      <c r="N6" s="82" t="s">
         <v>366</v>
       </c>
-      <c r="P6" s="2" t="s">
-        <v>524</v>
-      </c>
-      <c r="Q6" s="2" t="s">
-        <v>502</v>
-      </c>
-      <c r="R6" s="2" t="s">
-        <v>382</v>
+      <c r="O6" s="82"/>
+      <c r="P6" s="82" t="s">
+        <v>525</v>
+      </c>
+      <c r="Q6" s="82" t="s">
+        <v>511</v>
+      </c>
+      <c r="R6" s="82" t="s">
+        <v>519</v>
       </c>
       <c r="S6" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="T6" s="2" t="s">
-        <v>503</v>
+      <c r="T6" s="82" t="s">
+        <v>510</v>
       </c>
       <c r="V6" s="2"/>
     </row>
-    <row r="7" spans="1:28" ht="57" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:28" ht="142.5" x14ac:dyDescent="0.45">
       <c r="B7" s="2" t="s">
-        <v>436</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>394</v>
-      </c>
-      <c r="E7" s="88">
-        <v>45505</v>
-      </c>
-      <c r="F7" s="84" t="s">
-        <v>366</v>
+        <v>646</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>389</v>
+        <v>594</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>394</v>
+        <v>387</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>391</v>
+        <v>600</v>
       </c>
       <c r="N7" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="P7" s="82" t="s">
-        <v>650</v>
+      <c r="P7" s="2" t="s">
+        <v>602</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>499</v>
+        <v>511</v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>379</v>
+        <v>601</v>
       </c>
       <c r="S7" s="2" t="s">
-        <v>380</v>
+        <v>374</v>
       </c>
       <c r="T7" s="2" t="s">
-        <v>391</v>
+        <v>600</v>
       </c>
       <c r="V7" s="2"/>
     </row>
-    <row r="8" spans="1:28" ht="409.5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:28" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="B8" s="2" t="s">
+        <v>512</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="E8" s="87" t="s">
+        <v>591</v>
+      </c>
+      <c r="F8" s="84" t="s">
+        <v>440</v>
+      </c>
       <c r="J8" s="2" t="s">
-        <v>454</v>
+        <v>383</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>605</v>
+        <v>460</v>
       </c>
       <c r="L8" s="2" t="s">
         <v>387</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>615</v>
+        <v>459</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>498</v>
+        <v>366</v>
       </c>
       <c r="P8" s="2" t="s">
+        <v>521</v>
+      </c>
+      <c r="Q8" s="2" t="s">
         <v>614</v>
       </c>
-      <c r="Q8" s="2" t="s">
-        <v>511</v>
-      </c>
       <c r="R8" s="2" t="s">
-        <v>613</v>
+        <v>382</v>
       </c>
       <c r="S8" s="2" t="s">
-        <v>374</v>
+        <v>461</v>
       </c>
       <c r="T8" s="2" t="s">
-        <v>615</v>
+        <v>459</v>
       </c>
       <c r="V8" s="2"/>
     </row>
-    <row r="9" spans="1:28" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:28" ht="71.25" x14ac:dyDescent="0.45">
       <c r="B9" s="2" t="s">
-        <v>606</v>
+        <v>436</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>387</v>
-      </c>
-      <c r="E9" s="87" t="s">
-        <v>408</v>
+        <v>394</v>
+      </c>
+      <c r="E9" s="88">
+        <v>45505</v>
       </c>
       <c r="F9" s="84" t="s">
+        <v>366</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="P9" s="82" t="s">
+        <v>640</v>
+      </c>
+      <c r="Q9" s="2" t="s">
+        <v>499</v>
+      </c>
+      <c r="R9" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="S9" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="T9" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="V9" s="2"/>
+    </row>
+    <row r="10" spans="1:28" ht="409.5" x14ac:dyDescent="0.45">
+      <c r="B10" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="E10" s="87">
+        <v>12345678</v>
+      </c>
+      <c r="F10" s="84" t="s">
         <v>440</v>
       </c>
-      <c r="J9" s="82" t="s">
-        <v>518</v>
-      </c>
-      <c r="K9" s="82" t="s">
-        <v>508</v>
-      </c>
-      <c r="L9" s="82" t="s">
-        <v>387</v>
-      </c>
-      <c r="M9" s="82" t="s">
-        <v>510</v>
-      </c>
-      <c r="N9" s="82" t="s">
-        <v>366</v>
-      </c>
-      <c r="O9" s="82"/>
-      <c r="P9" s="82" t="s">
-        <v>526</v>
-      </c>
-      <c r="Q9" s="82" t="s">
-        <v>511</v>
-      </c>
-      <c r="R9" s="82" t="s">
-        <v>519</v>
-      </c>
-      <c r="S9" s="82" t="s">
-        <v>520</v>
-      </c>
-      <c r="T9" s="82" t="s">
-        <v>510</v>
-      </c>
-      <c r="V9" s="2"/>
-    </row>
-    <row r="10" spans="1:28" ht="142.5" x14ac:dyDescent="0.45">
       <c r="J10" s="2" t="s">
-        <v>383</v>
+        <v>454</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>604</v>
+        <v>463</v>
       </c>
       <c r="L10" s="2" t="s">
         <v>387</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>610</v>
+        <v>462</v>
       </c>
       <c r="N10" s="2" t="s">
         <v>366</v>
       </c>
       <c r="P10" s="2" t="s">
-        <v>612</v>
-      </c>
-      <c r="Q10" s="2" t="s">
-        <v>511</v>
+        <v>638</v>
       </c>
       <c r="R10" s="2" t="s">
-        <v>611</v>
+        <v>464</v>
       </c>
       <c r="S10" s="2" t="s">
         <v>374</v>
       </c>
       <c r="T10" s="2" t="s">
-        <v>610</v>
+        <v>462</v>
       </c>
       <c r="V10" s="2"/>
     </row>
-    <row r="11" spans="1:28" ht="85.5" x14ac:dyDescent="0.45">
-      <c r="B11" s="2" t="s">
-        <v>512</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>387</v>
-      </c>
-      <c r="E11" s="87" t="s">
-        <v>601</v>
-      </c>
-      <c r="F11" s="84" t="s">
-        <v>440</v>
-      </c>
+    <row r="11" spans="1:28" ht="409.5" x14ac:dyDescent="0.45">
       <c r="J11" s="2" t="s">
-        <v>383</v>
+        <v>454</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>460</v>
+        <v>595</v>
       </c>
       <c r="L11" s="2" t="s">
         <v>387</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>459</v>
+        <v>604</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>366</v>
+        <v>498</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>522</v>
+        <v>639</v>
       </c>
       <c r="Q11" s="2" t="s">
-        <v>625</v>
+        <v>511</v>
       </c>
       <c r="R11" s="2" t="s">
-        <v>382</v>
+        <v>603</v>
       </c>
       <c r="S11" s="2" t="s">
-        <v>461</v>
+        <v>374</v>
       </c>
       <c r="T11" s="2" t="s">
-        <v>459</v>
+        <v>604</v>
       </c>
       <c r="V11" s="2"/>
     </row>
@@ -7949,7 +7967,7 @@
         <v>366</v>
       </c>
       <c r="P12" s="82" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="Q12" s="2" t="s">
         <v>497</v>
@@ -7976,7 +7994,7 @@
         <v>409</v>
       </c>
       <c r="E13" s="87" t="s">
-        <v>591</v>
+        <v>408</v>
       </c>
       <c r="F13" s="84" t="s">
         <v>366</v>
@@ -7985,31 +8003,31 @@
         <v>454</v>
       </c>
       <c r="K13" s="82" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="L13" s="82" t="s">
         <v>509</v>
       </c>
       <c r="M13" s="82" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="N13" s="82">
         <v>1</v>
       </c>
       <c r="P13" s="82" t="s">
-        <v>641</v>
+        <v>630</v>
       </c>
       <c r="Q13" s="82" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="R13" s="82" t="s">
+        <v>528</v>
+      </c>
+      <c r="S13" s="82" t="s">
         <v>529</v>
       </c>
-      <c r="S13" s="82" t="s">
-        <v>530</v>
-      </c>
       <c r="T13" s="82" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="V13" s="2"/>
     </row>
@@ -8023,6 +8041,9 @@
       <c r="D14" s="2" t="s">
         <v>411</v>
       </c>
+      <c r="E14" s="87" t="s">
+        <v>410</v>
+      </c>
       <c r="F14" s="84" t="s">
         <v>366</v>
       </c>
@@ -8030,31 +8051,31 @@
         <v>454</v>
       </c>
       <c r="K14" s="82" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="L14" s="82" t="s">
         <v>509</v>
       </c>
       <c r="M14" s="82" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="N14" s="82">
         <v>1</v>
       </c>
       <c r="P14" s="82" t="s">
-        <v>641</v>
+        <v>630</v>
       </c>
       <c r="Q14" s="82" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="R14" s="82" t="s">
+        <v>528</v>
+      </c>
+      <c r="S14" s="82" t="s">
         <v>529</v>
       </c>
-      <c r="S14" s="82" t="s">
-        <v>530</v>
-      </c>
       <c r="T14" s="82" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="V14" s="2"/>
     </row>
@@ -8065,6 +8086,9 @@
       <c r="C15" s="2" t="s">
         <v>404</v>
       </c>
+      <c r="E15" s="87" t="s">
+        <v>412</v>
+      </c>
       <c r="F15" s="84" t="s">
         <v>366</v>
       </c>
@@ -8072,31 +8096,31 @@
         <v>454</v>
       </c>
       <c r="K15" s="82" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="L15" s="82" t="s">
         <v>509</v>
       </c>
       <c r="M15" s="82" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="N15" s="82">
         <v>1</v>
       </c>
       <c r="P15" s="82" t="s">
-        <v>641</v>
+        <v>630</v>
       </c>
       <c r="Q15" s="82" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="R15" s="82" t="s">
+        <v>528</v>
+      </c>
+      <c r="S15" s="82" t="s">
         <v>529</v>
       </c>
-      <c r="S15" s="82" t="s">
-        <v>530</v>
-      </c>
       <c r="T15" s="82" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="V15" s="2"/>
     </row>
@@ -8110,6 +8134,9 @@
       <c r="C16" s="2" t="s">
         <v>404</v>
       </c>
+      <c r="E16" s="87" t="s">
+        <v>416</v>
+      </c>
       <c r="F16" s="84" t="s">
         <v>366</v>
       </c>
@@ -8117,119 +8144,121 @@
         <v>454</v>
       </c>
       <c r="K16" s="82" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="L16" s="82" t="s">
         <v>509</v>
       </c>
       <c r="M16" s="82" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="N16" s="82">
         <v>1</v>
       </c>
       <c r="P16" s="82" t="s">
-        <v>641</v>
+        <v>630</v>
       </c>
       <c r="Q16" s="82" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="R16" s="82" t="s">
+        <v>528</v>
+      </c>
+      <c r="S16" s="82" t="s">
         <v>529</v>
       </c>
-      <c r="S16" s="82" t="s">
-        <v>530</v>
-      </c>
       <c r="T16" s="82" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="V16" s="2"/>
     </row>
-    <row r="17" spans="2:22" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:22" ht="142.5" x14ac:dyDescent="0.45">
       <c r="B17" s="2" t="s">
+        <v>512</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="E17" s="87" t="s">
+        <v>591</v>
+      </c>
+      <c r="F17" s="84" t="s">
+        <v>440</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>612</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>613</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>616</v>
+      </c>
+      <c r="N17" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="P17" s="82" t="s">
+        <v>632</v>
+      </c>
+      <c r="Q17" s="82" t="s">
+        <v>615</v>
+      </c>
+      <c r="R17" s="82" t="s">
+        <v>382</v>
+      </c>
+      <c r="S17" s="82" t="s">
+        <v>461</v>
+      </c>
+      <c r="T17" s="82" t="s">
+        <v>617</v>
+      </c>
+      <c r="V17" s="2"/>
+    </row>
+    <row r="18" spans="2:22" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="B18" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C18" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="E17" s="88">
+      <c r="E18" s="88">
         <v>45505</v>
       </c>
-      <c r="F17" s="84">
+      <c r="F18" s="84">
         <v>1</v>
       </c>
-      <c r="J17" s="82" t="s">
+      <c r="J18" s="82" t="s">
         <v>454</v>
       </c>
-      <c r="K17" s="82" t="s">
+      <c r="K18" s="82" t="s">
+        <v>532</v>
+      </c>
+      <c r="L18" s="82" t="s">
+        <v>394</v>
+      </c>
+      <c r="M18" s="82" t="s">
         <v>533</v>
       </c>
-      <c r="L17" s="82" t="s">
-        <v>394</v>
-      </c>
-      <c r="M17" s="82" t="s">
+      <c r="N18" s="82">
+        <v>1</v>
+      </c>
+      <c r="P18" s="82" t="s">
+        <v>631</v>
+      </c>
+      <c r="Q18" s="82" t="s">
         <v>534</v>
       </c>
-      <c r="N17" s="82"/>
-      <c r="P17" s="82" t="s">
-        <v>642</v>
-      </c>
-      <c r="Q17" s="82" t="s">
-        <v>535</v>
-      </c>
-      <c r="R17" s="82" t="s">
+      <c r="R18" s="82" t="s">
         <v>379</v>
       </c>
-      <c r="S17" s="82" t="s">
+      <c r="S18" s="82" t="s">
         <v>380</v>
       </c>
-      <c r="T17" s="82" t="s">
-        <v>534</v>
-      </c>
-      <c r="V17" s="2"/>
-    </row>
-    <row r="18" spans="2:22" ht="142.5" x14ac:dyDescent="0.45">
-      <c r="B18" s="2" t="s">
-        <v>512</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>387</v>
-      </c>
-      <c r="E18" s="87" t="s">
-        <v>601</v>
-      </c>
-      <c r="F18" s="84" t="s">
-        <v>440</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>623</v>
-      </c>
-      <c r="K18" s="2" t="s">
-        <v>624</v>
-      </c>
-      <c r="L18" s="2" t="s">
-        <v>387</v>
-      </c>
-      <c r="M18" s="2" t="s">
-        <v>627</v>
-      </c>
-      <c r="N18" s="2" t="s">
-        <v>366</v>
-      </c>
-      <c r="P18" s="82" t="s">
-        <v>643</v>
-      </c>
-      <c r="Q18" s="82" t="s">
-        <v>626</v>
-      </c>
-      <c r="R18" s="82" t="s">
-        <v>382</v>
-      </c>
-      <c r="S18" s="82" t="s">
-        <v>461</v>
-      </c>
       <c r="T18" s="82" t="s">
-        <v>628</v>
+        <v>533</v>
       </c>
       <c r="V18" s="2"/>
     </row>
@@ -8241,7 +8270,7 @@
         <v>387</v>
       </c>
       <c r="E19" s="87" t="s">
-        <v>590</v>
+        <v>647</v>
       </c>
       <c r="F19" s="84">
         <v>1</v>
@@ -8328,31 +8357,31 @@
         <v>484</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>607</v>
+        <v>597</v>
       </c>
       <c r="L21" s="2" t="s">
         <v>387</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>617</v>
+        <v>606</v>
       </c>
       <c r="N21" s="2" t="s">
         <v>366</v>
       </c>
       <c r="P21" s="2" t="s">
-        <v>618</v>
+        <v>607</v>
       </c>
       <c r="Q21" s="2" t="s">
-        <v>619</v>
+        <v>608</v>
       </c>
       <c r="R21" s="2" t="s">
-        <v>616</v>
+        <v>605</v>
       </c>
       <c r="S21" s="2" t="s">
         <v>374</v>
       </c>
       <c r="T21" s="2" t="s">
-        <v>621</v>
+        <v>610</v>
       </c>
       <c r="V21" s="2"/>
     </row>
@@ -8364,7 +8393,7 @@
         <v>426</v>
       </c>
       <c r="E22" s="87" t="s">
-        <v>595</v>
+        <v>587</v>
       </c>
       <c r="F22" s="84">
         <v>1</v>
@@ -8406,52 +8435,52 @@
         <v>484</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>608</v>
+        <v>598</v>
       </c>
       <c r="L23" s="2" t="s">
+        <v>599</v>
+      </c>
+      <c r="M23" s="2" t="s">
         <v>609</v>
-      </c>
-      <c r="M23" s="2" t="s">
-        <v>620</v>
       </c>
       <c r="N23" s="2" t="s">
         <v>498</v>
       </c>
       <c r="P23" s="2" t="s">
-        <v>644</v>
+        <v>633</v>
       </c>
       <c r="Q23" s="2" t="s">
-        <v>647</v>
+        <v>636</v>
       </c>
       <c r="R23" s="2" t="s">
-        <v>645</v>
+        <v>634</v>
       </c>
       <c r="S23" s="2" t="s">
-        <v>646</v>
+        <v>635</v>
       </c>
       <c r="T23" s="2" t="s">
-        <v>622</v>
+        <v>611</v>
       </c>
       <c r="V23" s="2"/>
     </row>
     <row r="24" spans="2:22" ht="71.25" x14ac:dyDescent="0.45">
       <c r="B24" s="2" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>357</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="F24" s="84" t="s">
         <v>498</v>
       </c>
       <c r="J24" s="2" t="s">
+        <v>557</v>
+      </c>
+      <c r="K24" s="2" t="s">
         <v>558</v>
-      </c>
-      <c r="K24" s="2" t="s">
-        <v>559</v>
       </c>
       <c r="L24" s="2" t="s">
         <v>387</v>
@@ -8463,19 +8492,19 @@
         <v>498</v>
       </c>
       <c r="P24" s="2" t="s">
+        <v>559</v>
+      </c>
+      <c r="Q24" s="2" t="s">
         <v>560</v>
       </c>
-      <c r="Q24" s="2" t="s">
-        <v>561</v>
-      </c>
       <c r="R24" s="2" t="s">
-        <v>588</v>
+        <v>583</v>
       </c>
       <c r="S24" s="2" t="s">
         <v>479</v>
       </c>
       <c r="T24" s="2" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="V24" s="2"/>
     </row>
@@ -8486,8 +8515,11 @@
       <c r="C25" s="2" t="s">
         <v>387</v>
       </c>
+      <c r="D25" s="2" t="s">
+        <v>586</v>
+      </c>
       <c r="E25" s="87" t="s">
-        <v>594</v>
+        <v>650</v>
       </c>
       <c r="F25" s="84">
         <v>1</v>
@@ -8531,6 +8563,12 @@
       <c r="C26" s="2" t="s">
         <v>387</v>
       </c>
+      <c r="D26" s="2" t="s">
+        <v>648</v>
+      </c>
+      <c r="E26" s="87" t="s">
+        <v>651</v>
+      </c>
       <c r="F26" s="84" t="s">
         <v>366</v>
       </c>
@@ -8573,8 +8611,11 @@
       <c r="C27" s="2" t="s">
         <v>387</v>
       </c>
+      <c r="D27" s="2" t="s">
+        <v>649</v>
+      </c>
       <c r="E27" s="87" t="s">
-        <v>593</v>
+        <v>652</v>
       </c>
       <c r="F27" s="84">
         <v>1</v>
@@ -8613,64 +8654,58 @@
     </row>
     <row r="28" spans="2:22" ht="99.75" x14ac:dyDescent="0.45">
       <c r="B28" s="2" t="s">
-        <v>423</v>
+        <v>433</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>387</v>
       </c>
-      <c r="D28" s="2" t="s">
-        <v>422</v>
-      </c>
-      <c r="E28" s="87" t="s">
-        <v>596</v>
-      </c>
       <c r="F28" s="84" t="s">
         <v>366</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="L28" s="2" t="s">
-        <v>395</v>
+        <v>387</v>
       </c>
       <c r="M28" s="2" t="s">
-        <v>376</v>
+        <v>381</v>
       </c>
       <c r="N28" s="2" t="s">
         <v>366</v>
       </c>
       <c r="P28" s="2" t="s">
-        <v>634</v>
+        <v>637</v>
       </c>
       <c r="Q28" s="2" t="s">
-        <v>493</v>
+        <v>495</v>
       </c>
       <c r="R28" s="2" t="s">
-        <v>635</v>
+        <v>382</v>
       </c>
       <c r="S28" s="2" t="s">
-        <v>637</v>
+        <v>374</v>
       </c>
       <c r="T28" s="2" t="s">
-        <v>376</v>
+        <v>496</v>
       </c>
       <c r="V28" s="2"/>
     </row>
-    <row r="29" spans="2:22" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:22" ht="99.75" x14ac:dyDescent="0.45">
       <c r="B29" s="2" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>387</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>428</v>
+        <v>422</v>
       </c>
       <c r="E29" s="87" t="s">
-        <v>597</v>
+        <v>588</v>
       </c>
       <c r="F29" s="84" t="s">
         <v>366</v>
@@ -8679,224 +8714,226 @@
         <v>448</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="L29" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M29" s="2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="N29" s="2" t="s">
         <v>366</v>
       </c>
       <c r="P29" s="2" t="s">
-        <v>639</v>
+        <v>623</v>
       </c>
       <c r="Q29" s="2" t="s">
         <v>493</v>
       </c>
       <c r="R29" s="2" t="s">
-        <v>636</v>
+        <v>624</v>
       </c>
       <c r="S29" s="2" t="s">
-        <v>638</v>
+        <v>626</v>
       </c>
       <c r="T29" s="2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="V29" s="2"/>
     </row>
-    <row r="30" spans="2:22" ht="142.5" x14ac:dyDescent="0.45">
+    <row r="30" spans="2:22" ht="71.25" x14ac:dyDescent="0.45">
       <c r="B30" s="2" t="s">
-        <v>435</v>
+        <v>427</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>430</v>
+        <v>387</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>470</v>
-      </c>
-      <c r="E30" s="87">
-        <v>999999</v>
+        <v>428</v>
+      </c>
+      <c r="E30" s="87" t="s">
+        <v>589</v>
       </c>
       <c r="F30" s="84" t="s">
         <v>366</v>
       </c>
-      <c r="J30" s="82" t="s">
+      <c r="J30" s="2" t="s">
+        <v>448</v>
+      </c>
+      <c r="K30" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="L30" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="M30" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="N30" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="P30" s="2" t="s">
+        <v>628</v>
+      </c>
+      <c r="Q30" s="2" t="s">
+        <v>493</v>
+      </c>
+      <c r="R30" s="2" t="s">
+        <v>625</v>
+      </c>
+      <c r="S30" s="2" t="s">
+        <v>627</v>
+      </c>
+      <c r="T30" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="V30" s="2"/>
+    </row>
+    <row r="31" spans="2:22" ht="133.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B31" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>470</v>
+      </c>
+      <c r="E31" s="87">
+        <v>999999</v>
+      </c>
+      <c r="F31" s="84" t="s">
+        <v>366</v>
+      </c>
+      <c r="J31" s="82" t="s">
+        <v>565</v>
+      </c>
+      <c r="K31" s="82" t="s">
         <v>566</v>
       </c>
-      <c r="K30" s="82" t="s">
-        <v>567</v>
-      </c>
-      <c r="L30" s="82" t="s">
+      <c r="L31" s="82" t="s">
         <v>387</v>
       </c>
-      <c r="M30" s="82" t="s">
+      <c r="M31" s="82" t="s">
         <v>470</v>
       </c>
-      <c r="N30" s="85" t="s">
+      <c r="N31" s="85" t="s">
         <v>366</v>
       </c>
-      <c r="P30" s="82" t="s">
-        <v>565</v>
-      </c>
-      <c r="Q30" s="82" t="s">
+      <c r="P31" s="82" t="s">
         <v>564</v>
       </c>
-      <c r="R30" s="82" t="s">
+      <c r="Q31" s="82" t="s">
+        <v>563</v>
+      </c>
+      <c r="R31" s="82" t="s">
         <v>382</v>
       </c>
-      <c r="S30" s="82" t="s">
+      <c r="S31" s="82" t="s">
         <v>374</v>
       </c>
-      <c r="T30" s="82" t="s">
+      <c r="T31" s="82" t="s">
         <v>470</v>
       </c>
-      <c r="V30" s="2"/>
-    </row>
-    <row r="31" spans="2:22" ht="28.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B31" s="2" t="s">
+      <c r="V31" s="2"/>
+    </row>
+    <row r="32" spans="2:22" ht="128.25" x14ac:dyDescent="0.45">
+      <c r="B32" s="2" t="s">
         <v>421</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>387</v>
-      </c>
-      <c r="E31" s="87" t="s">
-        <v>592</v>
-      </c>
-      <c r="F31" s="84">
-        <v>1</v>
-      </c>
-      <c r="J31" s="2" t="s">
-        <v>365</v>
-      </c>
-      <c r="K31" s="2" t="s">
-        <v>453</v>
-      </c>
-      <c r="L31" s="2" t="s">
-        <v>387</v>
-      </c>
-      <c r="M31" s="2" t="s">
-        <v>372</v>
-      </c>
-      <c r="N31" s="2" t="s">
-        <v>366</v>
-      </c>
-      <c r="P31" s="2" t="s">
-        <v>474</v>
-      </c>
-      <c r="Q31" s="2" t="s">
-        <v>475</v>
-      </c>
-      <c r="R31" s="2" t="s">
-        <v>375</v>
-      </c>
-      <c r="S31" s="2" t="s">
-        <v>374</v>
-      </c>
-      <c r="T31" s="2" t="s">
-        <v>476</v>
-      </c>
-      <c r="V31" s="2"/>
-    </row>
-    <row r="32" spans="2:22" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="B32" s="2" t="s">
-        <v>438</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>387</v>
       </c>
       <c r="E32" s="87" t="s">
-        <v>600</v>
-      </c>
-      <c r="F32" s="84" t="s">
-        <v>366</v>
+        <v>585</v>
+      </c>
+      <c r="F32" s="84">
+        <v>1</v>
       </c>
       <c r="J32" s="2" t="s">
         <v>365</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>574</v>
+        <v>453</v>
       </c>
       <c r="L32" s="2" t="s">
         <v>387</v>
       </c>
       <c r="M32" s="2" t="s">
-        <v>573</v>
+        <v>372</v>
       </c>
       <c r="N32" s="2" t="s">
         <v>366</v>
       </c>
       <c r="P32" s="2" t="s">
-        <v>575</v>
+        <v>474</v>
       </c>
       <c r="Q32" s="2" t="s">
-        <v>576</v>
+        <v>475</v>
       </c>
       <c r="R32" s="2" t="s">
-        <v>577</v>
+        <v>375</v>
       </c>
       <c r="S32" s="2" t="s">
-        <v>367</v>
+        <v>374</v>
       </c>
       <c r="T32" s="2" t="s">
-        <v>578</v>
+        <v>476</v>
       </c>
       <c r="V32" s="2"/>
     </row>
-    <row r="33" spans="1:22" ht="99.75" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:22" ht="42.75" x14ac:dyDescent="0.45">
       <c r="B33" s="2" t="s">
-        <v>420</v>
+        <v>438</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>387</v>
       </c>
+      <c r="E33" s="87" t="s">
+        <v>590</v>
+      </c>
       <c r="F33" s="84" t="s">
         <v>366</v>
       </c>
-      <c r="J33" s="82" t="s">
+      <c r="J33" s="2" t="s">
         <v>365</v>
       </c>
-      <c r="K33" s="82" t="s">
-        <v>549</v>
-      </c>
-      <c r="L33" s="82" t="s">
+      <c r="K33" s="2" t="s">
+        <v>573</v>
+      </c>
+      <c r="L33" s="2" t="s">
         <v>387</v>
       </c>
-      <c r="M33" s="82" t="s">
-        <v>539</v>
-      </c>
-      <c r="N33" s="82"/>
-      <c r="P33" s="82" t="s">
-        <v>544</v>
-      </c>
-      <c r="Q33" s="82" t="s">
-        <v>546</v>
-      </c>
-      <c r="R33" s="82" t="s">
-        <v>382</v>
-      </c>
-      <c r="S33" s="82" t="s">
-        <v>374</v>
-      </c>
-      <c r="T33" s="82" t="s">
-        <v>539</v>
+      <c r="M33" s="2" t="s">
+        <v>572</v>
+      </c>
+      <c r="N33" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="P33" s="2" t="s">
+        <v>574</v>
+      </c>
+      <c r="Q33" s="2" t="s">
+        <v>575</v>
+      </c>
+      <c r="R33" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="S33" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="T33" s="2" t="s">
+        <v>577</v>
       </c>
       <c r="V33" s="2"/>
     </row>
-    <row r="34" spans="1:22" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:22" ht="99.75" x14ac:dyDescent="0.45">
       <c r="B34" s="2" t="s">
-        <v>629</v>
+        <v>420</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>404</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>630</v>
-      </c>
-      <c r="E34" s="87" t="b">
-        <v>0</v>
+        <v>387</v>
       </c>
       <c r="F34" s="84" t="s">
         <v>366</v>
@@ -8905,42 +8942,47 @@
         <v>365</v>
       </c>
       <c r="K34" s="82" t="s">
-        <v>631</v>
+        <v>548</v>
       </c>
       <c r="L34" s="82" t="s">
-        <v>404</v>
+        <v>387</v>
       </c>
       <c r="M34" s="82" t="s">
-        <v>630</v>
+        <v>538</v>
       </c>
       <c r="N34" s="82" t="s">
         <v>366</v>
       </c>
-      <c r="O34" s="82"/>
       <c r="P34" s="82" t="s">
-        <v>632</v>
+        <v>543</v>
       </c>
       <c r="Q34" s="82" t="s">
-        <v>536</v>
+        <v>545</v>
       </c>
       <c r="R34" s="82" t="s">
-        <v>633</v>
+        <v>382</v>
       </c>
       <c r="S34" s="82" t="s">
-        <v>537</v>
+        <v>374</v>
       </c>
       <c r="T34" s="82" t="s">
-        <v>630</v>
+        <v>538</v>
       </c>
       <c r="V34" s="2"/>
     </row>
     <row r="35" spans="1:22" ht="85.5" x14ac:dyDescent="0.45">
       <c r="B35" s="2" t="s">
-        <v>417</v>
+        <v>618</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>404</v>
       </c>
+      <c r="D35" s="2" t="s">
+        <v>619</v>
+      </c>
+      <c r="E35" s="87" t="b">
+        <v>0</v>
+      </c>
       <c r="F35" s="84" t="s">
         <v>366</v>
       </c>
@@ -8948,41 +8990,41 @@
         <v>365</v>
       </c>
       <c r="K35" s="82" t="s">
-        <v>547</v>
+        <v>620</v>
       </c>
       <c r="L35" s="82" t="s">
         <v>404</v>
       </c>
       <c r="M35" s="82" t="s">
-        <v>540</v>
-      </c>
-      <c r="N35" s="82"/>
+        <v>619</v>
+      </c>
+      <c r="N35" s="82" t="s">
+        <v>366</v>
+      </c>
+      <c r="O35" s="82"/>
       <c r="P35" s="82" t="s">
-        <v>541</v>
+        <v>621</v>
       </c>
       <c r="Q35" s="82" t="s">
+        <v>535</v>
+      </c>
+      <c r="R35" s="82" t="s">
+        <v>622</v>
+      </c>
+      <c r="S35" s="82" t="s">
         <v>536</v>
       </c>
-      <c r="R35" s="82" t="s">
-        <v>542</v>
-      </c>
-      <c r="S35" s="82" t="s">
-        <v>537</v>
-      </c>
       <c r="T35" s="82" t="s">
-        <v>540</v>
+        <v>619</v>
       </c>
       <c r="V35" s="2"/>
     </row>
-    <row r="36" spans="1:22" ht="99.75" x14ac:dyDescent="0.45">
-      <c r="A36" s="2" t="s">
-        <v>418</v>
-      </c>
+    <row r="36" spans="1:22" ht="85.5" x14ac:dyDescent="0.45">
       <c r="B36" s="2" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>387</v>
+        <v>404</v>
       </c>
       <c r="F36" s="84" t="s">
         <v>366</v>
@@ -8991,35 +9033,40 @@
         <v>365</v>
       </c>
       <c r="K36" s="82" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="L36" s="82" t="s">
-        <v>387</v>
+        <v>404</v>
       </c>
       <c r="M36" s="82" t="s">
-        <v>538</v>
-      </c>
-      <c r="N36" s="82"/>
+        <v>539</v>
+      </c>
+      <c r="N36" s="82" t="s">
+        <v>366</v>
+      </c>
       <c r="P36" s="82" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="Q36" s="82" t="s">
-        <v>545</v>
+        <v>535</v>
       </c>
       <c r="R36" s="82" t="s">
-        <v>382</v>
+        <v>541</v>
       </c>
       <c r="S36" s="82" t="s">
-        <v>374</v>
+        <v>536</v>
       </c>
       <c r="T36" s="82" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="V36" s="2"/>
     </row>
     <row r="37" spans="1:22" ht="99.75" x14ac:dyDescent="0.45">
+      <c r="A37" s="2" t="s">
+        <v>418</v>
+      </c>
       <c r="B37" s="2" t="s">
-        <v>433</v>
+        <v>419</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>387</v>
@@ -9027,35 +9074,35 @@
       <c r="F37" s="84" t="s">
         <v>366</v>
       </c>
-      <c r="J37" s="2" t="s">
-        <v>447</v>
-      </c>
-      <c r="K37" s="2" t="s">
-        <v>360</v>
-      </c>
-      <c r="L37" s="2" t="s">
+      <c r="J37" s="82" t="s">
+        <v>365</v>
+      </c>
+      <c r="K37" s="82" t="s">
+        <v>547</v>
+      </c>
+      <c r="L37" s="82" t="s">
         <v>387</v>
       </c>
-      <c r="M37" s="2" t="s">
-        <v>381</v>
-      </c>
-      <c r="N37" s="2" t="s">
+      <c r="M37" s="82" t="s">
+        <v>537</v>
+      </c>
+      <c r="N37" s="82" t="s">
         <v>366</v>
       </c>
-      <c r="P37" s="2" t="s">
-        <v>648</v>
-      </c>
-      <c r="Q37" s="2" t="s">
-        <v>495</v>
-      </c>
-      <c r="R37" s="2" t="s">
+      <c r="P37" s="82" t="s">
+        <v>542</v>
+      </c>
+      <c r="Q37" s="82" t="s">
+        <v>544</v>
+      </c>
+      <c r="R37" s="82" t="s">
         <v>382</v>
       </c>
-      <c r="S37" s="2" t="s">
+      <c r="S37" s="82" t="s">
         <v>374</v>
       </c>
-      <c r="T37" s="2" t="s">
-        <v>496</v>
+      <c r="T37" s="82" t="s">
+        <v>537</v>
       </c>
       <c r="V37" s="2"/>
     </row>
@@ -9067,7 +9114,7 @@
         <v>430</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="E38" s="87">
         <v>9999999</v>
@@ -9076,34 +9123,34 @@
         <v>366</v>
       </c>
       <c r="J38" s="82" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="K38" s="82" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="L38" s="82" t="s">
         <v>387</v>
       </c>
       <c r="M38" s="82" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="N38" s="85" t="s">
         <v>366</v>
       </c>
       <c r="P38" s="82" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="Q38" s="82" t="s">
         <v>475</v>
       </c>
       <c r="R38" s="82" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="S38" s="82" t="s">
         <v>374</v>
       </c>
       <c r="T38" s="82" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="V38" s="2"/>
     </row>
@@ -9115,43 +9162,43 @@
         <v>357</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="E39" s="87" t="s">
-        <v>599</v>
+        <v>653</v>
       </c>
       <c r="F39" s="84" t="s">
         <v>366</v>
       </c>
       <c r="J39" s="82" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="K39" s="82" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="L39" s="82" t="s">
         <v>387</v>
       </c>
       <c r="M39" s="82" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="N39" s="85" t="s">
         <v>366</v>
       </c>
       <c r="P39" s="82" t="s">
-        <v>585</v>
+        <v>641</v>
       </c>
       <c r="Q39" s="82" t="s">
-        <v>587</v>
+        <v>644</v>
       </c>
       <c r="R39" s="82" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="S39" s="82" t="s">
         <v>479</v>
       </c>
       <c r="T39" s="82" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="V39" s="2"/>
     </row>
@@ -9163,7 +9210,7 @@
         <v>394</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="E40" s="88">
         <v>45566</v>
@@ -9172,25 +9219,25 @@
         <v>366</v>
       </c>
       <c r="J40" s="82" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="K40" s="82" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="L40" s="82" t="s">
         <v>394</v>
       </c>
       <c r="M40" s="82" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="N40" s="85" t="s">
         <v>366</v>
       </c>
       <c r="P40" s="82" t="s">
+        <v>581</v>
+      </c>
+      <c r="Q40" s="82" t="s">
         <v>582</v>
-      </c>
-      <c r="Q40" s="82" t="s">
-        <v>583</v>
       </c>
       <c r="R40" s="82" t="s">
         <v>379</v>
@@ -9199,7 +9246,7 @@
         <v>380</v>
       </c>
       <c r="T40" s="82" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="V40" s="2"/>
     </row>
@@ -9211,43 +9258,43 @@
         <v>357</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="E41" s="87" t="s">
-        <v>598</v>
+        <v>654</v>
       </c>
       <c r="F41" s="84" t="s">
         <v>366</v>
       </c>
       <c r="J41" s="82" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="K41" s="82" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="L41" s="82" t="s">
         <v>387</v>
       </c>
       <c r="M41" s="82" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="N41" s="85" t="s">
         <v>366</v>
       </c>
       <c r="P41" s="82" t="s">
-        <v>584</v>
+        <v>642</v>
       </c>
       <c r="Q41" s="82" t="s">
-        <v>586</v>
+        <v>643</v>
       </c>
       <c r="R41" s="82" t="s">
-        <v>588</v>
+        <v>583</v>
       </c>
       <c r="S41" s="82" t="s">
         <v>479</v>
       </c>
       <c r="T41" s="82" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="V41" s="2"/>
     </row>
@@ -9277,7 +9324,7 @@
     </row>
   </sheetData>
   <phoneticPr fontId="19" type="noConversion"/>
-  <dataValidations count="3">
+  <dataValidations disablePrompts="1" count="3">
     <dataValidation errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1" xr:uid="{00000000-0002-0000-0300-000000000000}"/>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid value" error="Valid property styles are &quot;element&quot;, &quot;attribute&quot;, or &quot;abstract&quot;.  Leave the cell blank to use the default value &quot;element&quot;." promptTitle="Property Style" prompt="- &quot;element&quot; or blank (default) - Represents a typical NIEM property._x000a_- &quot;abstract&quot; - Used to create a substitution group_x000a_- &quot;attribute&quot; - Use sparingly, if at all; for values tightly-coupled to an element." sqref="X50:X1048576 W2:W41" xr:uid="{00000000-0002-0000-0300-000002000000}">
       <formula1>"element,attribute,abstract"</formula1>

</xml_diff>

<commit_message>
Added DocumentBinary to UniformCommitmentOrder and ChargeFiling
</commit_message>
<xml_diff>
--- a/schemas/ChargeFiling_iepd/artifacts/ChargeFiling_MappingSpreadsheet.xlsx
+++ b/schemas/ChargeFiling_iepd/artifacts/ChargeFiling_MappingSpreadsheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28526"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mcp911gov-my.sharepoint.com/personal/jimpingel_missioncriticalpartners_com/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JamesCabral\git\JTMP-Data-Exchange-Specs\schemas\ChargeFiling_iepd\artifacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{BD75C440-E7A6-46B9-A2FB-5025BB798305}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A861E288-2FAC-4CA4-83BA-92B9A9B544F6}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F1CC14B-EF9C-48D7-BCAA-2BBD869654AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2220" yWindow="1830" windowWidth="25005" windowHeight="15015" tabRatio="781" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-4080" yWindow="-21720" windowWidth="51840" windowHeight="21120" tabRatio="781" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="9" state="hidden" r:id="rId1"/>
@@ -26,7 +26,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Codes | Facets'!$A$1:$M$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7">Namespace!$A$1:$N$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Property!$A$1:$W$41</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Property!$A$1:$W$47</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4">Type!$A$1:$L$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5">'Type-Has-Property'!$A$1:$P$1</definedName>
     <definedName name="CODES_NamespaceStyle">'Field Descriptions'!$B$165:$B$176</definedName>
@@ -139,7 +139,7 @@
     <definedName name="Type_Target_NamespacePrefix">Type!$H$1</definedName>
     <definedName name="Type_Target_Style">Type!$L$1</definedName>
   </definedNames>
-  <calcPr calcId="191028" calcOnSave="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -163,7 +163,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1088" uniqueCount="655">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1168" uniqueCount="687">
   <si>
     <t xml:space="preserve">Template last updated: </t>
   </si>
@@ -2826,6 +2826,102 @@
   </si>
   <si>
     <t xml:space="preserve">Literal </t>
+  </si>
+  <si>
+    <t>Attachment</t>
+  </si>
+  <si>
+    <t>A binary attachment to a report or document.</t>
+  </si>
+  <si>
+    <t>nc:DocumentBinary</t>
+  </si>
+  <si>
+    <t>AtachmentSize</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>A size of a binary object in kilobytes.</t>
+  </si>
+  <si>
+    <t>nc:BinarySizeValue</t>
+  </si>
+  <si>
+    <t>nc:NonNegativeDecimalType</t>
+  </si>
+  <si>
+    <t>AttachmentFormat</t>
+  </si>
+  <si>
+    <t>A file format or content type of a binary object.</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>nc:BinaryFormatText</t>
+  </si>
+  <si>
+    <t>AttachmentID</t>
+  </si>
+  <si>
+    <t>An identifier that references a binary object.</t>
+  </si>
+  <si>
+    <t>nc:BinaryID</t>
+  </si>
+  <si>
+    <t>AttachmentURI</t>
+  </si>
+  <si>
+    <t>As-is Process.URI</t>
+  </si>
+  <si>
+    <t>A URL or file reference of a binary object.</t>
+  </si>
+  <si>
+    <t>nc:BinaryURI</t>
+  </si>
+  <si>
+    <t>niem-xs:anyURI</t>
+  </si>
+  <si>
+    <t>BinaryObject</t>
+  </si>
+  <si>
+    <t>As-is Process.Object</t>
+  </si>
+  <si>
+    <t>A base64 binary encoding of data.</t>
+  </si>
+  <si>
+    <t>nc:Base64BinaryObject</t>
+  </si>
+  <si>
+    <t>niem-xs:base64Binary</t>
+  </si>
+  <si>
+    <t>binary object</t>
+  </si>
+  <si>
+    <t>nc:Document/nc:DocumentBinary/</t>
+  </si>
+  <si>
+    <t>nc:Document/nc:DocumentBinary/nc:BinarySizeValue</t>
+  </si>
+  <si>
+    <t>nc:Document/nc:DocumentBinarync:BinaryFormatText</t>
+  </si>
+  <si>
+    <t>nc:Document/nc:DocumentBinary/nc:BinaryID</t>
+  </si>
+  <si>
+    <t>nc:Document/nc:DocumentBinary/nc:BinaryURI</t>
+  </si>
+  <si>
+    <t>nc:Document/nc:DocumentBinarync:Base64BinaryObject</t>
   </si>
 </sst>
 </file>
@@ -3192,7 +3288,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3440,6 +3536,9 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="71">
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
@@ -4762,8 +4861,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table3" displayName="Table3" ref="A1:Z41" totalsRowShown="0" headerRowDxfId="107" dataDxfId="106" headerRowCellStyle="Accent2">
-  <autoFilter ref="A1:Z41" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table3" displayName="Table3" ref="A1:Z47" totalsRowShown="0" headerRowDxfId="107" dataDxfId="106" headerRowCellStyle="Accent2">
+  <autoFilter ref="A1:Z47" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Z41">
     <sortCondition ref="P1:P41"/>
   </sortState>
@@ -5163,14 +5262,14 @@
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="28.7109375" style="17" customWidth="1"/>
-    <col min="2" max="2" width="51.28515625" style="17" customWidth="1"/>
+    <col min="1" max="1" width="28.73046875" style="17" customWidth="1"/>
+    <col min="2" max="2" width="51.265625" style="17" customWidth="1"/>
     <col min="3" max="4" width="35" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" s="81" t="s">
         <v>0</v>
       </c>
@@ -5178,21 +5277,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" s="16"/>
       <c r="B2" s="16"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" s="27" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="28"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" s="28"/>
       <c r="B4" s="28"/>
     </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A5" s="29" t="s">
         <v>3</v>
       </c>
@@ -5206,7 +5305,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" s="30" t="s">
         <v>7</v>
       </c>
@@ -5220,7 +5319,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" s="30" t="s">
         <v>11</v>
       </c>
@@ -5234,7 +5333,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" s="30" t="s">
         <v>15</v>
       </c>
@@ -5248,7 +5347,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" s="30" t="s">
         <v>18</v>
       </c>
@@ -5262,7 +5361,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A10" s="30" t="s">
         <v>21</v>
       </c>
@@ -5276,7 +5375,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" s="30" t="s">
         <v>24</v>
       </c>
@@ -5290,7 +5389,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" s="30" t="s">
         <v>27</v>
       </c>
@@ -5304,7 +5403,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" s="30" t="s">
         <v>31</v>
       </c>
@@ -5318,15 +5417,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" s="28"/>
       <c r="B14" s="28"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" s="28"/>
       <c r="B15" s="28"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" s="28" t="s">
         <v>34</v>
       </c>
@@ -5335,7 +5434,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A18" s="29" t="s">
         <v>36</v>
       </c>
@@ -5349,7 +5448,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A19" s="31" t="s">
         <v>37</v>
       </c>
@@ -5363,7 +5462,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A20" s="31" t="s">
         <v>41</v>
       </c>
@@ -5377,7 +5476,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A21" s="31" t="s">
         <v>45</v>
       </c>
@@ -5391,7 +5490,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A22" s="31" t="s">
         <v>49</v>
       </c>
@@ -5405,7 +5504,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A23" s="31" t="s">
         <v>52</v>
       </c>
@@ -5419,7 +5518,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A24" s="31" t="s">
         <v>56</v>
       </c>
@@ -5433,7 +5532,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A25" s="31" t="s">
         <v>60</v>
       </c>
@@ -5447,7 +5546,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A26" s="31" t="s">
         <v>63</v>
       </c>
@@ -5461,7 +5560,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A27" s="31" t="s">
         <v>67</v>
       </c>
@@ -5475,7 +5574,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A28" s="31" t="s">
         <v>71</v>
       </c>
@@ -5489,7 +5588,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A31" s="29" t="s">
         <v>75</v>
       </c>
@@ -5497,7 +5596,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A32" s="5" t="s">
         <v>76</v>
       </c>
@@ -5505,7 +5604,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" ht="57" x14ac:dyDescent="0.45">
       <c r="A33" s="5" t="s">
         <v>78</v>
       </c>
@@ -5513,7 +5612,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A34" s="5" t="s">
         <v>80</v>
       </c>
@@ -5521,7 +5620,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A35" s="5" t="s">
         <v>82</v>
       </c>
@@ -5529,7 +5628,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A36" s="5" t="s">
         <v>84</v>
       </c>
@@ -5537,7 +5636,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A37" s="5" t="s">
         <v>86</v>
       </c>
@@ -5545,7 +5644,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A38" s="5" t="s">
         <v>88</v>
       </c>
@@ -5553,7 +5652,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" ht="99.75" x14ac:dyDescent="0.45">
       <c r="A39" s="30" t="s">
         <v>90</v>
       </c>
@@ -5561,7 +5660,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A40" s="30" t="s">
         <v>92</v>
       </c>
@@ -5587,30 +5686,30 @@
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" style="16" customWidth="1"/>
-    <col min="2" max="2" width="28.7109375" style="17" customWidth="1"/>
+    <col min="1" max="1" width="3.73046875" style="16" customWidth="1"/>
+    <col min="2" max="2" width="28.73046875" style="17" customWidth="1"/>
     <col min="3" max="3" width="76" style="17" customWidth="1"/>
-    <col min="4" max="5" width="29.28515625" style="16" customWidth="1"/>
-    <col min="6" max="16384" width="8.85546875" style="16"/>
+    <col min="4" max="5" width="29.265625" style="16" customWidth="1"/>
+    <col min="6" max="16384" width="8.86328125" style="16"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" s="68" t="s">
         <v>94</v>
       </c>
       <c r="B3" s="68"/>
       <c r="C3" s="68"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" s="38" t="s">
         <v>95</v>
       </c>
       <c r="B4" s="38"/>
       <c r="C4" s="38"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" s="69"/>
       <c r="B5" s="70" t="s">
         <v>96</v>
@@ -5619,7 +5718,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" s="69"/>
       <c r="B6" s="70" t="s">
         <v>98</v>
@@ -5628,7 +5727,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" s="69"/>
       <c r="B7" s="70" t="s">
         <v>100</v>
@@ -5637,7 +5736,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" s="69"/>
       <c r="B8" s="70" t="s">
         <v>4</v>
@@ -5646,7 +5745,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9" s="69"/>
       <c r="B9" s="70" t="s">
         <v>103</v>
@@ -5655,7 +5754,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A10" s="69"/>
       <c r="B10" s="70" t="s">
         <v>105</v>
@@ -5664,7 +5763,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" s="69"/>
       <c r="B11" s="70" t="s">
         <v>107</v>
@@ -5673,14 +5772,14 @@
         <v>108</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12" s="50" t="s">
         <v>109</v>
       </c>
       <c r="B12" s="50"/>
       <c r="C12" s="50"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13" s="69"/>
       <c r="B13" s="70" t="s">
         <v>110</v>
@@ -5689,14 +5788,14 @@
         <v>111</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14" s="69"/>
       <c r="B14" s="70" t="s">
         <v>112</v>
       </c>
       <c r="C14" s="33"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15" s="69"/>
       <c r="B15" s="71" t="s">
         <v>113</v>
@@ -5705,7 +5804,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A16" s="69"/>
       <c r="B16" s="71" t="s">
         <v>115</v>
@@ -5714,7 +5813,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17" s="69"/>
       <c r="B17" s="71" t="s">
         <v>117</v>
@@ -5723,7 +5822,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A18" s="69"/>
       <c r="B18" s="71" t="s">
         <v>119</v>
@@ -5732,7 +5831,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19" s="69"/>
       <c r="B19" s="71" t="s">
         <v>121</v>
@@ -5741,7 +5840,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A20" s="69"/>
       <c r="B20" s="71" t="s">
         <v>71</v>
@@ -5750,7 +5849,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21" s="69"/>
       <c r="B21" s="71" t="s">
         <v>124</v>
@@ -5759,14 +5858,14 @@
         <v>125</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22" s="69"/>
       <c r="B22" s="71" t="s">
         <v>126</v>
       </c>
       <c r="C22" s="33"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A23" s="69"/>
       <c r="B23" s="70" t="s">
         <v>4</v>
@@ -5775,7 +5874,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A24" s="69"/>
       <c r="B24" s="70" t="s">
         <v>128</v>
@@ -5784,7 +5883,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A25" s="69"/>
       <c r="B25" s="70" t="s">
         <v>107</v>
@@ -5793,14 +5892,14 @@
         <v>130</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A26" s="41" t="s">
         <v>131</v>
       </c>
       <c r="B26" s="41"/>
       <c r="C26" s="41"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A27" s="69"/>
       <c r="B27" s="70" t="s">
         <v>132</v>
@@ -5809,7 +5908,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A28" s="69"/>
       <c r="B28" s="70" t="s">
         <v>4</v>
@@ -5818,7 +5917,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A29" s="69"/>
       <c r="B29" s="70" t="s">
         <v>10</v>
@@ -5827,7 +5926,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A30" s="69"/>
       <c r="B30" s="70" t="s">
         <v>103</v>
@@ -5836,7 +5935,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A31" s="69"/>
       <c r="B31" s="70" t="s">
         <v>105</v>
@@ -5845,7 +5944,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A32" s="69"/>
       <c r="B32" s="70" t="s">
         <v>107</v>
@@ -5854,25 +5953,25 @@
         <v>138</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B33" s="16"/>
       <c r="C33" s="16"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A35" s="37" t="s">
         <v>139</v>
       </c>
       <c r="B35" s="37"/>
       <c r="C35" s="37"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A36" s="38" t="s">
         <v>140</v>
       </c>
       <c r="B36" s="38"/>
       <c r="C36" s="38"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A37" s="39"/>
       <c r="B37" s="32" t="s">
         <v>141</v>
@@ -5881,7 +5980,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A38" s="39"/>
       <c r="B38" s="32" t="s">
         <v>143</v>
@@ -5890,7 +5989,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A39" s="39"/>
       <c r="B39" s="32" t="s">
         <v>145</v>
@@ -5899,7 +5998,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A40" s="39"/>
       <c r="B40" s="32" t="s">
         <v>147</v>
@@ -5908,14 +6007,14 @@
         <v>148</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A41" s="50" t="s">
         <v>109</v>
       </c>
       <c r="B41" s="50"/>
       <c r="C41" s="50"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A42" s="40"/>
       <c r="B42" s="33" t="s">
         <v>149</v>
@@ -5924,14 +6023,14 @@
         <v>150</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A43" s="41" t="s">
         <v>151</v>
       </c>
       <c r="B43" s="41"/>
       <c r="C43" s="41"/>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A44" s="42"/>
       <c r="B44" s="32" t="s">
         <v>141</v>
@@ -5940,7 +6039,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A45" s="42"/>
       <c r="B45" s="32" t="s">
         <v>143</v>
@@ -5949,7 +6048,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A46" s="42"/>
       <c r="B46" s="32" t="s">
         <v>152</v>
@@ -5958,7 +6057,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A47" s="42"/>
       <c r="B47" s="32" t="s">
         <v>147</v>
@@ -5967,7 +6066,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A48" s="42"/>
       <c r="B48" s="32" t="s">
         <v>154</v>
@@ -5976,14 +6075,14 @@
         <v>155</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A49" s="42"/>
       <c r="B49" s="32" t="s">
         <v>156</v>
       </c>
       <c r="C49" s="43"/>
     </row>
-    <row r="50" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A50" s="42"/>
       <c r="B50" s="49" t="s">
         <v>157</v>
@@ -5992,7 +6091,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A51" s="42"/>
       <c r="B51" s="49" t="s">
         <v>159</v>
@@ -6001,7 +6100,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A52" s="42"/>
       <c r="B52" s="49" t="s">
         <v>161</v>
@@ -6010,7 +6109,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A53" s="42"/>
       <c r="B53" s="32" t="s">
         <v>163</v>
@@ -6019,7 +6118,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A54" s="42"/>
       <c r="B54" s="32" t="s">
         <v>165</v>
@@ -6028,7 +6127,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A55" s="42"/>
       <c r="B55" s="32" t="s">
         <v>167</v>
@@ -6037,14 +6136,14 @@
         <v>168</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A56" s="52" t="s">
         <v>169</v>
       </c>
       <c r="B56" s="52"/>
       <c r="C56" s="52"/>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A57" s="8"/>
       <c r="B57" s="7" t="s">
         <v>170</v>
@@ -6053,7 +6152,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A58" s="8"/>
       <c r="B58" s="7" t="s">
         <v>172</v>
@@ -6062,7 +6161,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A59" s="8"/>
       <c r="B59" s="7" t="s">
         <v>174</v>
@@ -6071,7 +6170,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A60" s="8"/>
       <c r="B60" s="7" t="s">
         <v>176</v>
@@ -6080,7 +6179,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A61" s="8"/>
       <c r="B61" s="7" t="s">
         <v>178</v>
@@ -6089,36 +6188,36 @@
         <v>179</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A62" s="44"/>
       <c r="B62" s="30"/>
       <c r="C62" s="30"/>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A63" s="44"/>
       <c r="B63" s="30"/>
       <c r="C63" s="30"/>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A64" s="44"/>
       <c r="B64" s="30"/>
       <c r="C64" s="30"/>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A65" s="45" t="s">
         <v>180</v>
       </c>
       <c r="B65" s="46"/>
       <c r="C65" s="47"/>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A66" s="38" t="s">
         <v>140</v>
       </c>
       <c r="B66" s="38"/>
       <c r="C66" s="38"/>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A67" s="39"/>
       <c r="B67" s="32" t="s">
         <v>181</v>
@@ -6127,7 +6226,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A68" s="39"/>
       <c r="B68" s="32" t="s">
         <v>183</v>
@@ -6136,7 +6235,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A69" s="39"/>
       <c r="B69" s="32" t="s">
         <v>185</v>
@@ -6145,7 +6244,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A70" s="39"/>
       <c r="B70" s="32" t="s">
         <v>147</v>
@@ -6154,14 +6253,14 @@
         <v>187</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A71" s="50" t="s">
         <v>109</v>
       </c>
       <c r="B71" s="50"/>
       <c r="C71" s="50"/>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A72" s="40"/>
       <c r="B72" s="33" t="s">
         <v>149</v>
@@ -6170,14 +6269,14 @@
         <v>150</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A73" s="41" t="s">
         <v>151</v>
       </c>
       <c r="B73" s="41"/>
       <c r="C73" s="41"/>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A74" s="40"/>
       <c r="B74" s="32" t="s">
         <v>181</v>
@@ -6186,7 +6285,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A75" s="40"/>
       <c r="B75" s="32" t="s">
         <v>183</v>
@@ -6195,7 +6294,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A76" s="40"/>
       <c r="B76" s="32" t="s">
         <v>147</v>
@@ -6204,7 +6303,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A77" s="40"/>
       <c r="B77" s="32" t="s">
         <v>185</v>
@@ -6213,14 +6312,14 @@
         <v>186</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A78" s="40"/>
       <c r="B78" s="32" t="s">
         <v>188</v>
       </c>
       <c r="C78" s="32"/>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A79" s="40"/>
       <c r="B79" s="49" t="s">
         <v>189</v>
@@ -6229,7 +6328,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A80" s="40"/>
       <c r="B80" s="49" t="s">
         <v>191</v>
@@ -6238,7 +6337,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="81" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A81" s="40"/>
       <c r="B81" s="49" t="s">
         <v>193</v>
@@ -6247,7 +6346,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A82" s="40"/>
       <c r="B82" s="49" t="s">
         <v>195</v>
@@ -6256,7 +6355,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A83" s="40"/>
       <c r="B83" s="49" t="s">
         <v>197</v>
@@ -6265,7 +6364,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A84" s="40"/>
       <c r="B84" s="49" t="s">
         <v>199</v>
@@ -6274,7 +6373,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A85" s="40"/>
       <c r="B85" s="49" t="s">
         <v>201</v>
@@ -6283,7 +6382,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="86" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A86" s="40"/>
       <c r="B86" s="49" t="s">
         <v>203</v>
@@ -6292,7 +6391,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="87" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A87" s="40"/>
       <c r="B87" s="49" t="s">
         <v>205</v>
@@ -6301,7 +6400,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="88" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A88" s="40"/>
       <c r="B88" s="32" t="s">
         <v>207</v>
@@ -6310,7 +6409,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="89" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" ht="57" x14ac:dyDescent="0.45">
       <c r="A89" s="40"/>
       <c r="B89" s="32" t="s">
         <v>209</v>
@@ -6319,7 +6418,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="90" spans="1:3" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" ht="57" hidden="1" x14ac:dyDescent="0.45">
       <c r="A90" s="40"/>
       <c r="B90" s="32" t="s">
         <v>211</v>
@@ -6328,14 +6427,14 @@
         <v>212</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A91" s="52" t="s">
         <v>169</v>
       </c>
       <c r="B91" s="52"/>
       <c r="C91" s="52"/>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A92" s="8"/>
       <c r="B92" s="7" t="s">
         <v>170</v>
@@ -6344,7 +6443,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="93" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A93" s="8"/>
       <c r="B93" s="7" t="s">
         <v>214</v>
@@ -6353,7 +6452,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="94" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A94" s="8"/>
       <c r="B94" s="7" t="s">
         <v>216</v>
@@ -6362,36 +6461,36 @@
         <v>217</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A95" s="44"/>
       <c r="B95" s="30"/>
       <c r="C95" s="30"/>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A96" s="44"/>
       <c r="B96" s="30"/>
       <c r="C96" s="30"/>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A97" s="44"/>
       <c r="B97" s="30"/>
       <c r="C97" s="30"/>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A98" s="45" t="s">
         <v>218</v>
       </c>
       <c r="B98" s="46"/>
       <c r="C98" s="47"/>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A99" s="38" t="s">
         <v>140</v>
       </c>
       <c r="B99" s="38"/>
       <c r="C99" s="38"/>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A100" s="39"/>
       <c r="B100" s="32" t="s">
         <v>219</v>
@@ -6400,7 +6499,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A101" s="39"/>
       <c r="B101" s="32" t="s">
         <v>183</v>
@@ -6409,7 +6508,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A102" s="39"/>
       <c r="B102" s="32" t="s">
         <v>221</v>
@@ -6418,7 +6517,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A103" s="39"/>
       <c r="B103" s="32" t="s">
         <v>143</v>
@@ -6427,7 +6526,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="104" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A104" s="39"/>
       <c r="B104" s="32" t="s">
         <v>223</v>
@@ -6436,7 +6535,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="105" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A105" s="39"/>
       <c r="B105" s="32" t="s">
         <v>225</v>
@@ -6445,14 +6544,14 @@
         <v>226</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A106" s="50" t="s">
         <v>109</v>
       </c>
       <c r="B106" s="50"/>
       <c r="C106" s="50"/>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A107" s="40"/>
       <c r="B107" s="33" t="s">
         <v>149</v>
@@ -6461,14 +6560,14 @@
         <v>150</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A108" s="41" t="s">
         <v>151</v>
       </c>
       <c r="B108" s="41"/>
       <c r="C108" s="41"/>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A109" s="39"/>
       <c r="B109" s="32" t="s">
         <v>219</v>
@@ -6477,7 +6576,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A110" s="39"/>
       <c r="B110" s="32" t="s">
         <v>183</v>
@@ -6486,7 +6585,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A111" s="39"/>
       <c r="B111" s="32" t="s">
         <v>221</v>
@@ -6495,7 +6594,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="112" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A112" s="39"/>
       <c r="B112" s="32" t="s">
         <v>143</v>
@@ -6504,7 +6603,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="113" spans="1:3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A113" s="39"/>
       <c r="B113" s="32" t="s">
         <v>223</v>
@@ -6513,7 +6612,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A114" s="39"/>
       <c r="B114" s="49" t="s">
         <v>227</v>
@@ -6522,7 +6621,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="115" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A115" s="39"/>
       <c r="B115" s="32" t="s">
         <v>225</v>
@@ -6531,7 +6630,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A116" s="39"/>
       <c r="B116" s="49" t="s">
         <v>230</v>
@@ -6540,7 +6639,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A117" s="39"/>
       <c r="B117" s="32" t="s">
         <v>147</v>
@@ -6549,7 +6648,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A118" s="39"/>
       <c r="B118" s="32" t="s">
         <v>233</v>
@@ -6558,14 +6657,14 @@
         <v>234</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A119" s="52" t="s">
         <v>169</v>
       </c>
       <c r="B119" s="52"/>
       <c r="C119" s="52"/>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A120" s="8"/>
       <c r="B120" s="8" t="s">
         <v>170</v>
@@ -6574,26 +6673,26 @@
         <v>235</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A121" s="48"/>
       <c r="B121" s="30"/>
       <c r="C121" s="30"/>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A124" s="45" t="s">
         <v>236</v>
       </c>
       <c r="B124" s="46"/>
       <c r="C124" s="51"/>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A125" s="38" t="s">
         <v>140</v>
       </c>
       <c r="B125" s="38"/>
       <c r="C125" s="38"/>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A126" s="39"/>
       <c r="B126" s="32" t="s">
         <v>237</v>
@@ -6602,7 +6701,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A127" s="39"/>
       <c r="B127" s="32" t="s">
         <v>183</v>
@@ -6611,7 +6710,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A128" s="39"/>
       <c r="B128" s="32" t="s">
         <v>238</v>
@@ -6620,7 +6719,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A129" s="39"/>
       <c r="B129" s="32" t="s">
         <v>147</v>
@@ -6629,14 +6728,14 @@
         <v>240</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A130" s="50" t="s">
         <v>109</v>
       </c>
       <c r="B130" s="50"/>
       <c r="C130" s="50"/>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A131" s="40"/>
       <c r="B131" s="33" t="s">
         <v>149</v>
@@ -6645,14 +6744,14 @@
         <v>150</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A132" s="41" t="s">
         <v>151</v>
       </c>
       <c r="B132" s="41"/>
       <c r="C132" s="41"/>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A133" s="39"/>
       <c r="B133" s="32" t="s">
         <v>237</v>
@@ -6661,7 +6760,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A134" s="39"/>
       <c r="B134" s="32" t="s">
         <v>183</v>
@@ -6670,7 +6769,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A135" s="40"/>
       <c r="B135" s="32" t="s">
         <v>238</v>
@@ -6679,7 +6778,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A136" s="40"/>
       <c r="B136" s="32" t="s">
         <v>147</v>
@@ -6688,7 +6787,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="137" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A137" s="40"/>
       <c r="B137" s="32" t="s">
         <v>242</v>
@@ -6697,7 +6796,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A138" s="40"/>
       <c r="B138" s="49" t="s">
         <v>244</v>
@@ -6706,7 +6805,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A139" s="40"/>
       <c r="B139" s="49" t="s">
         <v>246</v>
@@ -6715,7 +6814,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A140" s="40"/>
       <c r="B140" s="49" t="s">
         <v>248</v>
@@ -6724,7 +6823,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A141" s="40"/>
       <c r="B141" s="49" t="s">
         <v>250</v>
@@ -6733,7 +6832,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A142" s="40"/>
       <c r="B142" s="49" t="s">
         <v>252</v>
@@ -6742,7 +6841,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A143" s="40"/>
       <c r="B143" s="49" t="s">
         <v>254</v>
@@ -6751,7 +6850,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A144" s="40"/>
       <c r="B144" s="49" t="s">
         <v>256</v>
@@ -6760,7 +6859,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A145" s="40"/>
       <c r="B145" s="49" t="s">
         <v>258</v>
@@ -6769,7 +6868,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A146" s="40"/>
       <c r="B146" s="49" t="s">
         <v>260</v>
@@ -6778,7 +6877,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A147" s="40"/>
       <c r="B147" s="49" t="s">
         <v>262</v>
@@ -6787,7 +6886,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A148" s="40"/>
       <c r="B148" s="49" t="s">
         <v>264</v>
@@ -6796,7 +6895,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A149" s="40"/>
       <c r="B149" s="49" t="s">
         <v>266</v>
@@ -6805,14 +6904,14 @@
         <v>267</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A150" s="52" t="s">
         <v>169</v>
       </c>
       <c r="B150" s="52"/>
       <c r="C150" s="52"/>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A151" s="8"/>
       <c r="B151" s="8" t="s">
         <v>170</v>
@@ -6821,36 +6920,36 @@
         <v>268</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A152" s="44"/>
       <c r="B152" s="30"/>
       <c r="C152" s="30"/>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A153" s="44"/>
       <c r="B153" s="30"/>
       <c r="C153" s="30"/>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A154" s="44"/>
       <c r="B154" s="30"/>
       <c r="C154" s="30"/>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A155" s="45" t="s">
         <v>269</v>
       </c>
       <c r="B155" s="46"/>
       <c r="C155" s="47"/>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A156" s="38" t="s">
         <v>140</v>
       </c>
       <c r="B156" s="38"/>
       <c r="C156" s="38"/>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A157" s="39"/>
       <c r="B157" s="32" t="s">
         <v>237</v>
@@ -6859,7 +6958,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A158" s="39"/>
       <c r="B158" s="32" t="s">
         <v>271</v>
@@ -6868,7 +6967,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A159" s="39"/>
       <c r="B159" s="32" t="s">
         <v>147</v>
@@ -6877,14 +6976,14 @@
         <v>273</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A160" s="50" t="s">
         <v>109</v>
       </c>
       <c r="B160" s="50"/>
       <c r="C160" s="50"/>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A161" s="40"/>
       <c r="B161" s="33" t="s">
         <v>149</v>
@@ -6893,14 +6992,14 @@
         <v>150</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A162" s="41" t="s">
         <v>151</v>
       </c>
       <c r="B162" s="41"/>
       <c r="C162" s="41"/>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A163" s="40"/>
       <c r="B163" s="32" t="s">
         <v>237</v>
@@ -6909,14 +7008,14 @@
         <v>270</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A164" s="40"/>
       <c r="B164" s="32" t="s">
         <v>188</v>
       </c>
       <c r="C164" s="32"/>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A165" s="40"/>
       <c r="B165" s="49" t="s">
         <v>274</v>
@@ -6925,7 +7024,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A166" s="40"/>
       <c r="B166" s="49" t="s">
         <v>276</v>
@@ -6934,7 +7033,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A167" s="40"/>
       <c r="B167" s="49" t="s">
         <v>278</v>
@@ -6943,7 +7042,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A168" s="40"/>
       <c r="B168" s="49" t="s">
         <v>280</v>
@@ -6952,7 +7051,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A169" s="40"/>
       <c r="B169" s="49" t="s">
         <v>191</v>
@@ -6961,7 +7060,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="170" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A170" s="40"/>
       <c r="B170" s="49" t="s">
         <v>283</v>
@@ -6970,7 +7069,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A171" s="40"/>
       <c r="B171" s="49" t="s">
         <v>285</v>
@@ -6979,7 +7078,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A172" s="40"/>
       <c r="B172" s="49" t="s">
         <v>287</v>
@@ -6988,7 +7087,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A173" s="40"/>
       <c r="B173" s="49" t="s">
         <v>289</v>
@@ -6997,7 +7096,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A174" s="40"/>
       <c r="B174" s="49" t="s">
         <v>291</v>
@@ -7006,7 +7105,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="175" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A175" s="40"/>
       <c r="B175" s="49" t="s">
         <v>293</v>
@@ -7015,7 +7114,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="176" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A176" s="40"/>
       <c r="B176" s="49" t="s">
         <v>295</v>
@@ -7024,7 +7123,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A177" s="40"/>
       <c r="B177" s="32" t="s">
         <v>271</v>
@@ -7033,7 +7132,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A178" s="40"/>
       <c r="B178" s="32" t="s">
         <v>147</v>
@@ -7042,7 +7141,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A179" s="40"/>
       <c r="B179" s="32" t="s">
         <v>297</v>
@@ -7051,7 +7150,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A180" s="40"/>
       <c r="B180" s="49" t="s">
         <v>299</v>
@@ -7060,7 +7159,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A181" s="40"/>
       <c r="B181" s="49" t="s">
         <v>301</v>
@@ -7069,7 +7168,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A182" s="40"/>
       <c r="B182" s="32" t="s">
         <v>303</v>
@@ -7078,7 +7177,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A183" s="40"/>
       <c r="B183" s="32" t="s">
         <v>305</v>
@@ -7087,7 +7186,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A184" s="40"/>
       <c r="B184" s="32" t="s">
         <v>307</v>
@@ -7096,14 +7195,14 @@
         <v>308</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A185" s="52" t="s">
         <v>169</v>
       </c>
       <c r="B185" s="52"/>
       <c r="C185" s="52"/>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A186" s="8"/>
       <c r="B186" s="8" t="s">
         <v>170</v>
@@ -7112,21 +7211,21 @@
         <v>309</v>
       </c>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A190" s="45" t="s">
         <v>310</v>
       </c>
       <c r="B190" s="46"/>
       <c r="C190" s="47"/>
     </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A191" s="38" t="s">
         <v>140</v>
       </c>
       <c r="B191" s="38"/>
       <c r="C191" s="38"/>
     </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A192" s="39"/>
       <c r="B192" s="32" t="s">
         <v>311</v>
@@ -7135,7 +7234,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="193" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A193" s="39"/>
       <c r="B193" s="32" t="s">
         <v>313</v>
@@ -7144,7 +7243,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A194" s="39"/>
       <c r="B194" s="32" t="s">
         <v>315</v>
@@ -7153,7 +7252,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A195" s="39"/>
       <c r="B195" s="32" t="s">
         <v>147</v>
@@ -7162,14 +7261,14 @@
         <v>317</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A196" s="50" t="s">
         <v>109</v>
       </c>
       <c r="B196" s="50"/>
       <c r="C196" s="50"/>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A197" s="40"/>
       <c r="B197" s="33" t="s">
         <v>149</v>
@@ -7178,14 +7277,14 @@
         <v>150</v>
       </c>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A198" s="41" t="s">
         <v>151</v>
       </c>
       <c r="B198" s="41"/>
       <c r="C198" s="41"/>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A199" s="40"/>
       <c r="B199" s="32" t="s">
         <v>311</v>
@@ -7194,7 +7293,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="200" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A200" s="40"/>
       <c r="B200" s="32" t="s">
         <v>313</v>
@@ -7203,7 +7302,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A201" s="40"/>
       <c r="B201" s="32" t="s">
         <v>315</v>
@@ -7212,7 +7311,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A202" s="40"/>
       <c r="B202" s="32" t="s">
         <v>147</v>
@@ -7221,14 +7320,14 @@
         <v>317</v>
       </c>
     </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A203" s="52" t="s">
         <v>169</v>
       </c>
       <c r="B203" s="52"/>
       <c r="C203" s="52"/>
     </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A204" s="8"/>
       <c r="B204" s="8" t="s">
         <v>170</v>
@@ -7270,14 +7369,14 @@
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="24.140625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="86.42578125" style="5" customWidth="1"/>
-    <col min="3" max="16384" width="8.85546875" style="4"/>
+    <col min="1" max="1" width="24.1328125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="86.3984375" style="5" customWidth="1"/>
+    <col min="3" max="16384" width="8.86328125" style="4"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" s="18" t="s">
         <v>320</v>
       </c>
@@ -7285,42 +7384,42 @@
         <v>321</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="20" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" s="20" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" s="20" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="43.35" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="43.35" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="20" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" s="20" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" s="20" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" s="20" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" s="23" t="s">
         <v>322</v>
       </c>
@@ -7328,32 +7427,32 @@
         <v>321</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" s="20" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14" s="67" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="43.35" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" ht="43.35" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="20" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16" s="20" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A17" s="20" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A20" s="21" t="s">
         <v>323</v>
       </c>
@@ -7361,37 +7460,37 @@
         <v>321</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A21" s="20" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="43.35" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" ht="43.35" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="20" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A23" s="20" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A24" s="20" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A25" s="20" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A26" s="20" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A29" s="4" t="s">
         <v>324</v>
       </c>
@@ -7422,42 +7521,42 @@
   <dimension ref="A1:AB49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C37" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E7" sqref="E7"/>
+      <selection pane="bottomRight" activeCell="P46" sqref="P46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" style="2" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="7.28515625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" style="87" customWidth="1"/>
-    <col min="6" max="6" width="17.140625" style="84" customWidth="1"/>
-    <col min="7" max="7" width="5" style="2" hidden="1" customWidth="1"/>
-    <col min="8" max="9" width="22.7109375" style="2" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="8.85546875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="8.46484375" style="2" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="16.59765625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="7.265625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="12.3984375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="12.3984375" style="87" customWidth="1"/>
+    <col min="6" max="6" width="17.1328125" style="84" customWidth="1"/>
+    <col min="7" max="7" width="5" style="2" customWidth="1"/>
+    <col min="8" max="9" width="22.73046875" style="2" customWidth="1"/>
+    <col min="10" max="10" width="8.86328125" style="2" customWidth="1"/>
     <col min="11" max="12" width="13" style="2" customWidth="1"/>
-    <col min="13" max="13" width="22.7109375" style="2" customWidth="1"/>
+    <col min="13" max="13" width="22.73046875" style="2" customWidth="1"/>
     <col min="14" max="14" width="7" style="2" customWidth="1"/>
-    <col min="15" max="15" width="5" style="2" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="5" style="2" customWidth="1"/>
     <col min="16" max="16" width="16" style="2" customWidth="1"/>
-    <col min="17" max="17" width="11.7109375" style="2" customWidth="1"/>
-    <col min="18" max="18" width="19.5703125" style="2" customWidth="1"/>
-    <col min="19" max="19" width="11.5703125" style="2" customWidth="1"/>
-    <col min="20" max="20" width="14.42578125" style="2" customWidth="1"/>
-    <col min="21" max="21" width="4.85546875" style="2" hidden="1" customWidth="1"/>
-    <col min="23" max="23" width="29.7109375" style="2" hidden="1" customWidth="1"/>
-    <col min="24" max="24" width="17.28515625" style="2" hidden="1" customWidth="1"/>
-    <col min="25" max="25" width="31.28515625" style="2" hidden="1" customWidth="1"/>
-    <col min="26" max="27" width="31.85546875" style="2" hidden="1" customWidth="1"/>
-    <col min="28" max="28" width="31.85546875" style="2" customWidth="1"/>
-    <col min="29" max="16384" width="8.85546875" style="2"/>
+    <col min="17" max="17" width="11.73046875" style="2" customWidth="1"/>
+    <col min="18" max="18" width="19.59765625" style="2" customWidth="1"/>
+    <col min="19" max="19" width="11.59765625" style="2" customWidth="1"/>
+    <col min="20" max="20" width="14.3984375" style="2" customWidth="1"/>
+    <col min="21" max="21" width="4.86328125" style="2" hidden="1" customWidth="1"/>
+    <col min="23" max="23" width="29.73046875" style="2" hidden="1" customWidth="1"/>
+    <col min="24" max="24" width="17.265625" style="2" hidden="1" customWidth="1"/>
+    <col min="25" max="25" width="31.265625" style="2" hidden="1" customWidth="1"/>
+    <col min="26" max="27" width="31.86328125" style="2" hidden="1" customWidth="1"/>
+    <col min="28" max="28" width="31.86328125" style="2" customWidth="1"/>
+    <col min="29" max="16384" width="8.86328125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="56" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" s="56" customFormat="1" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>325</v>
       </c>
@@ -7540,7 +7639,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="2" spans="1:28" ht="120" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" ht="99.75" x14ac:dyDescent="0.45">
       <c r="B2" s="2" t="s">
         <v>345</v>
       </c>
@@ -7585,7 +7684,7 @@
       </c>
       <c r="V2" s="2"/>
     </row>
-    <row r="3" spans="1:28" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" ht="42.75" x14ac:dyDescent="0.45">
       <c r="B3" s="2" t="s">
         <v>357</v>
       </c>
@@ -7627,7 +7726,7 @@
       </c>
       <c r="V3" s="2"/>
     </row>
-    <row r="4" spans="1:28" ht="270" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" ht="228" x14ac:dyDescent="0.45">
       <c r="B4" s="2" t="s">
         <v>363</v>
       </c>
@@ -7672,7 +7771,7 @@
       </c>
       <c r="V4" s="2"/>
     </row>
-    <row r="5" spans="1:28" ht="90" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" ht="71.25" x14ac:dyDescent="0.45">
       <c r="B5" s="2" t="s">
         <v>368</v>
       </c>
@@ -7717,7 +7816,7 @@
       </c>
       <c r="V5" s="2"/>
     </row>
-    <row r="6" spans="1:28" ht="90" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" ht="85.5" x14ac:dyDescent="0.45">
       <c r="B6" s="2" t="s">
         <v>377</v>
       </c>
@@ -7763,7 +7862,7 @@
       </c>
       <c r="V6" s="2"/>
     </row>
-    <row r="7" spans="1:28" ht="180" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" ht="156.75" x14ac:dyDescent="0.45">
       <c r="B7" s="2" t="s">
         <v>385</v>
       </c>
@@ -7802,7 +7901,7 @@
       </c>
       <c r="V7" s="2"/>
     </row>
-    <row r="8" spans="1:28" ht="120" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" ht="85.5" x14ac:dyDescent="0.45">
       <c r="B8" s="2" t="s">
         <v>390</v>
       </c>
@@ -7847,7 +7946,7 @@
       </c>
       <c r="V8" s="2"/>
     </row>
-    <row r="9" spans="1:28" ht="75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" ht="71.25" x14ac:dyDescent="0.45">
       <c r="B9" s="2" t="s">
         <v>397</v>
       </c>
@@ -7892,7 +7991,7 @@
       </c>
       <c r="V9" s="2"/>
     </row>
-    <row r="10" spans="1:28" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" ht="409.5" x14ac:dyDescent="0.45">
       <c r="B10" s="2" t="s">
         <v>406</v>
       </c>
@@ -7934,7 +8033,7 @@
       </c>
       <c r="V10" s="2"/>
     </row>
-    <row r="11" spans="1:28" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" ht="409.5" x14ac:dyDescent="0.45">
       <c r="J11" s="2" t="s">
         <v>408</v>
       </c>
@@ -7967,7 +8066,7 @@
       </c>
       <c r="V11" s="2"/>
     </row>
-    <row r="12" spans="1:28" ht="108.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" ht="108.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B12" s="2" t="s">
         <v>418</v>
       </c>
@@ -8012,7 +8111,7 @@
       </c>
       <c r="V12" s="2"/>
     </row>
-    <row r="13" spans="1:28" ht="105" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28" ht="99.75" x14ac:dyDescent="0.45">
       <c r="B13" s="2" t="s">
         <v>427</v>
       </c>
@@ -8060,7 +8159,7 @@
       </c>
       <c r="V13" s="2"/>
     </row>
-    <row r="14" spans="1:28" ht="105" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" ht="99.75" x14ac:dyDescent="0.45">
       <c r="B14" s="2" t="s">
         <v>438</v>
       </c>
@@ -8108,7 +8207,7 @@
       </c>
       <c r="V14" s="2"/>
     </row>
-    <row r="15" spans="1:28" ht="105" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" ht="99.75" x14ac:dyDescent="0.45">
       <c r="B15" s="2" t="s">
         <v>440</v>
       </c>
@@ -8153,7 +8252,7 @@
       </c>
       <c r="V15" s="2"/>
     </row>
-    <row r="16" spans="1:28" ht="105" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" ht="99.75" x14ac:dyDescent="0.45">
       <c r="A16" s="2" t="s">
         <v>441</v>
       </c>
@@ -8201,7 +8300,7 @@
       </c>
       <c r="V16" s="2"/>
     </row>
-    <row r="17" spans="2:22" ht="165" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:22" ht="142.5" x14ac:dyDescent="0.45">
       <c r="B17" s="2" t="s">
         <v>390</v>
       </c>
@@ -8246,7 +8345,7 @@
       </c>
       <c r="V17" s="2"/>
     </row>
-    <row r="18" spans="2:22" ht="75" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:22" ht="71.25" x14ac:dyDescent="0.45">
       <c r="B18" s="2" t="s">
         <v>448</v>
       </c>
@@ -8291,7 +8390,7 @@
       </c>
       <c r="V18" s="2"/>
     </row>
-    <row r="19" spans="2:22" ht="120" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:22" ht="99.75" x14ac:dyDescent="0.45">
       <c r="B19" s="2" t="s">
         <v>453</v>
       </c>
@@ -8336,7 +8435,7 @@
       </c>
       <c r="V19" s="2"/>
     </row>
-    <row r="20" spans="2:22" ht="105" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:22" ht="85.5" x14ac:dyDescent="0.45">
       <c r="B20" s="2" t="s">
         <v>463</v>
       </c>
@@ -8381,7 +8480,7 @@
       </c>
       <c r="V20" s="2"/>
     </row>
-    <row r="21" spans="2:22" ht="120" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:22" ht="99.75" x14ac:dyDescent="0.45">
       <c r="J21" s="2" t="s">
         <v>469</v>
       </c>
@@ -8414,7 +8513,7 @@
       </c>
       <c r="V21" s="2"/>
     </row>
-    <row r="22" spans="2:22" ht="150" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:22" ht="114" x14ac:dyDescent="0.45">
       <c r="B22" s="2" t="s">
         <v>476</v>
       </c>
@@ -8459,7 +8558,7 @@
       </c>
       <c r="V22" s="2"/>
     </row>
-    <row r="23" spans="2:22" ht="150" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:22" ht="128.25" x14ac:dyDescent="0.45">
       <c r="J23" s="2" t="s">
         <v>469</v>
       </c>
@@ -8492,7 +8591,7 @@
       </c>
       <c r="V23" s="2"/>
     </row>
-    <row r="24" spans="2:22" ht="90" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:22" ht="71.25" x14ac:dyDescent="0.45">
       <c r="B24" s="2" t="s">
         <v>494</v>
       </c>
@@ -8537,7 +8636,7 @@
       </c>
       <c r="V24" s="2"/>
     </row>
-    <row r="25" spans="2:22" ht="127.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:22" ht="127.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B25" s="2" t="s">
         <v>505</v>
       </c>
@@ -8585,7 +8684,7 @@
       </c>
       <c r="V25" s="2"/>
     </row>
-    <row r="26" spans="2:22" ht="105" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:22" ht="99.75" x14ac:dyDescent="0.45">
       <c r="B26" s="2" t="s">
         <v>514</v>
       </c>
@@ -8633,7 +8732,7 @@
       </c>
       <c r="V26" s="2"/>
     </row>
-    <row r="27" spans="2:22" ht="105" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:22" ht="85.5" x14ac:dyDescent="0.45">
       <c r="B27" s="2" t="s">
         <v>522</v>
       </c>
@@ -8681,7 +8780,7 @@
       </c>
       <c r="V27" s="2"/>
     </row>
-    <row r="28" spans="2:22" ht="120" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:22" ht="99.75" x14ac:dyDescent="0.45">
       <c r="B28" s="2" t="s">
         <v>529</v>
       </c>
@@ -8723,7 +8822,7 @@
       </c>
       <c r="V28" s="2"/>
     </row>
-    <row r="29" spans="2:22" ht="105" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:22" ht="99.75" x14ac:dyDescent="0.45">
       <c r="B29" s="2" t="s">
         <v>535</v>
       </c>
@@ -8771,7 +8870,7 @@
       </c>
       <c r="V29" s="2"/>
     </row>
-    <row r="30" spans="2:22" ht="90" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:22" ht="71.25" x14ac:dyDescent="0.45">
       <c r="B30" s="2" t="s">
         <v>546</v>
       </c>
@@ -8819,7 +8918,7 @@
       </c>
       <c r="V30" s="2"/>
     </row>
-    <row r="31" spans="2:22" ht="133.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:22" ht="133.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B31" s="2" t="s">
         <v>555</v>
       </c>
@@ -8867,7 +8966,7 @@
       </c>
       <c r="V31" s="2"/>
     </row>
-    <row r="32" spans="2:22" ht="165" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:22" ht="128.25" x14ac:dyDescent="0.45">
       <c r="B32" s="2" t="s">
         <v>561</v>
       </c>
@@ -8912,7 +9011,7 @@
       </c>
       <c r="V32" s="2"/>
     </row>
-    <row r="33" spans="1:22" ht="45" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:22" ht="42.75" x14ac:dyDescent="0.45">
       <c r="B33" s="2" t="s">
         <v>570</v>
       </c>
@@ -8957,7 +9056,7 @@
       </c>
       <c r="V33" s="2"/>
     </row>
-    <row r="34" spans="1:22" ht="120" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:22" ht="99.75" x14ac:dyDescent="0.45">
       <c r="B34" s="2" t="s">
         <v>578</v>
       </c>
@@ -8999,7 +9098,7 @@
       </c>
       <c r="V34" s="2"/>
     </row>
-    <row r="35" spans="1:22" ht="105" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:22" ht="85.5" x14ac:dyDescent="0.45">
       <c r="B35" s="2" t="s">
         <v>583</v>
       </c>
@@ -9048,7 +9147,7 @@
       </c>
       <c r="V35" s="2"/>
     </row>
-    <row r="36" spans="1:22" ht="105" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:22" ht="85.5" x14ac:dyDescent="0.45">
       <c r="B36" s="2" t="s">
         <v>590</v>
       </c>
@@ -9090,7 +9189,7 @@
       </c>
       <c r="V36" s="2"/>
     </row>
-    <row r="37" spans="1:22" ht="120" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:22" ht="99.75" x14ac:dyDescent="0.45">
       <c r="A37" s="2" t="s">
         <v>595</v>
       </c>
@@ -9135,7 +9234,7 @@
       </c>
       <c r="V37" s="2"/>
     </row>
-    <row r="38" spans="1:22" ht="75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:22" ht="57" x14ac:dyDescent="0.45">
       <c r="B38" s="2" t="s">
         <v>601</v>
       </c>
@@ -9183,7 +9282,7 @@
       </c>
       <c r="V38" s="2"/>
     </row>
-    <row r="39" spans="1:22" ht="105" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:22" ht="85.5" x14ac:dyDescent="0.45">
       <c r="B39" s="2" t="s">
         <v>608</v>
       </c>
@@ -9231,7 +9330,7 @@
       </c>
       <c r="V39" s="2"/>
     </row>
-    <row r="40" spans="1:22" ht="90" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:22" ht="85.5" x14ac:dyDescent="0.45">
       <c r="B40" s="2" t="s">
         <v>616</v>
       </c>
@@ -9279,7 +9378,7 @@
       </c>
       <c r="V40" s="2"/>
     </row>
-    <row r="41" spans="1:22" ht="105" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:22" ht="85.5" x14ac:dyDescent="0.45">
       <c r="B41" s="2" t="s">
         <v>621</v>
       </c>
@@ -9327,38 +9426,318 @@
       </c>
       <c r="V41" s="2"/>
     </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="V42" s="2"/>
-    </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="V43" s="2"/>
-    </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="V44" s="2"/>
-    </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="V45" s="2"/>
-    </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="V46" s="2"/>
-    </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="V47" s="2"/>
-    </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:22" ht="57" x14ac:dyDescent="0.45">
+      <c r="B42" s="82" t="s">
+        <v>655</v>
+      </c>
+      <c r="C42" s="82" t="s">
+        <v>3</v>
+      </c>
+      <c r="D42" s="91" t="s">
+        <v>656</v>
+      </c>
+      <c r="E42" s="91"/>
+      <c r="F42" s="85"/>
+      <c r="G42" s="82" t="s">
+        <v>655</v>
+      </c>
+      <c r="H42" s="82"/>
+      <c r="I42" s="82" t="s">
+        <v>657</v>
+      </c>
+      <c r="J42" s="82" t="s">
+        <v>655</v>
+      </c>
+      <c r="K42" s="82" t="s">
+        <v>321</v>
+      </c>
+      <c r="L42" s="82"/>
+      <c r="M42" s="91" t="s">
+        <v>656</v>
+      </c>
+      <c r="N42" s="85"/>
+      <c r="O42" s="82"/>
+      <c r="P42" s="82" t="s">
+        <v>681</v>
+      </c>
+      <c r="Q42" s="82"/>
+      <c r="R42" s="82" t="s">
+        <v>657</v>
+      </c>
+      <c r="S42" s="82"/>
+      <c r="T42" s="82"/>
+      <c r="U42" s="82"/>
+      <c r="V42" s="82"/>
+    </row>
+    <row r="43" spans="1:22" ht="57" x14ac:dyDescent="0.45">
+      <c r="B43" s="82" t="s">
+        <v>658</v>
+      </c>
+      <c r="C43" s="82" t="s">
+        <v>659</v>
+      </c>
+      <c r="D43" s="91" t="s">
+        <v>660</v>
+      </c>
+      <c r="E43" s="91"/>
+      <c r="F43" s="85" t="s">
+        <v>351</v>
+      </c>
+      <c r="G43" s="82" t="s">
+        <v>658</v>
+      </c>
+      <c r="H43" s="82"/>
+      <c r="I43" s="82" t="s">
+        <v>661</v>
+      </c>
+      <c r="J43" s="82" t="s">
+        <v>655</v>
+      </c>
+      <c r="K43" s="82" t="s">
+        <v>658</v>
+      </c>
+      <c r="L43" s="82" t="s">
+        <v>659</v>
+      </c>
+      <c r="M43" s="91" t="s">
+        <v>660</v>
+      </c>
+      <c r="N43" s="85" t="s">
+        <v>351</v>
+      </c>
+      <c r="O43" s="82"/>
+      <c r="P43" s="82" t="s">
+        <v>682</v>
+      </c>
+      <c r="Q43" s="82"/>
+      <c r="R43" s="82" t="s">
+        <v>661</v>
+      </c>
+      <c r="S43" s="82" t="s">
+        <v>662</v>
+      </c>
+      <c r="T43" s="82"/>
+      <c r="U43" s="82"/>
+      <c r="V43" s="82"/>
+    </row>
+    <row r="44" spans="1:22" ht="57" x14ac:dyDescent="0.45">
+      <c r="B44" s="82" t="s">
+        <v>663</v>
+      </c>
+      <c r="C44" s="82" t="s">
+        <v>346</v>
+      </c>
+      <c r="D44" s="91" t="s">
+        <v>664</v>
+      </c>
+      <c r="E44" s="91"/>
+      <c r="F44" s="85" t="s">
+        <v>665</v>
+      </c>
+      <c r="G44" s="82" t="s">
+        <v>663</v>
+      </c>
+      <c r="H44" s="82"/>
+      <c r="I44" s="82" t="s">
+        <v>666</v>
+      </c>
+      <c r="J44" s="82" t="s">
+        <v>655</v>
+      </c>
+      <c r="K44" s="82" t="s">
+        <v>663</v>
+      </c>
+      <c r="L44" s="82" t="s">
+        <v>346</v>
+      </c>
+      <c r="M44" s="91" t="s">
+        <v>664</v>
+      </c>
+      <c r="N44" s="85" t="s">
+        <v>665</v>
+      </c>
+      <c r="O44" s="82"/>
+      <c r="P44" s="82" t="s">
+        <v>683</v>
+      </c>
+      <c r="Q44" s="82"/>
+      <c r="R44" s="82" t="s">
+        <v>666</v>
+      </c>
+      <c r="S44" s="82" t="s">
+        <v>355</v>
+      </c>
+      <c r="T44" s="82"/>
+      <c r="U44" s="82"/>
+      <c r="V44" s="82"/>
+    </row>
+    <row r="45" spans="1:22" ht="57" x14ac:dyDescent="0.45">
+      <c r="B45" s="82" t="s">
+        <v>667</v>
+      </c>
+      <c r="C45" s="82" t="s">
+        <v>346</v>
+      </c>
+      <c r="D45" s="91" t="s">
+        <v>668</v>
+      </c>
+      <c r="E45" s="91"/>
+      <c r="F45" s="85" t="s">
+        <v>665</v>
+      </c>
+      <c r="G45" s="82" t="s">
+        <v>667</v>
+      </c>
+      <c r="H45" s="82"/>
+      <c r="I45" s="82" t="s">
+        <v>669</v>
+      </c>
+      <c r="J45" s="82" t="s">
+        <v>655</v>
+      </c>
+      <c r="K45" s="82" t="s">
+        <v>667</v>
+      </c>
+      <c r="L45" s="82" t="s">
+        <v>346</v>
+      </c>
+      <c r="M45" s="91" t="s">
+        <v>668</v>
+      </c>
+      <c r="N45" s="85" t="s">
+        <v>665</v>
+      </c>
+      <c r="O45" s="82"/>
+      <c r="P45" s="82" t="s">
+        <v>684</v>
+      </c>
+      <c r="Q45" s="82"/>
+      <c r="R45" s="82" t="s">
+        <v>669</v>
+      </c>
+      <c r="S45" s="82" t="s">
+        <v>375</v>
+      </c>
+      <c r="T45" s="82"/>
+      <c r="U45" s="82"/>
+      <c r="V45" s="82"/>
+    </row>
+    <row r="46" spans="1:22" ht="57" x14ac:dyDescent="0.45">
+      <c r="B46" s="82" t="s">
+        <v>670</v>
+      </c>
+      <c r="C46" s="82" t="s">
+        <v>271</v>
+      </c>
+      <c r="D46" s="91" t="s">
+        <v>672</v>
+      </c>
+      <c r="E46" s="91"/>
+      <c r="F46" s="85" t="s">
+        <v>351</v>
+      </c>
+      <c r="G46" s="82" t="s">
+        <v>670</v>
+      </c>
+      <c r="H46" s="82"/>
+      <c r="I46" s="82" t="s">
+        <v>673</v>
+      </c>
+      <c r="J46" s="82" t="s">
+        <v>655</v>
+      </c>
+      <c r="K46" s="82" t="s">
+        <v>670</v>
+      </c>
+      <c r="L46" s="82" t="s">
+        <v>671</v>
+      </c>
+      <c r="M46" s="91" t="s">
+        <v>672</v>
+      </c>
+      <c r="N46" s="85" t="s">
+        <v>351</v>
+      </c>
+      <c r="O46" s="82"/>
+      <c r="P46" s="82" t="s">
+        <v>685</v>
+      </c>
+      <c r="Q46" s="82"/>
+      <c r="R46" s="82" t="s">
+        <v>673</v>
+      </c>
+      <c r="S46" s="82" t="s">
+        <v>674</v>
+      </c>
+      <c r="T46" s="82"/>
+      <c r="U46" s="82"/>
+      <c r="V46" s="82"/>
+    </row>
+    <row r="47" spans="1:22" ht="57" x14ac:dyDescent="0.45">
+      <c r="B47" s="82" t="s">
+        <v>675</v>
+      </c>
+      <c r="C47" s="82" t="s">
+        <v>680</v>
+      </c>
+      <c r="D47" s="91" t="s">
+        <v>677</v>
+      </c>
+      <c r="E47" s="91"/>
+      <c r="F47" s="85" t="s">
+        <v>351</v>
+      </c>
+      <c r="G47" s="82" t="s">
+        <v>675</v>
+      </c>
+      <c r="H47" s="82"/>
+      <c r="I47" s="82" t="s">
+        <v>678</v>
+      </c>
+      <c r="J47" s="82" t="s">
+        <v>655</v>
+      </c>
+      <c r="K47" s="82" t="s">
+        <v>675</v>
+      </c>
+      <c r="L47" s="82" t="s">
+        <v>676</v>
+      </c>
+      <c r="M47" s="91" t="s">
+        <v>677</v>
+      </c>
+      <c r="N47" s="85" t="s">
+        <v>351</v>
+      </c>
+      <c r="O47" s="82"/>
+      <c r="P47" s="82" t="s">
+        <v>686</v>
+      </c>
+      <c r="Q47" s="82"/>
+      <c r="R47" s="82" t="s">
+        <v>678</v>
+      </c>
+      <c r="S47" s="82" t="s">
+        <v>679</v>
+      </c>
+      <c r="T47" s="82"/>
+      <c r="U47" s="82"/>
+      <c r="V47" s="82"/>
+    </row>
+    <row r="48" spans="1:22" x14ac:dyDescent="0.45">
       <c r="V48" s="2"/>
     </row>
-    <row r="49" spans="22:22" x14ac:dyDescent="0.25">
+    <row r="49" spans="22:22" x14ac:dyDescent="0.45">
       <c r="V49" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="19" type="noConversion"/>
-  <dataValidations disablePrompts="1" count="3">
+  <dataValidations count="3">
     <dataValidation errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1" xr:uid="{00000000-0002-0000-0300-000000000000}"/>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid value" error="Valid property styles are &quot;element&quot;, &quot;attribute&quot;, or &quot;abstract&quot;.  Leave the cell blank to use the default value &quot;element&quot;." promptTitle="Property Style" prompt="- &quot;element&quot; or blank (default) - Represents a typical NIEM property._x000a_- &quot;abstract&quot; - Used to create a substitution group_x000a_- &quot;attribute&quot; - Use sparingly, if at all; for values tightly-coupled to an element." sqref="X50:X1048576 W2:W41" xr:uid="{00000000-0002-0000-0300-000002000000}">
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid value" error="Valid property styles are &quot;element&quot;, &quot;attribute&quot;, or &quot;abstract&quot;.  Leave the cell blank to use the default value &quot;element&quot;." promptTitle="Property Style" prompt="- &quot;element&quot; or blank (default) - Represents a typical NIEM property._x000a_- &quot;abstract&quot; - Used to create a substitution group_x000a_- &quot;attribute&quot; - Use sparingly, if at all; for values tightly-coupled to an element." sqref="X50:X1048576 W2:W47" xr:uid="{00000000-0002-0000-0300-000002000000}">
       <formula1>"element,attribute,abstract"</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576" xr:uid="{00000000-0002-0000-0300-000001000000}">
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576 O42:O47" xr:uid="{00000000-0002-0000-0300-000001000000}">
       <formula1>MAPPING_CODES</formula1>
     </dataValidation>
   </dataValidations>
@@ -9384,23 +9763,23 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" style="2" customWidth="1"/>
-    <col min="2" max="3" width="29.7109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="45.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" style="2" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="22.28515625" style="2" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="11.7109375" style="2" customWidth="1"/>
-    <col min="9" max="10" width="29.7109375" style="2" customWidth="1"/>
-    <col min="11" max="11" width="45.7109375" style="2" customWidth="1"/>
-    <col min="12" max="12" width="16.5703125" style="2" customWidth="1"/>
-    <col min="13" max="14" width="45.7109375" style="2" customWidth="1"/>
-    <col min="15" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="11.73046875" style="2" customWidth="1"/>
+    <col min="2" max="3" width="29.73046875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="45.73046875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11.73046875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="16.1328125" style="2" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="22.265625" style="2" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="11.73046875" style="2" customWidth="1"/>
+    <col min="9" max="10" width="29.73046875" style="2" customWidth="1"/>
+    <col min="11" max="11" width="45.73046875" style="2" customWidth="1"/>
+    <col min="12" max="12" width="16.59765625" style="2" customWidth="1"/>
+    <col min="13" max="14" width="45.73046875" style="2" customWidth="1"/>
+    <col min="15" max="16384" width="8.86328125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="56" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="56" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>325</v>
       </c>
@@ -9476,28 +9855,28 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="29.7109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="29.7109375" style="2" customWidth="1"/>
-    <col min="5" max="6" width="11.7109375" style="17" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="18.7109375" style="2" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="11.73046875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="29.73046875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13.1328125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="29.73046875" style="2" customWidth="1"/>
+    <col min="5" max="6" width="11.73046875" style="17" customWidth="1"/>
+    <col min="7" max="7" width="11.73046875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="18.73046875" style="2" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="12" style="2" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" style="2" customWidth="1"/>
-    <col min="11" max="11" width="23.85546875" style="2" customWidth="1"/>
+    <col min="10" max="10" width="11.73046875" style="2" customWidth="1"/>
+    <col min="11" max="11" width="23.86328125" style="2" customWidth="1"/>
     <col min="12" max="12" width="14" style="2" customWidth="1"/>
-    <col min="13" max="13" width="30.7109375" style="2" customWidth="1"/>
-    <col min="14" max="14" width="11.7109375" style="17" customWidth="1"/>
-    <col min="15" max="15" width="14.42578125" style="17" customWidth="1"/>
-    <col min="16" max="16" width="43.7109375" style="2" customWidth="1"/>
-    <col min="17" max="17" width="12.7109375" style="2" hidden="1" customWidth="1"/>
-    <col min="18" max="16384" width="8.85546875" style="2"/>
+    <col min="13" max="13" width="30.73046875" style="2" customWidth="1"/>
+    <col min="14" max="14" width="11.73046875" style="17" customWidth="1"/>
+    <col min="15" max="15" width="14.3984375" style="17" customWidth="1"/>
+    <col min="16" max="16" width="43.73046875" style="2" customWidth="1"/>
+    <col min="17" max="17" width="12.73046875" style="2" hidden="1" customWidth="1"/>
+    <col min="18" max="16384" width="8.86328125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="56" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" s="56" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A1" s="10" t="s">
         <v>635</v>
       </c>
@@ -9550,7 +9929,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B2" s="72"/>
       <c r="G2" s="72"/>
     </row>
@@ -9583,25 +9962,25 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" style="17" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" style="17" customWidth="1"/>
-    <col min="3" max="3" width="21.28515625" style="17" customWidth="1"/>
-    <col min="4" max="4" width="24.42578125" style="17" customWidth="1"/>
-    <col min="5" max="5" width="21.28515625" style="17" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.73046875" style="17" customWidth="1"/>
+    <col min="2" max="2" width="30.73046875" style="17" customWidth="1"/>
+    <col min="3" max="3" width="21.265625" style="17" customWidth="1"/>
+    <col min="4" max="4" width="24.3984375" style="17" customWidth="1"/>
+    <col min="5" max="5" width="21.265625" style="17" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15" style="17" customWidth="1"/>
-    <col min="7" max="7" width="20.28515625" style="17" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="16.85546875" style="17" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="12.28515625" style="17" customWidth="1"/>
-    <col min="10" max="10" width="32.85546875" style="17" customWidth="1"/>
-    <col min="11" max="11" width="17.42578125" style="17" customWidth="1"/>
-    <col min="12" max="12" width="40.7109375" style="17" customWidth="1"/>
-    <col min="13" max="13" width="22.140625" style="17" customWidth="1"/>
-    <col min="14" max="16384" width="8.85546875" style="17"/>
+    <col min="7" max="7" width="20.265625" style="17" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="16.86328125" style="17" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="12.265625" style="17" customWidth="1"/>
+    <col min="10" max="10" width="32.86328125" style="17" customWidth="1"/>
+    <col min="11" max="11" width="17.3984375" style="17" customWidth="1"/>
+    <col min="12" max="12" width="40.73046875" style="17" customWidth="1"/>
+    <col min="13" max="13" width="22.1328125" style="17" customWidth="1"/>
+    <col min="14" max="16384" width="8.86328125" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="57" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="57" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A1" s="60" t="s">
         <v>642</v>
       </c>
@@ -9676,26 +10055,26 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="55.7109375" style="58" customWidth="1"/>
-    <col min="3" max="3" width="35.7109375" style="58" customWidth="1"/>
+    <col min="1" max="1" width="15.73046875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="55.73046875" style="58" customWidth="1"/>
+    <col min="3" max="3" width="35.73046875" style="58" customWidth="1"/>
     <col min="4" max="4" width="15" style="2" customWidth="1"/>
-    <col min="5" max="6" width="29.140625" style="2" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="23.7109375" style="58" customWidth="1"/>
+    <col min="5" max="6" width="29.1328125" style="2" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="23.73046875" style="58" customWidth="1"/>
     <col min="8" max="8" width="13" style="58" customWidth="1"/>
-    <col min="9" max="9" width="55.7109375" style="58" customWidth="1"/>
-    <col min="10" max="10" width="35.7109375" style="58" customWidth="1"/>
-    <col min="11" max="11" width="14.7109375" style="2" customWidth="1"/>
-    <col min="12" max="12" width="23.5703125" style="2" customWidth="1"/>
-    <col min="13" max="13" width="35.42578125" style="2" customWidth="1"/>
-    <col min="14" max="14" width="23.7109375" style="59" customWidth="1"/>
-    <col min="15" max="15" width="9.140625" style="2" customWidth="1"/>
-    <col min="16" max="16384" width="8.85546875" style="2"/>
+    <col min="9" max="9" width="55.73046875" style="58" customWidth="1"/>
+    <col min="10" max="10" width="35.73046875" style="58" customWidth="1"/>
+    <col min="11" max="11" width="14.73046875" style="2" customWidth="1"/>
+    <col min="12" max="12" width="23.59765625" style="2" customWidth="1"/>
+    <col min="13" max="13" width="35.3984375" style="2" customWidth="1"/>
+    <col min="14" max="14" width="23.73046875" style="59" customWidth="1"/>
+    <col min="15" max="15" width="9.1328125" style="2" customWidth="1"/>
+    <col min="16" max="16384" width="8.86328125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="56" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="56" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A1" s="79" t="s">
         <v>648</v>
       </c>
@@ -9774,21 +10153,21 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" style="2" customWidth="1"/>
-    <col min="2" max="4" width="20.5703125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" style="17" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="16.85546875" style="17" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="15.7109375" style="2" customWidth="1"/>
-    <col min="9" max="9" width="20.7109375" style="2" customWidth="1"/>
-    <col min="10" max="10" width="23.85546875" style="2" customWidth="1"/>
-    <col min="11" max="11" width="30.7109375" style="2" customWidth="1"/>
-    <col min="12" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="15.73046875" style="2" customWidth="1"/>
+    <col min="2" max="4" width="20.59765625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11.73046875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="20.265625" style="17" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="16.86328125" style="17" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="15.73046875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="20.73046875" style="2" customWidth="1"/>
+    <col min="10" max="10" width="23.86328125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="30.73046875" style="2" customWidth="1"/>
+    <col min="12" max="16384" width="8.86328125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A1" s="10" t="s">
         <v>652</v>
       </c>

</xml_diff>

<commit_message>
Add DocumentType to ChargeFiling and UniformCommitmentOrder, allow multiple attachments
</commit_message>
<xml_diff>
--- a/schemas/ChargeFiling_iepd/artifacts/ChargeFiling_MappingSpreadsheet.xlsx
+++ b/schemas/ChargeFiling_iepd/artifacts/ChargeFiling_MappingSpreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JamesCabral\git\JTMP-Data-Exchange-Specs\schemas\ChargeFiling_iepd\artifacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F1CC14B-EF9C-48D7-BCAA-2BBD869654AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C31E1079-9A7D-49F6-B915-B45011BAB5B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4080" yWindow="-21720" windowWidth="51840" windowHeight="21120" tabRatio="781" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22980" yWindow="-21360" windowWidth="26865" windowHeight="19245" tabRatio="781" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="9" state="hidden" r:id="rId1"/>
@@ -26,7 +26,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Codes | Facets'!$A$1:$M$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7">Namespace!$A$1:$N$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Property!$A$1:$W$47</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Property!$A$1:$W$48</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4">Type!$A$1:$L$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5">'Type-Has-Property'!$A$1:$P$1</definedName>
     <definedName name="CODES_NamespaceStyle">'Field Descriptions'!$B$165:$B$176</definedName>
@@ -163,7 +163,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1168" uniqueCount="687">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1190" uniqueCount="697">
   <si>
     <t xml:space="preserve">Template last updated: </t>
   </si>
@@ -2923,12 +2923,42 @@
   <si>
     <t>nc:Document/nc:DocumentBinarync:Base64BinaryObject</t>
   </si>
+  <si>
+    <t>Attribute</t>
+  </si>
+  <si>
+    <t>DocumentType</t>
+  </si>
+  <si>
+    <t>A kind of document; a nature or genre of the content. Includes terms describing general categories, functions, or genres.</t>
+  </si>
+  <si>
+    <t>nc:DocumentType</t>
+  </si>
+  <si>
+    <t>nc:DocumentCategoryText</t>
+  </si>
+  <si>
+    <t>A kind of document; a nature or genre of the content.</t>
+  </si>
+  <si>
+    <t>0..unbounded</t>
+  </si>
+  <si>
+    <t>nc:BinaryType</t>
+  </si>
+  <si>
+    <t>nc:BinaryType (nc:BinaryFormatAbstract)</t>
+  </si>
+  <si>
+    <t>nc:BinaryType (nc:BinaryObjectAbstract)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3082,8 +3112,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3133,6 +3176,11 @@
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="22"/>
       </patternFill>
     </fill>
   </fills>
@@ -3288,7 +3336,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3536,7 +3584,30 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4861,8 +4932,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table3" displayName="Table3" ref="A1:Z47" totalsRowShown="0" headerRowDxfId="107" dataDxfId="106" headerRowCellStyle="Accent2">
-  <autoFilter ref="A1:Z47" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table3" displayName="Table3" ref="A1:Z48" totalsRowShown="0" headerRowDxfId="107" dataDxfId="106" headerRowCellStyle="Accent2">
+  <autoFilter ref="A1:Z48" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Z41">
     <sortCondition ref="P1:P41"/>
   </sortState>
@@ -7518,13 +7589,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:AB49"/>
+  <dimension ref="A1:AB50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C37" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C39" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P46" sqref="P46"/>
+      <selection pane="bottomRight" activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -9426,318 +9497,386 @@
       </c>
       <c r="V41" s="2"/>
     </row>
-    <row r="42" spans="1:22" ht="57" x14ac:dyDescent="0.45">
-      <c r="B42" s="82" t="s">
+    <row r="42" spans="1:22" s="94" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A42" s="95" t="s">
+        <v>687</v>
+      </c>
+      <c r="B42" s="97" t="s">
+        <v>688</v>
+      </c>
+      <c r="C42" s="97" t="s">
+        <v>346</v>
+      </c>
+      <c r="D42" s="97" t="s">
+        <v>689</v>
+      </c>
+      <c r="E42" s="97"/>
+      <c r="F42" s="98" t="s">
+        <v>693</v>
+      </c>
+      <c r="G42" s="97"/>
+      <c r="H42" s="97"/>
+      <c r="I42" s="93"/>
+      <c r="J42" s="96" t="s">
+        <v>3</v>
+      </c>
+      <c r="K42" s="96" t="s">
+        <v>688</v>
+      </c>
+      <c r="L42" s="96" t="s">
+        <v>346</v>
+      </c>
+      <c r="M42" s="96" t="s">
+        <v>689</v>
+      </c>
+      <c r="N42" s="92" t="s">
+        <v>415</v>
+      </c>
+      <c r="O42" s="97"/>
+      <c r="P42" s="97" t="s">
+        <v>690</v>
+      </c>
+      <c r="Q42" s="93" t="s">
+        <v>690</v>
+      </c>
+      <c r="R42" s="96" t="s">
+        <v>691</v>
+      </c>
+      <c r="S42" s="97" t="s">
+        <v>355</v>
+      </c>
+      <c r="T42" s="99" t="s">
+        <v>692</v>
+      </c>
+      <c r="U42" s="99"/>
+      <c r="V42" s="99"/>
+    </row>
+    <row r="43" spans="1:22" ht="57" x14ac:dyDescent="0.45">
+      <c r="B43" s="91" t="s">
         <v>655</v>
       </c>
-      <c r="C42" s="82" t="s">
+      <c r="C43" s="91" t="s">
         <v>3</v>
       </c>
-      <c r="D42" s="91" t="s">
+      <c r="D43" s="100" t="s">
         <v>656</v>
       </c>
-      <c r="E42" s="91"/>
-      <c r="F42" s="85"/>
-      <c r="G42" s="82" t="s">
+      <c r="E43" s="100"/>
+      <c r="F43" s="92"/>
+      <c r="G43" s="91" t="s">
         <v>655</v>
       </c>
-      <c r="H42" s="82"/>
-      <c r="I42" s="82" t="s">
+      <c r="H43" s="91"/>
+      <c r="I43" s="91"/>
+      <c r="J43" s="91" t="s">
+        <v>655</v>
+      </c>
+      <c r="K43" s="91" t="s">
+        <v>321</v>
+      </c>
+      <c r="L43" s="91"/>
+      <c r="M43" s="100" t="s">
+        <v>656</v>
+      </c>
+      <c r="N43" s="92"/>
+      <c r="O43" s="91"/>
+      <c r="P43" s="91" t="s">
+        <v>681</v>
+      </c>
+      <c r="Q43" s="91" t="s">
+        <v>694</v>
+      </c>
+      <c r="R43" s="91" t="s">
         <v>657</v>
       </c>
-      <c r="J42" s="82" t="s">
+      <c r="S43" s="91" t="s">
+        <v>694</v>
+      </c>
+      <c r="T43" s="91" t="s">
+        <v>694</v>
+      </c>
+      <c r="U43" s="91"/>
+      <c r="V43" s="91"/>
+    </row>
+    <row r="44" spans="1:22" ht="57" x14ac:dyDescent="0.45">
+      <c r="B44" s="91" t="s">
+        <v>658</v>
+      </c>
+      <c r="C44" s="91" t="s">
+        <v>659</v>
+      </c>
+      <c r="D44" s="100" t="s">
+        <v>660</v>
+      </c>
+      <c r="E44" s="100"/>
+      <c r="F44" s="92" t="s">
+        <v>351</v>
+      </c>
+      <c r="G44" s="91" t="s">
+        <v>658</v>
+      </c>
+      <c r="H44" s="91"/>
+      <c r="I44" s="91"/>
+      <c r="J44" s="91" t="s">
         <v>655</v>
       </c>
-      <c r="K42" s="82" t="s">
-        <v>321</v>
-      </c>
-      <c r="L42" s="82"/>
-      <c r="M42" s="91" t="s">
-        <v>656</v>
-      </c>
-      <c r="N42" s="85"/>
-      <c r="O42" s="82"/>
-      <c r="P42" s="82" t="s">
-        <v>681</v>
-      </c>
-      <c r="Q42" s="82"/>
-      <c r="R42" s="82" t="s">
-        <v>657</v>
-      </c>
-      <c r="S42" s="82"/>
-      <c r="T42" s="82"/>
-      <c r="U42" s="82"/>
-      <c r="V42" s="82"/>
-    </row>
-    <row r="43" spans="1:22" ht="57" x14ac:dyDescent="0.45">
-      <c r="B43" s="82" t="s">
+      <c r="K44" s="91" t="s">
         <v>658</v>
       </c>
-      <c r="C43" s="82" t="s">
+      <c r="L44" s="91" t="s">
         <v>659</v>
       </c>
-      <c r="D43" s="91" t="s">
+      <c r="M44" s="100" t="s">
         <v>660</v>
       </c>
-      <c r="E43" s="91"/>
-      <c r="F43" s="85" t="s">
+      <c r="N44" s="92" t="s">
         <v>351</v>
       </c>
-      <c r="G43" s="82" t="s">
-        <v>658</v>
-      </c>
-      <c r="H43" s="82"/>
-      <c r="I43" s="82" t="s">
+      <c r="O44" s="91"/>
+      <c r="P44" s="91" t="s">
+        <v>682</v>
+      </c>
+      <c r="Q44" s="91" t="s">
+        <v>694</v>
+      </c>
+      <c r="R44" s="91" t="s">
         <v>661</v>
       </c>
-      <c r="J43" s="82" t="s">
+      <c r="S44" s="91" t="s">
+        <v>662</v>
+      </c>
+      <c r="T44" s="91" t="s">
+        <v>694</v>
+      </c>
+      <c r="U44" s="91"/>
+      <c r="V44" s="91"/>
+    </row>
+    <row r="45" spans="1:22" ht="57" x14ac:dyDescent="0.45">
+      <c r="B45" s="91" t="s">
+        <v>663</v>
+      </c>
+      <c r="C45" s="91" t="s">
+        <v>346</v>
+      </c>
+      <c r="D45" s="100" t="s">
+        <v>664</v>
+      </c>
+      <c r="E45" s="100"/>
+      <c r="F45" s="92" t="s">
+        <v>665</v>
+      </c>
+      <c r="G45" s="91" t="s">
+        <v>663</v>
+      </c>
+      <c r="H45" s="91"/>
+      <c r="I45" s="91"/>
+      <c r="J45" s="91" t="s">
         <v>655</v>
       </c>
-      <c r="K43" s="82" t="s">
-        <v>658</v>
-      </c>
-      <c r="L43" s="82" t="s">
-        <v>659</v>
-      </c>
-      <c r="M43" s="91" t="s">
-        <v>660</v>
-      </c>
-      <c r="N43" s="85" t="s">
+      <c r="K45" s="91" t="s">
+        <v>663</v>
+      </c>
+      <c r="L45" s="91" t="s">
+        <v>346</v>
+      </c>
+      <c r="M45" s="100" t="s">
+        <v>664</v>
+      </c>
+      <c r="N45" s="92" t="s">
+        <v>665</v>
+      </c>
+      <c r="O45" s="91"/>
+      <c r="P45" s="91" t="s">
+        <v>683</v>
+      </c>
+      <c r="Q45" s="91" t="s">
+        <v>695</v>
+      </c>
+      <c r="R45" s="91" t="s">
+        <v>666</v>
+      </c>
+      <c r="S45" s="91" t="s">
+        <v>355</v>
+      </c>
+      <c r="T45" s="91" t="s">
+        <v>695</v>
+      </c>
+      <c r="U45" s="91"/>
+      <c r="V45" s="91"/>
+    </row>
+    <row r="46" spans="1:22" ht="57" x14ac:dyDescent="0.45">
+      <c r="B46" s="91" t="s">
+        <v>667</v>
+      </c>
+      <c r="C46" s="91" t="s">
+        <v>346</v>
+      </c>
+      <c r="D46" s="100" t="s">
+        <v>668</v>
+      </c>
+      <c r="E46" s="100"/>
+      <c r="F46" s="92" t="s">
+        <v>665</v>
+      </c>
+      <c r="G46" s="91" t="s">
+        <v>667</v>
+      </c>
+      <c r="H46" s="91"/>
+      <c r="I46" s="91"/>
+      <c r="J46" s="91" t="s">
+        <v>655</v>
+      </c>
+      <c r="K46" s="91" t="s">
+        <v>667</v>
+      </c>
+      <c r="L46" s="91" t="s">
+        <v>346</v>
+      </c>
+      <c r="M46" s="100" t="s">
+        <v>668</v>
+      </c>
+      <c r="N46" s="92" t="s">
+        <v>665</v>
+      </c>
+      <c r="O46" s="91"/>
+      <c r="P46" s="91" t="s">
+        <v>684</v>
+      </c>
+      <c r="Q46" s="91" t="s">
+        <v>694</v>
+      </c>
+      <c r="R46" s="91" t="s">
+        <v>669</v>
+      </c>
+      <c r="S46" s="91" t="s">
+        <v>375</v>
+      </c>
+      <c r="T46" s="91" t="s">
+        <v>694</v>
+      </c>
+      <c r="U46" s="91"/>
+      <c r="V46" s="91"/>
+    </row>
+    <row r="47" spans="1:22" ht="57" x14ac:dyDescent="0.45">
+      <c r="B47" s="91" t="s">
+        <v>670</v>
+      </c>
+      <c r="C47" s="91" t="s">
+        <v>271</v>
+      </c>
+      <c r="D47" s="100" t="s">
+        <v>672</v>
+      </c>
+      <c r="E47" s="100"/>
+      <c r="F47" s="92" t="s">
         <v>351</v>
       </c>
-      <c r="O43" s="82"/>
-      <c r="P43" s="82" t="s">
-        <v>682</v>
-      </c>
-      <c r="Q43" s="82"/>
-      <c r="R43" s="82" t="s">
-        <v>661</v>
-      </c>
-      <c r="S43" s="82" t="s">
-        <v>662</v>
-      </c>
-      <c r="T43" s="82"/>
-      <c r="U43" s="82"/>
-      <c r="V43" s="82"/>
-    </row>
-    <row r="44" spans="1:22" ht="57" x14ac:dyDescent="0.45">
-      <c r="B44" s="82" t="s">
-        <v>663</v>
-      </c>
-      <c r="C44" s="82" t="s">
-        <v>346</v>
-      </c>
-      <c r="D44" s="91" t="s">
-        <v>664</v>
-      </c>
-      <c r="E44" s="91"/>
-      <c r="F44" s="85" t="s">
-        <v>665</v>
-      </c>
-      <c r="G44" s="82" t="s">
-        <v>663</v>
-      </c>
-      <c r="H44" s="82"/>
-      <c r="I44" s="82" t="s">
-        <v>666</v>
-      </c>
-      <c r="J44" s="82" t="s">
+      <c r="G47" s="91" t="s">
+        <v>670</v>
+      </c>
+      <c r="H47" s="91"/>
+      <c r="I47" s="91"/>
+      <c r="J47" s="91" t="s">
         <v>655</v>
       </c>
-      <c r="K44" s="82" t="s">
-        <v>663</v>
-      </c>
-      <c r="L44" s="82" t="s">
-        <v>346</v>
-      </c>
-      <c r="M44" s="91" t="s">
-        <v>664</v>
-      </c>
-      <c r="N44" s="85" t="s">
-        <v>665</v>
-      </c>
-      <c r="O44" s="82"/>
-      <c r="P44" s="82" t="s">
-        <v>683</v>
-      </c>
-      <c r="Q44" s="82"/>
-      <c r="R44" s="82" t="s">
-        <v>666</v>
-      </c>
-      <c r="S44" s="82" t="s">
-        <v>355</v>
-      </c>
-      <c r="T44" s="82"/>
-      <c r="U44" s="82"/>
-      <c r="V44" s="82"/>
-    </row>
-    <row r="45" spans="1:22" ht="57" x14ac:dyDescent="0.45">
-      <c r="B45" s="82" t="s">
-        <v>667</v>
-      </c>
-      <c r="C45" s="82" t="s">
-        <v>346</v>
-      </c>
-      <c r="D45" s="91" t="s">
-        <v>668</v>
-      </c>
-      <c r="E45" s="91"/>
-      <c r="F45" s="85" t="s">
-        <v>665</v>
-      </c>
-      <c r="G45" s="82" t="s">
-        <v>667</v>
-      </c>
-      <c r="H45" s="82"/>
-      <c r="I45" s="82" t="s">
-        <v>669</v>
-      </c>
-      <c r="J45" s="82" t="s">
+      <c r="K47" s="91" t="s">
+        <v>670</v>
+      </c>
+      <c r="L47" s="91" t="s">
+        <v>671</v>
+      </c>
+      <c r="M47" s="100" t="s">
+        <v>672</v>
+      </c>
+      <c r="N47" s="92" t="s">
+        <v>351</v>
+      </c>
+      <c r="O47" s="91"/>
+      <c r="P47" s="91" t="s">
+        <v>685</v>
+      </c>
+      <c r="Q47" s="91" t="s">
+        <v>694</v>
+      </c>
+      <c r="R47" s="91" t="s">
+        <v>673</v>
+      </c>
+      <c r="S47" s="91" t="s">
+        <v>674</v>
+      </c>
+      <c r="T47" s="91" t="s">
+        <v>694</v>
+      </c>
+      <c r="U47" s="91"/>
+      <c r="V47" s="91"/>
+    </row>
+    <row r="48" spans="1:22" ht="57" x14ac:dyDescent="0.45">
+      <c r="B48" s="91" t="s">
+        <v>675</v>
+      </c>
+      <c r="C48" s="91" t="s">
+        <v>680</v>
+      </c>
+      <c r="D48" s="100" t="s">
+        <v>677</v>
+      </c>
+      <c r="E48" s="100"/>
+      <c r="F48" s="92" t="s">
+        <v>351</v>
+      </c>
+      <c r="G48" s="91" t="s">
+        <v>675</v>
+      </c>
+      <c r="H48" s="91"/>
+      <c r="I48" s="91"/>
+      <c r="J48" s="91" t="s">
         <v>655</v>
       </c>
-      <c r="K45" s="82" t="s">
-        <v>667</v>
-      </c>
-      <c r="L45" s="82" t="s">
-        <v>346</v>
-      </c>
-      <c r="M45" s="91" t="s">
-        <v>668</v>
-      </c>
-      <c r="N45" s="85" t="s">
-        <v>665</v>
-      </c>
-      <c r="O45" s="82"/>
-      <c r="P45" s="82" t="s">
-        <v>684</v>
-      </c>
-      <c r="Q45" s="82"/>
-      <c r="R45" s="82" t="s">
-        <v>669</v>
-      </c>
-      <c r="S45" s="82" t="s">
-        <v>375</v>
-      </c>
-      <c r="T45" s="82"/>
-      <c r="U45" s="82"/>
-      <c r="V45" s="82"/>
-    </row>
-    <row r="46" spans="1:22" ht="57" x14ac:dyDescent="0.45">
-      <c r="B46" s="82" t="s">
-        <v>670</v>
-      </c>
-      <c r="C46" s="82" t="s">
-        <v>271</v>
-      </c>
-      <c r="D46" s="91" t="s">
-        <v>672</v>
-      </c>
-      <c r="E46" s="91"/>
-      <c r="F46" s="85" t="s">
+      <c r="K48" s="91" t="s">
+        <v>675</v>
+      </c>
+      <c r="L48" s="91" t="s">
+        <v>676</v>
+      </c>
+      <c r="M48" s="100" t="s">
+        <v>677</v>
+      </c>
+      <c r="N48" s="92" t="s">
         <v>351</v>
       </c>
-      <c r="G46" s="82" t="s">
-        <v>670</v>
-      </c>
-      <c r="H46" s="82"/>
-      <c r="I46" s="82" t="s">
-        <v>673</v>
-      </c>
-      <c r="J46" s="82" t="s">
-        <v>655</v>
-      </c>
-      <c r="K46" s="82" t="s">
-        <v>670</v>
-      </c>
-      <c r="L46" s="82" t="s">
-        <v>671</v>
-      </c>
-      <c r="M46" s="91" t="s">
-        <v>672</v>
-      </c>
-      <c r="N46" s="85" t="s">
-        <v>351</v>
-      </c>
-      <c r="O46" s="82"/>
-      <c r="P46" s="82" t="s">
-        <v>685</v>
-      </c>
-      <c r="Q46" s="82"/>
-      <c r="R46" s="82" t="s">
-        <v>673</v>
-      </c>
-      <c r="S46" s="82" t="s">
-        <v>674</v>
-      </c>
-      <c r="T46" s="82"/>
-      <c r="U46" s="82"/>
-      <c r="V46" s="82"/>
-    </row>
-    <row r="47" spans="1:22" ht="57" x14ac:dyDescent="0.45">
-      <c r="B47" s="82" t="s">
-        <v>675</v>
-      </c>
-      <c r="C47" s="82" t="s">
-        <v>680</v>
-      </c>
-      <c r="D47" s="91" t="s">
-        <v>677</v>
-      </c>
-      <c r="E47" s="91"/>
-      <c r="F47" s="85" t="s">
-        <v>351</v>
-      </c>
-      <c r="G47" s="82" t="s">
-        <v>675</v>
-      </c>
-      <c r="H47" s="82"/>
-      <c r="I47" s="82" t="s">
+      <c r="O48" s="91"/>
+      <c r="P48" s="91" t="s">
+        <v>686</v>
+      </c>
+      <c r="Q48" s="91" t="s">
+        <v>696</v>
+      </c>
+      <c r="R48" s="91" t="s">
         <v>678</v>
       </c>
-      <c r="J47" s="82" t="s">
-        <v>655</v>
-      </c>
-      <c r="K47" s="82" t="s">
-        <v>675</v>
-      </c>
-      <c r="L47" s="82" t="s">
-        <v>676</v>
-      </c>
-      <c r="M47" s="91" t="s">
-        <v>677</v>
-      </c>
-      <c r="N47" s="85" t="s">
-        <v>351</v>
-      </c>
-      <c r="O47" s="82"/>
-      <c r="P47" s="82" t="s">
-        <v>686</v>
-      </c>
-      <c r="Q47" s="82"/>
-      <c r="R47" s="82" t="s">
-        <v>678</v>
-      </c>
-      <c r="S47" s="82" t="s">
+      <c r="S48" s="91" t="s">
         <v>679</v>
       </c>
-      <c r="T47" s="82"/>
-      <c r="U47" s="82"/>
-      <c r="V47" s="82"/>
-    </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.45">
-      <c r="V48" s="2"/>
+      <c r="T48" s="91" t="s">
+        <v>696</v>
+      </c>
+      <c r="U48" s="91"/>
+      <c r="V48" s="91"/>
     </row>
     <row r="49" spans="22:22" x14ac:dyDescent="0.45">
       <c r="V49" s="2"/>
+    </row>
+    <row r="50" spans="22:22" x14ac:dyDescent="0.45">
+      <c r="V50" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="19" type="noConversion"/>
   <dataValidations count="3">
     <dataValidation errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1" xr:uid="{00000000-0002-0000-0300-000000000000}"/>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid value" error="Valid property styles are &quot;element&quot;, &quot;attribute&quot;, or &quot;abstract&quot;.  Leave the cell blank to use the default value &quot;element&quot;." promptTitle="Property Style" prompt="- &quot;element&quot; or blank (default) - Represents a typical NIEM property._x000a_- &quot;abstract&quot; - Used to create a substitution group_x000a_- &quot;attribute&quot; - Use sparingly, if at all; for values tightly-coupled to an element." sqref="X50:X1048576 W2:W47" xr:uid="{00000000-0002-0000-0300-000002000000}">
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid value" error="Valid property styles are &quot;element&quot;, &quot;attribute&quot;, or &quot;abstract&quot;.  Leave the cell blank to use the default value &quot;element&quot;." promptTitle="Property Style" prompt="- &quot;element&quot; or blank (default) - Represents a typical NIEM property._x000a_- &quot;abstract&quot; - Used to create a substitution group_x000a_- &quot;attribute&quot; - Use sparingly, if at all; for values tightly-coupled to an element." sqref="X51:X1048576 W2:W41 W43:W48 V42" xr:uid="{00000000-0002-0000-0300-000002000000}">
       <formula1>"element,attribute,abstract"</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576 O42:O47" xr:uid="{00000000-0002-0000-0300-000001000000}">
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O43:O48 G2:G41 G43:G1048576" xr:uid="{00000000-0002-0000-0300-000001000000}">
       <formula1>MAPPING_CODES</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Added j:BookingDocumentControlIndeitifcation to ChargeFiling
</commit_message>
<xml_diff>
--- a/schemas/ChargeFiling_iepd/artifacts/ChargeFiling_MappingSpreadsheet.xlsx
+++ b/schemas/ChargeFiling_iepd/artifacts/ChargeFiling_MappingSpreadsheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JamesCabral\git\JTMP-Data-Exchange-Specs\schemas\ChargeFiling_iepd\artifacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C31E1079-9A7D-49F6-B915-B45011BAB5B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75F8218F-E832-496F-BFB8-56EB16D65AD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22980" yWindow="-21360" windowWidth="26865" windowHeight="19245" tabRatio="781" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21735" yWindow="-21600" windowWidth="26010" windowHeight="20985" tabRatio="781" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="9" state="hidden" r:id="rId1"/>
@@ -163,7 +163,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1190" uniqueCount="697">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1205" uniqueCount="701">
   <si>
     <t xml:space="preserve">Template last updated: </t>
   </si>
@@ -2952,6 +2952,18 @@
   </si>
   <si>
     <t>nc:BinaryType (nc:BinaryObjectAbstract)</t>
+  </si>
+  <si>
+    <t>FolderNumber</t>
+  </si>
+  <si>
+    <t>A Person ID for single continuous term of incarceration. If the individual is released today and returns tomorrow, a new folder number will be issued.</t>
+  </si>
+  <si>
+    <t>j:Arrest/nola-ext:ArrestAugmentation/j:Booking/j:BookingDocumentControlIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>An identification assigned by a booking system to identify a unique booking event within a specific jail.</t>
   </si>
 </sst>
 </file>
@@ -3126,7 +3138,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3181,6 +3193,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="22"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -3584,31 +3602,29 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="71">
@@ -7592,10 +7608,10 @@
   <dimension ref="A1:AB50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C39" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="J40" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E39" sqref="E39"/>
+      <selection pane="bottomRight" activeCell="V44" sqref="V44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -9497,376 +9513,392 @@
       </c>
       <c r="V41" s="2"/>
     </row>
-    <row r="42" spans="1:22" s="94" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A42" s="95" t="s">
+    <row r="42" spans="1:22" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A42" s="91" t="s">
         <v>687</v>
       </c>
-      <c r="B42" s="97" t="s">
+      <c r="B42" s="93" t="s">
         <v>688</v>
       </c>
-      <c r="C42" s="97" t="s">
+      <c r="C42" s="93" t="s">
         <v>346</v>
       </c>
-      <c r="D42" s="97" t="s">
+      <c r="D42" s="93" t="s">
         <v>689</v>
       </c>
-      <c r="E42" s="97"/>
-      <c r="F42" s="98" t="s">
+      <c r="E42" s="93"/>
+      <c r="F42" s="84" t="s">
         <v>693</v>
       </c>
-      <c r="G42" s="97"/>
-      <c r="H42" s="97"/>
-      <c r="I42" s="93"/>
-      <c r="J42" s="96" t="s">
+      <c r="G42" s="93"/>
+      <c r="H42" s="93"/>
+      <c r="I42" s="2"/>
+      <c r="J42" s="92" t="s">
         <v>3</v>
       </c>
-      <c r="K42" s="96" t="s">
+      <c r="K42" s="92" t="s">
         <v>688</v>
       </c>
-      <c r="L42" s="96" t="s">
+      <c r="L42" s="92" t="s">
         <v>346</v>
       </c>
-      <c r="M42" s="96" t="s">
+      <c r="M42" s="92" t="s">
         <v>689</v>
       </c>
-      <c r="N42" s="92" t="s">
+      <c r="N42" s="84" t="s">
         <v>415</v>
       </c>
-      <c r="O42" s="97"/>
-      <c r="P42" s="97" t="s">
+      <c r="O42" s="93"/>
+      <c r="P42" s="93" t="s">
         <v>690</v>
       </c>
-      <c r="Q42" s="93" t="s">
+      <c r="Q42" s="2" t="s">
         <v>690</v>
       </c>
-      <c r="R42" s="96" t="s">
+      <c r="R42" s="92" t="s">
         <v>691</v>
       </c>
-      <c r="S42" s="97" t="s">
+      <c r="S42" s="93" t="s">
         <v>355</v>
       </c>
-      <c r="T42" s="99" t="s">
+      <c r="T42" t="s">
         <v>692</v>
       </c>
-      <c r="U42" s="99"/>
-      <c r="V42" s="99"/>
     </row>
     <row r="43" spans="1:22" ht="57" x14ac:dyDescent="0.45">
-      <c r="B43" s="91" t="s">
+      <c r="B43" s="2" t="s">
         <v>655</v>
       </c>
-      <c r="C43" s="91" t="s">
+      <c r="C43" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D43" s="100" t="s">
+      <c r="D43" s="87" t="s">
         <v>656</v>
       </c>
-      <c r="E43" s="100"/>
-      <c r="F43" s="92"/>
-      <c r="G43" s="91" t="s">
+      <c r="G43" s="2" t="s">
         <v>655</v>
       </c>
-      <c r="H43" s="91"/>
-      <c r="I43" s="91"/>
-      <c r="J43" s="91" t="s">
+      <c r="J43" s="2" t="s">
         <v>655</v>
       </c>
-      <c r="K43" s="91" t="s">
+      <c r="K43" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="L43" s="91"/>
-      <c r="M43" s="100" t="s">
+      <c r="M43" s="87" t="s">
         <v>656</v>
       </c>
-      <c r="N43" s="92"/>
-      <c r="O43" s="91"/>
-      <c r="P43" s="91" t="s">
+      <c r="N43" s="84"/>
+      <c r="P43" s="2" t="s">
         <v>681</v>
       </c>
-      <c r="Q43" s="91" t="s">
+      <c r="Q43" s="2" t="s">
         <v>694</v>
       </c>
-      <c r="R43" s="91" t="s">
+      <c r="R43" s="2" t="s">
         <v>657</v>
       </c>
-      <c r="S43" s="91" t="s">
+      <c r="S43" s="2" t="s">
         <v>694</v>
       </c>
-      <c r="T43" s="91" t="s">
+      <c r="T43" s="87" t="s">
+        <v>656</v>
+      </c>
+      <c r="V43" s="2"/>
+    </row>
+    <row r="44" spans="1:22" ht="57" x14ac:dyDescent="0.45">
+      <c r="B44" s="2" t="s">
+        <v>658</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>659</v>
+      </c>
+      <c r="D44" s="87" t="s">
+        <v>660</v>
+      </c>
+      <c r="F44" s="84" t="s">
+        <v>351</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>658</v>
+      </c>
+      <c r="J44" s="2" t="s">
+        <v>655</v>
+      </c>
+      <c r="K44" s="2" t="s">
+        <v>658</v>
+      </c>
+      <c r="L44" s="2" t="s">
+        <v>659</v>
+      </c>
+      <c r="M44" s="87" t="s">
+        <v>660</v>
+      </c>
+      <c r="N44" s="84" t="s">
+        <v>351</v>
+      </c>
+      <c r="P44" s="2" t="s">
+        <v>682</v>
+      </c>
+      <c r="Q44" s="2" t="s">
         <v>694</v>
       </c>
-      <c r="U43" s="91"/>
-      <c r="V43" s="91"/>
-    </row>
-    <row r="44" spans="1:22" ht="57" x14ac:dyDescent="0.45">
-      <c r="B44" s="91" t="s">
-        <v>658</v>
-      </c>
-      <c r="C44" s="91" t="s">
-        <v>659</v>
-      </c>
-      <c r="D44" s="100" t="s">
+      <c r="R44" s="2" t="s">
+        <v>661</v>
+      </c>
+      <c r="S44" s="2" t="s">
+        <v>662</v>
+      </c>
+      <c r="T44" s="87" t="s">
         <v>660</v>
       </c>
-      <c r="E44" s="100"/>
-      <c r="F44" s="92" t="s">
+      <c r="V44" s="2"/>
+    </row>
+    <row r="45" spans="1:22" ht="57" x14ac:dyDescent="0.45">
+      <c r="B45" s="2" t="s">
+        <v>663</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="D45" s="87" t="s">
+        <v>664</v>
+      </c>
+      <c r="F45" s="84" t="s">
+        <v>665</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>663</v>
+      </c>
+      <c r="J45" s="2" t="s">
+        <v>655</v>
+      </c>
+      <c r="K45" s="2" t="s">
+        <v>663</v>
+      </c>
+      <c r="L45" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="M45" s="87" t="s">
+        <v>664</v>
+      </c>
+      <c r="N45" s="84" t="s">
+        <v>665</v>
+      </c>
+      <c r="P45" s="2" t="s">
+        <v>683</v>
+      </c>
+      <c r="Q45" s="2" t="s">
+        <v>695</v>
+      </c>
+      <c r="R45" s="2" t="s">
+        <v>666</v>
+      </c>
+      <c r="S45" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="T45" s="87" t="s">
+        <v>664</v>
+      </c>
+      <c r="V45" s="2"/>
+    </row>
+    <row r="46" spans="1:22" ht="57" x14ac:dyDescent="0.45">
+      <c r="B46" s="2" t="s">
+        <v>667</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="D46" s="87" t="s">
+        <v>668</v>
+      </c>
+      <c r="F46" s="84" t="s">
+        <v>665</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>667</v>
+      </c>
+      <c r="J46" s="2" t="s">
+        <v>655</v>
+      </c>
+      <c r="K46" s="2" t="s">
+        <v>667</v>
+      </c>
+      <c r="L46" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="M46" s="87" t="s">
+        <v>668</v>
+      </c>
+      <c r="N46" s="84" t="s">
+        <v>665</v>
+      </c>
+      <c r="P46" s="2" t="s">
+        <v>684</v>
+      </c>
+      <c r="Q46" s="2" t="s">
+        <v>694</v>
+      </c>
+      <c r="R46" s="2" t="s">
+        <v>669</v>
+      </c>
+      <c r="S46" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="T46" s="87" t="s">
+        <v>668</v>
+      </c>
+      <c r="V46" s="2"/>
+    </row>
+    <row r="47" spans="1:22" ht="57" x14ac:dyDescent="0.45">
+      <c r="B47" s="2" t="s">
+        <v>670</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="D47" s="87" t="s">
+        <v>672</v>
+      </c>
+      <c r="F47" s="84" t="s">
         <v>351</v>
       </c>
-      <c r="G44" s="91" t="s">
-        <v>658</v>
-      </c>
-      <c r="H44" s="91"/>
-      <c r="I44" s="91"/>
-      <c r="J44" s="91" t="s">
+      <c r="G47" s="2" t="s">
+        <v>670</v>
+      </c>
+      <c r="J47" s="2" t="s">
         <v>655</v>
       </c>
-      <c r="K44" s="91" t="s">
-        <v>658</v>
-      </c>
-      <c r="L44" s="91" t="s">
-        <v>659</v>
-      </c>
-      <c r="M44" s="100" t="s">
-        <v>660</v>
-      </c>
-      <c r="N44" s="92" t="s">
+      <c r="K47" s="2" t="s">
+        <v>670</v>
+      </c>
+      <c r="L47" s="2" t="s">
+        <v>671</v>
+      </c>
+      <c r="M47" s="87" t="s">
+        <v>672</v>
+      </c>
+      <c r="N47" s="84" t="s">
         <v>351</v>
       </c>
-      <c r="O44" s="91"/>
-      <c r="P44" s="91" t="s">
-        <v>682</v>
-      </c>
-      <c r="Q44" s="91" t="s">
+      <c r="P47" s="2" t="s">
+        <v>685</v>
+      </c>
+      <c r="Q47" s="2" t="s">
         <v>694</v>
       </c>
-      <c r="R44" s="91" t="s">
-        <v>661</v>
-      </c>
-      <c r="S44" s="91" t="s">
-        <v>662</v>
-      </c>
-      <c r="T44" s="91" t="s">
-        <v>694</v>
-      </c>
-      <c r="U44" s="91"/>
-      <c r="V44" s="91"/>
-    </row>
-    <row r="45" spans="1:22" ht="57" x14ac:dyDescent="0.45">
-      <c r="B45" s="91" t="s">
-        <v>663</v>
-      </c>
-      <c r="C45" s="91" t="s">
+      <c r="R47" s="2" t="s">
+        <v>673</v>
+      </c>
+      <c r="S47" s="2" t="s">
+        <v>674</v>
+      </c>
+      <c r="T47" s="87" t="s">
+        <v>672</v>
+      </c>
+      <c r="V47" s="2"/>
+    </row>
+    <row r="48" spans="1:22" ht="57" x14ac:dyDescent="0.45">
+      <c r="B48" s="2" t="s">
+        <v>675</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>680</v>
+      </c>
+      <c r="D48" s="87" t="s">
+        <v>677</v>
+      </c>
+      <c r="F48" s="84" t="s">
+        <v>351</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>675</v>
+      </c>
+      <c r="J48" s="2" t="s">
+        <v>655</v>
+      </c>
+      <c r="K48" s="2" t="s">
+        <v>675</v>
+      </c>
+      <c r="L48" s="2" t="s">
+        <v>676</v>
+      </c>
+      <c r="M48" s="87" t="s">
+        <v>677</v>
+      </c>
+      <c r="N48" s="84" t="s">
+        <v>351</v>
+      </c>
+      <c r="P48" s="2" t="s">
+        <v>686</v>
+      </c>
+      <c r="Q48" s="2" t="s">
+        <v>696</v>
+      </c>
+      <c r="R48" s="2" t="s">
+        <v>678</v>
+      </c>
+      <c r="S48" s="2" t="s">
+        <v>679</v>
+      </c>
+      <c r="T48" s="87" t="s">
+        <v>677</v>
+      </c>
+      <c r="V48" s="2"/>
+    </row>
+    <row r="49" spans="1:22" s="97" customFormat="1" ht="99.75" x14ac:dyDescent="0.45">
+      <c r="A49" s="96" t="s">
+        <v>687</v>
+      </c>
+      <c r="B49" s="100" t="s">
+        <v>697</v>
+      </c>
+      <c r="C49" s="99" t="s">
         <v>346</v>
       </c>
-      <c r="D45" s="100" t="s">
-        <v>664</v>
-      </c>
-      <c r="E45" s="100"/>
-      <c r="F45" s="92" t="s">
-        <v>665</v>
-      </c>
-      <c r="G45" s="91" t="s">
-        <v>663</v>
-      </c>
-      <c r="H45" s="91"/>
-      <c r="I45" s="91"/>
-      <c r="J45" s="91" t="s">
-        <v>655</v>
-      </c>
-      <c r="K45" s="91" t="s">
-        <v>663</v>
-      </c>
-      <c r="L45" s="91" t="s">
+      <c r="D49" s="100" t="s">
+        <v>698</v>
+      </c>
+      <c r="E49" s="99"/>
+      <c r="F49" s="99"/>
+      <c r="G49" s="100" t="s">
+        <v>351</v>
+      </c>
+      <c r="H49" s="100" t="s">
+        <v>697</v>
+      </c>
+      <c r="I49" s="100"/>
+      <c r="J49" s="94" t="s">
+        <v>408</v>
+      </c>
+      <c r="K49" s="94" t="s">
+        <v>697</v>
+      </c>
+      <c r="L49" s="94" t="s">
         <v>346</v>
       </c>
-      <c r="M45" s="100" t="s">
-        <v>664</v>
-      </c>
-      <c r="N45" s="92" t="s">
-        <v>665</v>
-      </c>
-      <c r="O45" s="91"/>
-      <c r="P45" s="91" t="s">
-        <v>683</v>
-      </c>
-      <c r="Q45" s="91" t="s">
-        <v>695</v>
-      </c>
-      <c r="R45" s="91" t="s">
-        <v>666</v>
-      </c>
-      <c r="S45" s="91" t="s">
-        <v>355</v>
-      </c>
-      <c r="T45" s="91" t="s">
-        <v>695</v>
-      </c>
-      <c r="U45" s="91"/>
-      <c r="V45" s="91"/>
-    </row>
-    <row r="46" spans="1:22" ht="57" x14ac:dyDescent="0.45">
-      <c r="B46" s="91" t="s">
-        <v>667</v>
-      </c>
-      <c r="C46" s="91" t="s">
-        <v>346</v>
-      </c>
-      <c r="D46" s="100" t="s">
-        <v>668</v>
-      </c>
-      <c r="E46" s="100"/>
-      <c r="F46" s="92" t="s">
-        <v>665</v>
-      </c>
-      <c r="G46" s="91" t="s">
-        <v>667</v>
-      </c>
-      <c r="H46" s="91"/>
-      <c r="I46" s="91"/>
-      <c r="J46" s="91" t="s">
-        <v>655</v>
-      </c>
-      <c r="K46" s="91" t="s">
-        <v>667</v>
-      </c>
-      <c r="L46" s="91" t="s">
-        <v>346</v>
-      </c>
-      <c r="M46" s="100" t="s">
-        <v>668</v>
-      </c>
-      <c r="N46" s="92" t="s">
-        <v>665</v>
-      </c>
-      <c r="O46" s="91"/>
-      <c r="P46" s="91" t="s">
-        <v>684</v>
-      </c>
-      <c r="Q46" s="91" t="s">
-        <v>694</v>
-      </c>
-      <c r="R46" s="91" t="s">
-        <v>669</v>
-      </c>
-      <c r="S46" s="91" t="s">
+      <c r="M49" s="94" t="s">
+        <v>698</v>
+      </c>
+      <c r="N49" s="94" t="s">
+        <v>351</v>
+      </c>
+      <c r="O49" s="94"/>
+      <c r="P49" s="94" t="s">
+        <v>699</v>
+      </c>
+      <c r="Q49" s="95"/>
+      <c r="R49" s="98" t="s">
+        <v>374</v>
+      </c>
+      <c r="S49" s="98" t="s">
         <v>375</v>
       </c>
-      <c r="T46" s="91" t="s">
-        <v>694</v>
-      </c>
-      <c r="U46" s="91"/>
-      <c r="V46" s="91"/>
-    </row>
-    <row r="47" spans="1:22" ht="57" x14ac:dyDescent="0.45">
-      <c r="B47" s="91" t="s">
-        <v>670</v>
-      </c>
-      <c r="C47" s="91" t="s">
-        <v>271</v>
-      </c>
-      <c r="D47" s="100" t="s">
-        <v>672</v>
-      </c>
-      <c r="E47" s="100"/>
-      <c r="F47" s="92" t="s">
-        <v>351</v>
-      </c>
-      <c r="G47" s="91" t="s">
-        <v>670</v>
-      </c>
-      <c r="H47" s="91"/>
-      <c r="I47" s="91"/>
-      <c r="J47" s="91" t="s">
-        <v>655</v>
-      </c>
-      <c r="K47" s="91" t="s">
-        <v>670</v>
-      </c>
-      <c r="L47" s="91" t="s">
-        <v>671</v>
-      </c>
-      <c r="M47" s="100" t="s">
-        <v>672</v>
-      </c>
-      <c r="N47" s="92" t="s">
-        <v>351</v>
-      </c>
-      <c r="O47" s="91"/>
-      <c r="P47" s="91" t="s">
-        <v>685</v>
-      </c>
-      <c r="Q47" s="91" t="s">
-        <v>694</v>
-      </c>
-      <c r="R47" s="91" t="s">
-        <v>673</v>
-      </c>
-      <c r="S47" s="91" t="s">
-        <v>674</v>
-      </c>
-      <c r="T47" s="91" t="s">
-        <v>694</v>
-      </c>
-      <c r="U47" s="91"/>
-      <c r="V47" s="91"/>
-    </row>
-    <row r="48" spans="1:22" ht="57" x14ac:dyDescent="0.45">
-      <c r="B48" s="91" t="s">
-        <v>675</v>
-      </c>
-      <c r="C48" s="91" t="s">
-        <v>680</v>
-      </c>
-      <c r="D48" s="100" t="s">
-        <v>677</v>
-      </c>
-      <c r="E48" s="100"/>
-      <c r="F48" s="92" t="s">
-        <v>351</v>
-      </c>
-      <c r="G48" s="91" t="s">
-        <v>675</v>
-      </c>
-      <c r="H48" s="91"/>
-      <c r="I48" s="91"/>
-      <c r="J48" s="91" t="s">
-        <v>655</v>
-      </c>
-      <c r="K48" s="91" t="s">
-        <v>675</v>
-      </c>
-      <c r="L48" s="91" t="s">
-        <v>676</v>
-      </c>
-      <c r="M48" s="100" t="s">
-        <v>677</v>
-      </c>
-      <c r="N48" s="92" t="s">
-        <v>351</v>
-      </c>
-      <c r="O48" s="91"/>
-      <c r="P48" s="91" t="s">
-        <v>686</v>
-      </c>
-      <c r="Q48" s="91" t="s">
-        <v>696</v>
-      </c>
-      <c r="R48" s="91" t="s">
-        <v>678</v>
-      </c>
-      <c r="S48" s="91" t="s">
-        <v>679</v>
-      </c>
-      <c r="T48" s="91" t="s">
-        <v>696</v>
-      </c>
-      <c r="U48" s="91"/>
-      <c r="V48" s="91"/>
-    </row>
-    <row r="49" spans="22:22" x14ac:dyDescent="0.45">
-      <c r="V49" s="2"/>
-    </row>
-    <row r="50" spans="22:22" x14ac:dyDescent="0.45">
+      <c r="T49" s="98" t="s">
+        <v>700</v>
+      </c>
+      <c r="V49" s="99"/>
+    </row>
+    <row r="50" spans="1:22" x14ac:dyDescent="0.45">
       <c r="V50" s="2"/>
     </row>
   </sheetData>
@@ -9876,7 +9908,7 @@
     <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid value" error="Valid property styles are &quot;element&quot;, &quot;attribute&quot;, or &quot;abstract&quot;.  Leave the cell blank to use the default value &quot;element&quot;." promptTitle="Property Style" prompt="- &quot;element&quot; or blank (default) - Represents a typical NIEM property._x000a_- &quot;abstract&quot; - Used to create a substitution group_x000a_- &quot;attribute&quot; - Use sparingly, if at all; for values tightly-coupled to an element." sqref="X51:X1048576 W2:W41 W43:W48 V42" xr:uid="{00000000-0002-0000-0300-000002000000}">
       <formula1>"element,attribute,abstract"</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O43:O48 G2:G41 G43:G1048576" xr:uid="{00000000-0002-0000-0300-000001000000}">
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O43:O48 G2:G41 G43:G1048576 N49" xr:uid="{00000000-0002-0000-0300-000001000000}">
       <formula1>MAPPING_CODES</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Moved ArrestIncident in ChargeFiling to ChargeAugmentation
</commit_message>
<xml_diff>
--- a/schemas/ChargeFiling_iepd/artifacts/ChargeFiling_MappingSpreadsheet.xlsx
+++ b/schemas/ChargeFiling_iepd/artifacts/ChargeFiling_MappingSpreadsheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JamesCabral\git\JTMP-Data-Exchange-Specs\schemas\ChargeFiling_iepd\artifacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75F8218F-E832-496F-BFB8-56EB16D65AD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05ACBEA7-0281-4E10-91D5-B37EFA98F6F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21735" yWindow="-21600" windowWidth="26010" windowHeight="20985" tabRatio="781" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-4080" yWindow="-21720" windowWidth="51840" windowHeight="21120" tabRatio="781" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="9" state="hidden" r:id="rId1"/>
@@ -1900,9 +1900,6 @@
 The Item # is the incident number assigned by the Computer Aided Dispatching. It will be included on all arrest paperwork submitted by the arresting officer.</t>
   </si>
   <si>
-    <t>j:Arrest/nola-ext:ArrestAugmentation/nola-ext:ArrestIncident/nc:ActivityIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
     <t>nc:IdentificationType (nc:ActivityIdentification)</t>
   </si>
   <si>
@@ -2964,6 +2961,9 @@
   </si>
   <si>
     <t>An identification assigned by a booking system to identify a unique booking event within a specific jail.</t>
+  </si>
+  <si>
+    <t>j:Arrest/j:ArrestCharge/nola-ext:ChargeAugmentation/nola-ext:ArrestIncident/nc:ActivityIdentification/nc:IdentificationID</t>
   </si>
 </sst>
 </file>
@@ -3354,7 +3354,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3619,11 +3619,7 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -7608,10 +7604,10 @@
   <dimension ref="A1:AB50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="J40" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="J12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="V44" sqref="V44"/>
+      <selection pane="bottomRight" activeCell="P18" sqref="P18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -8416,10 +8412,10 @@
         <v>351</v>
       </c>
       <c r="P17" s="82" t="s">
+        <v>700</v>
+      </c>
+      <c r="Q17" s="82" t="s">
         <v>445</v>
-      </c>
-      <c r="Q17" s="82" t="s">
-        <v>446</v>
       </c>
       <c r="R17" s="82" t="s">
         <v>374</v>
@@ -8428,13 +8424,13 @@
         <v>396</v>
       </c>
       <c r="T17" s="82" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="V17" s="2"/>
     </row>
     <row r="18" spans="2:22" ht="71.25" x14ac:dyDescent="0.45">
       <c r="B18" s="2" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>100</v>
@@ -8449,22 +8445,22 @@
         <v>408</v>
       </c>
       <c r="K18" s="82" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="L18" s="82" t="s">
         <v>398</v>
       </c>
       <c r="M18" s="82" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="N18" s="82">
         <v>1</v>
       </c>
       <c r="P18" s="82" t="s">
+        <v>450</v>
+      </c>
+      <c r="Q18" s="82" t="s">
         <v>451</v>
-      </c>
-      <c r="Q18" s="82" t="s">
-        <v>452</v>
       </c>
       <c r="R18" s="82" t="s">
         <v>404</v>
@@ -8473,58 +8469,58 @@
         <v>405</v>
       </c>
       <c r="T18" s="82" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="V18" s="2"/>
     </row>
     <row r="19" spans="2:22" ht="99.75" x14ac:dyDescent="0.45">
       <c r="B19" s="2" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>346</v>
       </c>
       <c r="E19" s="87" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="F19" s="84">
         <v>1</v>
       </c>
       <c r="J19" s="2" t="s">
+        <v>454</v>
+      </c>
+      <c r="K19" s="2" t="s">
         <v>455</v>
-      </c>
-      <c r="K19" s="2" t="s">
-        <v>456</v>
       </c>
       <c r="L19" s="2" t="s">
         <v>346</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="N19" s="2" t="s">
         <v>351</v>
       </c>
       <c r="P19" s="2" t="s">
+        <v>457</v>
+      </c>
+      <c r="Q19" s="2" t="s">
         <v>458</v>
       </c>
-      <c r="Q19" s="2" t="s">
+      <c r="R19" s="2" t="s">
         <v>459</v>
       </c>
-      <c r="R19" s="2" t="s">
+      <c r="S19" s="2" t="s">
         <v>460</v>
       </c>
-      <c r="S19" s="2" t="s">
+      <c r="T19" s="2" t="s">
         <v>461</v>
-      </c>
-      <c r="T19" s="2" t="s">
-        <v>462</v>
       </c>
       <c r="V19" s="2"/>
     </row>
     <row r="20" spans="2:22" ht="85.5" x14ac:dyDescent="0.45">
       <c r="B20" s="2" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>398</v>
@@ -8536,25 +8532,25 @@
         <v>1</v>
       </c>
       <c r="J20" s="2" t="s">
+        <v>463</v>
+      </c>
+      <c r="K20" s="2" t="s">
         <v>464</v>
-      </c>
-      <c r="K20" s="2" t="s">
-        <v>465</v>
       </c>
       <c r="L20" s="2" t="s">
         <v>398</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="N20" s="2" t="s">
         <v>351</v>
       </c>
       <c r="P20" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="Q20" s="2" t="s">
         <v>467</v>
-      </c>
-      <c r="Q20" s="2" t="s">
-        <v>468</v>
       </c>
       <c r="R20" s="2" t="s">
         <v>404</v>
@@ -8563,313 +8559,313 @@
         <v>405</v>
       </c>
       <c r="T20" s="2" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="V20" s="2"/>
     </row>
     <row r="21" spans="2:22" ht="99.75" x14ac:dyDescent="0.45">
       <c r="J21" s="2" t="s">
+        <v>468</v>
+      </c>
+      <c r="K21" s="2" t="s">
         <v>469</v>
-      </c>
-      <c r="K21" s="2" t="s">
-        <v>470</v>
       </c>
       <c r="L21" s="2" t="s">
         <v>346</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="N21" s="2" t="s">
         <v>351</v>
       </c>
       <c r="P21" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="Q21" s="2" t="s">
         <v>472</v>
       </c>
-      <c r="Q21" s="2" t="s">
+      <c r="R21" s="2" t="s">
         <v>473</v>
-      </c>
-      <c r="R21" s="2" t="s">
-        <v>474</v>
       </c>
       <c r="S21" s="2" t="s">
         <v>375</v>
       </c>
       <c r="T21" s="2" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="V21" s="2"/>
     </row>
     <row r="22" spans="2:22" ht="114" x14ac:dyDescent="0.45">
       <c r="B22" s="2" t="s">
+        <v>475</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>476</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="E22" s="87" t="s">
         <v>477</v>
-      </c>
-      <c r="E22" s="87" t="s">
-        <v>478</v>
       </c>
       <c r="F22" s="84">
         <v>1</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="K22" s="2" t="s">
+        <v>478</v>
+      </c>
+      <c r="L22" s="2" t="s">
         <v>479</v>
       </c>
-      <c r="L22" s="2" t="s">
+      <c r="M22" s="2" t="s">
         <v>480</v>
-      </c>
-      <c r="M22" s="2" t="s">
-        <v>481</v>
       </c>
       <c r="N22" s="2" t="s">
         <v>351</v>
       </c>
       <c r="P22" s="2" t="s">
+        <v>481</v>
+      </c>
+      <c r="Q22" s="2" t="s">
         <v>482</v>
       </c>
-      <c r="Q22" s="2" t="s">
+      <c r="R22" s="2" t="s">
         <v>483</v>
-      </c>
-      <c r="R22" s="2" t="s">
-        <v>484</v>
       </c>
       <c r="S22" s="2" t="s">
         <v>355</v>
       </c>
       <c r="T22" s="2" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="V22" s="2"/>
     </row>
     <row r="23" spans="2:22" ht="128.25" x14ac:dyDescent="0.45">
       <c r="J23" s="2" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="K23" s="2" t="s">
+        <v>485</v>
+      </c>
+      <c r="L23" s="2" t="s">
         <v>486</v>
       </c>
-      <c r="L23" s="2" t="s">
+      <c r="M23" s="2" t="s">
         <v>487</v>
-      </c>
-      <c r="M23" s="2" t="s">
-        <v>488</v>
       </c>
       <c r="N23" s="2" t="s">
         <v>415</v>
       </c>
       <c r="P23" s="2" t="s">
+        <v>488</v>
+      </c>
+      <c r="Q23" s="2" t="s">
         <v>489</v>
       </c>
-      <c r="Q23" s="2" t="s">
+      <c r="R23" s="2" t="s">
         <v>490</v>
       </c>
-      <c r="R23" s="2" t="s">
+      <c r="S23" s="2" t="s">
         <v>491</v>
       </c>
-      <c r="S23" s="2" t="s">
+      <c r="T23" s="2" t="s">
         <v>492</v>
-      </c>
-      <c r="T23" s="2" t="s">
-        <v>493</v>
       </c>
       <c r="V23" s="2"/>
     </row>
     <row r="24" spans="2:22" ht="71.25" x14ac:dyDescent="0.45">
       <c r="B24" s="2" t="s">
+        <v>493</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>494</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="D24" s="2" t="s">
         <v>495</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>496</v>
       </c>
       <c r="F24" s="84" t="s">
         <v>415</v>
       </c>
       <c r="J24" s="2" t="s">
+        <v>496</v>
+      </c>
+      <c r="K24" s="2" t="s">
         <v>497</v>
-      </c>
-      <c r="K24" s="2" t="s">
-        <v>498</v>
       </c>
       <c r="L24" s="2" t="s">
         <v>346</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="N24" s="84" t="s">
         <v>415</v>
       </c>
       <c r="P24" s="2" t="s">
+        <v>499</v>
+      </c>
+      <c r="Q24" s="2" t="s">
         <v>500</v>
       </c>
-      <c r="Q24" s="2" t="s">
+      <c r="R24" s="2" t="s">
         <v>501</v>
       </c>
-      <c r="R24" s="2" t="s">
+      <c r="S24" s="2" t="s">
         <v>502</v>
       </c>
-      <c r="S24" s="2" t="s">
+      <c r="T24" s="2" t="s">
         <v>503</v>
-      </c>
-      <c r="T24" s="2" t="s">
-        <v>504</v>
       </c>
       <c r="V24" s="2"/>
     </row>
     <row r="25" spans="2:22" ht="127.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B25" s="2" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>346</v>
       </c>
       <c r="D25" s="2" t="s">
+        <v>505</v>
+      </c>
+      <c r="E25" s="87" t="s">
         <v>506</v>
-      </c>
-      <c r="E25" s="87" t="s">
-        <v>507</v>
       </c>
       <c r="F25" s="84">
         <v>1</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="L25" s="2" t="s">
         <v>346</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="N25" s="2" t="s">
         <v>351</v>
       </c>
       <c r="P25" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="Q25" s="2" t="s">
+        <v>502</v>
+      </c>
+      <c r="R25" s="2" t="s">
         <v>510</v>
       </c>
-      <c r="Q25" s="2" t="s">
-        <v>503</v>
-      </c>
-      <c r="R25" s="2" t="s">
+      <c r="S25" s="2" t="s">
         <v>511</v>
       </c>
-      <c r="S25" s="2" t="s">
+      <c r="T25" s="2" t="s">
         <v>512</v>
-      </c>
-      <c r="T25" s="2" t="s">
-        <v>513</v>
       </c>
       <c r="V25" s="2"/>
     </row>
     <row r="26" spans="2:22" ht="99.75" x14ac:dyDescent="0.45">
       <c r="B26" s="2" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>346</v>
       </c>
       <c r="D26" s="2" t="s">
+        <v>514</v>
+      </c>
+      <c r="E26" s="87" t="s">
         <v>515</v>
-      </c>
-      <c r="E26" s="87" t="s">
-        <v>516</v>
       </c>
       <c r="F26" s="84" t="s">
         <v>351</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="L26" s="2" t="s">
         <v>346</v>
       </c>
       <c r="M26" s="2" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="N26" s="2" t="s">
         <v>351</v>
       </c>
       <c r="P26" s="2" t="s">
+        <v>518</v>
+      </c>
+      <c r="Q26" s="2" t="s">
+        <v>502</v>
+      </c>
+      <c r="R26" s="2" t="s">
         <v>519</v>
       </c>
-      <c r="Q26" s="2" t="s">
-        <v>503</v>
-      </c>
-      <c r="R26" s="2" t="s">
+      <c r="S26" s="2" t="s">
+        <v>511</v>
+      </c>
+      <c r="T26" s="2" t="s">
         <v>520</v>
-      </c>
-      <c r="S26" s="2" t="s">
-        <v>512</v>
-      </c>
-      <c r="T26" s="2" t="s">
-        <v>521</v>
       </c>
       <c r="V26" s="2"/>
     </row>
     <row r="27" spans="2:22" ht="85.5" x14ac:dyDescent="0.45">
       <c r="B27" s="2" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>346</v>
       </c>
       <c r="D27" s="2" t="s">
+        <v>522</v>
+      </c>
+      <c r="E27" s="87" t="s">
         <v>523</v>
-      </c>
-      <c r="E27" s="87" t="s">
-        <v>524</v>
       </c>
       <c r="F27" s="84">
         <v>1</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="L27" s="2" t="s">
         <v>346</v>
       </c>
       <c r="M27" s="2" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="N27" s="2" t="s">
         <v>351</v>
       </c>
       <c r="P27" s="2" t="s">
+        <v>525</v>
+      </c>
+      <c r="Q27" s="2" t="s">
+        <v>502</v>
+      </c>
+      <c r="R27" s="2" t="s">
         <v>526</v>
       </c>
-      <c r="Q27" s="2" t="s">
-        <v>503</v>
-      </c>
-      <c r="R27" s="2" t="s">
+      <c r="S27" s="2" t="s">
+        <v>511</v>
+      </c>
+      <c r="T27" s="2" t="s">
         <v>527</v>
-      </c>
-      <c r="S27" s="2" t="s">
-        <v>512</v>
-      </c>
-      <c r="T27" s="2" t="s">
-        <v>528</v>
       </c>
       <c r="V27" s="2"/>
     </row>
     <row r="28" spans="2:22" ht="99.75" x14ac:dyDescent="0.45">
       <c r="B28" s="2" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>346</v>
@@ -8878,25 +8874,25 @@
         <v>351</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="L28" s="2" t="s">
         <v>346</v>
       </c>
       <c r="M28" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="N28" s="2" t="s">
         <v>351</v>
       </c>
       <c r="P28" s="2" t="s">
+        <v>531</v>
+      </c>
+      <c r="Q28" s="2" t="s">
         <v>532</v>
-      </c>
-      <c r="Q28" s="2" t="s">
-        <v>533</v>
       </c>
       <c r="R28" s="2" t="s">
         <v>374</v>
@@ -8905,115 +8901,115 @@
         <v>375</v>
       </c>
       <c r="T28" s="2" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="V28" s="2"/>
     </row>
     <row r="29" spans="2:22" ht="99.75" x14ac:dyDescent="0.45">
       <c r="B29" s="2" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>346</v>
       </c>
       <c r="D29" s="2" t="s">
+        <v>535</v>
+      </c>
+      <c r="E29" s="87" t="s">
         <v>536</v>
-      </c>
-      <c r="E29" s="87" t="s">
-        <v>537</v>
       </c>
       <c r="F29" s="84" t="s">
         <v>351</v>
       </c>
       <c r="J29" s="2" t="s">
+        <v>537</v>
+      </c>
+      <c r="K29" s="2" t="s">
         <v>538</v>
       </c>
-      <c r="K29" s="2" t="s">
+      <c r="L29" s="2" t="s">
         <v>539</v>
       </c>
-      <c r="L29" s="2" t="s">
+      <c r="M29" s="2" t="s">
         <v>540</v>
-      </c>
-      <c r="M29" s="2" t="s">
-        <v>541</v>
       </c>
       <c r="N29" s="2" t="s">
         <v>351</v>
       </c>
       <c r="P29" s="2" t="s">
+        <v>541</v>
+      </c>
+      <c r="Q29" s="2" t="s">
         <v>542</v>
       </c>
-      <c r="Q29" s="2" t="s">
+      <c r="R29" s="2" t="s">
         <v>543</v>
       </c>
-      <c r="R29" s="2" t="s">
+      <c r="S29" s="2" t="s">
         <v>544</v>
       </c>
-      <c r="S29" s="2" t="s">
-        <v>545</v>
-      </c>
       <c r="T29" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="V29" s="2"/>
     </row>
     <row r="30" spans="2:22" ht="71.25" x14ac:dyDescent="0.45">
       <c r="B30" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>346</v>
       </c>
       <c r="D30" s="2" t="s">
+        <v>546</v>
+      </c>
+      <c r="E30" s="87" t="s">
         <v>547</v>
-      </c>
-      <c r="E30" s="87" t="s">
-        <v>548</v>
       </c>
       <c r="F30" s="84" t="s">
         <v>351</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="K30" s="2" t="s">
+        <v>548</v>
+      </c>
+      <c r="L30" s="2" t="s">
         <v>549</v>
       </c>
-      <c r="L30" s="2" t="s">
+      <c r="M30" s="2" t="s">
         <v>550</v>
-      </c>
-      <c r="M30" s="2" t="s">
-        <v>551</v>
       </c>
       <c r="N30" s="2" t="s">
         <v>351</v>
       </c>
       <c r="P30" s="2" t="s">
+        <v>551</v>
+      </c>
+      <c r="Q30" s="2" t="s">
+        <v>542</v>
+      </c>
+      <c r="R30" s="2" t="s">
         <v>552</v>
       </c>
-      <c r="Q30" s="2" t="s">
-        <v>543</v>
-      </c>
-      <c r="R30" s="2" t="s">
+      <c r="S30" s="2" t="s">
         <v>553</v>
       </c>
-      <c r="S30" s="2" t="s">
-        <v>554</v>
-      </c>
       <c r="T30" s="2" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="V30" s="2"/>
     </row>
     <row r="31" spans="2:22" ht="133.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B31" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>407</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="E31" s="87">
         <v>999999</v>
@@ -9022,25 +9018,25 @@
         <v>351</v>
       </c>
       <c r="J31" s="82" t="s">
+        <v>556</v>
+      </c>
+      <c r="K31" s="82" t="s">
         <v>557</v>
-      </c>
-      <c r="K31" s="82" t="s">
-        <v>558</v>
       </c>
       <c r="L31" s="82" t="s">
         <v>346</v>
       </c>
       <c r="M31" s="82" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="N31" s="85" t="s">
         <v>351</v>
       </c>
       <c r="P31" s="82" t="s">
+        <v>558</v>
+      </c>
+      <c r="Q31" s="82" t="s">
         <v>559</v>
-      </c>
-      <c r="Q31" s="82" t="s">
-        <v>560</v>
       </c>
       <c r="R31" s="82" t="s">
         <v>374</v>
@@ -9049,103 +9045,103 @@
         <v>375</v>
       </c>
       <c r="T31" s="82" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="V31" s="2"/>
     </row>
     <row r="32" spans="2:22" ht="128.25" x14ac:dyDescent="0.45">
       <c r="B32" s="2" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>346</v>
       </c>
       <c r="E32" s="87" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="F32" s="84">
         <v>1</v>
       </c>
       <c r="J32" s="2" t="s">
+        <v>562</v>
+      </c>
+      <c r="K32" s="2" t="s">
         <v>563</v>
-      </c>
-      <c r="K32" s="2" t="s">
-        <v>564</v>
       </c>
       <c r="L32" s="2" t="s">
         <v>346</v>
       </c>
       <c r="M32" s="2" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="N32" s="2" t="s">
         <v>351</v>
       </c>
       <c r="P32" s="2" t="s">
+        <v>565</v>
+      </c>
+      <c r="Q32" s="2" t="s">
         <v>566</v>
       </c>
-      <c r="Q32" s="2" t="s">
+      <c r="R32" s="2" t="s">
         <v>567</v>
-      </c>
-      <c r="R32" s="2" t="s">
-        <v>568</v>
       </c>
       <c r="S32" s="2" t="s">
         <v>375</v>
       </c>
       <c r="T32" s="2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="V32" s="2"/>
     </row>
     <row r="33" spans="1:22" ht="42.75" x14ac:dyDescent="0.45">
       <c r="B33" s="2" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>346</v>
       </c>
       <c r="E33" s="87" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="F33" s="84" t="s">
         <v>351</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="L33" s="2" t="s">
         <v>346</v>
       </c>
       <c r="M33" s="2" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="N33" s="2" t="s">
         <v>351</v>
       </c>
       <c r="P33" s="2" t="s">
+        <v>573</v>
+      </c>
+      <c r="Q33" s="2" t="s">
         <v>574</v>
       </c>
-      <c r="Q33" s="2" t="s">
+      <c r="R33" s="2" t="s">
         <v>575</v>
-      </c>
-      <c r="R33" s="2" t="s">
-        <v>576</v>
       </c>
       <c r="S33" s="2" t="s">
         <v>355</v>
       </c>
       <c r="T33" s="2" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="V33" s="2"/>
     </row>
     <row r="34" spans="1:22" ht="99.75" x14ac:dyDescent="0.45">
       <c r="B34" s="2" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>346</v>
@@ -9154,25 +9150,25 @@
         <v>351</v>
       </c>
       <c r="J34" s="82" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="K34" s="82" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="L34" s="82" t="s">
         <v>346</v>
       </c>
       <c r="M34" s="82" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="N34" s="82" t="s">
         <v>351</v>
       </c>
       <c r="P34" s="82" t="s">
+        <v>580</v>
+      </c>
+      <c r="Q34" s="82" t="s">
         <v>581</v>
-      </c>
-      <c r="Q34" s="82" t="s">
-        <v>582</v>
       </c>
       <c r="R34" s="82" t="s">
         <v>374</v>
@@ -9181,19 +9177,19 @@
         <v>375</v>
       </c>
       <c r="T34" s="82" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="V34" s="2"/>
     </row>
     <row r="35" spans="1:22" ht="85.5" x14ac:dyDescent="0.45">
       <c r="B35" s="2" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>428</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="E35" s="87" t="b">
         <v>0</v>
@@ -9202,41 +9198,41 @@
         <v>351</v>
       </c>
       <c r="J35" s="82" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="K35" s="82" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="L35" s="82" t="s">
         <v>428</v>
       </c>
       <c r="M35" s="82" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="N35" s="82" t="s">
         <v>351</v>
       </c>
       <c r="O35" s="82"/>
       <c r="P35" s="82" t="s">
+        <v>585</v>
+      </c>
+      <c r="Q35" s="82" t="s">
         <v>586</v>
       </c>
-      <c r="Q35" s="82" t="s">
+      <c r="R35" s="82" t="s">
         <v>587</v>
       </c>
-      <c r="R35" s="82" t="s">
+      <c r="S35" s="82" t="s">
         <v>588</v>
       </c>
-      <c r="S35" s="82" t="s">
-        <v>589</v>
-      </c>
       <c r="T35" s="82" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="V35" s="2"/>
     </row>
     <row r="36" spans="1:22" ht="85.5" x14ac:dyDescent="0.45">
       <c r="B36" s="2" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>428</v>
@@ -9245,43 +9241,43 @@
         <v>351</v>
       </c>
       <c r="J36" s="82" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="K36" s="82" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="L36" s="82" t="s">
         <v>428</v>
       </c>
       <c r="M36" s="82" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="N36" s="82" t="s">
         <v>351</v>
       </c>
       <c r="P36" s="82" t="s">
+        <v>592</v>
+      </c>
+      <c r="Q36" s="82" t="s">
+        <v>586</v>
+      </c>
+      <c r="R36" s="82" t="s">
         <v>593</v>
       </c>
-      <c r="Q36" s="82" t="s">
-        <v>587</v>
-      </c>
-      <c r="R36" s="82" t="s">
-        <v>594</v>
-      </c>
       <c r="S36" s="82" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="T36" s="82" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="V36" s="2"/>
     </row>
     <row r="37" spans="1:22" ht="99.75" x14ac:dyDescent="0.45">
       <c r="A37" s="2" t="s">
+        <v>594</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>595</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>596</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>346</v>
@@ -9290,25 +9286,25 @@
         <v>351</v>
       </c>
       <c r="J37" s="82" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="K37" s="82" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="L37" s="82" t="s">
         <v>346</v>
       </c>
       <c r="M37" s="82" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="N37" s="82" t="s">
         <v>351</v>
       </c>
       <c r="P37" s="82" t="s">
+        <v>598</v>
+      </c>
+      <c r="Q37" s="82" t="s">
         <v>599</v>
-      </c>
-      <c r="Q37" s="82" t="s">
-        <v>600</v>
       </c>
       <c r="R37" s="82" t="s">
         <v>374</v>
@@ -9317,19 +9313,19 @@
         <v>375</v>
       </c>
       <c r="T37" s="82" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="V37" s="2"/>
     </row>
     <row r="38" spans="1:22" ht="57" x14ac:dyDescent="0.45">
       <c r="B38" s="2" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>407</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="E38" s="87">
         <v>9999999</v>
@@ -9338,94 +9334,94 @@
         <v>351</v>
       </c>
       <c r="J38" s="82" t="s">
+        <v>602</v>
+      </c>
+      <c r="K38" s="82" t="s">
         <v>603</v>
-      </c>
-      <c r="K38" s="82" t="s">
-        <v>604</v>
       </c>
       <c r="L38" s="82" t="s">
         <v>346</v>
       </c>
       <c r="M38" s="82" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="N38" s="85" t="s">
         <v>351</v>
       </c>
       <c r="P38" s="82" t="s">
+        <v>604</v>
+      </c>
+      <c r="Q38" s="82" t="s">
+        <v>566</v>
+      </c>
+      <c r="R38" s="82" t="s">
         <v>605</v>
-      </c>
-      <c r="Q38" s="82" t="s">
-        <v>567</v>
-      </c>
-      <c r="R38" s="82" t="s">
-        <v>606</v>
       </c>
       <c r="S38" s="82" t="s">
         <v>375</v>
       </c>
       <c r="T38" s="82" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="V38" s="2"/>
     </row>
     <row r="39" spans="1:22" ht="85.5" x14ac:dyDescent="0.45">
       <c r="B39" s="2" t="s">
+        <v>607</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>494</v>
+      </c>
+      <c r="D39" s="2" t="s">
         <v>608</v>
       </c>
-      <c r="C39" s="2" t="s">
-        <v>495</v>
-      </c>
-      <c r="D39" s="2" t="s">
+      <c r="E39" s="87" t="s">
         <v>609</v>
-      </c>
-      <c r="E39" s="87" t="s">
-        <v>610</v>
       </c>
       <c r="F39" s="84" t="s">
         <v>351</v>
       </c>
       <c r="J39" s="82" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="K39" s="82" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="L39" s="82" t="s">
         <v>346</v>
       </c>
       <c r="M39" s="82" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="N39" s="85" t="s">
         <v>351</v>
       </c>
       <c r="P39" s="82" t="s">
+        <v>612</v>
+      </c>
+      <c r="Q39" s="82" t="s">
         <v>613</v>
       </c>
-      <c r="Q39" s="82" t="s">
+      <c r="R39" s="82" t="s">
         <v>614</v>
       </c>
-      <c r="R39" s="82" t="s">
-        <v>615</v>
-      </c>
       <c r="S39" s="82" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="T39" s="82" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="V39" s="2"/>
     </row>
     <row r="40" spans="1:22" ht="85.5" x14ac:dyDescent="0.45">
       <c r="B40" s="2" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>398</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="E40" s="88">
         <v>45566</v>
@@ -9434,25 +9430,25 @@
         <v>351</v>
       </c>
       <c r="J40" s="82" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="K40" s="82" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="L40" s="82" t="s">
         <v>398</v>
       </c>
       <c r="M40" s="82" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="N40" s="85" t="s">
         <v>351</v>
       </c>
       <c r="P40" s="82" t="s">
+        <v>618</v>
+      </c>
+      <c r="Q40" s="82" t="s">
         <v>619</v>
-      </c>
-      <c r="Q40" s="82" t="s">
-        <v>620</v>
       </c>
       <c r="R40" s="82" t="s">
         <v>404</v>
@@ -9461,74 +9457,74 @@
         <v>405</v>
       </c>
       <c r="T40" s="82" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="V40" s="2"/>
     </row>
     <row r="41" spans="1:22" ht="85.5" x14ac:dyDescent="0.45">
       <c r="B41" s="2" t="s">
+        <v>620</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>494</v>
+      </c>
+      <c r="D41" s="2" t="s">
         <v>621</v>
       </c>
-      <c r="C41" s="2" t="s">
-        <v>495</v>
-      </c>
-      <c r="D41" s="2" t="s">
+      <c r="E41" s="87" t="s">
         <v>622</v>
-      </c>
-      <c r="E41" s="87" t="s">
-        <v>623</v>
       </c>
       <c r="F41" s="84" t="s">
         <v>351</v>
       </c>
       <c r="J41" s="82" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="K41" s="82" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="L41" s="82" t="s">
         <v>346</v>
       </c>
       <c r="M41" s="82" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="N41" s="85" t="s">
         <v>351</v>
       </c>
       <c r="P41" s="82" t="s">
+        <v>625</v>
+      </c>
+      <c r="Q41" s="82" t="s">
         <v>626</v>
       </c>
-      <c r="Q41" s="82" t="s">
-        <v>627</v>
-      </c>
       <c r="R41" s="82" t="s">
+        <v>501</v>
+      </c>
+      <c r="S41" s="82" t="s">
         <v>502</v>
       </c>
-      <c r="S41" s="82" t="s">
-        <v>503</v>
-      </c>
       <c r="T41" s="82" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="V41" s="2"/>
     </row>
     <row r="42" spans="1:22" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A42" s="91" t="s">
+        <v>686</v>
+      </c>
+      <c r="B42" s="93" t="s">
         <v>687</v>
-      </c>
-      <c r="B42" s="93" t="s">
-        <v>688</v>
       </c>
       <c r="C42" s="93" t="s">
         <v>346</v>
       </c>
       <c r="D42" s="93" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="E42" s="93"/>
       <c r="F42" s="84" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="G42" s="93"/>
       <c r="H42" s="93"/>
@@ -9537,366 +9533,366 @@
         <v>3</v>
       </c>
       <c r="K42" s="92" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="L42" s="92" t="s">
         <v>346</v>
       </c>
       <c r="M42" s="92" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="N42" s="84" t="s">
         <v>415</v>
       </c>
       <c r="O42" s="93"/>
       <c r="P42" s="93" t="s">
+        <v>689</v>
+      </c>
+      <c r="Q42" s="2" t="s">
+        <v>689</v>
+      </c>
+      <c r="R42" s="92" t="s">
         <v>690</v>
-      </c>
-      <c r="Q42" s="2" t="s">
-        <v>690</v>
-      </c>
-      <c r="R42" s="92" t="s">
-        <v>691</v>
       </c>
       <c r="S42" s="93" t="s">
         <v>355</v>
       </c>
       <c r="T42" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="43" spans="1:22" ht="57" x14ac:dyDescent="0.45">
       <c r="B43" s="2" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D43" s="87" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="J43" s="2" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="K43" s="2" t="s">
         <v>321</v>
       </c>
       <c r="M43" s="87" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="N43" s="84"/>
       <c r="P43" s="2" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="Q43" s="2" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="R43" s="2" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="S43" s="2" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="T43" s="87" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="V43" s="2"/>
     </row>
     <row r="44" spans="1:22" ht="57" x14ac:dyDescent="0.45">
       <c r="B44" s="2" t="s">
+        <v>657</v>
+      </c>
+      <c r="C44" s="2" t="s">
         <v>658</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="D44" s="87" t="s">
         <v>659</v>
-      </c>
-      <c r="D44" s="87" t="s">
-        <v>660</v>
       </c>
       <c r="F44" s="84" t="s">
         <v>351</v>
       </c>
       <c r="G44" s="2" t="s">
+        <v>657</v>
+      </c>
+      <c r="J44" s="2" t="s">
+        <v>654</v>
+      </c>
+      <c r="K44" s="2" t="s">
+        <v>657</v>
+      </c>
+      <c r="L44" s="2" t="s">
         <v>658</v>
       </c>
-      <c r="J44" s="2" t="s">
-        <v>655</v>
-      </c>
-      <c r="K44" s="2" t="s">
-        <v>658</v>
-      </c>
-      <c r="L44" s="2" t="s">
+      <c r="M44" s="87" t="s">
         <v>659</v>
-      </c>
-      <c r="M44" s="87" t="s">
-        <v>660</v>
       </c>
       <c r="N44" s="84" t="s">
         <v>351</v>
       </c>
       <c r="P44" s="2" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="Q44" s="2" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="R44" s="2" t="s">
+        <v>660</v>
+      </c>
+      <c r="S44" s="2" t="s">
         <v>661</v>
       </c>
-      <c r="S44" s="2" t="s">
-        <v>662</v>
-      </c>
       <c r="T44" s="87" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="V44" s="2"/>
     </row>
     <row r="45" spans="1:22" ht="57" x14ac:dyDescent="0.45">
       <c r="B45" s="2" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>346</v>
       </c>
       <c r="D45" s="87" t="s">
+        <v>663</v>
+      </c>
+      <c r="F45" s="84" t="s">
         <v>664</v>
       </c>
-      <c r="F45" s="84" t="s">
-        <v>665</v>
-      </c>
       <c r="G45" s="2" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="J45" s="2" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="K45" s="2" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="L45" s="2" t="s">
         <v>346</v>
       </c>
       <c r="M45" s="87" t="s">
+        <v>663</v>
+      </c>
+      <c r="N45" s="84" t="s">
         <v>664</v>
       </c>
-      <c r="N45" s="84" t="s">
+      <c r="P45" s="2" t="s">
+        <v>682</v>
+      </c>
+      <c r="Q45" s="2" t="s">
+        <v>694</v>
+      </c>
+      <c r="R45" s="2" t="s">
         <v>665</v>
-      </c>
-      <c r="P45" s="2" t="s">
-        <v>683</v>
-      </c>
-      <c r="Q45" s="2" t="s">
-        <v>695</v>
-      </c>
-      <c r="R45" s="2" t="s">
-        <v>666</v>
       </c>
       <c r="S45" s="2" t="s">
         <v>355</v>
       </c>
       <c r="T45" s="87" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="V45" s="2"/>
     </row>
     <row r="46" spans="1:22" ht="57" x14ac:dyDescent="0.45">
       <c r="B46" s="2" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>346</v>
       </c>
       <c r="D46" s="87" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="F46" s="84" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="J46" s="2" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="K46" s="2" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="L46" s="2" t="s">
         <v>346</v>
       </c>
       <c r="M46" s="87" t="s">
+        <v>667</v>
+      </c>
+      <c r="N46" s="84" t="s">
+        <v>664</v>
+      </c>
+      <c r="P46" s="2" t="s">
+        <v>683</v>
+      </c>
+      <c r="Q46" s="2" t="s">
+        <v>693</v>
+      </c>
+      <c r="R46" s="2" t="s">
         <v>668</v>
-      </c>
-      <c r="N46" s="84" t="s">
-        <v>665</v>
-      </c>
-      <c r="P46" s="2" t="s">
-        <v>684</v>
-      </c>
-      <c r="Q46" s="2" t="s">
-        <v>694</v>
-      </c>
-      <c r="R46" s="2" t="s">
-        <v>669</v>
       </c>
       <c r="S46" s="2" t="s">
         <v>375</v>
       </c>
       <c r="T46" s="87" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="V46" s="2"/>
     </row>
     <row r="47" spans="1:22" ht="57" x14ac:dyDescent="0.45">
       <c r="B47" s="2" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>271</v>
       </c>
       <c r="D47" s="87" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="F47" s="84" t="s">
         <v>351</v>
       </c>
       <c r="G47" s="2" t="s">
+        <v>669</v>
+      </c>
+      <c r="J47" s="2" t="s">
+        <v>654</v>
+      </c>
+      <c r="K47" s="2" t="s">
+        <v>669</v>
+      </c>
+      <c r="L47" s="2" t="s">
         <v>670</v>
       </c>
-      <c r="J47" s="2" t="s">
-        <v>655</v>
-      </c>
-      <c r="K47" s="2" t="s">
-        <v>670</v>
-      </c>
-      <c r="L47" s="2" t="s">
+      <c r="M47" s="87" t="s">
         <v>671</v>
-      </c>
-      <c r="M47" s="87" t="s">
-        <v>672</v>
       </c>
       <c r="N47" s="84" t="s">
         <v>351</v>
       </c>
       <c r="P47" s="2" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="Q47" s="2" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="R47" s="2" t="s">
+        <v>672</v>
+      </c>
+      <c r="S47" s="2" t="s">
         <v>673</v>
       </c>
-      <c r="S47" s="2" t="s">
-        <v>674</v>
-      </c>
       <c r="T47" s="87" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="V47" s="2"/>
     </row>
     <row r="48" spans="1:22" ht="57" x14ac:dyDescent="0.45">
       <c r="B48" s="2" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="D48" s="87" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="F48" s="84" t="s">
         <v>351</v>
       </c>
       <c r="G48" s="2" t="s">
+        <v>674</v>
+      </c>
+      <c r="J48" s="2" t="s">
+        <v>654</v>
+      </c>
+      <c r="K48" s="2" t="s">
+        <v>674</v>
+      </c>
+      <c r="L48" s="2" t="s">
         <v>675</v>
       </c>
-      <c r="J48" s="2" t="s">
-        <v>655</v>
-      </c>
-      <c r="K48" s="2" t="s">
-        <v>675</v>
-      </c>
-      <c r="L48" s="2" t="s">
+      <c r="M48" s="87" t="s">
         <v>676</v>
-      </c>
-      <c r="M48" s="87" t="s">
-        <v>677</v>
       </c>
       <c r="N48" s="84" t="s">
         <v>351</v>
       </c>
       <c r="P48" s="2" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="Q48" s="2" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="R48" s="2" t="s">
+        <v>677</v>
+      </c>
+      <c r="S48" s="2" t="s">
         <v>678</v>
       </c>
-      <c r="S48" s="2" t="s">
-        <v>679</v>
-      </c>
       <c r="T48" s="87" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="V48" s="2"/>
     </row>
     <row r="49" spans="1:22" s="97" customFormat="1" ht="99.75" x14ac:dyDescent="0.45">
       <c r="A49" s="96" t="s">
-        <v>687</v>
-      </c>
-      <c r="B49" s="100" t="s">
+        <v>686</v>
+      </c>
+      <c r="B49" s="98" t="s">
+        <v>696</v>
+      </c>
+      <c r="C49" t="s">
+        <v>346</v>
+      </c>
+      <c r="D49" s="98" t="s">
         <v>697</v>
       </c>
-      <c r="C49" s="99" t="s">
-        <v>346</v>
-      </c>
-      <c r="D49" s="100" t="s">
-        <v>698</v>
-      </c>
-      <c r="E49" s="99"/>
-      <c r="F49" s="99"/>
-      <c r="G49" s="100" t="s">
+      <c r="E49"/>
+      <c r="F49"/>
+      <c r="G49" s="98" t="s">
         <v>351</v>
       </c>
-      <c r="H49" s="100" t="s">
-        <v>697</v>
-      </c>
-      <c r="I49" s="100"/>
+      <c r="H49" s="98" t="s">
+        <v>696</v>
+      </c>
+      <c r="I49" s="98"/>
       <c r="J49" s="94" t="s">
         <v>408</v>
       </c>
       <c r="K49" s="94" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="L49" s="94" t="s">
         <v>346</v>
       </c>
       <c r="M49" s="94" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="N49" s="94" t="s">
         <v>351</v>
       </c>
       <c r="O49" s="94"/>
       <c r="P49" s="94" t="s">
+        <v>698</v>
+      </c>
+      <c r="Q49" s="95"/>
+      <c r="R49" s="82" t="s">
+        <v>374</v>
+      </c>
+      <c r="S49" s="82" t="s">
+        <v>375</v>
+      </c>
+      <c r="T49" s="82" t="s">
         <v>699</v>
       </c>
-      <c r="Q49" s="95"/>
-      <c r="R49" s="98" t="s">
-        <v>374</v>
-      </c>
-      <c r="S49" s="98" t="s">
-        <v>375</v>
-      </c>
-      <c r="T49" s="98" t="s">
-        <v>700</v>
-      </c>
-      <c r="V49" s="99"/>
+      <c r="V49"/>
     </row>
     <row r="50" spans="1:22" x14ac:dyDescent="0.45">
       <c r="V50" s="2"/>
@@ -9964,7 +9960,7 @@
         <v>147</v>
       </c>
       <c r="E1" s="25" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="F1" s="9" t="s">
         <v>4</v>
@@ -9976,22 +9972,22 @@
         <v>335</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>628</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>629</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>630</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>631</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>632</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>633</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>634</v>
       </c>
     </row>
   </sheetData>
@@ -10049,7 +10045,7 @@
   <sheetData>
     <row r="1" spans="1:17" s="56" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A1" s="10" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>183</v>
@@ -10076,25 +10072,25 @@
         <v>329</v>
       </c>
       <c r="J1" s="11" t="s">
+        <v>635</v>
+      </c>
+      <c r="K1" s="11" t="s">
+        <v>628</v>
+      </c>
+      <c r="L1" s="11" t="s">
         <v>636</v>
       </c>
-      <c r="K1" s="11" t="s">
-        <v>629</v>
-      </c>
-      <c r="L1" s="11" t="s">
+      <c r="M1" s="1" t="s">
         <v>637</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="15" t="s">
         <v>638</v>
       </c>
-      <c r="N1" s="15" t="s">
+      <c r="O1" s="15" t="s">
         <v>639</v>
       </c>
-      <c r="O1" s="15" t="s">
+      <c r="P1" s="1" t="s">
         <v>640</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>641</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>233</v>
@@ -10153,7 +10149,7 @@
   <sheetData>
     <row r="1" spans="1:13" s="57" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A1" s="60" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="B1" s="61" t="s">
         <v>183</v>
@@ -10165,10 +10161,10 @@
         <v>147</v>
       </c>
       <c r="E1" s="62" t="s">
+        <v>642</v>
+      </c>
+      <c r="F1" s="63" t="s">
         <v>643</v>
-      </c>
-      <c r="F1" s="63" t="s">
-        <v>644</v>
       </c>
       <c r="G1" s="63" t="s">
         <v>4</v>
@@ -10177,19 +10173,19 @@
         <v>329</v>
       </c>
       <c r="I1" s="64" t="s">
+        <v>644</v>
+      </c>
+      <c r="J1" s="65" t="s">
+        <v>628</v>
+      </c>
+      <c r="K1" s="66" t="s">
         <v>645</v>
       </c>
-      <c r="J1" s="65" t="s">
-        <v>629</v>
-      </c>
-      <c r="K1" s="66" t="s">
+      <c r="L1" s="66" t="s">
+        <v>630</v>
+      </c>
+      <c r="M1" s="66" t="s">
         <v>646</v>
-      </c>
-      <c r="L1" s="66" t="s">
-        <v>631</v>
-      </c>
-      <c r="M1" s="66" t="s">
-        <v>647</v>
       </c>
     </row>
   </sheetData>
@@ -10247,7 +10243,7 @@
   <sheetData>
     <row r="1" spans="1:14" s="56" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A1" s="79" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="B1" s="75" t="s">
         <v>271</v>
@@ -10256,7 +10252,7 @@
         <v>147</v>
       </c>
       <c r="D1" s="76" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="E1" s="77" t="s">
         <v>4</v>
@@ -10265,16 +10261,16 @@
         <v>329</v>
       </c>
       <c r="G1" s="78" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="H1" s="78" t="s">
         <v>188</v>
       </c>
       <c r="I1" s="78" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="J1" s="78" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="K1" s="74" t="s">
         <v>297</v>
@@ -10340,7 +10336,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A1" s="10" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>313</v>
@@ -10352,7 +10348,7 @@
         <v>147</v>
       </c>
       <c r="E1" s="73" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="F1" s="63" t="s">
         <v>4</v>
@@ -10364,13 +10360,13 @@
         <v>335</v>
       </c>
       <c r="I1" s="11" t="s">
+        <v>652</v>
+      </c>
+      <c r="J1" s="11" t="s">
         <v>653</v>
       </c>
-      <c r="J1" s="11" t="s">
-        <v>654</v>
-      </c>
       <c r="K1" s="11" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Replaced JMSChargeNumber with ChargeSequenceID in ChargeFiling
</commit_message>
<xml_diff>
--- a/schemas/ChargeFiling_iepd/artifacts/ChargeFiling_MappingSpreadsheet.xlsx
+++ b/schemas/ChargeFiling_iepd/artifacts/ChargeFiling_MappingSpreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JamesCabral\git\JTMP-Data-Exchange-Specs\schemas\ChargeFiling_iepd\artifacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05ACBEA7-0281-4E10-91D5-B37EFA98F6F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F53A321B-904E-47C0-B3DF-10E6681DDE74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-4080" yWindow="-21720" windowWidth="51840" windowHeight="21120" tabRatio="781" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1900,12 +1900,6 @@
 The Item # is the incident number assigned by the Computer Aided Dispatching. It will be included on all arrest paperwork submitted by the arresting officer.</t>
   </si>
   <si>
-    <t>nc:IdentificationType (nc:ActivityIdentification)</t>
-  </si>
-  <si>
-    <t>An identification that references an activity.</t>
-  </si>
-  <si>
     <t>Data received from NOPD</t>
   </si>
   <si>
@@ -2963,7 +2957,13 @@
     <t>An identification assigned by a booking system to identify a unique booking event within a specific jail.</t>
   </si>
   <si>
-    <t>j:Arrest/j:ArrestCharge/nola-ext:ChargeAugmentation/nola-ext:ArrestIncident/nc:ActivityIdentification/nc:IdentificationID</t>
+    <t>j:Arrest/j:ArrestCharge/j:ChargeSequenceID</t>
+  </si>
+  <si>
+    <t>j:ChargeSequenceID</t>
+  </si>
+  <si>
+    <t>A sequentially assigned identifier for charge tracking purposes.</t>
   </si>
 </sst>
 </file>
@@ -7604,10 +7604,10 @@
   <dimension ref="A1:AB50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="J12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P18" sqref="P18"/>
+      <selection pane="bottomRight" activeCell="Q17" sqref="Q17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -8412,25 +8412,25 @@
         <v>351</v>
       </c>
       <c r="P17" s="82" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="Q17" s="82" t="s">
-        <v>445</v>
+        <v>353</v>
       </c>
       <c r="R17" s="82" t="s">
-        <v>374</v>
+        <v>699</v>
       </c>
       <c r="S17" s="82" t="s">
         <v>396</v>
       </c>
       <c r="T17" s="82" t="s">
-        <v>446</v>
+        <v>700</v>
       </c>
       <c r="V17" s="2"/>
     </row>
     <row r="18" spans="2:22" ht="71.25" x14ac:dyDescent="0.45">
       <c r="B18" s="2" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>100</v>
@@ -8445,22 +8445,22 @@
         <v>408</v>
       </c>
       <c r="K18" s="82" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="L18" s="82" t="s">
         <v>398</v>
       </c>
       <c r="M18" s="82" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="N18" s="82">
         <v>1</v>
       </c>
       <c r="P18" s="82" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="Q18" s="82" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="R18" s="82" t="s">
         <v>404</v>
@@ -8469,58 +8469,58 @@
         <v>405</v>
       </c>
       <c r="T18" s="82" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="V18" s="2"/>
     </row>
     <row r="19" spans="2:22" ht="99.75" x14ac:dyDescent="0.45">
       <c r="B19" s="2" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>346</v>
       </c>
       <c r="E19" s="87" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="F19" s="84">
         <v>1</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="L19" s="2" t="s">
         <v>346</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="N19" s="2" t="s">
         <v>351</v>
       </c>
       <c r="P19" s="2" t="s">
+        <v>455</v>
+      </c>
+      <c r="Q19" s="2" t="s">
+        <v>456</v>
+      </c>
+      <c r="R19" s="2" t="s">
         <v>457</v>
       </c>
-      <c r="Q19" s="2" t="s">
+      <c r="S19" s="2" t="s">
         <v>458</v>
       </c>
-      <c r="R19" s="2" t="s">
+      <c r="T19" s="2" t="s">
         <v>459</v>
-      </c>
-      <c r="S19" s="2" t="s">
-        <v>460</v>
-      </c>
-      <c r="T19" s="2" t="s">
-        <v>461</v>
       </c>
       <c r="V19" s="2"/>
     </row>
     <row r="20" spans="2:22" ht="85.5" x14ac:dyDescent="0.45">
       <c r="B20" s="2" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>398</v>
@@ -8532,25 +8532,25 @@
         <v>1</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="L20" s="2" t="s">
         <v>398</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="N20" s="2" t="s">
         <v>351</v>
       </c>
       <c r="P20" s="2" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="Q20" s="2" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="R20" s="2" t="s">
         <v>404</v>
@@ -8559,313 +8559,313 @@
         <v>405</v>
       </c>
       <c r="T20" s="2" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="V20" s="2"/>
     </row>
     <row r="21" spans="2:22" ht="99.75" x14ac:dyDescent="0.45">
       <c r="J21" s="2" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="L21" s="2" t="s">
         <v>346</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="N21" s="2" t="s">
         <v>351</v>
       </c>
       <c r="P21" s="2" t="s">
+        <v>469</v>
+      </c>
+      <c r="Q21" s="2" t="s">
+        <v>470</v>
+      </c>
+      <c r="R21" s="2" t="s">
         <v>471</v>
-      </c>
-      <c r="Q21" s="2" t="s">
-        <v>472</v>
-      </c>
-      <c r="R21" s="2" t="s">
-        <v>473</v>
       </c>
       <c r="S21" s="2" t="s">
         <v>375</v>
       </c>
       <c r="T21" s="2" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="V21" s="2"/>
     </row>
     <row r="22" spans="2:22" ht="114" x14ac:dyDescent="0.45">
       <c r="B22" s="2" t="s">
+        <v>473</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="E22" s="87" t="s">
         <v>475</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>476</v>
-      </c>
-      <c r="E22" s="87" t="s">
-        <v>477</v>
       </c>
       <c r="F22" s="84">
         <v>1</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="K22" s="2" t="s">
+        <v>476</v>
+      </c>
+      <c r="L22" s="2" t="s">
+        <v>477</v>
+      </c>
+      <c r="M22" s="2" t="s">
         <v>478</v>
-      </c>
-      <c r="L22" s="2" t="s">
-        <v>479</v>
-      </c>
-      <c r="M22" s="2" t="s">
-        <v>480</v>
       </c>
       <c r="N22" s="2" t="s">
         <v>351</v>
       </c>
       <c r="P22" s="2" t="s">
+        <v>479</v>
+      </c>
+      <c r="Q22" s="2" t="s">
+        <v>480</v>
+      </c>
+      <c r="R22" s="2" t="s">
         <v>481</v>
-      </c>
-      <c r="Q22" s="2" t="s">
-        <v>482</v>
-      </c>
-      <c r="R22" s="2" t="s">
-        <v>483</v>
       </c>
       <c r="S22" s="2" t="s">
         <v>355</v>
       </c>
       <c r="T22" s="2" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="V22" s="2"/>
     </row>
     <row r="23" spans="2:22" ht="128.25" x14ac:dyDescent="0.45">
       <c r="J23" s="2" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="K23" s="2" t="s">
+        <v>483</v>
+      </c>
+      <c r="L23" s="2" t="s">
+        <v>484</v>
+      </c>
+      <c r="M23" s="2" t="s">
         <v>485</v>
-      </c>
-      <c r="L23" s="2" t="s">
-        <v>486</v>
-      </c>
-      <c r="M23" s="2" t="s">
-        <v>487</v>
       </c>
       <c r="N23" s="2" t="s">
         <v>415</v>
       </c>
       <c r="P23" s="2" t="s">
+        <v>486</v>
+      </c>
+      <c r="Q23" s="2" t="s">
+        <v>487</v>
+      </c>
+      <c r="R23" s="2" t="s">
         <v>488</v>
       </c>
-      <c r="Q23" s="2" t="s">
+      <c r="S23" s="2" t="s">
         <v>489</v>
       </c>
-      <c r="R23" s="2" t="s">
+      <c r="T23" s="2" t="s">
         <v>490</v>
-      </c>
-      <c r="S23" s="2" t="s">
-        <v>491</v>
-      </c>
-      <c r="T23" s="2" t="s">
-        <v>492</v>
       </c>
       <c r="V23" s="2"/>
     </row>
     <row r="24" spans="2:22" ht="71.25" x14ac:dyDescent="0.45">
       <c r="B24" s="2" t="s">
+        <v>491</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>492</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>493</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>494</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>495</v>
       </c>
       <c r="F24" s="84" t="s">
         <v>415</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="L24" s="2" t="s">
         <v>346</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="N24" s="84" t="s">
         <v>415</v>
       </c>
       <c r="P24" s="2" t="s">
+        <v>497</v>
+      </c>
+      <c r="Q24" s="2" t="s">
+        <v>498</v>
+      </c>
+      <c r="R24" s="2" t="s">
         <v>499</v>
       </c>
-      <c r="Q24" s="2" t="s">
+      <c r="S24" s="2" t="s">
         <v>500</v>
       </c>
-      <c r="R24" s="2" t="s">
+      <c r="T24" s="2" t="s">
         <v>501</v>
-      </c>
-      <c r="S24" s="2" t="s">
-        <v>502</v>
-      </c>
-      <c r="T24" s="2" t="s">
-        <v>503</v>
       </c>
       <c r="V24" s="2"/>
     </row>
     <row r="25" spans="2:22" ht="127.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B25" s="2" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>346</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="E25" s="87" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="F25" s="84">
         <v>1</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="L25" s="2" t="s">
         <v>346</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="N25" s="2" t="s">
         <v>351</v>
       </c>
       <c r="P25" s="2" t="s">
+        <v>507</v>
+      </c>
+      <c r="Q25" s="2" t="s">
+        <v>500</v>
+      </c>
+      <c r="R25" s="2" t="s">
+        <v>508</v>
+      </c>
+      <c r="S25" s="2" t="s">
         <v>509</v>
       </c>
-      <c r="Q25" s="2" t="s">
-        <v>502</v>
-      </c>
-      <c r="R25" s="2" t="s">
+      <c r="T25" s="2" t="s">
         <v>510</v>
-      </c>
-      <c r="S25" s="2" t="s">
-        <v>511</v>
-      </c>
-      <c r="T25" s="2" t="s">
-        <v>512</v>
       </c>
       <c r="V25" s="2"/>
     </row>
     <row r="26" spans="2:22" ht="99.75" x14ac:dyDescent="0.45">
       <c r="B26" s="2" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>346</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="E26" s="87" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="F26" s="84" t="s">
         <v>351</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="L26" s="2" t="s">
         <v>346</v>
       </c>
       <c r="M26" s="2" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="N26" s="2" t="s">
         <v>351</v>
       </c>
       <c r="P26" s="2" t="s">
+        <v>516</v>
+      </c>
+      <c r="Q26" s="2" t="s">
+        <v>500</v>
+      </c>
+      <c r="R26" s="2" t="s">
+        <v>517</v>
+      </c>
+      <c r="S26" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="T26" s="2" t="s">
         <v>518</v>
-      </c>
-      <c r="Q26" s="2" t="s">
-        <v>502</v>
-      </c>
-      <c r="R26" s="2" t="s">
-        <v>519</v>
-      </c>
-      <c r="S26" s="2" t="s">
-        <v>511</v>
-      </c>
-      <c r="T26" s="2" t="s">
-        <v>520</v>
       </c>
       <c r="V26" s="2"/>
     </row>
     <row r="27" spans="2:22" ht="85.5" x14ac:dyDescent="0.45">
       <c r="B27" s="2" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>346</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="E27" s="87" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="F27" s="84">
         <v>1</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="L27" s="2" t="s">
         <v>346</v>
       </c>
       <c r="M27" s="2" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="N27" s="2" t="s">
         <v>351</v>
       </c>
       <c r="P27" s="2" t="s">
+        <v>523</v>
+      </c>
+      <c r="Q27" s="2" t="s">
+        <v>500</v>
+      </c>
+      <c r="R27" s="2" t="s">
+        <v>524</v>
+      </c>
+      <c r="S27" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="T27" s="2" t="s">
         <v>525</v>
-      </c>
-      <c r="Q27" s="2" t="s">
-        <v>502</v>
-      </c>
-      <c r="R27" s="2" t="s">
-        <v>526</v>
-      </c>
-      <c r="S27" s="2" t="s">
-        <v>511</v>
-      </c>
-      <c r="T27" s="2" t="s">
-        <v>527</v>
       </c>
       <c r="V27" s="2"/>
     </row>
     <row r="28" spans="2:22" ht="99.75" x14ac:dyDescent="0.45">
       <c r="B28" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>346</v>
@@ -8874,25 +8874,25 @@
         <v>351</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="L28" s="2" t="s">
         <v>346</v>
       </c>
       <c r="M28" s="2" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="N28" s="2" t="s">
         <v>351</v>
       </c>
       <c r="P28" s="2" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="Q28" s="2" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="R28" s="2" t="s">
         <v>374</v>
@@ -8901,115 +8901,115 @@
         <v>375</v>
       </c>
       <c r="T28" s="2" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="V28" s="2"/>
     </row>
     <row r="29" spans="2:22" ht="99.75" x14ac:dyDescent="0.45">
       <c r="B29" s="2" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>346</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="E29" s="87" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="F29" s="84" t="s">
         <v>351</v>
       </c>
       <c r="J29" s="2" t="s">
+        <v>535</v>
+      </c>
+      <c r="K29" s="2" t="s">
+        <v>536</v>
+      </c>
+      <c r="L29" s="2" t="s">
         <v>537</v>
       </c>
-      <c r="K29" s="2" t="s">
+      <c r="M29" s="2" t="s">
         <v>538</v>
-      </c>
-      <c r="L29" s="2" t="s">
-        <v>539</v>
-      </c>
-      <c r="M29" s="2" t="s">
-        <v>540</v>
       </c>
       <c r="N29" s="2" t="s">
         <v>351</v>
       </c>
       <c r="P29" s="2" t="s">
+        <v>539</v>
+      </c>
+      <c r="Q29" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="R29" s="2" t="s">
         <v>541</v>
       </c>
-      <c r="Q29" s="2" t="s">
+      <c r="S29" s="2" t="s">
         <v>542</v>
       </c>
-      <c r="R29" s="2" t="s">
-        <v>543</v>
-      </c>
-      <c r="S29" s="2" t="s">
-        <v>544</v>
-      </c>
       <c r="T29" s="2" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="V29" s="2"/>
     </row>
     <row r="30" spans="2:22" ht="71.25" x14ac:dyDescent="0.45">
       <c r="B30" s="2" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>346</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="E30" s="87" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="F30" s="84" t="s">
         <v>351</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="K30" s="2" t="s">
+        <v>546</v>
+      </c>
+      <c r="L30" s="2" t="s">
+        <v>547</v>
+      </c>
+      <c r="M30" s="2" t="s">
         <v>548</v>
-      </c>
-      <c r="L30" s="2" t="s">
-        <v>549</v>
-      </c>
-      <c r="M30" s="2" t="s">
-        <v>550</v>
       </c>
       <c r="N30" s="2" t="s">
         <v>351</v>
       </c>
       <c r="P30" s="2" t="s">
+        <v>549</v>
+      </c>
+      <c r="Q30" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="R30" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="S30" s="2" t="s">
         <v>551</v>
       </c>
-      <c r="Q30" s="2" t="s">
-        <v>542</v>
-      </c>
-      <c r="R30" s="2" t="s">
-        <v>552</v>
-      </c>
-      <c r="S30" s="2" t="s">
-        <v>553</v>
-      </c>
       <c r="T30" s="2" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="V30" s="2"/>
     </row>
     <row r="31" spans="2:22" ht="133.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B31" s="2" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>407</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="E31" s="87">
         <v>999999</v>
@@ -9018,25 +9018,25 @@
         <v>351</v>
       </c>
       <c r="J31" s="82" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="K31" s="82" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="L31" s="82" t="s">
         <v>346</v>
       </c>
       <c r="M31" s="82" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="N31" s="85" t="s">
         <v>351</v>
       </c>
       <c r="P31" s="82" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="Q31" s="82" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="R31" s="82" t="s">
         <v>374</v>
@@ -9045,103 +9045,103 @@
         <v>375</v>
       </c>
       <c r="T31" s="82" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="V31" s="2"/>
     </row>
     <row r="32" spans="2:22" ht="128.25" x14ac:dyDescent="0.45">
       <c r="B32" s="2" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>346</v>
       </c>
       <c r="E32" s="87" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="F32" s="84">
         <v>1</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="L32" s="2" t="s">
         <v>346</v>
       </c>
       <c r="M32" s="2" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="N32" s="2" t="s">
         <v>351</v>
       </c>
       <c r="P32" s="2" t="s">
+        <v>563</v>
+      </c>
+      <c r="Q32" s="2" t="s">
+        <v>564</v>
+      </c>
+      <c r="R32" s="2" t="s">
         <v>565</v>
-      </c>
-      <c r="Q32" s="2" t="s">
-        <v>566</v>
-      </c>
-      <c r="R32" s="2" t="s">
-        <v>567</v>
       </c>
       <c r="S32" s="2" t="s">
         <v>375</v>
       </c>
       <c r="T32" s="2" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="V32" s="2"/>
     </row>
     <row r="33" spans="1:22" ht="42.75" x14ac:dyDescent="0.45">
       <c r="B33" s="2" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>346</v>
       </c>
       <c r="E33" s="87" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="F33" s="84" t="s">
         <v>351</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="L33" s="2" t="s">
         <v>346</v>
       </c>
       <c r="M33" s="2" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="N33" s="2" t="s">
         <v>351</v>
       </c>
       <c r="P33" s="2" t="s">
+        <v>571</v>
+      </c>
+      <c r="Q33" s="2" t="s">
+        <v>572</v>
+      </c>
+      <c r="R33" s="2" t="s">
         <v>573</v>
-      </c>
-      <c r="Q33" s="2" t="s">
-        <v>574</v>
-      </c>
-      <c r="R33" s="2" t="s">
-        <v>575</v>
       </c>
       <c r="S33" s="2" t="s">
         <v>355</v>
       </c>
       <c r="T33" s="2" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="V33" s="2"/>
     </row>
     <row r="34" spans="1:22" ht="99.75" x14ac:dyDescent="0.45">
       <c r="B34" s="2" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>346</v>
@@ -9150,25 +9150,25 @@
         <v>351</v>
       </c>
       <c r="J34" s="82" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="K34" s="82" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="L34" s="82" t="s">
         <v>346</v>
       </c>
       <c r="M34" s="82" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="N34" s="82" t="s">
         <v>351</v>
       </c>
       <c r="P34" s="82" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="Q34" s="82" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="R34" s="82" t="s">
         <v>374</v>
@@ -9177,19 +9177,19 @@
         <v>375</v>
       </c>
       <c r="T34" s="82" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="V34" s="2"/>
     </row>
     <row r="35" spans="1:22" ht="85.5" x14ac:dyDescent="0.45">
       <c r="B35" s="2" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>428</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="E35" s="87" t="b">
         <v>0</v>
@@ -9198,41 +9198,41 @@
         <v>351</v>
       </c>
       <c r="J35" s="82" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="K35" s="82" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="L35" s="82" t="s">
         <v>428</v>
       </c>
       <c r="M35" s="82" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="N35" s="82" t="s">
         <v>351</v>
       </c>
       <c r="O35" s="82"/>
       <c r="P35" s="82" t="s">
+        <v>583</v>
+      </c>
+      <c r="Q35" s="82" t="s">
+        <v>584</v>
+      </c>
+      <c r="R35" s="82" t="s">
         <v>585</v>
       </c>
-      <c r="Q35" s="82" t="s">
+      <c r="S35" s="82" t="s">
         <v>586</v>
       </c>
-      <c r="R35" s="82" t="s">
-        <v>587</v>
-      </c>
-      <c r="S35" s="82" t="s">
-        <v>588</v>
-      </c>
       <c r="T35" s="82" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="V35" s="2"/>
     </row>
     <row r="36" spans="1:22" ht="85.5" x14ac:dyDescent="0.45">
       <c r="B36" s="2" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>428</v>
@@ -9241,43 +9241,43 @@
         <v>351</v>
       </c>
       <c r="J36" s="82" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="K36" s="82" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="L36" s="82" t="s">
         <v>428</v>
       </c>
       <c r="M36" s="82" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="N36" s="82" t="s">
         <v>351</v>
       </c>
       <c r="P36" s="82" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="Q36" s="82" t="s">
+        <v>584</v>
+      </c>
+      <c r="R36" s="82" t="s">
+        <v>591</v>
+      </c>
+      <c r="S36" s="82" t="s">
         <v>586</v>
       </c>
-      <c r="R36" s="82" t="s">
-        <v>593</v>
-      </c>
-      <c r="S36" s="82" t="s">
-        <v>588</v>
-      </c>
       <c r="T36" s="82" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="V36" s="2"/>
     </row>
     <row r="37" spans="1:22" ht="99.75" x14ac:dyDescent="0.45">
       <c r="A37" s="2" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>346</v>
@@ -9286,25 +9286,25 @@
         <v>351</v>
       </c>
       <c r="J37" s="82" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="K37" s="82" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="L37" s="82" t="s">
         <v>346</v>
       </c>
       <c r="M37" s="82" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="N37" s="82" t="s">
         <v>351</v>
       </c>
       <c r="P37" s="82" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="Q37" s="82" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="R37" s="82" t="s">
         <v>374</v>
@@ -9313,19 +9313,19 @@
         <v>375</v>
       </c>
       <c r="T37" s="82" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="V37" s="2"/>
     </row>
     <row r="38" spans="1:22" ht="57" x14ac:dyDescent="0.45">
       <c r="B38" s="2" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>407</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="E38" s="87">
         <v>9999999</v>
@@ -9334,94 +9334,94 @@
         <v>351</v>
       </c>
       <c r="J38" s="82" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="K38" s="82" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="L38" s="82" t="s">
         <v>346</v>
       </c>
       <c r="M38" s="82" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="N38" s="85" t="s">
         <v>351</v>
       </c>
       <c r="P38" s="82" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="Q38" s="82" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="R38" s="82" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="S38" s="82" t="s">
         <v>375</v>
       </c>
       <c r="T38" s="82" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="V38" s="2"/>
     </row>
     <row r="39" spans="1:22" ht="85.5" x14ac:dyDescent="0.45">
       <c r="B39" s="2" t="s">
+        <v>605</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>492</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>606</v>
+      </c>
+      <c r="E39" s="87" t="s">
         <v>607</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>494</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>608</v>
-      </c>
-      <c r="E39" s="87" t="s">
-        <v>609</v>
       </c>
       <c r="F39" s="84" t="s">
         <v>351</v>
       </c>
       <c r="J39" s="82" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="K39" s="82" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="L39" s="82" t="s">
         <v>346</v>
       </c>
       <c r="M39" s="82" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="N39" s="85" t="s">
         <v>351</v>
       </c>
       <c r="P39" s="82" t="s">
+        <v>610</v>
+      </c>
+      <c r="Q39" s="82" t="s">
+        <v>611</v>
+      </c>
+      <c r="R39" s="82" t="s">
         <v>612</v>
       </c>
-      <c r="Q39" s="82" t="s">
-        <v>613</v>
-      </c>
-      <c r="R39" s="82" t="s">
-        <v>614</v>
-      </c>
       <c r="S39" s="82" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="T39" s="82" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="V39" s="2"/>
     </row>
     <row r="40" spans="1:22" ht="85.5" x14ac:dyDescent="0.45">
       <c r="B40" s="2" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>398</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="E40" s="88">
         <v>45566</v>
@@ -9430,25 +9430,25 @@
         <v>351</v>
       </c>
       <c r="J40" s="82" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="K40" s="82" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="L40" s="82" t="s">
         <v>398</v>
       </c>
       <c r="M40" s="82" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="N40" s="85" t="s">
         <v>351</v>
       </c>
       <c r="P40" s="82" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="Q40" s="82" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="R40" s="82" t="s">
         <v>404</v>
@@ -9457,74 +9457,74 @@
         <v>405</v>
       </c>
       <c r="T40" s="82" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="V40" s="2"/>
     </row>
     <row r="41" spans="1:22" ht="85.5" x14ac:dyDescent="0.45">
       <c r="B41" s="2" t="s">
+        <v>618</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>492</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>619</v>
+      </c>
+      <c r="E41" s="87" t="s">
         <v>620</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>494</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>621</v>
-      </c>
-      <c r="E41" s="87" t="s">
-        <v>622</v>
       </c>
       <c r="F41" s="84" t="s">
         <v>351</v>
       </c>
       <c r="J41" s="82" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="K41" s="82" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="L41" s="82" t="s">
         <v>346</v>
       </c>
       <c r="M41" s="82" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="N41" s="85" t="s">
         <v>351</v>
       </c>
       <c r="P41" s="82" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="Q41" s="82" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="R41" s="82" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="S41" s="82" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="T41" s="82" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="V41" s="2"/>
     </row>
     <row r="42" spans="1:22" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A42" s="91" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="B42" s="93" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="C42" s="93" t="s">
         <v>346</v>
       </c>
       <c r="D42" s="93" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="E42" s="93"/>
       <c r="F42" s="84" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="G42" s="93"/>
       <c r="H42" s="93"/>
@@ -9533,326 +9533,326 @@
         <v>3</v>
       </c>
       <c r="K42" s="92" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="L42" s="92" t="s">
         <v>346</v>
       </c>
       <c r="M42" s="92" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="N42" s="84" t="s">
         <v>415</v>
       </c>
       <c r="O42" s="93"/>
       <c r="P42" s="93" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="Q42" s="2" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="R42" s="92" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="S42" s="93" t="s">
         <v>355</v>
       </c>
       <c r="T42" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
     </row>
     <row r="43" spans="1:22" ht="57" x14ac:dyDescent="0.45">
       <c r="B43" s="2" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D43" s="87" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="J43" s="2" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="K43" s="2" t="s">
         <v>321</v>
       </c>
       <c r="M43" s="87" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="N43" s="84"/>
       <c r="P43" s="2" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="Q43" s="2" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="R43" s="2" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="S43" s="2" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="T43" s="87" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="V43" s="2"/>
     </row>
     <row r="44" spans="1:22" ht="57" x14ac:dyDescent="0.45">
       <c r="B44" s="2" t="s">
+        <v>655</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>656</v>
+      </c>
+      <c r="D44" s="87" t="s">
         <v>657</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>658</v>
-      </c>
-      <c r="D44" s="87" t="s">
-        <v>659</v>
       </c>
       <c r="F44" s="84" t="s">
         <v>351</v>
       </c>
       <c r="G44" s="2" t="s">
+        <v>655</v>
+      </c>
+      <c r="J44" s="2" t="s">
+        <v>652</v>
+      </c>
+      <c r="K44" s="2" t="s">
+        <v>655</v>
+      </c>
+      <c r="L44" s="2" t="s">
+        <v>656</v>
+      </c>
+      <c r="M44" s="87" t="s">
         <v>657</v>
-      </c>
-      <c r="J44" s="2" t="s">
-        <v>654</v>
-      </c>
-      <c r="K44" s="2" t="s">
-        <v>657</v>
-      </c>
-      <c r="L44" s="2" t="s">
-        <v>658</v>
-      </c>
-      <c r="M44" s="87" t="s">
-        <v>659</v>
       </c>
       <c r="N44" s="84" t="s">
         <v>351</v>
       </c>
       <c r="P44" s="2" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="Q44" s="2" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="R44" s="2" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="S44" s="2" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="T44" s="87" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="V44" s="2"/>
     </row>
     <row r="45" spans="1:22" ht="57" x14ac:dyDescent="0.45">
       <c r="B45" s="2" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>346</v>
       </c>
       <c r="D45" s="87" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="F45" s="84" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="J45" s="2" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="K45" s="2" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="L45" s="2" t="s">
         <v>346</v>
       </c>
       <c r="M45" s="87" t="s">
+        <v>661</v>
+      </c>
+      <c r="N45" s="84" t="s">
+        <v>662</v>
+      </c>
+      <c r="P45" s="2" t="s">
+        <v>680</v>
+      </c>
+      <c r="Q45" s="2" t="s">
+        <v>692</v>
+      </c>
+      <c r="R45" s="2" t="s">
         <v>663</v>
-      </c>
-      <c r="N45" s="84" t="s">
-        <v>664</v>
-      </c>
-      <c r="P45" s="2" t="s">
-        <v>682</v>
-      </c>
-      <c r="Q45" s="2" t="s">
-        <v>694</v>
-      </c>
-      <c r="R45" s="2" t="s">
-        <v>665</v>
       </c>
       <c r="S45" s="2" t="s">
         <v>355</v>
       </c>
       <c r="T45" s="87" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="V45" s="2"/>
     </row>
     <row r="46" spans="1:22" ht="57" x14ac:dyDescent="0.45">
       <c r="B46" s="2" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>346</v>
       </c>
       <c r="D46" s="87" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="F46" s="84" t="s">
+        <v>662</v>
+      </c>
+      <c r="G46" s="2" t="s">
         <v>664</v>
       </c>
-      <c r="G46" s="2" t="s">
-        <v>666</v>
-      </c>
       <c r="J46" s="2" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="K46" s="2" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="L46" s="2" t="s">
         <v>346</v>
       </c>
       <c r="M46" s="87" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="N46" s="84" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="P46" s="2" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="Q46" s="2" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="R46" s="2" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="S46" s="2" t="s">
         <v>375</v>
       </c>
       <c r="T46" s="87" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="V46" s="2"/>
     </row>
     <row r="47" spans="1:22" ht="57" x14ac:dyDescent="0.45">
       <c r="B47" s="2" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>271</v>
       </c>
       <c r="D47" s="87" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="F47" s="84" t="s">
         <v>351</v>
       </c>
       <c r="G47" s="2" t="s">
+        <v>667</v>
+      </c>
+      <c r="J47" s="2" t="s">
+        <v>652</v>
+      </c>
+      <c r="K47" s="2" t="s">
+        <v>667</v>
+      </c>
+      <c r="L47" s="2" t="s">
+        <v>668</v>
+      </c>
+      <c r="M47" s="87" t="s">
         <v>669</v>
-      </c>
-      <c r="J47" s="2" t="s">
-        <v>654</v>
-      </c>
-      <c r="K47" s="2" t="s">
-        <v>669</v>
-      </c>
-      <c r="L47" s="2" t="s">
-        <v>670</v>
-      </c>
-      <c r="M47" s="87" t="s">
-        <v>671</v>
       </c>
       <c r="N47" s="84" t="s">
         <v>351</v>
       </c>
       <c r="P47" s="2" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="Q47" s="2" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="R47" s="2" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="S47" s="2" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="T47" s="87" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="V47" s="2"/>
     </row>
     <row r="48" spans="1:22" ht="57" x14ac:dyDescent="0.45">
       <c r="B48" s="2" t="s">
+        <v>672</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>677</v>
+      </c>
+      <c r="D48" s="87" t="s">
         <v>674</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>679</v>
-      </c>
-      <c r="D48" s="87" t="s">
-        <v>676</v>
       </c>
       <c r="F48" s="84" t="s">
         <v>351</v>
       </c>
       <c r="G48" s="2" t="s">
+        <v>672</v>
+      </c>
+      <c r="J48" s="2" t="s">
+        <v>652</v>
+      </c>
+      <c r="K48" s="2" t="s">
+        <v>672</v>
+      </c>
+      <c r="L48" s="2" t="s">
+        <v>673</v>
+      </c>
+      <c r="M48" s="87" t="s">
         <v>674</v>
-      </c>
-      <c r="J48" s="2" t="s">
-        <v>654</v>
-      </c>
-      <c r="K48" s="2" t="s">
-        <v>674</v>
-      </c>
-      <c r="L48" s="2" t="s">
-        <v>675</v>
-      </c>
-      <c r="M48" s="87" t="s">
-        <v>676</v>
       </c>
       <c r="N48" s="84" t="s">
         <v>351</v>
       </c>
       <c r="P48" s="2" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="Q48" s="2" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="R48" s="2" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="S48" s="2" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="T48" s="87" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="V48" s="2"/>
     </row>
     <row r="49" spans="1:22" s="97" customFormat="1" ht="99.75" x14ac:dyDescent="0.45">
       <c r="A49" s="96" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="B49" s="98" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="C49" t="s">
         <v>346</v>
       </c>
       <c r="D49" s="98" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="E49"/>
       <c r="F49"/>
@@ -9860,27 +9860,27 @@
         <v>351</v>
       </c>
       <c r="H49" s="98" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="I49" s="98"/>
       <c r="J49" s="94" t="s">
         <v>408</v>
       </c>
       <c r="K49" s="94" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="L49" s="94" t="s">
         <v>346</v>
       </c>
       <c r="M49" s="94" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="N49" s="94" t="s">
         <v>351</v>
       </c>
       <c r="O49" s="94"/>
       <c r="P49" s="94" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="Q49" s="95"/>
       <c r="R49" s="82" t="s">
@@ -9890,7 +9890,7 @@
         <v>375</v>
       </c>
       <c r="T49" s="82" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="V49"/>
     </row>
@@ -9960,7 +9960,7 @@
         <v>147</v>
       </c>
       <c r="E1" s="25" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="F1" s="9" t="s">
         <v>4</v>
@@ -9972,22 +9972,22 @@
         <v>335</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>626</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>627</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>628</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>629</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>630</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>631</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>632</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>633</v>
       </c>
     </row>
   </sheetData>
@@ -10045,7 +10045,7 @@
   <sheetData>
     <row r="1" spans="1:17" s="56" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A1" s="10" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>183</v>
@@ -10072,25 +10072,25 @@
         <v>329</v>
       </c>
       <c r="J1" s="11" t="s">
+        <v>633</v>
+      </c>
+      <c r="K1" s="11" t="s">
+        <v>626</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>634</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>635</v>
       </c>
-      <c r="K1" s="11" t="s">
-        <v>628</v>
-      </c>
-      <c r="L1" s="11" t="s">
+      <c r="N1" s="15" t="s">
         <v>636</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="15" t="s">
         <v>637</v>
       </c>
-      <c r="N1" s="15" t="s">
+      <c r="P1" s="1" t="s">
         <v>638</v>
-      </c>
-      <c r="O1" s="15" t="s">
-        <v>639</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>640</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>233</v>
@@ -10149,7 +10149,7 @@
   <sheetData>
     <row r="1" spans="1:13" s="57" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A1" s="60" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="B1" s="61" t="s">
         <v>183</v>
@@ -10161,10 +10161,10 @@
         <v>147</v>
       </c>
       <c r="E1" s="62" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="F1" s="63" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="G1" s="63" t="s">
         <v>4</v>
@@ -10173,19 +10173,19 @@
         <v>329</v>
       </c>
       <c r="I1" s="64" t="s">
+        <v>642</v>
+      </c>
+      <c r="J1" s="65" t="s">
+        <v>626</v>
+      </c>
+      <c r="K1" s="66" t="s">
+        <v>643</v>
+      </c>
+      <c r="L1" s="66" t="s">
+        <v>628</v>
+      </c>
+      <c r="M1" s="66" t="s">
         <v>644</v>
-      </c>
-      <c r="J1" s="65" t="s">
-        <v>628</v>
-      </c>
-      <c r="K1" s="66" t="s">
-        <v>645</v>
-      </c>
-      <c r="L1" s="66" t="s">
-        <v>630</v>
-      </c>
-      <c r="M1" s="66" t="s">
-        <v>646</v>
       </c>
     </row>
   </sheetData>
@@ -10243,7 +10243,7 @@
   <sheetData>
     <row r="1" spans="1:14" s="56" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A1" s="79" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="B1" s="75" t="s">
         <v>271</v>
@@ -10252,7 +10252,7 @@
         <v>147</v>
       </c>
       <c r="D1" s="76" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="E1" s="77" t="s">
         <v>4</v>
@@ -10261,16 +10261,16 @@
         <v>329</v>
       </c>
       <c r="G1" s="78" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="H1" s="78" t="s">
         <v>188</v>
       </c>
       <c r="I1" s="78" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="J1" s="78" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="K1" s="74" t="s">
         <v>297</v>
@@ -10336,7 +10336,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A1" s="10" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>313</v>
@@ -10348,7 +10348,7 @@
         <v>147</v>
       </c>
       <c r="E1" s="73" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="F1" s="63" t="s">
         <v>4</v>
@@ -10360,13 +10360,13 @@
         <v>335</v>
       </c>
       <c r="I1" s="11" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="J1" s="11" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="K1" s="11" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
     </row>
   </sheetData>

</xml_diff>